<commit_message>
Added mathematica plot and prepared measurement statistics
	new file:   exp3/data/collision.nb
	modified:   exp3/data/values.xlsx
</commit_message>
<xml_diff>
--- a/exp3/data/values.xlsx
+++ b/exp3/data/values.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="294" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="364" uniqueCount="30">
   <si>
     <t>Balls</t>
   </si>
@@ -92,12 +92,27 @@
   <si>
     <t>ball 3 vs ball 1</t>
   </si>
+  <si>
+    <t>Mean</t>
+  </si>
+  <si>
+    <t>Stdev</t>
+  </si>
+  <si>
+    <t>StdErrMean</t>
+  </si>
+  <si>
+    <t>a1</t>
+  </si>
+  <si>
+    <t>a2</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -105,8 +120,22 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -137,6 +166,17 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -147,17 +187,26 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="2"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="2" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="1" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="3">
+    <cellStyle name="20% - Akzent1" xfId="2" builtinId="30"/>
+    <cellStyle name="Gut" xfId="1" builtinId="26"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -450,24 +499,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A2:H279"/>
+  <dimension ref="A2:L282"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A129" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B146" activeCellId="1" sqref="S153 B146"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="K11" sqref="K11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="23" customWidth="1"/>
     <col min="7" max="7" width="18.28515625" customWidth="1"/>
+    <col min="11" max="12" width="11.42578125" style="7"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:11">
       <c r="B2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" spans="1:11">
       <c r="A3" s="1"/>
       <c r="B3" s="1" t="s">
         <v>1</v>
@@ -479,7 +529,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" spans="1:11">
       <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
@@ -493,7 +543,7 @@
         <v>1049</v>
       </c>
     </row>
-    <row r="5" spans="1:8">
+    <row r="5" spans="1:11">
       <c r="A5" s="1" t="s">
         <v>5</v>
       </c>
@@ -507,7 +557,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="9" spans="1:8">
+    <row r="9" spans="1:11">
       <c r="A9" s="4" t="s">
         <v>6</v>
       </c>
@@ -515,7 +565,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="1:8">
+    <row r="10" spans="1:11">
       <c r="B10" t="s">
         <v>9</v>
       </c>
@@ -525,8 +575,14 @@
       <c r="H10" s="2" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="11" spans="1:8">
+      <c r="J10" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="K10" s="8" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11">
       <c r="B11" t="s">
         <v>7</v>
       </c>
@@ -546,8 +602,16 @@
       <c r="H11" s="2">
         <v>34</v>
       </c>
-    </row>
-    <row r="12" spans="1:8">
+      <c r="J11">
+        <f>E14-E16</f>
+        <v>159</v>
+      </c>
+      <c r="K11" s="7">
+        <f>$C$18+H11-$C$5/2-$E$11</f>
+        <v>143</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11">
       <c r="B12" t="s">
         <v>10</v>
       </c>
@@ -557,8 +621,12 @@
       <c r="H12" s="2">
         <v>34</v>
       </c>
-    </row>
-    <row r="13" spans="1:8">
+      <c r="K12" s="7">
+        <f t="shared" ref="K12:K20" si="0">$C$18+H12-$C$5/2-$E$11</f>
+        <v>143</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11">
       <c r="B13" t="s">
         <v>11</v>
       </c>
@@ -568,8 +636,12 @@
       <c r="H13" s="2">
         <v>35</v>
       </c>
-    </row>
-    <row r="14" spans="1:8">
+      <c r="K13" s="7">
+        <f t="shared" si="0"/>
+        <v>144</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11">
       <c r="B14" t="s">
         <v>7</v>
       </c>
@@ -590,8 +662,12 @@
       <c r="H14" s="2">
         <v>35</v>
       </c>
-    </row>
-    <row r="15" spans="1:8">
+      <c r="K14" s="7">
+        <f t="shared" si="0"/>
+        <v>144</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11">
       <c r="B15" t="s">
         <v>12</v>
       </c>
@@ -601,8 +677,12 @@
       <c r="H15" s="2">
         <v>36</v>
       </c>
-    </row>
-    <row r="16" spans="1:8">
+      <c r="K15" s="7">
+        <f t="shared" si="0"/>
+        <v>145</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11">
       <c r="B16" t="s">
         <v>7</v>
       </c>
@@ -622,16 +702,24 @@
       <c r="H16" s="2">
         <v>34</v>
       </c>
-    </row>
-    <row r="17" spans="1:8">
+      <c r="K16" s="7">
+        <f t="shared" si="0"/>
+        <v>143</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12">
       <c r="G17" s="2">
         <v>7</v>
       </c>
       <c r="H17" s="2">
         <v>34</v>
       </c>
-    </row>
-    <row r="18" spans="1:8">
+      <c r="K17" s="7">
+        <f t="shared" si="0"/>
+        <v>143</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12">
       <c r="B18" t="s">
         <v>16</v>
       </c>
@@ -644,29 +732,41 @@
       <c r="H18" s="2">
         <v>34</v>
       </c>
-    </row>
-    <row r="19" spans="1:8">
+      <c r="K18" s="7">
+        <f t="shared" si="0"/>
+        <v>143</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12">
       <c r="G19" s="2">
         <v>9</v>
       </c>
       <c r="H19" s="2">
         <v>34</v>
       </c>
-    </row>
-    <row r="20" spans="1:8">
+      <c r="K19" s="7">
+        <f t="shared" si="0"/>
+        <v>143</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12">
       <c r="G20" s="2">
         <v>10</v>
       </c>
       <c r="H20" s="2">
         <v>34</v>
       </c>
-    </row>
-    <row r="21" spans="1:8">
+      <c r="K20" s="7">
+        <f t="shared" si="0"/>
+        <v>143</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12">
       <c r="B21" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:8">
+    <row r="22" spans="1:12">
       <c r="A22" s="1"/>
       <c r="B22" s="1" t="s">
         <v>1</v>
@@ -677,8 +777,17 @@
       <c r="D22" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="23" spans="1:8">
+      <c r="J22" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="K22" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="L22" s="9" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12">
       <c r="A23" s="1" t="s">
         <v>4</v>
       </c>
@@ -691,8 +800,20 @@
       <c r="D23" s="1">
         <v>1049</v>
       </c>
-    </row>
-    <row r="24" spans="1:8">
+      <c r="J23">
+        <f>AVERAGE(K11:K20)</f>
+        <v>143.4</v>
+      </c>
+      <c r="K23" s="7">
+        <f>STDEV(K11:K20)</f>
+        <v>0.69920589877963857</v>
+      </c>
+      <c r="L23" s="7">
+        <f>K23/SQRT(COUNT(K11:K20))</f>
+        <v>0.22110831935688041</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12">
       <c r="A24" s="1" t="s">
         <v>5</v>
       </c>
@@ -706,7 +827,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="28" spans="1:8">
+    <row r="28" spans="1:12">
       <c r="A28" s="4" t="s">
         <v>6</v>
       </c>
@@ -714,7 +835,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="29" spans="1:8">
+    <row r="29" spans="1:12">
       <c r="B29" t="s">
         <v>9</v>
       </c>
@@ -724,8 +845,14 @@
       <c r="H29" s="2" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="30" spans="1:8">
+      <c r="J29" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="K29" s="8" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12">
       <c r="B30" t="s">
         <v>7</v>
       </c>
@@ -745,8 +872,16 @@
       <c r="H30" s="2">
         <v>36</v>
       </c>
-    </row>
-    <row r="31" spans="1:8">
+      <c r="J30">
+        <f>E33-E35</f>
+        <v>159</v>
+      </c>
+      <c r="K30" s="7">
+        <f>$C$37+H30-$C$24/2-$E$30</f>
+        <v>95</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12">
       <c r="B31" t="s">
         <v>10</v>
       </c>
@@ -756,8 +891,12 @@
       <c r="H31" s="2">
         <v>38</v>
       </c>
-    </row>
-    <row r="32" spans="1:8">
+      <c r="K31" s="7">
+        <f t="shared" ref="K31:K39" si="1">$C$37+H31-$C$24/2-$E$30</f>
+        <v>97</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12">
       <c r="B32" t="s">
         <v>11</v>
       </c>
@@ -767,8 +906,12 @@
       <c r="H32" s="2">
         <v>40</v>
       </c>
-    </row>
-    <row r="33" spans="1:8">
+      <c r="K32" s="7">
+        <f t="shared" si="1"/>
+        <v>99</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12">
       <c r="B33" t="s">
         <v>7</v>
       </c>
@@ -789,8 +932,12 @@
       <c r="H33" s="2">
         <v>36</v>
       </c>
-    </row>
-    <row r="34" spans="1:8">
+      <c r="K33" s="7">
+        <f t="shared" si="1"/>
+        <v>95</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12">
       <c r="B34" t="s">
         <v>12</v>
       </c>
@@ -800,8 +947,12 @@
       <c r="H34" s="2">
         <v>37</v>
       </c>
-    </row>
-    <row r="35" spans="1:8">
+      <c r="K34" s="7">
+        <f t="shared" si="1"/>
+        <v>96</v>
+      </c>
+    </row>
+    <row r="35" spans="1:12">
       <c r="B35" t="s">
         <v>7</v>
       </c>
@@ -821,16 +972,24 @@
       <c r="H35" s="2">
         <v>36</v>
       </c>
-    </row>
-    <row r="36" spans="1:8">
+      <c r="K35" s="7">
+        <f t="shared" si="1"/>
+        <v>95</v>
+      </c>
+    </row>
+    <row r="36" spans="1:12">
       <c r="G36" s="2">
         <v>7</v>
       </c>
       <c r="H36" s="2">
         <v>35</v>
       </c>
-    </row>
-    <row r="37" spans="1:8">
+      <c r="K36" s="7">
+        <f t="shared" si="1"/>
+        <v>94</v>
+      </c>
+    </row>
+    <row r="37" spans="1:12">
       <c r="B37" t="s">
         <v>16</v>
       </c>
@@ -843,29 +1002,50 @@
       <c r="H37" s="2">
         <v>35</v>
       </c>
-    </row>
-    <row r="38" spans="1:8">
+      <c r="K37" s="7">
+        <f t="shared" si="1"/>
+        <v>94</v>
+      </c>
+    </row>
+    <row r="38" spans="1:12">
       <c r="G38" s="2">
         <v>9</v>
       </c>
       <c r="H38" s="2">
         <v>36</v>
       </c>
-    </row>
-    <row r="39" spans="1:8">
+      <c r="K38" s="7">
+        <f t="shared" si="1"/>
+        <v>95</v>
+      </c>
+    </row>
+    <row r="39" spans="1:12">
       <c r="G39" s="2">
         <v>10</v>
       </c>
       <c r="H39" s="2">
         <v>36</v>
       </c>
-    </row>
-    <row r="41" spans="1:8">
+      <c r="K39" s="7">
+        <f t="shared" si="1"/>
+        <v>95</v>
+      </c>
+    </row>
+    <row r="41" spans="1:12">
       <c r="B41" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="42" spans="1:8">
+      <c r="J41" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="K41" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="L41" s="9" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="42" spans="1:12">
       <c r="A42" s="1"/>
       <c r="B42" s="1" t="s">
         <v>1</v>
@@ -876,8 +1056,20 @@
       <c r="D42" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="43" spans="1:8">
+      <c r="J42">
+        <f>AVERAGE(K30:K39)</f>
+        <v>95.5</v>
+      </c>
+      <c r="K42" s="7">
+        <f>STDEV(K30:K39)</f>
+        <v>1.509230856356236</v>
+      </c>
+      <c r="L42" s="7">
+        <f>K42/SQRT(COUNT(K30:K39))</f>
+        <v>0.47726070210921173</v>
+      </c>
+    </row>
+    <row r="43" spans="1:12">
       <c r="A43" s="1" t="s">
         <v>4</v>
       </c>
@@ -890,8 +1082,10 @@
       <c r="D43" s="1">
         <v>1049</v>
       </c>
-    </row>
-    <row r="44" spans="1:8">
+      <c r="K43"/>
+      <c r="L43"/>
+    </row>
+    <row r="44" spans="1:12">
       <c r="A44" s="1" t="s">
         <v>5</v>
       </c>
@@ -904,16 +1098,32 @@
       <c r="D44" s="1">
         <v>65</v>
       </c>
-    </row>
-    <row r="48" spans="1:8">
+      <c r="K44"/>
+      <c r="L44"/>
+    </row>
+    <row r="45" spans="1:12">
+      <c r="K45"/>
+      <c r="L45"/>
+    </row>
+    <row r="46" spans="1:12">
+      <c r="K46"/>
+      <c r="L46"/>
+    </row>
+    <row r="47" spans="1:12">
+      <c r="K47"/>
+      <c r="L47"/>
+    </row>
+    <row r="48" spans="1:12">
       <c r="A48" s="4" t="s">
         <v>18</v>
       </c>
       <c r="B48" s="4" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="49" spans="1:8">
+      <c r="K48"/>
+      <c r="L48"/>
+    </row>
+    <row r="49" spans="1:12">
       <c r="B49" t="s">
         <v>19</v>
       </c>
@@ -923,8 +1133,14 @@
       <c r="H49" s="2" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="50" spans="1:8">
+      <c r="J49" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="K49" s="8" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="50" spans="1:12">
       <c r="B50" t="s">
         <v>7</v>
       </c>
@@ -944,8 +1160,16 @@
       <c r="H50" s="2">
         <v>39</v>
       </c>
-    </row>
-    <row r="51" spans="1:8">
+      <c r="J50">
+        <f>E53-E55</f>
+        <v>158</v>
+      </c>
+      <c r="K50" s="7">
+        <f>$C$57+H50-$D$44/2-$E$50</f>
+        <v>106</v>
+      </c>
+    </row>
+    <row r="51" spans="1:12">
       <c r="B51" t="s">
         <v>10</v>
       </c>
@@ -955,8 +1179,12 @@
       <c r="H51" s="2">
         <v>39</v>
       </c>
-    </row>
-    <row r="52" spans="1:8">
+      <c r="K51" s="7">
+        <f t="shared" ref="K51:K59" si="2">$C$57+H51-$D$44/2-$E$50</f>
+        <v>106</v>
+      </c>
+    </row>
+    <row r="52" spans="1:12">
       <c r="B52" t="s">
         <v>11</v>
       </c>
@@ -966,8 +1194,12 @@
       <c r="H52" s="2">
         <v>38</v>
       </c>
-    </row>
-    <row r="53" spans="1:8">
+      <c r="K52" s="7">
+        <f t="shared" si="2"/>
+        <v>105</v>
+      </c>
+    </row>
+    <row r="53" spans="1:12">
       <c r="B53" t="s">
         <v>7</v>
       </c>
@@ -988,8 +1220,12 @@
       <c r="H53" s="2">
         <v>38.5</v>
       </c>
-    </row>
-    <row r="54" spans="1:8">
+      <c r="K53" s="7">
+        <f t="shared" si="2"/>
+        <v>105.5</v>
+      </c>
+    </row>
+    <row r="54" spans="1:12">
       <c r="B54" t="s">
         <v>12</v>
       </c>
@@ -999,8 +1235,12 @@
       <c r="H54" s="2">
         <v>38.5</v>
       </c>
-    </row>
-    <row r="55" spans="1:8">
+      <c r="K54" s="7">
+        <f t="shared" si="2"/>
+        <v>105.5</v>
+      </c>
+    </row>
+    <row r="55" spans="1:12">
       <c r="B55" t="s">
         <v>7</v>
       </c>
@@ -1020,16 +1260,24 @@
       <c r="H55" s="2">
         <v>38.5</v>
       </c>
-    </row>
-    <row r="56" spans="1:8">
+      <c r="K55" s="7">
+        <f t="shared" si="2"/>
+        <v>105.5</v>
+      </c>
+    </row>
+    <row r="56" spans="1:12">
       <c r="G56" s="2">
         <v>7</v>
       </c>
       <c r="H56" s="2">
         <v>38</v>
       </c>
-    </row>
-    <row r="57" spans="1:8">
+      <c r="K56" s="7">
+        <f t="shared" si="2"/>
+        <v>105</v>
+      </c>
+    </row>
+    <row r="57" spans="1:12">
       <c r="B57" t="s">
         <v>16</v>
       </c>
@@ -1042,29 +1290,50 @@
       <c r="H57" s="2">
         <v>37.5</v>
       </c>
-    </row>
-    <row r="58" spans="1:8">
+      <c r="K57" s="7">
+        <f t="shared" si="2"/>
+        <v>104.5</v>
+      </c>
+    </row>
+    <row r="58" spans="1:12">
       <c r="G58" s="2">
         <v>9</v>
       </c>
       <c r="H58" s="2">
         <v>39</v>
       </c>
-    </row>
-    <row r="59" spans="1:8">
+      <c r="K58" s="7">
+        <f t="shared" si="2"/>
+        <v>106</v>
+      </c>
+    </row>
+    <row r="59" spans="1:12">
       <c r="G59" s="2">
         <v>10</v>
       </c>
       <c r="H59" s="2">
         <v>39</v>
       </c>
-    </row>
-    <row r="61" spans="1:8">
+      <c r="K59" s="7">
+        <f t="shared" si="2"/>
+        <v>106</v>
+      </c>
+    </row>
+    <row r="61" spans="1:12">
       <c r="B61" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="62" spans="1:8">
+      <c r="J61" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="K61" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="L61" s="9" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="62" spans="1:12">
       <c r="A62" s="1"/>
       <c r="B62" s="1" t="s">
         <v>1</v>
@@ -1075,8 +1344,20 @@
       <c r="D62" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="63" spans="1:8">
+      <c r="J62">
+        <f>AVERAGE(K50:K59)</f>
+        <v>105.5</v>
+      </c>
+      <c r="K62" s="7">
+        <f>STDEV(K50:K59)</f>
+        <v>0.52704627669472992</v>
+      </c>
+      <c r="L62" s="7">
+        <f>K62/SQRT(COUNT(K50:K59))</f>
+        <v>0.16666666666666666</v>
+      </c>
+    </row>
+    <row r="63" spans="1:12">
       <c r="A63" s="1" t="s">
         <v>4</v>
       </c>
@@ -1089,8 +1370,10 @@
       <c r="D63" s="1">
         <v>1049</v>
       </c>
-    </row>
-    <row r="64" spans="1:8">
+      <c r="K63"/>
+      <c r="L63"/>
+    </row>
+    <row r="64" spans="1:12">
       <c r="A64" s="1" t="s">
         <v>5</v>
       </c>
@@ -1103,16 +1386,32 @@
       <c r="D64" s="1">
         <v>65</v>
       </c>
-    </row>
-    <row r="68" spans="1:8">
+      <c r="K64"/>
+      <c r="L64"/>
+    </row>
+    <row r="65" spans="1:12">
+      <c r="K65"/>
+      <c r="L65"/>
+    </row>
+    <row r="66" spans="1:12">
+      <c r="K66"/>
+      <c r="L66"/>
+    </row>
+    <row r="67" spans="1:12">
+      <c r="K67"/>
+      <c r="L67"/>
+    </row>
+    <row r="68" spans="1:12">
       <c r="A68" s="4" t="s">
         <v>18</v>
       </c>
       <c r="B68" s="4" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="69" spans="1:8">
+      <c r="K68"/>
+      <c r="L68"/>
+    </row>
+    <row r="69" spans="1:12">
       <c r="B69" t="s">
         <v>19</v>
       </c>
@@ -1122,8 +1421,14 @@
       <c r="H69" s="2" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="70" spans="1:8">
+      <c r="J69" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="K69" s="8" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="70" spans="1:12">
       <c r="B70" t="s">
         <v>7</v>
       </c>
@@ -1143,8 +1448,16 @@
       <c r="H70" s="2">
         <v>31</v>
       </c>
-    </row>
-    <row r="71" spans="1:8">
+      <c r="J70">
+        <f>E73-E75</f>
+        <v>158</v>
+      </c>
+      <c r="K70" s="7">
+        <f>$C$77+H70-$D$64/2-$E$70</f>
+        <v>78</v>
+      </c>
+    </row>
+    <row r="71" spans="1:12">
       <c r="B71" t="s">
         <v>10</v>
       </c>
@@ -1154,8 +1467,12 @@
       <c r="H71" s="2">
         <v>30</v>
       </c>
-    </row>
-    <row r="72" spans="1:8">
+      <c r="K71" s="7">
+        <f t="shared" ref="K71:K79" si="3">$C$77+H71-$D$64/2-$E$70</f>
+        <v>77</v>
+      </c>
+    </row>
+    <row r="72" spans="1:12">
       <c r="B72" t="s">
         <v>11</v>
       </c>
@@ -1165,8 +1482,12 @@
       <c r="H72" s="2">
         <v>30</v>
       </c>
-    </row>
-    <row r="73" spans="1:8">
+      <c r="K72" s="7">
+        <f t="shared" si="3"/>
+        <v>77</v>
+      </c>
+    </row>
+    <row r="73" spans="1:12">
       <c r="B73" t="s">
         <v>7</v>
       </c>
@@ -1187,8 +1508,12 @@
       <c r="H73" s="2">
         <v>29</v>
       </c>
-    </row>
-    <row r="74" spans="1:8">
+      <c r="K73" s="7">
+        <f t="shared" si="3"/>
+        <v>76</v>
+      </c>
+    </row>
+    <row r="74" spans="1:12">
       <c r="B74" t="s">
         <v>12</v>
       </c>
@@ -1198,8 +1523,12 @@
       <c r="H74" s="2">
         <v>29.5</v>
       </c>
-    </row>
-    <row r="75" spans="1:8">
+      <c r="K74" s="7">
+        <f t="shared" si="3"/>
+        <v>76.5</v>
+      </c>
+    </row>
+    <row r="75" spans="1:12">
       <c r="B75" t="s">
         <v>7</v>
       </c>
@@ -1219,16 +1548,24 @@
       <c r="H75" s="2">
         <v>29</v>
       </c>
-    </row>
-    <row r="76" spans="1:8">
+      <c r="K75" s="7">
+        <f t="shared" si="3"/>
+        <v>76</v>
+      </c>
+    </row>
+    <row r="76" spans="1:12">
       <c r="G76" s="2">
         <v>7</v>
       </c>
       <c r="H76" s="2">
         <v>30</v>
       </c>
-    </row>
-    <row r="77" spans="1:8">
+      <c r="K76" s="7">
+        <f t="shared" si="3"/>
+        <v>77</v>
+      </c>
+    </row>
+    <row r="77" spans="1:12">
       <c r="B77" t="s">
         <v>16</v>
       </c>
@@ -1241,29 +1578,50 @@
       <c r="H77" s="2">
         <v>29.5</v>
       </c>
-    </row>
-    <row r="78" spans="1:8">
+      <c r="K77" s="7">
+        <f t="shared" si="3"/>
+        <v>76.5</v>
+      </c>
+    </row>
+    <row r="78" spans="1:12">
       <c r="G78" s="2">
         <v>9</v>
       </c>
       <c r="H78" s="2">
         <v>30</v>
       </c>
-    </row>
-    <row r="79" spans="1:8">
+      <c r="K78" s="7">
+        <f t="shared" si="3"/>
+        <v>77</v>
+      </c>
+    </row>
+    <row r="79" spans="1:12">
       <c r="G79" s="2">
         <v>10</v>
       </c>
       <c r="H79" s="2">
         <v>29</v>
       </c>
-    </row>
-    <row r="81" spans="1:8">
+      <c r="K79" s="7">
+        <f t="shared" si="3"/>
+        <v>76</v>
+      </c>
+    </row>
+    <row r="81" spans="1:12">
       <c r="B81" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="82" spans="1:8">
+      <c r="J81" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="K81" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="L81" s="9" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="82" spans="1:12">
       <c r="A82" s="1"/>
       <c r="B82" s="1" t="s">
         <v>1</v>
@@ -1274,8 +1632,20 @@
       <c r="D82" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="83" spans="1:8">
+      <c r="J82">
+        <f>AVERAGE(K70:K79)</f>
+        <v>76.7</v>
+      </c>
+      <c r="K82" s="7">
+        <f>STDEV(K70:K79)</f>
+        <v>0.6324555320335481</v>
+      </c>
+      <c r="L82" s="7">
+        <f>K82/SQRT(COUNT(K70:K79))</f>
+        <v>0.19999999999995957</v>
+      </c>
+    </row>
+    <row r="83" spans="1:12">
       <c r="A83" s="1" t="s">
         <v>4</v>
       </c>
@@ -1288,8 +1658,10 @@
       <c r="D83" s="1">
         <v>1049</v>
       </c>
-    </row>
-    <row r="84" spans="1:8">
+      <c r="K83"/>
+      <c r="L83"/>
+    </row>
+    <row r="84" spans="1:12">
       <c r="A84" s="1" t="s">
         <v>5</v>
       </c>
@@ -1302,16 +1674,32 @@
       <c r="D84" s="1">
         <v>65</v>
       </c>
-    </row>
-    <row r="88" spans="1:8">
+      <c r="K84"/>
+      <c r="L84"/>
+    </row>
+    <row r="85" spans="1:12">
+      <c r="K85"/>
+      <c r="L85"/>
+    </row>
+    <row r="86" spans="1:12">
+      <c r="K86"/>
+      <c r="L86"/>
+    </row>
+    <row r="87" spans="1:12">
+      <c r="K87"/>
+      <c r="L87"/>
+    </row>
+    <row r="88" spans="1:12">
       <c r="A88" s="4" t="s">
         <v>20</v>
       </c>
       <c r="B88" s="4" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="89" spans="1:8">
+      <c r="K88"/>
+      <c r="L88"/>
+    </row>
+    <row r="89" spans="1:12">
       <c r="B89" t="s">
         <v>10</v>
       </c>
@@ -1321,8 +1709,14 @@
       <c r="H89" s="2" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="90" spans="1:8">
+      <c r="J89" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="K89" s="8" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="90" spans="1:12">
       <c r="B90" t="s">
         <v>7</v>
       </c>
@@ -1342,8 +1736,16 @@
       <c r="H90" s="2">
         <v>18</v>
       </c>
-    </row>
-    <row r="91" spans="1:8">
+      <c r="J90">
+        <f>E93-E95</f>
+        <v>86</v>
+      </c>
+      <c r="K90" s="7">
+        <f>$C$97+H90-$B$84/2-$E$90</f>
+        <v>164</v>
+      </c>
+    </row>
+    <row r="91" spans="1:12">
       <c r="B91" t="s">
         <v>9</v>
       </c>
@@ -1353,8 +1755,12 @@
       <c r="H91" s="2">
         <v>19</v>
       </c>
-    </row>
-    <row r="92" spans="1:8">
+      <c r="K91" s="7">
+        <f t="shared" ref="K91:K99" si="4">$C$97+H91-$B$84/2-$E$90</f>
+        <v>165</v>
+      </c>
+    </row>
+    <row r="92" spans="1:12">
       <c r="B92" t="s">
         <v>11</v>
       </c>
@@ -1364,8 +1770,12 @@
       <c r="H92" s="2">
         <v>19</v>
       </c>
-    </row>
-    <row r="93" spans="1:8">
+      <c r="K92" s="7">
+        <f t="shared" si="4"/>
+        <v>165</v>
+      </c>
+    </row>
+    <row r="93" spans="1:12">
       <c r="B93" t="s">
         <v>7</v>
       </c>
@@ -1386,8 +1796,12 @@
       <c r="H93" s="2">
         <v>18.5</v>
       </c>
-    </row>
-    <row r="94" spans="1:8">
+      <c r="K93" s="7">
+        <f t="shared" si="4"/>
+        <v>164.5</v>
+      </c>
+    </row>
+    <row r="94" spans="1:12">
       <c r="B94" t="s">
         <v>12</v>
       </c>
@@ -1397,8 +1811,12 @@
       <c r="H94" s="2">
         <v>18</v>
       </c>
-    </row>
-    <row r="95" spans="1:8">
+      <c r="K94" s="7">
+        <f t="shared" si="4"/>
+        <v>164</v>
+      </c>
+    </row>
+    <row r="95" spans="1:12">
       <c r="B95" t="s">
         <v>7</v>
       </c>
@@ -1418,16 +1836,24 @@
       <c r="H95" s="2">
         <v>18</v>
       </c>
-    </row>
-    <row r="96" spans="1:8">
+      <c r="K95" s="7">
+        <f t="shared" si="4"/>
+        <v>164</v>
+      </c>
+    </row>
+    <row r="96" spans="1:12">
       <c r="G96" s="2">
         <v>7</v>
       </c>
       <c r="H96" s="2">
         <v>18.5</v>
       </c>
-    </row>
-    <row r="97" spans="1:8">
+      <c r="K96" s="7">
+        <f t="shared" si="4"/>
+        <v>164.5</v>
+      </c>
+    </row>
+    <row r="97" spans="1:12">
       <c r="B97" t="s">
         <v>16</v>
       </c>
@@ -1440,29 +1866,50 @@
       <c r="H97" s="2">
         <v>18.5</v>
       </c>
-    </row>
-    <row r="98" spans="1:8">
+      <c r="K97" s="7">
+        <f t="shared" si="4"/>
+        <v>164.5</v>
+      </c>
+    </row>
+    <row r="98" spans="1:12">
       <c r="G98" s="2">
         <v>9</v>
       </c>
       <c r="H98" s="2">
         <v>19</v>
       </c>
-    </row>
-    <row r="99" spans="1:8">
+      <c r="K98" s="7">
+        <f t="shared" si="4"/>
+        <v>165</v>
+      </c>
+    </row>
+    <row r="99" spans="1:12">
       <c r="G99" s="2">
         <v>10</v>
       </c>
       <c r="H99" s="2">
         <v>19</v>
       </c>
-    </row>
-    <row r="101" spans="1:8">
+      <c r="K99" s="7">
+        <f t="shared" si="4"/>
+        <v>165</v>
+      </c>
+    </row>
+    <row r="101" spans="1:12">
       <c r="B101" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="102" spans="1:8">
+      <c r="J101" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="K101" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="L101" s="9" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="102" spans="1:12">
       <c r="A102" s="1"/>
       <c r="B102" s="1" t="s">
         <v>1</v>
@@ -1473,8 +1920,20 @@
       <c r="D102" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="103" spans="1:8">
+      <c r="J102">
+        <f>AVERAGE(K90:K99)</f>
+        <v>164.55</v>
+      </c>
+      <c r="K102" s="7">
+        <f>STDEV(K90:K99)</f>
+        <v>0.43779751788250199</v>
+      </c>
+      <c r="L102" s="7">
+        <f>K102/SQRT(COUNT(K90:K99))</f>
+        <v>0.13844373104770025</v>
+      </c>
+    </row>
+    <row r="103" spans="1:12">
       <c r="A103" s="1" t="s">
         <v>4</v>
       </c>
@@ -1487,8 +1946,10 @@
       <c r="D103" s="1">
         <v>1049</v>
       </c>
-    </row>
-    <row r="104" spans="1:8">
+      <c r="K103"/>
+      <c r="L103"/>
+    </row>
+    <row r="104" spans="1:12">
       <c r="A104" s="1" t="s">
         <v>5</v>
       </c>
@@ -1501,16 +1962,32 @@
       <c r="D104" s="1">
         <v>65</v>
       </c>
-    </row>
-    <row r="108" spans="1:8">
+      <c r="K104"/>
+      <c r="L104"/>
+    </row>
+    <row r="105" spans="1:12">
+      <c r="K105"/>
+      <c r="L105"/>
+    </row>
+    <row r="106" spans="1:12">
+      <c r="K106"/>
+      <c r="L106"/>
+    </row>
+    <row r="107" spans="1:12">
+      <c r="K107"/>
+      <c r="L107"/>
+    </row>
+    <row r="108" spans="1:12">
       <c r="A108" s="4" t="s">
         <v>20</v>
       </c>
       <c r="B108" s="4" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="109" spans="1:8">
+      <c r="K108"/>
+      <c r="L108"/>
+    </row>
+    <row r="109" spans="1:12">
       <c r="B109" t="s">
         <v>10</v>
       </c>
@@ -1520,8 +1997,14 @@
       <c r="H109" s="2" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="110" spans="1:8">
+      <c r="J109" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="K109" s="8" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="110" spans="1:12">
       <c r="B110" t="s">
         <v>7</v>
       </c>
@@ -1541,8 +2024,16 @@
       <c r="H110" s="2">
         <v>20</v>
       </c>
-    </row>
-    <row r="111" spans="1:8">
+      <c r="J110">
+        <f>E113-E115</f>
+        <v>86</v>
+      </c>
+      <c r="K110" s="7">
+        <f>$C$117+H110-$B$104/2-$E$110</f>
+        <v>106</v>
+      </c>
+    </row>
+    <row r="111" spans="1:12">
       <c r="B111" t="s">
         <v>9</v>
       </c>
@@ -1552,8 +2043,12 @@
       <c r="H111" s="2">
         <v>20.5</v>
       </c>
-    </row>
-    <row r="112" spans="1:8">
+      <c r="K111" s="7">
+        <f t="shared" ref="K111:K119" si="5">$C$117+H111-$B$104/2-$E$110</f>
+        <v>106.5</v>
+      </c>
+    </row>
+    <row r="112" spans="1:12">
       <c r="B112" t="s">
         <v>11</v>
       </c>
@@ -1563,8 +2058,12 @@
       <c r="H112" s="2">
         <v>20.5</v>
       </c>
-    </row>
-    <row r="113" spans="1:8">
+      <c r="K112" s="7">
+        <f t="shared" si="5"/>
+        <v>106.5</v>
+      </c>
+    </row>
+    <row r="113" spans="1:12">
       <c r="B113" t="s">
         <v>7</v>
       </c>
@@ -1585,8 +2084,12 @@
       <c r="H113" s="2">
         <v>20</v>
       </c>
-    </row>
-    <row r="114" spans="1:8">
+      <c r="K113" s="7">
+        <f t="shared" si="5"/>
+        <v>106</v>
+      </c>
+    </row>
+    <row r="114" spans="1:12">
       <c r="B114" t="s">
         <v>12</v>
       </c>
@@ -1596,8 +2099,12 @@
       <c r="H114" s="2">
         <v>20</v>
       </c>
-    </row>
-    <row r="115" spans="1:8">
+      <c r="K114" s="7">
+        <f t="shared" si="5"/>
+        <v>106</v>
+      </c>
+    </row>
+    <row r="115" spans="1:12">
       <c r="B115" t="s">
         <v>7</v>
       </c>
@@ -1617,16 +2124,24 @@
       <c r="H115" s="2">
         <v>23</v>
       </c>
-    </row>
-    <row r="116" spans="1:8">
+      <c r="K115" s="7">
+        <f t="shared" si="5"/>
+        <v>109</v>
+      </c>
+    </row>
+    <row r="116" spans="1:12">
       <c r="G116" s="2">
         <v>7</v>
       </c>
       <c r="H116" s="2">
         <v>23</v>
       </c>
-    </row>
-    <row r="117" spans="1:8">
+      <c r="K116" s="7">
+        <f t="shared" si="5"/>
+        <v>109</v>
+      </c>
+    </row>
+    <row r="117" spans="1:12">
       <c r="B117" t="s">
         <v>16</v>
       </c>
@@ -1639,29 +2154,50 @@
       <c r="H117" s="2">
         <v>21.5</v>
       </c>
-    </row>
-    <row r="118" spans="1:8">
+      <c r="K117" s="7">
+        <f t="shared" si="5"/>
+        <v>107.5</v>
+      </c>
+    </row>
+    <row r="118" spans="1:12">
       <c r="G118" s="2">
         <v>9</v>
       </c>
       <c r="H118" s="2">
         <v>23</v>
       </c>
-    </row>
-    <row r="119" spans="1:8">
+      <c r="K118" s="7">
+        <f t="shared" si="5"/>
+        <v>109</v>
+      </c>
+    </row>
+    <row r="119" spans="1:12">
       <c r="G119" s="2">
         <v>10</v>
       </c>
       <c r="H119" s="2">
         <v>22</v>
       </c>
-    </row>
-    <row r="121" spans="1:8">
+      <c r="K119" s="7">
+        <f t="shared" si="5"/>
+        <v>108</v>
+      </c>
+    </row>
+    <row r="121" spans="1:12">
       <c r="B121" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="122" spans="1:8">
+      <c r="J121" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="K121" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="L121" s="9" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="122" spans="1:12">
       <c r="A122" s="1"/>
       <c r="B122" s="1" t="s">
         <v>1</v>
@@ -1672,8 +2208,20 @@
       <c r="D122" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="123" spans="1:8">
+      <c r="J122">
+        <f>AVERAGE(K110:K119)</f>
+        <v>107.35</v>
+      </c>
+      <c r="K122" s="7">
+        <f>STDEV(K110:K119)</f>
+        <v>1.3133925536561235</v>
+      </c>
+      <c r="L122" s="7">
+        <f>K122/SQRT(COUNT(K110:K119))</f>
+        <v>0.41533119314582584</v>
+      </c>
+    </row>
+    <row r="123" spans="1:12">
       <c r="A123" s="1" t="s">
         <v>4</v>
       </c>
@@ -1686,8 +2234,10 @@
       <c r="D123" s="1">
         <v>1049</v>
       </c>
-    </row>
-    <row r="124" spans="1:8">
+      <c r="K123"/>
+      <c r="L123"/>
+    </row>
+    <row r="124" spans="1:12">
       <c r="A124" s="1" t="s">
         <v>5</v>
       </c>
@@ -1700,16 +2250,32 @@
       <c r="D124" s="1">
         <v>65</v>
       </c>
-    </row>
-    <row r="128" spans="1:8">
+      <c r="K124"/>
+      <c r="L124"/>
+    </row>
+    <row r="125" spans="1:12">
+      <c r="K125"/>
+      <c r="L125"/>
+    </row>
+    <row r="126" spans="1:12">
+      <c r="K126"/>
+      <c r="L126"/>
+    </row>
+    <row r="127" spans="1:12">
+      <c r="K127"/>
+      <c r="L127"/>
+    </row>
+    <row r="128" spans="1:12">
       <c r="A128" s="4" t="s">
         <v>21</v>
       </c>
       <c r="B128" s="4" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="129" spans="1:8">
+      <c r="K128"/>
+      <c r="L128"/>
+    </row>
+    <row r="129" spans="1:12">
       <c r="B129" t="s">
         <v>9</v>
       </c>
@@ -1719,8 +2285,14 @@
       <c r="H129" s="2" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="130" spans="1:8">
+      <c r="J129" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="K129" s="8" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="130" spans="1:12">
       <c r="B130" t="s">
         <v>7</v>
       </c>
@@ -1740,8 +2312,16 @@
       <c r="H130" s="2">
         <v>29</v>
       </c>
-    </row>
-    <row r="131" spans="1:8">
+      <c r="J130">
+        <f>E133-E135</f>
+        <v>95</v>
+      </c>
+      <c r="K130" s="7">
+        <f>$C$137+H130-$C$124/2-$E$130</f>
+        <v>142</v>
+      </c>
+    </row>
+    <row r="131" spans="1:12">
       <c r="B131" t="s">
         <v>9</v>
       </c>
@@ -1751,8 +2331,12 @@
       <c r="H131" s="2">
         <v>30</v>
       </c>
-    </row>
-    <row r="132" spans="1:8">
+      <c r="K131" s="7">
+        <f t="shared" ref="K131:K139" si="6">$C$137+H131-$C$124/2-$E$130</f>
+        <v>143</v>
+      </c>
+    </row>
+    <row r="132" spans="1:12">
       <c r="B132" t="s">
         <v>11</v>
       </c>
@@ -1762,8 +2346,12 @@
       <c r="H132" s="2">
         <v>30</v>
       </c>
-    </row>
-    <row r="133" spans="1:8">
+      <c r="K132" s="7">
+        <f t="shared" si="6"/>
+        <v>143</v>
+      </c>
+    </row>
+    <row r="133" spans="1:12">
       <c r="B133" t="s">
         <v>7</v>
       </c>
@@ -1784,8 +2372,12 @@
       <c r="H133" s="2">
         <v>30</v>
       </c>
-    </row>
-    <row r="134" spans="1:8">
+      <c r="K133" s="7">
+        <f t="shared" si="6"/>
+        <v>143</v>
+      </c>
+    </row>
+    <row r="134" spans="1:12">
       <c r="B134" t="s">
         <v>12</v>
       </c>
@@ -1795,8 +2387,12 @@
       <c r="H134" s="2">
         <v>30</v>
       </c>
-    </row>
-    <row r="135" spans="1:8">
+      <c r="K134" s="7">
+        <f t="shared" si="6"/>
+        <v>143</v>
+      </c>
+    </row>
+    <row r="135" spans="1:12">
       <c r="B135" t="s">
         <v>7</v>
       </c>
@@ -1816,16 +2412,24 @@
       <c r="H135" s="2">
         <v>29.5</v>
       </c>
-    </row>
-    <row r="136" spans="1:8">
+      <c r="K135" s="7">
+        <f t="shared" si="6"/>
+        <v>142.5</v>
+      </c>
+    </row>
+    <row r="136" spans="1:12">
       <c r="G136" s="2">
         <v>7</v>
       </c>
       <c r="H136" s="2">
         <v>29</v>
       </c>
-    </row>
-    <row r="137" spans="1:8">
+      <c r="K136" s="7">
+        <f t="shared" si="6"/>
+        <v>142</v>
+      </c>
+    </row>
+    <row r="137" spans="1:12">
       <c r="B137" t="s">
         <v>16</v>
       </c>
@@ -1838,29 +2442,50 @@
       <c r="H137" s="2">
         <v>29</v>
       </c>
-    </row>
-    <row r="138" spans="1:8">
+      <c r="K137" s="7">
+        <f t="shared" si="6"/>
+        <v>142</v>
+      </c>
+    </row>
+    <row r="138" spans="1:12">
       <c r="G138" s="2">
         <v>9</v>
       </c>
       <c r="H138" s="2">
         <v>29.5</v>
       </c>
-    </row>
-    <row r="139" spans="1:8">
+      <c r="K138" s="7">
+        <f t="shared" si="6"/>
+        <v>142.5</v>
+      </c>
+    </row>
+    <row r="139" spans="1:12">
       <c r="G139" s="2">
         <v>10</v>
       </c>
       <c r="H139" s="2">
         <v>29</v>
       </c>
-    </row>
-    <row r="141" spans="1:8">
+      <c r="K139" s="7">
+        <f t="shared" si="6"/>
+        <v>142</v>
+      </c>
+    </row>
+    <row r="141" spans="1:12">
       <c r="B141" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="142" spans="1:8">
+      <c r="J141" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="K141" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="L141" s="9" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="142" spans="1:12">
       <c r="A142" s="1"/>
       <c r="B142" s="1" t="s">
         <v>1</v>
@@ -1871,8 +2496,20 @@
       <c r="D142" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="143" spans="1:8">
+      <c r="J142">
+        <f>AVERAGE(K130:K139)</f>
+        <v>142.5</v>
+      </c>
+      <c r="K142" s="7">
+        <f>STDEV(K130:K139)</f>
+        <v>0.47140452079103168</v>
+      </c>
+      <c r="L142" s="7">
+        <f>K142/SQRT(COUNT(K130:K139))</f>
+        <v>0.14907119849998596</v>
+      </c>
+    </row>
+    <row r="143" spans="1:12">
       <c r="A143" s="1" t="s">
         <v>4</v>
       </c>
@@ -1885,8 +2522,10 @@
       <c r="D143" s="1">
         <v>1049</v>
       </c>
-    </row>
-    <row r="144" spans="1:8">
+      <c r="K143"/>
+      <c r="L143"/>
+    </row>
+    <row r="144" spans="1:12">
       <c r="A144" s="1" t="s">
         <v>5</v>
       </c>
@@ -1899,16 +2538,32 @@
       <c r="D144" s="1">
         <v>65</v>
       </c>
-    </row>
-    <row r="148" spans="1:8">
+      <c r="K144"/>
+      <c r="L144"/>
+    </row>
+    <row r="145" spans="1:12">
+      <c r="K145"/>
+      <c r="L145"/>
+    </row>
+    <row r="146" spans="1:12">
+      <c r="K146"/>
+      <c r="L146"/>
+    </row>
+    <row r="147" spans="1:12">
+      <c r="K147"/>
+      <c r="L147"/>
+    </row>
+    <row r="148" spans="1:12">
       <c r="A148" s="4" t="s">
         <v>21</v>
       </c>
       <c r="B148" s="4" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="149" spans="1:8">
+      <c r="K148"/>
+      <c r="L148"/>
+    </row>
+    <row r="149" spans="1:12">
       <c r="B149" t="s">
         <v>9</v>
       </c>
@@ -1918,8 +2573,14 @@
       <c r="H149" s="2" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="150" spans="1:8">
+      <c r="J149" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="K149" s="8" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="150" spans="1:12">
       <c r="B150" t="s">
         <v>7</v>
       </c>
@@ -1939,8 +2600,16 @@
       <c r="H150" s="2">
         <v>32</v>
       </c>
-    </row>
-    <row r="151" spans="1:8">
+      <c r="J150">
+        <f>E153-E155</f>
+        <v>95</v>
+      </c>
+      <c r="K150" s="7">
+        <f>$C$18+H150-$C$5/2-$E$11</f>
+        <v>141</v>
+      </c>
+    </row>
+    <row r="151" spans="1:12">
       <c r="B151" t="s">
         <v>9</v>
       </c>
@@ -1950,8 +2619,12 @@
       <c r="H151" s="2">
         <v>33</v>
       </c>
-    </row>
-    <row r="152" spans="1:8">
+      <c r="K151" s="7">
+        <f t="shared" ref="K151:K159" si="7">$C$18+H151-$C$5/2-$E$11</f>
+        <v>142</v>
+      </c>
+    </row>
+    <row r="152" spans="1:12">
       <c r="B152" t="s">
         <v>11</v>
       </c>
@@ -1961,8 +2634,12 @@
       <c r="H152" s="2">
         <v>33</v>
       </c>
-    </row>
-    <row r="153" spans="1:8">
+      <c r="K152" s="7">
+        <f t="shared" si="7"/>
+        <v>142</v>
+      </c>
+    </row>
+    <row r="153" spans="1:12">
       <c r="B153" t="s">
         <v>7</v>
       </c>
@@ -1983,8 +2660,12 @@
       <c r="H153" s="2">
         <v>32</v>
       </c>
-    </row>
-    <row r="154" spans="1:8">
+      <c r="K153" s="7">
+        <f t="shared" si="7"/>
+        <v>141</v>
+      </c>
+    </row>
+    <row r="154" spans="1:12">
       <c r="B154" t="s">
         <v>12</v>
       </c>
@@ -1994,8 +2675,12 @@
       <c r="H154" s="2">
         <v>31</v>
       </c>
-    </row>
-    <row r="155" spans="1:8">
+      <c r="K154" s="7">
+        <f t="shared" si="7"/>
+        <v>140</v>
+      </c>
+    </row>
+    <row r="155" spans="1:12">
       <c r="B155" t="s">
         <v>7</v>
       </c>
@@ -2015,16 +2700,24 @@
       <c r="H155" s="2">
         <v>34.5</v>
       </c>
-    </row>
-    <row r="156" spans="1:8">
+      <c r="K155" s="7">
+        <f t="shared" si="7"/>
+        <v>143.5</v>
+      </c>
+    </row>
+    <row r="156" spans="1:12">
       <c r="G156" s="2">
         <v>7</v>
       </c>
       <c r="H156" s="2">
         <v>31</v>
       </c>
-    </row>
-    <row r="157" spans="1:8">
+      <c r="K156" s="7">
+        <f t="shared" si="7"/>
+        <v>140</v>
+      </c>
+    </row>
+    <row r="157" spans="1:12">
       <c r="B157" t="s">
         <v>16</v>
       </c>
@@ -2037,29 +2730,50 @@
       <c r="H157" s="2">
         <v>31</v>
       </c>
-    </row>
-    <row r="158" spans="1:8">
+      <c r="K157" s="7">
+        <f t="shared" si="7"/>
+        <v>140</v>
+      </c>
+    </row>
+    <row r="158" spans="1:12">
       <c r="G158" s="2">
         <v>9</v>
       </c>
       <c r="H158" s="2">
         <v>31.5</v>
       </c>
-    </row>
-    <row r="159" spans="1:8">
+      <c r="K158" s="7">
+        <f t="shared" si="7"/>
+        <v>140.5</v>
+      </c>
+    </row>
+    <row r="159" spans="1:12">
       <c r="G159" s="2">
         <v>10</v>
       </c>
       <c r="H159" s="2">
         <v>33.5</v>
       </c>
-    </row>
-    <row r="161" spans="1:8">
+      <c r="K159" s="7">
+        <f t="shared" si="7"/>
+        <v>142.5</v>
+      </c>
+    </row>
+    <row r="161" spans="1:12">
       <c r="B161" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="162" spans="1:8">
+      <c r="J161" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="K161" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="L161" s="9" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="162" spans="1:12">
       <c r="A162" s="1"/>
       <c r="B162" s="1" t="s">
         <v>1</v>
@@ -2070,8 +2784,20 @@
       <c r="D162" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="163" spans="1:8">
+      <c r="J162">
+        <f>AVERAGE(K150:K159)</f>
+        <v>141.25</v>
+      </c>
+      <c r="K162" s="7">
+        <f>STDEV(K150:K159)</f>
+        <v>1.2076147288491199</v>
+      </c>
+      <c r="L162" s="7">
+        <f>K162/SQRT(COUNT(K150:K159))</f>
+        <v>0.38188130791298663</v>
+      </c>
+    </row>
+    <row r="163" spans="1:12">
       <c r="A163" s="1" t="s">
         <v>4</v>
       </c>
@@ -2084,8 +2810,10 @@
       <c r="D163" s="1">
         <v>1049</v>
       </c>
-    </row>
-    <row r="164" spans="1:8">
+      <c r="K163"/>
+      <c r="L163"/>
+    </row>
+    <row r="164" spans="1:12">
       <c r="A164" s="1" t="s">
         <v>5</v>
       </c>
@@ -2098,16 +2826,32 @@
       <c r="D164" s="1">
         <v>65</v>
       </c>
-    </row>
-    <row r="168" spans="1:8">
+      <c r="K164"/>
+      <c r="L164"/>
+    </row>
+    <row r="165" spans="1:12">
+      <c r="K165"/>
+      <c r="L165"/>
+    </row>
+    <row r="166" spans="1:12">
+      <c r="K166"/>
+      <c r="L166"/>
+    </row>
+    <row r="167" spans="1:12">
+      <c r="K167"/>
+      <c r="L167"/>
+    </row>
+    <row r="168" spans="1:12">
       <c r="A168" s="4" t="s">
         <v>22</v>
       </c>
       <c r="B168" s="4" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="169" spans="1:8">
+      <c r="K168"/>
+      <c r="L168"/>
+    </row>
+    <row r="169" spans="1:12">
       <c r="B169" t="s">
         <v>19</v>
       </c>
@@ -2117,8 +2861,14 @@
       <c r="H169" s="2" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="170" spans="1:8">
+      <c r="J169" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="K169" s="8" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="170" spans="1:12">
       <c r="B170" t="s">
         <v>7</v>
       </c>
@@ -2138,8 +2888,16 @@
       <c r="H170" s="2">
         <v>36</v>
       </c>
-    </row>
-    <row r="171" spans="1:8">
+      <c r="J170">
+        <f>E173-E175</f>
+        <v>146</v>
+      </c>
+      <c r="K170" s="7">
+        <f>$C$18+H170-$C$5/2-$E$11</f>
+        <v>145</v>
+      </c>
+    </row>
+    <row r="171" spans="1:12">
       <c r="B171" t="s">
         <v>9</v>
       </c>
@@ -2149,8 +2907,12 @@
       <c r="H171" s="2">
         <v>37</v>
       </c>
-    </row>
-    <row r="172" spans="1:8">
+      <c r="K171" s="7">
+        <f t="shared" ref="K171:K179" si="8">$C$18+H171-$C$5/2-$E$11</f>
+        <v>146</v>
+      </c>
+    </row>
+    <row r="172" spans="1:12">
       <c r="B172" t="s">
         <v>11</v>
       </c>
@@ -2160,8 +2922,12 @@
       <c r="H172" s="2">
         <v>37</v>
       </c>
-    </row>
-    <row r="173" spans="1:8">
+      <c r="K172" s="7">
+        <f t="shared" si="8"/>
+        <v>146</v>
+      </c>
+    </row>
+    <row r="173" spans="1:12">
       <c r="B173" t="s">
         <v>7</v>
       </c>
@@ -2181,8 +2947,12 @@
       <c r="H173" s="2">
         <v>36.5</v>
       </c>
-    </row>
-    <row r="174" spans="1:8">
+      <c r="K173" s="7">
+        <f t="shared" si="8"/>
+        <v>145.5</v>
+      </c>
+    </row>
+    <row r="174" spans="1:12">
       <c r="B174" t="s">
         <v>12</v>
       </c>
@@ -2192,8 +2962,12 @@
       <c r="H174" s="2">
         <v>36</v>
       </c>
-    </row>
-    <row r="175" spans="1:8">
+      <c r="K174" s="7">
+        <f t="shared" si="8"/>
+        <v>145</v>
+      </c>
+    </row>
+    <row r="175" spans="1:12">
       <c r="B175" t="s">
         <v>7</v>
       </c>
@@ -2213,16 +2987,24 @@
       <c r="H175" s="2">
         <v>36</v>
       </c>
-    </row>
-    <row r="176" spans="1:8">
+      <c r="K175" s="7">
+        <f t="shared" si="8"/>
+        <v>145</v>
+      </c>
+    </row>
+    <row r="176" spans="1:12">
       <c r="G176" s="2">
         <v>7</v>
       </c>
       <c r="H176" s="2">
         <v>36</v>
       </c>
-    </row>
-    <row r="177" spans="1:8">
+      <c r="K176" s="7">
+        <f t="shared" si="8"/>
+        <v>145</v>
+      </c>
+    </row>
+    <row r="177" spans="1:12">
       <c r="B177" t="s">
         <v>16</v>
       </c>
@@ -2235,29 +3017,50 @@
       <c r="H177" s="2">
         <v>34.5</v>
       </c>
-    </row>
-    <row r="178" spans="1:8">
+      <c r="K177" s="7">
+        <f t="shared" si="8"/>
+        <v>143.5</v>
+      </c>
+    </row>
+    <row r="178" spans="1:12">
       <c r="G178" s="2">
         <v>9</v>
       </c>
       <c r="H178" s="2">
         <v>35</v>
       </c>
-    </row>
-    <row r="179" spans="1:8">
+      <c r="K178" s="7">
+        <f t="shared" si="8"/>
+        <v>144</v>
+      </c>
+    </row>
+    <row r="179" spans="1:12">
       <c r="G179" s="2">
         <v>10</v>
       </c>
       <c r="H179" s="2">
         <v>36</v>
       </c>
-    </row>
-    <row r="181" spans="1:8">
+      <c r="K179" s="7">
+        <f t="shared" si="8"/>
+        <v>145</v>
+      </c>
+    </row>
+    <row r="181" spans="1:12">
       <c r="B181" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="182" spans="1:8">
+      <c r="J181" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="K181" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="L181" s="9" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="182" spans="1:12">
       <c r="A182" s="1"/>
       <c r="B182" s="1" t="s">
         <v>1</v>
@@ -2268,8 +3071,20 @@
       <c r="D182" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="183" spans="1:8">
+      <c r="J182">
+        <f>AVERAGE(K170:K179)</f>
+        <v>145</v>
+      </c>
+      <c r="K182" s="7">
+        <f>STDEV(K170:K179)</f>
+        <v>0.78173595997057166</v>
+      </c>
+      <c r="L182" s="7">
+        <f>K182/SQRT(COUNT(K170:K179))</f>
+        <v>0.2472066162365221</v>
+      </c>
+    </row>
+    <row r="183" spans="1:12">
       <c r="A183" s="1" t="s">
         <v>4</v>
       </c>
@@ -2282,8 +3097,10 @@
       <c r="D183" s="1">
         <v>1049</v>
       </c>
-    </row>
-    <row r="184" spans="1:8">
+      <c r="K183"/>
+      <c r="L183"/>
+    </row>
+    <row r="184" spans="1:12">
       <c r="A184" s="1" t="s">
         <v>5</v>
       </c>
@@ -2296,16 +3113,32 @@
       <c r="D184" s="1">
         <v>65</v>
       </c>
-    </row>
-    <row r="188" spans="1:8">
+      <c r="K184"/>
+      <c r="L184"/>
+    </row>
+    <row r="185" spans="1:12">
+      <c r="K185"/>
+      <c r="L185"/>
+    </row>
+    <row r="186" spans="1:12">
+      <c r="K186"/>
+      <c r="L186"/>
+    </row>
+    <row r="187" spans="1:12">
+      <c r="K187"/>
+      <c r="L187"/>
+    </row>
+    <row r="188" spans="1:12">
       <c r="A188" s="4" t="s">
         <v>22</v>
       </c>
       <c r="B188" s="4" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="189" spans="1:8">
+      <c r="K188"/>
+      <c r="L188"/>
+    </row>
+    <row r="189" spans="1:12">
       <c r="B189" t="s">
         <v>19</v>
       </c>
@@ -2315,8 +3148,14 @@
       <c r="H189" s="2" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="190" spans="1:8">
+      <c r="J189" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="K189" s="8" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="190" spans="1:12">
       <c r="B190" t="s">
         <v>7</v>
       </c>
@@ -2336,8 +3175,16 @@
       <c r="H190" s="2">
         <v>35</v>
       </c>
-    </row>
-    <row r="191" spans="1:8">
+      <c r="J190">
+        <f>E193-E195</f>
+        <v>146</v>
+      </c>
+      <c r="K190" s="7">
+        <f>$C$18+H190-$C$5/2-$E$11</f>
+        <v>144</v>
+      </c>
+    </row>
+    <row r="191" spans="1:12">
       <c r="B191" t="s">
         <v>9</v>
       </c>
@@ -2347,8 +3194,12 @@
       <c r="H191" s="2">
         <v>35</v>
       </c>
-    </row>
-    <row r="192" spans="1:8">
+      <c r="K191" s="7">
+        <f t="shared" ref="K191:K199" si="9">$C$18+H191-$C$5/2-$E$11</f>
+        <v>144</v>
+      </c>
+    </row>
+    <row r="192" spans="1:12">
       <c r="B192" t="s">
         <v>11</v>
       </c>
@@ -2358,8 +3209,12 @@
       <c r="H192" s="2">
         <v>36</v>
       </c>
-    </row>
-    <row r="193" spans="1:8">
+      <c r="K192" s="7">
+        <f t="shared" si="9"/>
+        <v>145</v>
+      </c>
+    </row>
+    <row r="193" spans="1:12">
       <c r="B193" t="s">
         <v>7</v>
       </c>
@@ -2379,8 +3234,12 @@
       <c r="H193" s="2">
         <v>38</v>
       </c>
-    </row>
-    <row r="194" spans="1:8">
+      <c r="K193" s="7">
+        <f t="shared" si="9"/>
+        <v>147</v>
+      </c>
+    </row>
+    <row r="194" spans="1:12">
       <c r="B194" t="s">
         <v>12</v>
       </c>
@@ -2390,8 +3249,12 @@
       <c r="H194" s="2">
         <v>35</v>
       </c>
-    </row>
-    <row r="195" spans="1:8">
+      <c r="K194" s="7">
+        <f t="shared" si="9"/>
+        <v>144</v>
+      </c>
+    </row>
+    <row r="195" spans="1:12">
       <c r="B195" t="s">
         <v>7</v>
       </c>
@@ -2411,16 +3274,24 @@
       <c r="H195" s="2">
         <v>34</v>
       </c>
-    </row>
-    <row r="196" spans="1:8">
+      <c r="K195" s="7">
+        <f t="shared" si="9"/>
+        <v>143</v>
+      </c>
+    </row>
+    <row r="196" spans="1:12">
       <c r="G196" s="2">
         <v>7</v>
       </c>
       <c r="H196" s="2">
         <v>37.5</v>
       </c>
-    </row>
-    <row r="197" spans="1:8">
+      <c r="K196" s="7">
+        <f t="shared" si="9"/>
+        <v>146.5</v>
+      </c>
+    </row>
+    <row r="197" spans="1:12">
       <c r="B197" t="s">
         <v>16</v>
       </c>
@@ -2433,29 +3304,50 @@
       <c r="H197" s="2">
         <v>36.5</v>
       </c>
-    </row>
-    <row r="198" spans="1:8">
+      <c r="K197" s="7">
+        <f t="shared" si="9"/>
+        <v>145.5</v>
+      </c>
+    </row>
+    <row r="198" spans="1:12">
       <c r="G198" s="2">
         <v>9</v>
       </c>
       <c r="H198" s="2">
         <v>36</v>
       </c>
-    </row>
-    <row r="199" spans="1:8">
+      <c r="K198" s="7">
+        <f t="shared" si="9"/>
+        <v>145</v>
+      </c>
+    </row>
+    <row r="199" spans="1:12">
       <c r="G199" s="2">
         <v>10</v>
       </c>
       <c r="H199" s="2">
         <v>36.5</v>
       </c>
-    </row>
-    <row r="201" spans="1:8">
+      <c r="K199" s="7">
+        <f t="shared" si="9"/>
+        <v>145.5</v>
+      </c>
+    </row>
+    <row r="201" spans="1:12">
       <c r="B201" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="202" spans="1:8">
+      <c r="J201" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="K201" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="L201" s="9" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="202" spans="1:12">
       <c r="A202" s="1"/>
       <c r="B202" s="1" t="s">
         <v>1</v>
@@ -2466,8 +3358,20 @@
       <c r="D202" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="203" spans="1:8">
+      <c r="J202">
+        <f>AVERAGE(K190:K199)</f>
+        <v>144.94999999999999</v>
+      </c>
+      <c r="K202" s="7">
+        <f>STDEV(K190:K199)</f>
+        <v>1.2349089035231087</v>
+      </c>
+      <c r="L202" s="7">
+        <f>K202/SQRT(COUNT(K190:K199))</f>
+        <v>0.39051248379541548</v>
+      </c>
+    </row>
+    <row r="203" spans="1:12">
       <c r="A203" s="1" t="s">
         <v>4</v>
       </c>
@@ -2480,8 +3384,10 @@
       <c r="D203" s="1">
         <v>1049</v>
       </c>
-    </row>
-    <row r="204" spans="1:8">
+      <c r="K203"/>
+      <c r="L203"/>
+    </row>
+    <row r="204" spans="1:12">
       <c r="A204" s="1" t="s">
         <v>5</v>
       </c>
@@ -2494,16 +3400,32 @@
       <c r="D204" s="1">
         <v>65</v>
       </c>
-    </row>
-    <row r="208" spans="1:8">
+      <c r="K204"/>
+      <c r="L204"/>
+    </row>
+    <row r="205" spans="1:12">
+      <c r="K205"/>
+      <c r="L205"/>
+    </row>
+    <row r="206" spans="1:12">
+      <c r="K206"/>
+      <c r="L206"/>
+    </row>
+    <row r="207" spans="1:12">
+      <c r="K207"/>
+      <c r="L207"/>
+    </row>
+    <row r="208" spans="1:12">
       <c r="A208" s="4" t="s">
         <v>23</v>
       </c>
       <c r="B208" s="4" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="209" spans="1:8">
+      <c r="K208"/>
+      <c r="L208"/>
+    </row>
+    <row r="209" spans="1:12">
       <c r="B209" t="s">
         <v>9</v>
       </c>
@@ -2513,8 +3435,14 @@
       <c r="H209" s="2" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="210" spans="1:8">
+      <c r="J209" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="K209" s="8" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="210" spans="1:12">
       <c r="B210" t="s">
         <v>7</v>
       </c>
@@ -2534,8 +3462,16 @@
       <c r="H210" s="2">
         <v>43</v>
       </c>
-    </row>
-    <row r="211" spans="1:8">
+      <c r="J210">
+        <f>E213-E215</f>
+        <v>72.5</v>
+      </c>
+      <c r="K210" s="7">
+        <f>$C$18+H210-$C$5/2-$E$11</f>
+        <v>152</v>
+      </c>
+    </row>
+    <row r="211" spans="1:12">
       <c r="B211" t="s">
         <v>19</v>
       </c>
@@ -2545,8 +3481,12 @@
       <c r="H211" s="2">
         <v>43</v>
       </c>
-    </row>
-    <row r="212" spans="1:8">
+      <c r="K211" s="7">
+        <f t="shared" ref="K211:K219" si="10">$C$18+H211-$C$5/2-$E$11</f>
+        <v>152</v>
+      </c>
+    </row>
+    <row r="212" spans="1:12">
       <c r="B212" t="s">
         <v>11</v>
       </c>
@@ -2556,8 +3496,12 @@
       <c r="H212" s="2">
         <v>43</v>
       </c>
-    </row>
-    <row r="213" spans="1:8">
+      <c r="K212" s="7">
+        <f t="shared" si="10"/>
+        <v>152</v>
+      </c>
+    </row>
+    <row r="213" spans="1:12">
       <c r="B213" t="s">
         <v>7</v>
       </c>
@@ -2577,8 +3521,12 @@
       <c r="H213" s="2">
         <v>43</v>
       </c>
-    </row>
-    <row r="214" spans="1:8">
+      <c r="K213" s="7">
+        <f t="shared" si="10"/>
+        <v>152</v>
+      </c>
+    </row>
+    <row r="214" spans="1:12">
       <c r="B214" t="s">
         <v>12</v>
       </c>
@@ -2588,8 +3536,12 @@
       <c r="H214" s="2">
         <v>43</v>
       </c>
-    </row>
-    <row r="215" spans="1:8">
+      <c r="K214" s="7">
+        <f t="shared" si="10"/>
+        <v>152</v>
+      </c>
+    </row>
+    <row r="215" spans="1:12">
       <c r="B215" t="s">
         <v>7</v>
       </c>
@@ -2609,16 +3561,24 @@
       <c r="H215" s="2">
         <v>43</v>
       </c>
-    </row>
-    <row r="216" spans="1:8">
+      <c r="K215" s="7">
+        <f t="shared" si="10"/>
+        <v>152</v>
+      </c>
+    </row>
+    <row r="216" spans="1:12">
       <c r="G216" s="2">
         <v>7</v>
       </c>
       <c r="H216" s="2">
         <v>43.5</v>
       </c>
-    </row>
-    <row r="217" spans="1:8">
+      <c r="K216" s="7">
+        <f t="shared" si="10"/>
+        <v>152.5</v>
+      </c>
+    </row>
+    <row r="217" spans="1:12">
       <c r="B217" t="s">
         <v>16</v>
       </c>
@@ -2631,29 +3591,50 @@
       <c r="H217" s="2">
         <v>43</v>
       </c>
-    </row>
-    <row r="218" spans="1:8">
+      <c r="K217" s="7">
+        <f t="shared" si="10"/>
+        <v>152</v>
+      </c>
+    </row>
+    <row r="218" spans="1:12">
       <c r="G218" s="2">
         <v>9</v>
       </c>
       <c r="H218" s="2">
         <v>43.5</v>
       </c>
-    </row>
-    <row r="219" spans="1:8">
+      <c r="K218" s="7">
+        <f t="shared" si="10"/>
+        <v>152.5</v>
+      </c>
+    </row>
+    <row r="219" spans="1:12">
       <c r="G219" s="2">
         <v>10</v>
       </c>
       <c r="H219" s="2">
         <v>43</v>
       </c>
-    </row>
-    <row r="221" spans="1:8">
+      <c r="K219" s="7">
+        <f t="shared" si="10"/>
+        <v>152</v>
+      </c>
+    </row>
+    <row r="221" spans="1:12">
       <c r="B221" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="222" spans="1:8">
+      <c r="J221" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="K221" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="L221" s="9" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="222" spans="1:12">
       <c r="A222" s="1"/>
       <c r="B222" s="1" t="s">
         <v>1</v>
@@ -2664,8 +3645,20 @@
       <c r="D222" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="223" spans="1:8">
+      <c r="J222">
+        <f>AVERAGE(K210:K219)</f>
+        <v>152.1</v>
+      </c>
+      <c r="K222" s="7">
+        <f>STDEV(K210:K219)</f>
+        <v>0.21081851067789195</v>
+      </c>
+      <c r="L222" s="7">
+        <f>K222/SQRT(COUNT(K210:K219))</f>
+        <v>6.6666666666666666E-2</v>
+      </c>
+    </row>
+    <row r="223" spans="1:12">
       <c r="A223" s="1" t="s">
         <v>4</v>
       </c>
@@ -2678,8 +3671,10 @@
       <c r="D223" s="1">
         <v>1049</v>
       </c>
-    </row>
-    <row r="224" spans="1:8">
+      <c r="K223"/>
+      <c r="L223"/>
+    </row>
+    <row r="224" spans="1:12">
       <c r="A224" s="1" t="s">
         <v>5</v>
       </c>
@@ -2692,16 +3687,32 @@
       <c r="D224" s="1">
         <v>65</v>
       </c>
-    </row>
-    <row r="228" spans="1:8">
+      <c r="K224"/>
+      <c r="L224"/>
+    </row>
+    <row r="225" spans="1:12">
+      <c r="K225"/>
+      <c r="L225"/>
+    </row>
+    <row r="226" spans="1:12">
+      <c r="K226"/>
+      <c r="L226"/>
+    </row>
+    <row r="227" spans="1:12">
+      <c r="K227"/>
+      <c r="L227"/>
+    </row>
+    <row r="228" spans="1:12">
       <c r="A228" s="4" t="s">
         <v>23</v>
       </c>
       <c r="B228" s="4" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="229" spans="1:8">
+      <c r="K228"/>
+      <c r="L228"/>
+    </row>
+    <row r="229" spans="1:12">
       <c r="B229" t="s">
         <v>9</v>
       </c>
@@ -2711,8 +3722,14 @@
       <c r="H229" s="2" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="230" spans="1:8">
+      <c r="J229" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="K229" s="8" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="230" spans="1:12">
       <c r="B230" t="s">
         <v>7</v>
       </c>
@@ -2732,8 +3749,16 @@
       <c r="H230" s="2">
         <v>38</v>
       </c>
-    </row>
-    <row r="231" spans="1:8">
+      <c r="J230">
+        <f>E233-E235</f>
+        <v>72.5</v>
+      </c>
+      <c r="K230" s="7">
+        <f>$C$18+H230-$C$5/2-$E$11</f>
+        <v>147</v>
+      </c>
+    </row>
+    <row r="231" spans="1:12">
       <c r="B231" t="s">
         <v>19</v>
       </c>
@@ -2743,8 +3768,12 @@
       <c r="H231" s="2">
         <v>38.5</v>
       </c>
-    </row>
-    <row r="232" spans="1:8">
+      <c r="K231" s="7">
+        <f t="shared" ref="K231:K239" si="11">$C$18+H231-$C$5/2-$E$11</f>
+        <v>147.5</v>
+      </c>
+    </row>
+    <row r="232" spans="1:12">
       <c r="B232" t="s">
         <v>11</v>
       </c>
@@ -2754,8 +3783,12 @@
       <c r="H232" s="2">
         <v>37</v>
       </c>
-    </row>
-    <row r="233" spans="1:8">
+      <c r="K232" s="7">
+        <f t="shared" si="11"/>
+        <v>146</v>
+      </c>
+    </row>
+    <row r="233" spans="1:12">
       <c r="B233" t="s">
         <v>7</v>
       </c>
@@ -2775,8 +3808,12 @@
       <c r="H233" s="2">
         <v>37</v>
       </c>
-    </row>
-    <row r="234" spans="1:8">
+      <c r="K233" s="7">
+        <f t="shared" si="11"/>
+        <v>146</v>
+      </c>
+    </row>
+    <row r="234" spans="1:12">
       <c r="B234" t="s">
         <v>12</v>
       </c>
@@ -2786,8 +3823,12 @@
       <c r="H234" s="2">
         <v>37</v>
       </c>
-    </row>
-    <row r="235" spans="1:8">
+      <c r="K234" s="7">
+        <f t="shared" si="11"/>
+        <v>146</v>
+      </c>
+    </row>
+    <row r="235" spans="1:12">
       <c r="B235" t="s">
         <v>7</v>
       </c>
@@ -2807,16 +3848,24 @@
       <c r="H235" s="2">
         <v>37</v>
       </c>
-    </row>
-    <row r="236" spans="1:8">
+      <c r="K235" s="7">
+        <f t="shared" si="11"/>
+        <v>146</v>
+      </c>
+    </row>
+    <row r="236" spans="1:12">
       <c r="G236" s="2">
         <v>7</v>
       </c>
       <c r="H236" s="2">
         <v>36</v>
       </c>
-    </row>
-    <row r="237" spans="1:8">
+      <c r="K236" s="7">
+        <f t="shared" si="11"/>
+        <v>145</v>
+      </c>
+    </row>
+    <row r="237" spans="1:12">
       <c r="B237" t="s">
         <v>16</v>
       </c>
@@ -2829,29 +3878,50 @@
       <c r="H237" s="2">
         <v>37</v>
       </c>
-    </row>
-    <row r="238" spans="1:8">
+      <c r="K237" s="7">
+        <f t="shared" si="11"/>
+        <v>146</v>
+      </c>
+    </row>
+    <row r="238" spans="1:12">
       <c r="G238" s="2">
         <v>9</v>
       </c>
       <c r="H238" s="2">
         <v>36</v>
       </c>
-    </row>
-    <row r="239" spans="1:8">
+      <c r="K238" s="7">
+        <f t="shared" si="11"/>
+        <v>145</v>
+      </c>
+    </row>
+    <row r="239" spans="1:12">
       <c r="G239" s="2">
         <v>10</v>
       </c>
       <c r="H239" s="2">
         <v>37.5</v>
       </c>
-    </row>
-    <row r="241" spans="1:8">
+      <c r="K239" s="7">
+        <f t="shared" si="11"/>
+        <v>146.5</v>
+      </c>
+    </row>
+    <row r="241" spans="1:12">
       <c r="B241" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="242" spans="1:8">
+      <c r="J241" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="K241" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="L241" s="9" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="242" spans="1:12">
       <c r="A242" s="1"/>
       <c r="B242" s="1" t="s">
         <v>1</v>
@@ -2862,8 +3932,20 @@
       <c r="D242" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="243" spans="1:8">
+      <c r="J242">
+        <f>AVERAGE(K230:K239)</f>
+        <v>146.1</v>
+      </c>
+      <c r="K242" s="7">
+        <f>STDEV(K230:K239)</f>
+        <v>0.77459666924106596</v>
+      </c>
+      <c r="L242" s="7">
+        <f>K242/SQRT(COUNT(K230:K239))</f>
+        <v>0.24494897427818579</v>
+      </c>
+    </row>
+    <row r="243" spans="1:12">
       <c r="A243" s="1" t="s">
         <v>4</v>
       </c>
@@ -2876,8 +3958,10 @@
       <c r="D243" s="1">
         <v>1049</v>
       </c>
-    </row>
-    <row r="244" spans="1:8">
+      <c r="K243"/>
+      <c r="L243"/>
+    </row>
+    <row r="244" spans="1:12">
       <c r="A244" s="1" t="s">
         <v>5</v>
       </c>
@@ -2890,16 +3974,32 @@
       <c r="D244" s="1">
         <v>65</v>
       </c>
-    </row>
-    <row r="248" spans="1:8">
+      <c r="K244"/>
+      <c r="L244"/>
+    </row>
+    <row r="245" spans="1:12">
+      <c r="K245"/>
+      <c r="L245"/>
+    </row>
+    <row r="246" spans="1:12">
+      <c r="K246"/>
+      <c r="L246"/>
+    </row>
+    <row r="247" spans="1:12">
+      <c r="K247"/>
+      <c r="L247"/>
+    </row>
+    <row r="248" spans="1:12">
       <c r="A248" s="4" t="s">
         <v>24</v>
       </c>
       <c r="B248" s="4" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="249" spans="1:8">
+      <c r="K248"/>
+      <c r="L248"/>
+    </row>
+    <row r="249" spans="1:12">
       <c r="B249" t="s">
         <v>10</v>
       </c>
@@ -2909,8 +4009,14 @@
       <c r="H249" s="2" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="250" spans="1:8">
+      <c r="J249" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="K249" s="8" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="250" spans="1:12">
       <c r="B250" t="s">
         <v>7</v>
       </c>
@@ -2930,8 +4036,16 @@
       <c r="H250" s="2">
         <v>18</v>
       </c>
-    </row>
-    <row r="251" spans="1:8">
+      <c r="J250">
+        <f>E253-E255</f>
+        <v>72.5</v>
+      </c>
+      <c r="K250" s="7">
+        <f>$C$18+H250-$C$5/2-$E$11</f>
+        <v>127</v>
+      </c>
+    </row>
+    <row r="251" spans="1:12">
       <c r="B251" t="s">
         <v>19</v>
       </c>
@@ -2941,8 +4055,12 @@
       <c r="H251" s="2">
         <v>19</v>
       </c>
-    </row>
-    <row r="252" spans="1:8">
+      <c r="K251" s="7">
+        <f t="shared" ref="K251:K259" si="12">$C$18+H251-$C$5/2-$E$11</f>
+        <v>128</v>
+      </c>
+    </row>
+    <row r="252" spans="1:12">
       <c r="B252" t="s">
         <v>11</v>
       </c>
@@ -2952,8 +4070,12 @@
       <c r="H252" s="2">
         <v>18.5</v>
       </c>
-    </row>
-    <row r="253" spans="1:8">
+      <c r="K252" s="7">
+        <f t="shared" si="12"/>
+        <v>127.5</v>
+      </c>
+    </row>
+    <row r="253" spans="1:12">
       <c r="B253" t="s">
         <v>7</v>
       </c>
@@ -2973,8 +4095,12 @@
       <c r="H253" s="2">
         <v>20</v>
       </c>
-    </row>
-    <row r="254" spans="1:8">
+      <c r="K253" s="7">
+        <f t="shared" si="12"/>
+        <v>129</v>
+      </c>
+    </row>
+    <row r="254" spans="1:12">
       <c r="B254" t="s">
         <v>12</v>
       </c>
@@ -2984,8 +4110,12 @@
       <c r="H254" s="2">
         <v>20</v>
       </c>
-    </row>
-    <row r="255" spans="1:8">
+      <c r="K254" s="7">
+        <f t="shared" si="12"/>
+        <v>129</v>
+      </c>
+    </row>
+    <row r="255" spans="1:12">
       <c r="B255" t="s">
         <v>7</v>
       </c>
@@ -3005,16 +4135,24 @@
       <c r="H255" s="2">
         <v>20</v>
       </c>
-    </row>
-    <row r="256" spans="1:8">
+      <c r="K255" s="7">
+        <f t="shared" si="12"/>
+        <v>129</v>
+      </c>
+    </row>
+    <row r="256" spans="1:12">
       <c r="G256" s="2">
         <v>7</v>
       </c>
       <c r="H256" s="2">
         <v>21</v>
       </c>
-    </row>
-    <row r="257" spans="1:8">
+      <c r="K256" s="7">
+        <f t="shared" si="12"/>
+        <v>130</v>
+      </c>
+    </row>
+    <row r="257" spans="1:12">
       <c r="B257" t="s">
         <v>16</v>
       </c>
@@ -3027,29 +4165,50 @@
       <c r="H257" s="2">
         <v>18</v>
       </c>
-    </row>
-    <row r="258" spans="1:8">
+      <c r="K257" s="7">
+        <f t="shared" si="12"/>
+        <v>127</v>
+      </c>
+    </row>
+    <row r="258" spans="1:12">
       <c r="G258" s="2">
         <v>9</v>
       </c>
       <c r="H258" s="2">
         <v>20</v>
       </c>
-    </row>
-    <row r="259" spans="1:8">
+      <c r="K258" s="7">
+        <f t="shared" si="12"/>
+        <v>129</v>
+      </c>
+    </row>
+    <row r="259" spans="1:12">
       <c r="G259" s="2">
         <v>10</v>
       </c>
       <c r="H259" s="2">
         <v>19</v>
       </c>
-    </row>
-    <row r="261" spans="1:8">
+      <c r="K259" s="7">
+        <f t="shared" si="12"/>
+        <v>128</v>
+      </c>
+    </row>
+    <row r="261" spans="1:12">
       <c r="B261" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="262" spans="1:8">
+      <c r="J261" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="K261" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="L261" s="9" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="262" spans="1:12">
       <c r="A262" s="1"/>
       <c r="B262" s="1" t="s">
         <v>1</v>
@@ -3060,8 +4219,20 @@
       <c r="D262" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="263" spans="1:8">
+      <c r="J262">
+        <f>AVERAGE(K250:K259)</f>
+        <v>128.35</v>
+      </c>
+      <c r="K262" s="7">
+        <f>STDEV(K250:K259)</f>
+        <v>1.0013879257196638</v>
+      </c>
+      <c r="L262" s="7">
+        <f>K262/SQRT(COUNT(K250:K259))</f>
+        <v>0.31666666666656451</v>
+      </c>
+    </row>
+    <row r="263" spans="1:12">
       <c r="A263" s="1" t="s">
         <v>4</v>
       </c>
@@ -3074,8 +4245,10 @@
       <c r="D263" s="1">
         <v>1049</v>
       </c>
-    </row>
-    <row r="264" spans="1:8">
+      <c r="K263"/>
+      <c r="L263"/>
+    </row>
+    <row r="264" spans="1:12">
       <c r="A264" s="1" t="s">
         <v>5</v>
       </c>
@@ -3088,16 +4261,32 @@
       <c r="D264" s="1">
         <v>65</v>
       </c>
-    </row>
-    <row r="268" spans="1:8">
+      <c r="K264"/>
+      <c r="L264"/>
+    </row>
+    <row r="265" spans="1:12">
+      <c r="K265"/>
+      <c r="L265"/>
+    </row>
+    <row r="266" spans="1:12">
+      <c r="K266"/>
+      <c r="L266"/>
+    </row>
+    <row r="267" spans="1:12">
+      <c r="K267"/>
+      <c r="L267"/>
+    </row>
+    <row r="268" spans="1:12">
       <c r="A268" s="4" t="s">
         <v>24</v>
       </c>
       <c r="B268" s="4" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="269" spans="1:8">
+      <c r="K268"/>
+      <c r="L268"/>
+    </row>
+    <row r="269" spans="1:12">
       <c r="B269" t="s">
         <v>10</v>
       </c>
@@ -3107,8 +4296,14 @@
       <c r="H269" s="2" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="270" spans="1:8">
+      <c r="J269" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="K269" s="8" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="270" spans="1:12">
       <c r="B270" t="s">
         <v>7</v>
       </c>
@@ -3128,8 +4323,16 @@
       <c r="H270" s="2">
         <v>27</v>
       </c>
-    </row>
-    <row r="271" spans="1:8">
+      <c r="J270">
+        <f>E273-E275</f>
+        <v>72.5</v>
+      </c>
+      <c r="K270" s="7">
+        <f>$C$18+H270-$C$5/2-$E$11</f>
+        <v>136</v>
+      </c>
+    </row>
+    <row r="271" spans="1:12">
       <c r="B271" t="s">
         <v>19</v>
       </c>
@@ -3139,8 +4342,12 @@
       <c r="H271" s="2">
         <v>28</v>
       </c>
-    </row>
-    <row r="272" spans="1:8">
+      <c r="K271" s="7">
+        <f t="shared" ref="K271:K279" si="13">$C$18+H271-$C$5/2-$E$11</f>
+        <v>137</v>
+      </c>
+    </row>
+    <row r="272" spans="1:12">
       <c r="B272" t="s">
         <v>11</v>
       </c>
@@ -3150,8 +4357,12 @@
       <c r="H272" s="2">
         <v>28</v>
       </c>
-    </row>
-    <row r="273" spans="2:8">
+      <c r="K272" s="7">
+        <f t="shared" si="13"/>
+        <v>137</v>
+      </c>
+    </row>
+    <row r="273" spans="2:12">
       <c r="B273" t="s">
         <v>7</v>
       </c>
@@ -3171,8 +4382,12 @@
       <c r="H273" s="2">
         <v>28</v>
       </c>
-    </row>
-    <row r="274" spans="2:8">
+      <c r="K273" s="7">
+        <f t="shared" si="13"/>
+        <v>137</v>
+      </c>
+    </row>
+    <row r="274" spans="2:12">
       <c r="B274" t="s">
         <v>12</v>
       </c>
@@ -3182,8 +4397,12 @@
       <c r="H274" s="2">
         <v>27.5</v>
       </c>
-    </row>
-    <row r="275" spans="2:8">
+      <c r="K274" s="7">
+        <f t="shared" si="13"/>
+        <v>136.5</v>
+      </c>
+    </row>
+    <row r="275" spans="2:12">
       <c r="B275" t="s">
         <v>7</v>
       </c>
@@ -3203,16 +4422,24 @@
       <c r="H275" s="2">
         <v>27.5</v>
       </c>
-    </row>
-    <row r="276" spans="2:8">
+      <c r="K275" s="7">
+        <f t="shared" si="13"/>
+        <v>136.5</v>
+      </c>
+    </row>
+    <row r="276" spans="2:12">
       <c r="G276" s="2">
         <v>7</v>
       </c>
       <c r="H276" s="2">
         <v>27.5</v>
       </c>
-    </row>
-    <row r="277" spans="2:8">
+      <c r="K276" s="7">
+        <f t="shared" si="13"/>
+        <v>136.5</v>
+      </c>
+    </row>
+    <row r="277" spans="2:12">
       <c r="B277" t="s">
         <v>16</v>
       </c>
@@ -3225,26 +4452,63 @@
       <c r="H277" s="2">
         <v>27.5</v>
       </c>
-    </row>
-    <row r="278" spans="2:8">
+      <c r="K277" s="7">
+        <f t="shared" si="13"/>
+        <v>136.5</v>
+      </c>
+    </row>
+    <row r="278" spans="2:12">
       <c r="G278" s="2">
         <v>9</v>
       </c>
       <c r="H278" s="2">
         <v>27</v>
       </c>
-    </row>
-    <row r="279" spans="2:8">
+      <c r="K278" s="7">
+        <f t="shared" si="13"/>
+        <v>136</v>
+      </c>
+    </row>
+    <row r="279" spans="2:12">
       <c r="G279" s="2">
         <v>10</v>
       </c>
       <c r="H279" s="2">
         <v>27.5</v>
       </c>
+      <c r="K279" s="7">
+        <f t="shared" si="13"/>
+        <v>136.5</v>
+      </c>
+    </row>
+    <row r="281" spans="2:12">
+      <c r="J281" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="K281" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="L281" s="9" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="282" spans="2:12">
+      <c r="J282">
+        <f>AVERAGE(K270:K279)</f>
+        <v>136.55000000000001</v>
+      </c>
+      <c r="K282" s="7">
+        <f>STDEV(K270:K279)</f>
+        <v>0.36893239368631092</v>
+      </c>
+      <c r="L282" s="7">
+        <f>K282/SQRT(COUNT(K270:K279))</f>
+        <v>0.11666666666666665</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
updated excel with inelastic A and T2'/T1 calculations
	modified:   exp3/data/values.xlsx
</commit_message>
<xml_diff>
--- a/exp3/data/values.xlsx
+++ b/exp3/data/values.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="378" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="392" uniqueCount="32">
   <si>
     <t>Balls</t>
   </si>
@@ -119,9 +119,8 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
+  <numFmts count="1">
     <numFmt formatCode="GENERAL" numFmtId="164"/>
-    <numFmt formatCode="GENERAL" numFmtId="165"/>
   </numFmts>
   <fonts count="5">
     <font>
@@ -240,11 +239,7 @@
       <protection hidden="false" locked="true"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="9">
-    <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
+  <cellXfs count="8">
     <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0">
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
       <protection hidden="false" locked="true"/>
@@ -265,7 +260,7 @@
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
       <protection hidden="false" locked="true"/>
     </xf>
-    <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="165" xfId="0">
+    <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0">
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
       <protection hidden="false" locked="true"/>
     </xf>
@@ -285,8 +280,8 @@
     <cellStyle builtinId="4" customBuiltin="false" name="Currency" xfId="17"/>
     <cellStyle builtinId="7" customBuiltin="false" name="Currency [0]" xfId="18"/>
     <cellStyle builtinId="5" customBuiltin="false" name="Percent" xfId="19"/>
-    <cellStyle builtinId="54" customBuiltin="true" name="Excel Built-in 20% - Accent1" xfId="20"/>
-    <cellStyle builtinId="54" customBuiltin="true" name="Excel Built-in Good" xfId="21"/>
+    <cellStyle builtinId="54" customBuiltin="true" name="Excel Built-in Excel Built-in 20% - Accent1" xfId="20"/>
+    <cellStyle builtinId="54" customBuiltin="true" name="Excel Built-in Excel Built-in Good" xfId="21"/>
   </cellStyles>
   <colors>
     <indexedColors>
@@ -358,8 +353,8 @@
   </sheetPr>
   <dimension ref="A2:N282"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A181" view="normal" windowProtection="false" workbookViewId="0" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100">
-      <selection activeCell="M11" activeCellId="0" pane="topLeft" sqref="M11"/>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A244" view="normal" windowProtection="false" workbookViewId="0" zoomScale="55" zoomScaleNormal="55" zoomScalePageLayoutView="100">
+      <selection activeCell="N30" activeCellId="0" pane="topLeft" sqref="N30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -368,7 +363,7 @@
     <col collapsed="false" hidden="false" max="6" min="2" style="0" width="10.5748987854251"/>
     <col collapsed="false" hidden="false" max="7" min="7" style="0" width="18.2834008097166"/>
     <col collapsed="false" hidden="false" max="10" min="8" style="0" width="10.5748987854251"/>
-    <col collapsed="false" hidden="false" max="12" min="11" style="1" width="11.4251012145749"/>
+    <col collapsed="false" hidden="false" max="12" min="11" style="0" width="11.4251012145749"/>
     <col collapsed="false" hidden="false" max="1025" min="13" style="0" width="10.5748987854251"/>
   </cols>
   <sheetData>
@@ -378,50 +373,50 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="3">
-      <c r="A3" s="2"/>
-      <c r="B3" s="2" t="s">
+      <c r="A3" s="1"/>
+      <c r="B3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="D3" s="1" t="s">
         <v>3</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="4">
-      <c r="A4" s="2" t="s">
+      <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="2" t="n">
+      <c r="B4" s="1" t="n">
         <v>233</v>
       </c>
-      <c r="C4" s="2" t="n">
+      <c r="C4" s="1" t="n">
         <v>540</v>
       </c>
-      <c r="D4" s="2" t="n">
+      <c r="D4" s="1" t="n">
         <v>1049</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="5">
-      <c r="A5" s="2" t="s">
+      <c r="A5" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="2" t="n">
+      <c r="B5" s="1" t="n">
         <v>38</v>
       </c>
-      <c r="C5" s="2" t="n">
+      <c r="C5" s="1" t="n">
         <v>52</v>
       </c>
-      <c r="D5" s="2" t="n">
+      <c r="D5" s="1" t="n">
         <v>65</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="9">
-      <c r="A9" s="3" t="s">
+      <c r="A9" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B9" s="3" t="s">
+      <c r="B9" s="2" t="s">
         <v>7</v>
       </c>
     </row>
@@ -429,16 +424,16 @@
       <c r="B10" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="G10" s="4" t="s">
+      <c r="G10" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="H10" s="4" t="s">
+      <c r="H10" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="J10" s="5" t="s">
+      <c r="J10" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="K10" s="5" t="s">
+      <c r="K10" s="4" t="s">
         <v>12</v>
       </c>
       <c r="M10" s="0" t="s">
@@ -458,29 +453,29 @@
       <c r="D11" s="0" t="s">
         <v>16</v>
       </c>
-      <c r="E11" s="6" t="n">
+      <c r="E11" s="5" t="n">
         <f aca="false">C11-C5/2</f>
         <v>265</v>
       </c>
-      <c r="G11" s="4" t="n">
+      <c r="G11" s="3" t="n">
         <v>1</v>
       </c>
-      <c r="H11" s="4" t="n">
+      <c r="H11" s="3" t="n">
         <v>34</v>
       </c>
-      <c r="J11" s="6" t="n">
+      <c r="J11" s="5" t="n">
         <f aca="false">E14-E16</f>
         <v>159</v>
       </c>
-      <c r="K11" s="1" t="n">
+      <c r="K11" s="0" t="n">
         <f aca="false">$C$18+H11-$C$5/2-$E$11-50</f>
         <v>93</v>
       </c>
-      <c r="M11" s="6" t="n">
+      <c r="M11" s="5" t="n">
         <f aca="false">C4*0.001/(B4*0.001)</f>
         <v>2.31759656652361</v>
       </c>
-      <c r="N11" s="6" t="n">
+      <c r="N11" s="5" t="n">
         <f aca="false">$M$11*$J$23^2/$J$11^2</f>
         <v>0.799718868077318</v>
       </c>
@@ -489,13 +484,13 @@
       <c r="B12" s="0" t="s">
         <v>17</v>
       </c>
-      <c r="G12" s="4" t="n">
+      <c r="G12" s="3" t="n">
         <v>2</v>
       </c>
-      <c r="H12" s="4" t="n">
+      <c r="H12" s="3" t="n">
         <v>34</v>
       </c>
-      <c r="K12" s="1" t="n">
+      <c r="K12" s="0" t="n">
         <f aca="false">$C$18+H12-$C$5/2-$E$11-50</f>
         <v>93</v>
       </c>
@@ -504,13 +499,13 @@
       <c r="B13" s="0" t="s">
         <v>18</v>
       </c>
-      <c r="G13" s="4" t="n">
+      <c r="G13" s="3" t="n">
         <v>3</v>
       </c>
-      <c r="H13" s="4" t="n">
+      <c r="H13" s="3" t="n">
         <v>35</v>
       </c>
-      <c r="K13" s="1" t="n">
+      <c r="K13" s="0" t="n">
         <f aca="false">$C$18+H13-$C$5/2-$E$11-50</f>
         <v>94</v>
       </c>
@@ -519,24 +514,24 @@
       <c r="B14" s="0" t="s">
         <v>15</v>
       </c>
-      <c r="C14" s="6" t="n">
+      <c r="C14" s="5" t="n">
         <f aca="false">C11-C5</f>
         <v>239</v>
       </c>
       <c r="D14" s="0" t="s">
         <v>16</v>
       </c>
-      <c r="E14" s="6" t="n">
+      <c r="E14" s="5" t="n">
         <f aca="false">C14-B5/2</f>
         <v>220</v>
       </c>
-      <c r="G14" s="4" t="n">
+      <c r="G14" s="3" t="n">
         <v>4</v>
       </c>
-      <c r="H14" s="4" t="n">
+      <c r="H14" s="3" t="n">
         <v>35</v>
       </c>
-      <c r="K14" s="1" t="n">
+      <c r="K14" s="0" t="n">
         <f aca="false">$C$18+H14-$C$5/2-$E$11-50</f>
         <v>94</v>
       </c>
@@ -545,13 +540,13 @@
       <c r="B15" s="0" t="s">
         <v>19</v>
       </c>
-      <c r="G15" s="4" t="n">
+      <c r="G15" s="3" t="n">
         <v>5</v>
       </c>
-      <c r="H15" s="4" t="n">
+      <c r="H15" s="3" t="n">
         <v>36</v>
       </c>
-      <c r="K15" s="1" t="n">
+      <c r="K15" s="0" t="n">
         <f aca="false">$C$18+H15-$C$5/2-$E$11-50</f>
         <v>95</v>
       </c>
@@ -566,29 +561,29 @@
       <c r="D16" s="0" t="s">
         <v>16</v>
       </c>
-      <c r="E16" s="6" t="n">
+      <c r="E16" s="5" t="n">
         <f aca="false">C16-B5/2</f>
         <v>61</v>
       </c>
-      <c r="G16" s="4" t="n">
+      <c r="G16" s="3" t="n">
         <v>6</v>
       </c>
-      <c r="H16" s="4" t="n">
+      <c r="H16" s="3" t="n">
         <v>34</v>
       </c>
-      <c r="K16" s="1" t="n">
+      <c r="K16" s="0" t="n">
         <f aca="false">$C$18+H16-$C$5/2-$E$11-50</f>
         <v>93</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="17">
-      <c r="G17" s="4" t="n">
+      <c r="G17" s="3" t="n">
         <v>7</v>
       </c>
-      <c r="H17" s="4" t="n">
+      <c r="H17" s="3" t="n">
         <v>34</v>
       </c>
-      <c r="K17" s="1" t="n">
+      <c r="K17" s="0" t="n">
         <f aca="false">$C$18+H17-$C$5/2-$E$11-50</f>
         <v>93</v>
       </c>
@@ -597,40 +592,40 @@
       <c r="B18" s="0" t="s">
         <v>20</v>
       </c>
-      <c r="C18" s="7" t="n">
+      <c r="C18" s="6" t="n">
         <v>400</v>
       </c>
-      <c r="G18" s="4" t="n">
+      <c r="G18" s="3" t="n">
         <v>8</v>
       </c>
-      <c r="H18" s="4" t="n">
+      <c r="H18" s="3" t="n">
         <v>34</v>
       </c>
-      <c r="K18" s="1" t="n">
+      <c r="K18" s="0" t="n">
         <f aca="false">$C$18+H18-$C$5/2-$E$11-50</f>
         <v>93</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="19">
-      <c r="G19" s="4" t="n">
+      <c r="G19" s="3" t="n">
         <v>9</v>
       </c>
-      <c r="H19" s="4" t="n">
+      <c r="H19" s="3" t="n">
         <v>34</v>
       </c>
-      <c r="K19" s="1" t="n">
+      <c r="K19" s="0" t="n">
         <f aca="false">$C$18+H19-$C$5/2-$E$11-50</f>
         <v>93</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="20">
-      <c r="G20" s="4" t="n">
+      <c r="G20" s="3" t="n">
         <v>10</v>
       </c>
-      <c r="H20" s="4" t="n">
+      <c r="H20" s="3" t="n">
         <v>34</v>
       </c>
-      <c r="K20" s="1" t="n">
+      <c r="K20" s="0" t="n">
         <f aca="false">$C$18+H20-$C$5/2-$E$11-50</f>
         <v>93</v>
       </c>
@@ -641,71 +636,71 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="22">
-      <c r="A22" s="2"/>
-      <c r="B22" s="2" t="s">
+      <c r="A22" s="1"/>
+      <c r="B22" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C22" s="2" t="s">
+      <c r="C22" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D22" s="2" t="s">
+      <c r="D22" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="J22" s="8" t="s">
+      <c r="J22" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="K22" s="8" t="s">
+      <c r="K22" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="L22" s="8" t="s">
+      <c r="L22" s="7" t="s">
         <v>23</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="23">
-      <c r="A23" s="2" t="s">
+      <c r="A23" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B23" s="2" t="n">
+      <c r="B23" s="1" t="n">
         <v>233</v>
       </c>
-      <c r="C23" s="2" t="n">
+      <c r="C23" s="1" t="n">
         <v>540</v>
       </c>
-      <c r="D23" s="2" t="n">
+      <c r="D23" s="1" t="n">
         <v>1049</v>
       </c>
-      <c r="J23" s="6" t="n">
+      <c r="J23" s="5" t="n">
         <f aca="false">AVERAGE(K11:K20)</f>
         <v>93.4</v>
       </c>
-      <c r="K23" s="1" t="n">
+      <c r="K23" s="0" t="n">
         <f aca="false">STDEV(K11:K20)</f>
         <v>0.699205898779639</v>
       </c>
-      <c r="L23" s="1" t="n">
+      <c r="L23" s="0" t="n">
         <f aca="false">K23/SQRT(COUNT(K11:K20))</f>
         <v>0.22110831935688</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="24">
-      <c r="A24" s="2" t="s">
+      <c r="A24" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B24" s="2" t="n">
+      <c r="B24" s="1" t="n">
         <v>38</v>
       </c>
-      <c r="C24" s="2" t="n">
+      <c r="C24" s="1" t="n">
         <v>52</v>
       </c>
-      <c r="D24" s="2" t="n">
+      <c r="D24" s="1" t="n">
         <v>65</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="28">
-      <c r="A28" s="3" t="s">
+      <c r="A28" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B28" s="3" t="s">
+      <c r="B28" s="2" t="s">
         <v>24</v>
       </c>
     </row>
@@ -713,17 +708,23 @@
       <c r="B29" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="G29" s="4" t="s">
+      <c r="G29" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="H29" s="4" t="s">
+      <c r="H29" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="J29" s="5" t="s">
+      <c r="J29" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="K29" s="5" t="s">
+      <c r="K29" s="4" t="s">
         <v>12</v>
+      </c>
+      <c r="M29" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="N29" s="0" t="s">
+        <v>14</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="30">
@@ -736,36 +737,44 @@
       <c r="D30" s="0" t="s">
         <v>16</v>
       </c>
-      <c r="E30" s="6" t="n">
+      <c r="E30" s="5" t="n">
         <f aca="false">C30-C24/2</f>
         <v>265</v>
       </c>
-      <c r="G30" s="4" t="n">
+      <c r="G30" s="3" t="n">
         <v>1</v>
       </c>
-      <c r="H30" s="4" t="n">
+      <c r="H30" s="3" t="n">
         <v>36</v>
       </c>
-      <c r="J30" s="6" t="n">
+      <c r="J30" s="5" t="n">
         <f aca="false">E33-E35</f>
         <v>159</v>
       </c>
-      <c r="K30" s="1" t="n">
+      <c r="K30" s="0" t="n">
         <f aca="false">$C$37+H30-$C$24/2-$E$30-50</f>
         <v>45</v>
+      </c>
+      <c r="M30" s="5" t="n">
+        <f aca="false">C23*0.001/(B23*0.001)</f>
+        <v>2.31759656652361</v>
+      </c>
+      <c r="N30" s="5" t="n">
+        <f aca="false">$M$30*$J$42^2/$J$30^2</f>
+        <v>0.189786966174024</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="31">
       <c r="B31" s="0" t="s">
         <v>17</v>
       </c>
-      <c r="G31" s="4" t="n">
+      <c r="G31" s="3" t="n">
         <v>2</v>
       </c>
-      <c r="H31" s="4" t="n">
+      <c r="H31" s="3" t="n">
         <v>38</v>
       </c>
-      <c r="K31" s="1" t="n">
+      <c r="K31" s="0" t="n">
         <f aca="false">$C$37+H31-$C$24/2-$E$30-50</f>
         <v>47</v>
       </c>
@@ -774,13 +783,13 @@
       <c r="B32" s="0" t="s">
         <v>18</v>
       </c>
-      <c r="G32" s="4" t="n">
+      <c r="G32" s="3" t="n">
         <v>3</v>
       </c>
-      <c r="H32" s="4" t="n">
+      <c r="H32" s="3" t="n">
         <v>40</v>
       </c>
-      <c r="K32" s="1" t="n">
+      <c r="K32" s="0" t="n">
         <f aca="false">$C$37+H32-$C$24/2-$E$30-50</f>
         <v>49</v>
       </c>
@@ -789,24 +798,24 @@
       <c r="B33" s="0" t="s">
         <v>15</v>
       </c>
-      <c r="C33" s="6" t="n">
+      <c r="C33" s="5" t="n">
         <f aca="false">C30-C24</f>
         <v>239</v>
       </c>
       <c r="D33" s="0" t="s">
         <v>16</v>
       </c>
-      <c r="E33" s="6" t="n">
+      <c r="E33" s="5" t="n">
         <f aca="false">C33-B24/2</f>
         <v>220</v>
       </c>
-      <c r="G33" s="4" t="n">
+      <c r="G33" s="3" t="n">
         <v>4</v>
       </c>
-      <c r="H33" s="4" t="n">
+      <c r="H33" s="3" t="n">
         <v>36</v>
       </c>
-      <c r="K33" s="1" t="n">
+      <c r="K33" s="0" t="n">
         <f aca="false">$C$37+H33-$C$24/2-$E$30-50</f>
         <v>45</v>
       </c>
@@ -815,13 +824,13 @@
       <c r="B34" s="0" t="s">
         <v>19</v>
       </c>
-      <c r="G34" s="4" t="n">
+      <c r="G34" s="3" t="n">
         <v>5</v>
       </c>
-      <c r="H34" s="4" t="n">
+      <c r="H34" s="3" t="n">
         <v>37</v>
       </c>
-      <c r="K34" s="1" t="n">
+      <c r="K34" s="0" t="n">
         <f aca="false">$C$37+H34-$C$24/2-$E$30-50</f>
         <v>46</v>
       </c>
@@ -836,29 +845,29 @@
       <c r="D35" s="0" t="s">
         <v>16</v>
       </c>
-      <c r="E35" s="6" t="n">
+      <c r="E35" s="5" t="n">
         <f aca="false">C35-B24/2</f>
         <v>61</v>
       </c>
-      <c r="G35" s="4" t="n">
+      <c r="G35" s="3" t="n">
         <v>6</v>
       </c>
-      <c r="H35" s="4" t="n">
+      <c r="H35" s="3" t="n">
         <v>36</v>
       </c>
-      <c r="K35" s="1" t="n">
+      <c r="K35" s="0" t="n">
         <f aca="false">$C$37+H35-$C$24/2-$E$30-50</f>
         <v>45</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="36">
-      <c r="G36" s="4" t="n">
+      <c r="G36" s="3" t="n">
         <v>7</v>
       </c>
-      <c r="H36" s="4" t="n">
+      <c r="H36" s="3" t="n">
         <v>35</v>
       </c>
-      <c r="K36" s="1" t="n">
+      <c r="K36" s="0" t="n">
         <f aca="false">$C$37+H36-$C$24/2-$E$30-50</f>
         <v>44</v>
       </c>
@@ -867,40 +876,40 @@
       <c r="B37" s="0" t="s">
         <v>20</v>
       </c>
-      <c r="C37" s="7" t="n">
+      <c r="C37" s="6" t="n">
         <v>350</v>
       </c>
-      <c r="G37" s="4" t="n">
+      <c r="G37" s="3" t="n">
         <v>8</v>
       </c>
-      <c r="H37" s="4" t="n">
+      <c r="H37" s="3" t="n">
         <v>35</v>
       </c>
-      <c r="K37" s="1" t="n">
+      <c r="K37" s="0" t="n">
         <f aca="false">$C$37+H37-$C$24/2-$E$30-50</f>
         <v>44</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="38">
-      <c r="G38" s="4" t="n">
+      <c r="G38" s="3" t="n">
         <v>9</v>
       </c>
-      <c r="H38" s="4" t="n">
+      <c r="H38" s="3" t="n">
         <v>36</v>
       </c>
-      <c r="K38" s="1" t="n">
+      <c r="K38" s="0" t="n">
         <f aca="false">$C$37+H38-$C$24/2-$E$30-50</f>
         <v>45</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="39">
-      <c r="G39" s="4" t="n">
+      <c r="G39" s="3" t="n">
         <v>10</v>
       </c>
-      <c r="H39" s="4" t="n">
+      <c r="H39" s="3" t="n">
         <v>36</v>
       </c>
-      <c r="K39" s="1" t="n">
+      <c r="K39" s="0" t="n">
         <f aca="false">$C$37+H39-$C$24/2-$E$30-50</f>
         <v>45</v>
       </c>
@@ -909,73 +918,73 @@
       <c r="B41" s="0" t="s">
         <v>0</v>
       </c>
-      <c r="J41" s="8" t="s">
+      <c r="J41" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="K41" s="8" t="s">
+      <c r="K41" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="L41" s="8" t="s">
+      <c r="L41" s="7" t="s">
         <v>23</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="42">
-      <c r="A42" s="2"/>
-      <c r="B42" s="2" t="s">
+      <c r="A42" s="1"/>
+      <c r="B42" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C42" s="2" t="s">
+      <c r="C42" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D42" s="2" t="s">
+      <c r="D42" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="J42" s="6" t="n">
+      <c r="J42" s="5" t="n">
         <f aca="false">AVERAGE(K30:K39)</f>
         <v>45.5</v>
       </c>
-      <c r="K42" s="1" t="n">
+      <c r="K42" s="0" t="n">
         <f aca="false">STDEV(K30:K39)</f>
         <v>1.50923085635624</v>
       </c>
-      <c r="L42" s="1" t="n">
+      <c r="L42" s="0" t="n">
         <f aca="false">K42/SQRT(COUNT(K30:K39))</f>
         <v>0.477260702109212</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="43">
-      <c r="A43" s="2" t="s">
+      <c r="A43" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B43" s="2" t="n">
+      <c r="B43" s="1" t="n">
         <v>233</v>
       </c>
-      <c r="C43" s="2" t="n">
+      <c r="C43" s="1" t="n">
         <v>540</v>
       </c>
-      <c r="D43" s="2" t="n">
+      <c r="D43" s="1" t="n">
         <v>1049</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="44">
-      <c r="A44" s="2" t="s">
+      <c r="A44" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B44" s="2" t="n">
+      <c r="B44" s="1" t="n">
         <v>38</v>
       </c>
-      <c r="C44" s="2" t="n">
+      <c r="C44" s="1" t="n">
         <v>52</v>
       </c>
-      <c r="D44" s="2" t="n">
+      <c r="D44" s="1" t="n">
         <v>65</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="48">
-      <c r="A48" s="3" t="s">
+      <c r="A48" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="B48" s="3" t="s">
+      <c r="B48" s="2" t="s">
         <v>7</v>
       </c>
     </row>
@@ -983,16 +992,16 @@
       <c r="B49" s="0" t="s">
         <v>26</v>
       </c>
-      <c r="G49" s="4" t="s">
+      <c r="G49" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="H49" s="4" t="s">
+      <c r="H49" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="J49" s="5" t="s">
+      <c r="J49" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="K49" s="5" t="s">
+      <c r="K49" s="4" t="s">
         <v>12</v>
       </c>
       <c r="M49" s="0" t="s">
@@ -1012,29 +1021,29 @@
       <c r="D50" s="0" t="s">
         <v>16</v>
       </c>
-      <c r="E50" s="6" t="n">
+      <c r="E50" s="5" t="n">
         <f aca="false">C50-D44/2</f>
         <v>270.5</v>
       </c>
-      <c r="G50" s="4" t="n">
+      <c r="G50" s="3" t="n">
         <v>1</v>
       </c>
-      <c r="H50" s="4" t="n">
+      <c r="H50" s="3" t="n">
         <v>39</v>
       </c>
-      <c r="J50" s="6" t="n">
+      <c r="J50" s="5" t="n">
         <f aca="false">E53-E55</f>
         <v>158</v>
       </c>
-      <c r="K50" s="1" t="n">
+      <c r="K50" s="0" t="n">
         <f aca="false">$C$57+H50-$D$44/2-$E$50-50</f>
         <v>56</v>
       </c>
-      <c r="M50" s="6" t="n">
+      <c r="M50" s="5" t="n">
         <f aca="false">D43*0.001/(B43*0.001)</f>
         <v>4.50214592274678</v>
       </c>
-      <c r="N50" s="6" t="n">
+      <c r="N50" s="5" t="n">
         <f aca="false">$M$50*$J$62^2/$J$50^2</f>
         <v>0.555509332580547</v>
       </c>
@@ -1043,13 +1052,13 @@
       <c r="B51" s="0" t="s">
         <v>17</v>
       </c>
-      <c r="G51" s="4" t="n">
+      <c r="G51" s="3" t="n">
         <v>2</v>
       </c>
-      <c r="H51" s="4" t="n">
+      <c r="H51" s="3" t="n">
         <v>39</v>
       </c>
-      <c r="K51" s="1" t="n">
+      <c r="K51" s="0" t="n">
         <f aca="false">$C$57+H51-$D$44/2-$E$50-50</f>
         <v>56</v>
       </c>
@@ -1058,13 +1067,13 @@
       <c r="B52" s="0" t="s">
         <v>18</v>
       </c>
-      <c r="G52" s="4" t="n">
+      <c r="G52" s="3" t="n">
         <v>3</v>
       </c>
-      <c r="H52" s="4" t="n">
+      <c r="H52" s="3" t="n">
         <v>38</v>
       </c>
-      <c r="K52" s="1" t="n">
+      <c r="K52" s="0" t="n">
         <f aca="false">$C$57+H52-$D$44/2-$E$50-50</f>
         <v>55</v>
       </c>
@@ -1073,24 +1082,24 @@
       <c r="B53" s="0" t="s">
         <v>15</v>
       </c>
-      <c r="C53" s="6" t="n">
+      <c r="C53" s="5" t="n">
         <f aca="false">C50-D44</f>
         <v>238</v>
       </c>
       <c r="D53" s="0" t="s">
         <v>16</v>
       </c>
-      <c r="E53" s="6" t="n">
+      <c r="E53" s="5" t="n">
         <f aca="false">C53-B44/2</f>
         <v>219</v>
       </c>
-      <c r="G53" s="4" t="n">
+      <c r="G53" s="3" t="n">
         <v>4</v>
       </c>
-      <c r="H53" s="4" t="n">
+      <c r="H53" s="3" t="n">
         <v>38.5</v>
       </c>
-      <c r="K53" s="1" t="n">
+      <c r="K53" s="0" t="n">
         <f aca="false">$C$57+H53-$D$44/2-$E$50-50</f>
         <v>55.5</v>
       </c>
@@ -1099,13 +1108,13 @@
       <c r="B54" s="0" t="s">
         <v>19</v>
       </c>
-      <c r="G54" s="4" t="n">
+      <c r="G54" s="3" t="n">
         <v>5</v>
       </c>
-      <c r="H54" s="4" t="n">
+      <c r="H54" s="3" t="n">
         <v>38.5</v>
       </c>
-      <c r="K54" s="1" t="n">
+      <c r="K54" s="0" t="n">
         <f aca="false">$C$57+H54-$D$44/2-$E$50-50</f>
         <v>55.5</v>
       </c>
@@ -1120,29 +1129,29 @@
       <c r="D55" s="0" t="s">
         <v>16</v>
       </c>
-      <c r="E55" s="6" t="n">
+      <c r="E55" s="5" t="n">
         <f aca="false">C55-B44/2</f>
         <v>61</v>
       </c>
-      <c r="G55" s="4" t="n">
+      <c r="G55" s="3" t="n">
         <v>6</v>
       </c>
-      <c r="H55" s="4" t="n">
+      <c r="H55" s="3" t="n">
         <v>38.5</v>
       </c>
-      <c r="K55" s="1" t="n">
+      <c r="K55" s="0" t="n">
         <f aca="false">$C$57+H55-$D$44/2-$E$50-50</f>
         <v>55.5</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="56">
-      <c r="G56" s="4" t="n">
+      <c r="G56" s="3" t="n">
         <v>7</v>
       </c>
-      <c r="H56" s="4" t="n">
+      <c r="H56" s="3" t="n">
         <v>38</v>
       </c>
-      <c r="K56" s="1" t="n">
+      <c r="K56" s="0" t="n">
         <f aca="false">$C$57+H56-$D$44/2-$E$50-50</f>
         <v>55</v>
       </c>
@@ -1151,40 +1160,40 @@
       <c r="B57" s="0" t="s">
         <v>20</v>
       </c>
-      <c r="C57" s="7" t="n">
+      <c r="C57" s="6" t="n">
         <v>370</v>
       </c>
-      <c r="G57" s="4" t="n">
+      <c r="G57" s="3" t="n">
         <v>8</v>
       </c>
-      <c r="H57" s="4" t="n">
+      <c r="H57" s="3" t="n">
         <v>37.5</v>
       </c>
-      <c r="K57" s="1" t="n">
+      <c r="K57" s="0" t="n">
         <f aca="false">$C$57+H57-$D$44/2-$E$50-50</f>
         <v>54.5</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="58">
-      <c r="G58" s="4" t="n">
+      <c r="G58" s="3" t="n">
         <v>9</v>
       </c>
-      <c r="H58" s="4" t="n">
+      <c r="H58" s="3" t="n">
         <v>39</v>
       </c>
-      <c r="K58" s="1" t="n">
+      <c r="K58" s="0" t="n">
         <f aca="false">$C$57+H58-$D$44/2-$E$50-50</f>
         <v>56</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="59">
-      <c r="G59" s="4" t="n">
+      <c r="G59" s="3" t="n">
         <v>10</v>
       </c>
-      <c r="H59" s="4" t="n">
+      <c r="H59" s="3" t="n">
         <v>39</v>
       </c>
-      <c r="K59" s="1" t="n">
+      <c r="K59" s="0" t="n">
         <f aca="false">$C$57+H59-$D$44/2-$E$50-50</f>
         <v>56</v>
       </c>
@@ -1193,73 +1202,73 @@
       <c r="B61" s="0" t="s">
         <v>0</v>
       </c>
-      <c r="J61" s="8" t="s">
+      <c r="J61" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="K61" s="8" t="s">
+      <c r="K61" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="L61" s="8" t="s">
+      <c r="L61" s="7" t="s">
         <v>23</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="62">
-      <c r="A62" s="2"/>
-      <c r="B62" s="2" t="s">
+      <c r="A62" s="1"/>
+      <c r="B62" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C62" s="2" t="s">
+      <c r="C62" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D62" s="2" t="s">
+      <c r="D62" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="J62" s="6" t="n">
+      <c r="J62" s="5" t="n">
         <f aca="false">AVERAGE(K50:K59)</f>
         <v>55.5</v>
       </c>
-      <c r="K62" s="1" t="n">
+      <c r="K62" s="0" t="n">
         <f aca="false">STDEV(K50:K59)</f>
         <v>0.52704627669473</v>
       </c>
-      <c r="L62" s="1" t="n">
+      <c r="L62" s="0" t="n">
         <f aca="false">K62/SQRT(COUNT(K50:K59))</f>
         <v>0.166666666666667</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="63">
-      <c r="A63" s="2" t="s">
+      <c r="A63" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B63" s="2" t="n">
+      <c r="B63" s="1" t="n">
         <v>233</v>
       </c>
-      <c r="C63" s="2" t="n">
+      <c r="C63" s="1" t="n">
         <v>540</v>
       </c>
-      <c r="D63" s="2" t="n">
+      <c r="D63" s="1" t="n">
         <v>1049</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="64">
-      <c r="A64" s="2" t="s">
+      <c r="A64" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B64" s="2" t="n">
+      <c r="B64" s="1" t="n">
         <v>38</v>
       </c>
-      <c r="C64" s="2" t="n">
+      <c r="C64" s="1" t="n">
         <v>52</v>
       </c>
-      <c r="D64" s="2" t="n">
+      <c r="D64" s="1" t="n">
         <v>65</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="68">
-      <c r="A68" s="3" t="s">
+      <c r="A68" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="B68" s="3" t="s">
+      <c r="B68" s="2" t="s">
         <v>24</v>
       </c>
     </row>
@@ -1267,17 +1276,23 @@
       <c r="B69" s="0" t="s">
         <v>26</v>
       </c>
-      <c r="G69" s="4" t="s">
+      <c r="G69" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="H69" s="4" t="s">
+      <c r="H69" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="J69" s="5" t="s">
+      <c r="J69" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="K69" s="5" t="s">
+      <c r="K69" s="4" t="s">
         <v>12</v>
+      </c>
+      <c r="M69" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="N69" s="0" t="s">
+        <v>14</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="70">
@@ -1290,36 +1305,44 @@
       <c r="D70" s="0" t="s">
         <v>16</v>
       </c>
-      <c r="E70" s="6" t="n">
+      <c r="E70" s="5" t="n">
         <f aca="false">C70-D64/2</f>
         <v>270.5</v>
       </c>
-      <c r="G70" s="4" t="n">
+      <c r="G70" s="3" t="n">
         <v>1</v>
       </c>
-      <c r="H70" s="4" t="n">
+      <c r="H70" s="3" t="n">
         <v>31</v>
       </c>
-      <c r="J70" s="6" t="n">
+      <c r="J70" s="5" t="n">
         <f aca="false">E73-E75</f>
         <v>158</v>
       </c>
-      <c r="K70" s="1" t="n">
+      <c r="K70" s="0" t="n">
         <f aca="false">$C$77+H70-$D$64/2-$E$70-50</f>
         <v>28</v>
+      </c>
+      <c r="M70" s="5" t="n">
+        <f aca="false">D63*0.001/(B63*0.001)</f>
+        <v>4.50214592274678</v>
+      </c>
+      <c r="N70" s="5" t="n">
+        <f aca="false">$M$70*$J$82^2/$J$70^2</f>
+        <v>0.128566528075106</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="71">
       <c r="B71" s="0" t="s">
         <v>17</v>
       </c>
-      <c r="G71" s="4" t="n">
+      <c r="G71" s="3" t="n">
         <v>2</v>
       </c>
-      <c r="H71" s="4" t="n">
+      <c r="H71" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="K71" s="1" t="n">
+      <c r="K71" s="0" t="n">
         <f aca="false">$C$77+H71-$D$64/2-$E$70-50</f>
         <v>27</v>
       </c>
@@ -1328,13 +1351,13 @@
       <c r="B72" s="0" t="s">
         <v>18</v>
       </c>
-      <c r="G72" s="4" t="n">
+      <c r="G72" s="3" t="n">
         <v>3</v>
       </c>
-      <c r="H72" s="4" t="n">
+      <c r="H72" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="K72" s="1" t="n">
+      <c r="K72" s="0" t="n">
         <f aca="false">$C$77+H72-$D$64/2-$E$70-50</f>
         <v>27</v>
       </c>
@@ -1343,24 +1366,24 @@
       <c r="B73" s="0" t="s">
         <v>15</v>
       </c>
-      <c r="C73" s="6" t="n">
+      <c r="C73" s="5" t="n">
         <f aca="false">C70-D64</f>
         <v>238</v>
       </c>
       <c r="D73" s="0" t="s">
         <v>16</v>
       </c>
-      <c r="E73" s="6" t="n">
+      <c r="E73" s="5" t="n">
         <f aca="false">C73-B64/2</f>
         <v>219</v>
       </c>
-      <c r="G73" s="4" t="n">
+      <c r="G73" s="3" t="n">
         <v>4</v>
       </c>
-      <c r="H73" s="4" t="n">
+      <c r="H73" s="3" t="n">
         <v>29</v>
       </c>
-      <c r="K73" s="1" t="n">
+      <c r="K73" s="0" t="n">
         <f aca="false">$C$77+H73-$D$64/2-$E$70-50</f>
         <v>26</v>
       </c>
@@ -1369,13 +1392,13 @@
       <c r="B74" s="0" t="s">
         <v>19</v>
       </c>
-      <c r="G74" s="4" t="n">
+      <c r="G74" s="3" t="n">
         <v>5</v>
       </c>
-      <c r="H74" s="4" t="n">
+      <c r="H74" s="3" t="n">
         <v>29.5</v>
       </c>
-      <c r="K74" s="1" t="n">
+      <c r="K74" s="0" t="n">
         <f aca="false">$C$77+H74-$D$64/2-$E$70-50</f>
         <v>26.5</v>
       </c>
@@ -1390,29 +1413,29 @@
       <c r="D75" s="0" t="s">
         <v>16</v>
       </c>
-      <c r="E75" s="6" t="n">
+      <c r="E75" s="5" t="n">
         <f aca="false">C75-B64/2</f>
         <v>61</v>
       </c>
-      <c r="G75" s="4" t="n">
+      <c r="G75" s="3" t="n">
         <v>6</v>
       </c>
-      <c r="H75" s="4" t="n">
+      <c r="H75" s="3" t="n">
         <v>29</v>
       </c>
-      <c r="K75" s="1" t="n">
+      <c r="K75" s="0" t="n">
         <f aca="false">$C$77+H75-$D$64/2-$E$70-50</f>
         <v>26</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="76">
-      <c r="G76" s="4" t="n">
+      <c r="G76" s="3" t="n">
         <v>7</v>
       </c>
-      <c r="H76" s="4" t="n">
+      <c r="H76" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="K76" s="1" t="n">
+      <c r="K76" s="0" t="n">
         <f aca="false">$C$77+H76-$D$64/2-$E$70-50</f>
         <v>27</v>
       </c>
@@ -1421,40 +1444,40 @@
       <c r="B77" s="0" t="s">
         <v>20</v>
       </c>
-      <c r="C77" s="7" t="n">
+      <c r="C77" s="6" t="n">
         <v>350</v>
       </c>
-      <c r="G77" s="4" t="n">
+      <c r="G77" s="3" t="n">
         <v>8</v>
       </c>
-      <c r="H77" s="4" t="n">
+      <c r="H77" s="3" t="n">
         <v>29.5</v>
       </c>
-      <c r="K77" s="1" t="n">
+      <c r="K77" s="0" t="n">
         <f aca="false">$C$77+H77-$D$64/2-$E$70-50</f>
         <v>26.5</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="78">
-      <c r="G78" s="4" t="n">
+      <c r="G78" s="3" t="n">
         <v>9</v>
       </c>
-      <c r="H78" s="4" t="n">
+      <c r="H78" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="K78" s="1" t="n">
+      <c r="K78" s="0" t="n">
         <f aca="false">$C$77+H78-$D$64/2-$E$70-50</f>
         <v>27</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="79">
-      <c r="G79" s="4" t="n">
+      <c r="G79" s="3" t="n">
         <v>10</v>
       </c>
-      <c r="H79" s="4" t="n">
+      <c r="H79" s="3" t="n">
         <v>29</v>
       </c>
-      <c r="K79" s="1" t="n">
+      <c r="K79" s="0" t="n">
         <f aca="false">$C$77+H79-$D$64/2-$E$70-50</f>
         <v>26</v>
       </c>
@@ -1463,73 +1486,73 @@
       <c r="B81" s="0" t="s">
         <v>0</v>
       </c>
-      <c r="J81" s="8" t="s">
+      <c r="J81" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="K81" s="8" t="s">
+      <c r="K81" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="L81" s="8" t="s">
+      <c r="L81" s="7" t="s">
         <v>23</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="82">
-      <c r="A82" s="2"/>
-      <c r="B82" s="2" t="s">
+      <c r="A82" s="1"/>
+      <c r="B82" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C82" s="2" t="s">
+      <c r="C82" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D82" s="2" t="s">
+      <c r="D82" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="J82" s="6" t="n">
+      <c r="J82" s="5" t="n">
         <f aca="false">AVERAGE(K70:K79)</f>
         <v>26.7</v>
       </c>
-      <c r="K82" s="1" t="n">
+      <c r="K82" s="0" t="n">
         <f aca="false">STDEV(K70:K79)</f>
         <v>0.632455532033708</v>
       </c>
-      <c r="L82" s="1" t="n">
+      <c r="L82" s="0" t="n">
         <f aca="false">K82/SQRT(COUNT(K70:K79))</f>
         <v>0.20000000000001</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="83">
-      <c r="A83" s="2" t="s">
+      <c r="A83" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B83" s="2" t="n">
+      <c r="B83" s="1" t="n">
         <v>233</v>
       </c>
-      <c r="C83" s="2" t="n">
+      <c r="C83" s="1" t="n">
         <v>540</v>
       </c>
-      <c r="D83" s="2" t="n">
+      <c r="D83" s="1" t="n">
         <v>1049</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="84">
-      <c r="A84" s="2" t="s">
+      <c r="A84" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B84" s="2" t="n">
+      <c r="B84" s="1" t="n">
         <v>38</v>
       </c>
-      <c r="C84" s="2" t="n">
+      <c r="C84" s="1" t="n">
         <v>52</v>
       </c>
-      <c r="D84" s="2" t="n">
+      <c r="D84" s="1" t="n">
         <v>65</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="88">
-      <c r="A88" s="3" t="s">
+      <c r="A88" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="B88" s="3" t="s">
+      <c r="B88" s="2" t="s">
         <v>7</v>
       </c>
     </row>
@@ -1537,16 +1560,16 @@
       <c r="B89" s="0" t="s">
         <v>17</v>
       </c>
-      <c r="G89" s="4" t="s">
+      <c r="G89" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="H89" s="4" t="s">
+      <c r="H89" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="J89" s="5" t="s">
+      <c r="J89" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="K89" s="5" t="s">
+      <c r="K89" s="4" t="s">
         <v>12</v>
       </c>
       <c r="M89" s="0" t="s">
@@ -1566,29 +1589,29 @@
       <c r="D90" s="0" t="s">
         <v>16</v>
       </c>
-      <c r="E90" s="6" t="n">
+      <c r="E90" s="5" t="n">
         <f aca="false">C90-B84/2</f>
         <v>265</v>
       </c>
-      <c r="G90" s="4" t="n">
+      <c r="G90" s="3" t="n">
         <v>1</v>
       </c>
-      <c r="H90" s="4" t="n">
+      <c r="H90" s="3" t="n">
         <v>18</v>
       </c>
-      <c r="J90" s="6" t="n">
+      <c r="J90" s="5" t="n">
         <f aca="false">E93-E95</f>
         <v>86</v>
       </c>
-      <c r="K90" s="1" t="n">
+      <c r="K90" s="0" t="n">
         <f aca="false">$C$97+H90-$B$84/2-$E$90-50</f>
         <v>114</v>
       </c>
-      <c r="M90" s="6" t="n">
+      <c r="M90" s="5" t="n">
         <f aca="false">B83*0.001/(C83*0.001)</f>
         <v>0.431481481481481</v>
       </c>
-      <c r="N90" s="6" t="n">
+      <c r="N90" s="5" t="n">
         <f aca="false">$M$90*$J$102^2/$J$90^2</f>
         <v>0.765518068450414</v>
       </c>
@@ -1597,13 +1620,13 @@
       <c r="B91" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="G91" s="4" t="n">
+      <c r="G91" s="3" t="n">
         <v>2</v>
       </c>
-      <c r="H91" s="4" t="n">
+      <c r="H91" s="3" t="n">
         <v>19</v>
       </c>
-      <c r="K91" s="1" t="n">
+      <c r="K91" s="0" t="n">
         <f aca="false">$C$97+H91-$B$84/2-$E$90-50</f>
         <v>115</v>
       </c>
@@ -1612,13 +1635,13 @@
       <c r="B92" s="0" t="s">
         <v>18</v>
       </c>
-      <c r="G92" s="4" t="n">
+      <c r="G92" s="3" t="n">
         <v>3</v>
       </c>
-      <c r="H92" s="4" t="n">
+      <c r="H92" s="3" t="n">
         <v>19</v>
       </c>
-      <c r="K92" s="1" t="n">
+      <c r="K92" s="0" t="n">
         <f aca="false">$C$97+H92-$B$84/2-$E$90-50</f>
         <v>115</v>
       </c>
@@ -1627,24 +1650,24 @@
       <c r="B93" s="0" t="s">
         <v>15</v>
       </c>
-      <c r="C93" s="6" t="n">
+      <c r="C93" s="5" t="n">
         <f aca="false">C90-B84</f>
         <v>246</v>
       </c>
       <c r="D93" s="0" t="s">
         <v>16</v>
       </c>
-      <c r="E93" s="6" t="n">
+      <c r="E93" s="5" t="n">
         <f aca="false">C93-C84/2</f>
         <v>220</v>
       </c>
-      <c r="G93" s="4" t="n">
+      <c r="G93" s="3" t="n">
         <v>4</v>
       </c>
-      <c r="H93" s="4" t="n">
+      <c r="H93" s="3" t="n">
         <v>18.5</v>
       </c>
-      <c r="K93" s="1" t="n">
+      <c r="K93" s="0" t="n">
         <f aca="false">$C$97+H93-$B$84/2-$E$90-50</f>
         <v>114.5</v>
       </c>
@@ -1653,13 +1676,13 @@
       <c r="B94" s="0" t="s">
         <v>19</v>
       </c>
-      <c r="G94" s="4" t="n">
+      <c r="G94" s="3" t="n">
         <v>5</v>
       </c>
-      <c r="H94" s="4" t="n">
+      <c r="H94" s="3" t="n">
         <v>18</v>
       </c>
-      <c r="K94" s="1" t="n">
+      <c r="K94" s="0" t="n">
         <f aca="false">$C$97+H94-$B$84/2-$E$90-50</f>
         <v>114</v>
       </c>
@@ -1674,29 +1697,29 @@
       <c r="D95" s="0" t="s">
         <v>16</v>
       </c>
-      <c r="E95" s="6" t="n">
+      <c r="E95" s="5" t="n">
         <f aca="false">C95-C84/2</f>
         <v>134</v>
       </c>
-      <c r="G95" s="4" t="n">
+      <c r="G95" s="3" t="n">
         <v>6</v>
       </c>
-      <c r="H95" s="4" t="n">
+      <c r="H95" s="3" t="n">
         <v>18</v>
       </c>
-      <c r="K95" s="1" t="n">
+      <c r="K95" s="0" t="n">
         <f aca="false">$C$97+H95-$B$84/2-$E$90-50</f>
         <v>114</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="96">
-      <c r="G96" s="4" t="n">
+      <c r="G96" s="3" t="n">
         <v>7</v>
       </c>
-      <c r="H96" s="4" t="n">
+      <c r="H96" s="3" t="n">
         <v>18.5</v>
       </c>
-      <c r="K96" s="1" t="n">
+      <c r="K96" s="0" t="n">
         <f aca="false">$C$97+H96-$B$84/2-$E$90-50</f>
         <v>114.5</v>
       </c>
@@ -1705,40 +1728,40 @@
       <c r="B97" s="0" t="s">
         <v>20</v>
       </c>
-      <c r="C97" s="7" t="n">
+      <c r="C97" s="6" t="n">
         <v>430</v>
       </c>
-      <c r="G97" s="4" t="n">
+      <c r="G97" s="3" t="n">
         <v>8</v>
       </c>
-      <c r="H97" s="4" t="n">
+      <c r="H97" s="3" t="n">
         <v>18.5</v>
       </c>
-      <c r="K97" s="1" t="n">
+      <c r="K97" s="0" t="n">
         <f aca="false">$C$97+H97-$B$84/2-$E$90-50</f>
         <v>114.5</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="98">
-      <c r="G98" s="4" t="n">
+      <c r="G98" s="3" t="n">
         <v>9</v>
       </c>
-      <c r="H98" s="4" t="n">
+      <c r="H98" s="3" t="n">
         <v>19</v>
       </c>
-      <c r="K98" s="1" t="n">
+      <c r="K98" s="0" t="n">
         <f aca="false">$C$97+H98-$B$84/2-$E$90-50</f>
         <v>115</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="99">
-      <c r="G99" s="4" t="n">
+      <c r="G99" s="3" t="n">
         <v>10</v>
       </c>
-      <c r="H99" s="4" t="n">
+      <c r="H99" s="3" t="n">
         <v>19</v>
       </c>
-      <c r="K99" s="1" t="n">
+      <c r="K99" s="0" t="n">
         <f aca="false">$C$97+H99-$B$84/2-$E$90-50</f>
         <v>115</v>
       </c>
@@ -1747,73 +1770,73 @@
       <c r="B101" s="0" t="s">
         <v>0</v>
       </c>
-      <c r="J101" s="8" t="s">
+      <c r="J101" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="K101" s="8" t="s">
+      <c r="K101" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="L101" s="8" t="s">
+      <c r="L101" s="7" t="s">
         <v>23</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="102">
-      <c r="A102" s="2"/>
-      <c r="B102" s="2" t="s">
+      <c r="A102" s="1"/>
+      <c r="B102" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C102" s="2" t="s">
+      <c r="C102" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D102" s="2" t="s">
+      <c r="D102" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="J102" s="6" t="n">
+      <c r="J102" s="5" t="n">
         <f aca="false">AVERAGE(K90:K99)</f>
         <v>114.55</v>
       </c>
-      <c r="K102" s="1" t="n">
+      <c r="K102" s="0" t="n">
         <f aca="false">STDEV(K90:K99)</f>
         <v>0.437797517886195</v>
       </c>
-      <c r="L102" s="1" t="n">
+      <c r="L102" s="0" t="n">
         <f aca="false">K102/SQRT(COUNT(K90:K99))</f>
         <v>0.138443731048868</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="103">
-      <c r="A103" s="2" t="s">
+      <c r="A103" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B103" s="2" t="n">
+      <c r="B103" s="1" t="n">
         <v>233</v>
       </c>
-      <c r="C103" s="2" t="n">
+      <c r="C103" s="1" t="n">
         <v>540</v>
       </c>
-      <c r="D103" s="2" t="n">
+      <c r="D103" s="1" t="n">
         <v>1049</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="104">
-      <c r="A104" s="2" t="s">
+      <c r="A104" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B104" s="2" t="n">
+      <c r="B104" s="1" t="n">
         <v>38</v>
       </c>
-      <c r="C104" s="2" t="n">
+      <c r="C104" s="1" t="n">
         <v>52</v>
       </c>
-      <c r="D104" s="2" t="n">
+      <c r="D104" s="1" t="n">
         <v>65</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="108">
-      <c r="A108" s="3" t="s">
+      <c r="A108" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="B108" s="3" t="s">
+      <c r="B108" s="2" t="s">
         <v>24</v>
       </c>
     </row>
@@ -1821,17 +1844,23 @@
       <c r="B109" s="0" t="s">
         <v>17</v>
       </c>
-      <c r="G109" s="4" t="s">
+      <c r="G109" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="H109" s="4" t="s">
+      <c r="H109" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="J109" s="5" t="s">
+      <c r="J109" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="K109" s="5" t="s">
+      <c r="K109" s="4" t="s">
         <v>12</v>
+      </c>
+      <c r="M109" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="N109" s="0" t="s">
+        <v>14</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="110">
@@ -1844,36 +1873,44 @@
       <c r="D110" s="0" t="s">
         <v>16</v>
       </c>
-      <c r="E110" s="6" t="n">
+      <c r="E110" s="5" t="n">
         <f aca="false">C110-B104/2</f>
         <v>265</v>
       </c>
-      <c r="G110" s="4" t="n">
+      <c r="G110" s="3" t="n">
         <v>1</v>
       </c>
-      <c r="H110" s="4" t="n">
+      <c r="H110" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="J110" s="6" t="n">
+      <c r="J110" s="5" t="n">
         <f aca="false">E113-E115</f>
         <v>86</v>
       </c>
-      <c r="K110" s="1" t="n">
+      <c r="K110" s="0" t="n">
         <f aca="false">$C$117+H110-$B$104/2-$E$110-50</f>
         <v>56</v>
+      </c>
+      <c r="M110" s="5" t="n">
+        <f aca="false">B103*0.001/(C103*0.001)</f>
+        <v>0.431481481481481</v>
+      </c>
+      <c r="N110" s="5" t="n">
+        <f aca="false">$M$110*$J$122^2/$J$110^2</f>
+        <v>0.191881057453478</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="111">
       <c r="B111" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="G111" s="4" t="n">
+      <c r="G111" s="3" t="n">
         <v>2</v>
       </c>
-      <c r="H111" s="4" t="n">
+      <c r="H111" s="3" t="n">
         <v>20.5</v>
       </c>
-      <c r="K111" s="1" t="n">
+      <c r="K111" s="0" t="n">
         <f aca="false">$C$117+H111-$B$104/2-$E$110-50</f>
         <v>56.5</v>
       </c>
@@ -1882,13 +1919,13 @@
       <c r="B112" s="0" t="s">
         <v>18</v>
       </c>
-      <c r="G112" s="4" t="n">
+      <c r="G112" s="3" t="n">
         <v>3</v>
       </c>
-      <c r="H112" s="4" t="n">
+      <c r="H112" s="3" t="n">
         <v>20.5</v>
       </c>
-      <c r="K112" s="1" t="n">
+      <c r="K112" s="0" t="n">
         <f aca="false">$C$117+H112-$B$104/2-$E$110-50</f>
         <v>56.5</v>
       </c>
@@ -1897,24 +1934,24 @@
       <c r="B113" s="0" t="s">
         <v>15</v>
       </c>
-      <c r="C113" s="6" t="n">
+      <c r="C113" s="5" t="n">
         <f aca="false">C110-B104</f>
         <v>246</v>
       </c>
       <c r="D113" s="0" t="s">
         <v>16</v>
       </c>
-      <c r="E113" s="6" t="n">
+      <c r="E113" s="5" t="n">
         <f aca="false">C113-C104/2</f>
         <v>220</v>
       </c>
-      <c r="G113" s="4" t="n">
+      <c r="G113" s="3" t="n">
         <v>4</v>
       </c>
-      <c r="H113" s="4" t="n">
+      <c r="H113" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="K113" s="1" t="n">
+      <c r="K113" s="0" t="n">
         <f aca="false">$C$117+H113-$B$104/2-$E$110-50</f>
         <v>56</v>
       </c>
@@ -1923,13 +1960,13 @@
       <c r="B114" s="0" t="s">
         <v>19</v>
       </c>
-      <c r="G114" s="4" t="n">
+      <c r="G114" s="3" t="n">
         <v>5</v>
       </c>
-      <c r="H114" s="4" t="n">
+      <c r="H114" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="K114" s="1" t="n">
+      <c r="K114" s="0" t="n">
         <f aca="false">$C$117+H114-$B$104/2-$E$110-50</f>
         <v>56</v>
       </c>
@@ -1944,29 +1981,29 @@
       <c r="D115" s="0" t="s">
         <v>16</v>
       </c>
-      <c r="E115" s="6" t="n">
+      <c r="E115" s="5" t="n">
         <f aca="false">C115-C104/2</f>
         <v>134</v>
       </c>
-      <c r="G115" s="4" t="n">
+      <c r="G115" s="3" t="n">
         <v>6</v>
       </c>
-      <c r="H115" s="4" t="n">
+      <c r="H115" s="3" t="n">
         <v>23</v>
       </c>
-      <c r="K115" s="1" t="n">
+      <c r="K115" s="0" t="n">
         <f aca="false">$C$117+H115-$B$104/2-$E$110-50</f>
         <v>59</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="116">
-      <c r="G116" s="4" t="n">
+      <c r="G116" s="3" t="n">
         <v>7</v>
       </c>
-      <c r="H116" s="4" t="n">
+      <c r="H116" s="3" t="n">
         <v>23</v>
       </c>
-      <c r="K116" s="1" t="n">
+      <c r="K116" s="0" t="n">
         <f aca="false">$C$117+H116-$B$104/2-$E$110-50</f>
         <v>59</v>
       </c>
@@ -1975,40 +2012,40 @@
       <c r="B117" s="0" t="s">
         <v>20</v>
       </c>
-      <c r="C117" s="7" t="n">
+      <c r="C117" s="6" t="n">
         <v>370</v>
       </c>
-      <c r="G117" s="4" t="n">
+      <c r="G117" s="3" t="n">
         <v>8</v>
       </c>
-      <c r="H117" s="4" t="n">
+      <c r="H117" s="3" t="n">
         <v>21.5</v>
       </c>
-      <c r="K117" s="1" t="n">
+      <c r="K117" s="0" t="n">
         <f aca="false">$C$117+H117-$B$104/2-$E$110-50</f>
         <v>57.5</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="118">
-      <c r="G118" s="4" t="n">
+      <c r="G118" s="3" t="n">
         <v>9</v>
       </c>
-      <c r="H118" s="4" t="n">
+      <c r="H118" s="3" t="n">
         <v>23</v>
       </c>
-      <c r="K118" s="1" t="n">
+      <c r="K118" s="0" t="n">
         <f aca="false">$C$117+H118-$B$104/2-$E$110-50</f>
         <v>59</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="119">
-      <c r="G119" s="4" t="n">
+      <c r="G119" s="3" t="n">
         <v>10</v>
       </c>
-      <c r="H119" s="4" t="n">
+      <c r="H119" s="3" t="n">
         <v>22</v>
       </c>
-      <c r="K119" s="1" t="n">
+      <c r="K119" s="0" t="n">
         <f aca="false">$C$117+H119-$B$104/2-$E$110-50</f>
         <v>58</v>
       </c>
@@ -2017,73 +2054,73 @@
       <c r="B121" s="0" t="s">
         <v>0</v>
       </c>
-      <c r="J121" s="8" t="s">
+      <c r="J121" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="K121" s="8" t="s">
+      <c r="K121" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="L121" s="8" t="s">
+      <c r="L121" s="7" t="s">
         <v>23</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="122">
-      <c r="A122" s="2"/>
-      <c r="B122" s="2" t="s">
+      <c r="A122" s="1"/>
+      <c r="B122" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C122" s="2" t="s">
+      <c r="C122" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D122" s="2" t="s">
+      <c r="D122" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="J122" s="6" t="n">
+      <c r="J122" s="5" t="n">
         <f aca="false">AVERAGE(K110:K119)</f>
         <v>57.35</v>
       </c>
-      <c r="K122" s="1" t="n">
+      <c r="K122" s="0" t="n">
         <f aca="false">STDEV(K110:K119)</f>
         <v>1.31339255365643</v>
       </c>
-      <c r="L122" s="1" t="n">
+      <c r="L122" s="0" t="n">
         <f aca="false">K122/SQRT(COUNT(K110:K119))</f>
         <v>0.415331193145923</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="123">
-      <c r="A123" s="2" t="s">
+      <c r="A123" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B123" s="2" t="n">
+      <c r="B123" s="1" t="n">
         <v>233</v>
       </c>
-      <c r="C123" s="2" t="n">
+      <c r="C123" s="1" t="n">
         <v>540</v>
       </c>
-      <c r="D123" s="2" t="n">
+      <c r="D123" s="1" t="n">
         <v>1049</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="124">
-      <c r="A124" s="2" t="s">
+      <c r="A124" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B124" s="2" t="n">
+      <c r="B124" s="1" t="n">
         <v>38</v>
       </c>
-      <c r="C124" s="2" t="n">
+      <c r="C124" s="1" t="n">
         <v>52</v>
       </c>
-      <c r="D124" s="2" t="n">
+      <c r="D124" s="1" t="n">
         <v>65</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="128">
-      <c r="A128" s="3" t="s">
+      <c r="A128" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="B128" s="3" t="s">
+      <c r="B128" s="2" t="s">
         <v>7</v>
       </c>
     </row>
@@ -2091,16 +2128,16 @@
       <c r="B129" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="G129" s="4" t="s">
+      <c r="G129" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="H129" s="4" t="s">
+      <c r="H129" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="J129" s="5" t="s">
+      <c r="J129" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="K129" s="5" t="s">
+      <c r="K129" s="4" t="s">
         <v>12</v>
       </c>
       <c r="M129" s="0" t="s">
@@ -2120,29 +2157,29 @@
       <c r="D130" s="0" t="s">
         <v>16</v>
       </c>
-      <c r="E130" s="6" t="n">
+      <c r="E130" s="5" t="n">
         <f aca="false">C130-C124/2</f>
         <v>271</v>
       </c>
-      <c r="G130" s="4" t="n">
+      <c r="G130" s="3" t="n">
         <v>1</v>
       </c>
-      <c r="H130" s="4" t="n">
+      <c r="H130" s="3" t="n">
         <v>29</v>
       </c>
-      <c r="J130" s="6" t="n">
+      <c r="J130" s="5" t="n">
         <f aca="false">E133-E135</f>
         <v>95</v>
       </c>
-      <c r="K130" s="1" t="n">
+      <c r="K130" s="0" t="n">
         <f aca="false">$C$137+H130-$C$124/2-$E$130-50</f>
         <v>92</v>
       </c>
-      <c r="M130" s="6" t="n">
+      <c r="M130" s="5" t="n">
         <f aca="false">C123*0.001/(C123*0.001)</f>
         <v>1</v>
       </c>
-      <c r="N130" s="6" t="n">
+      <c r="N130" s="5" t="n">
         <f aca="false">$M$130*$J$142^2/$J$130^2</f>
         <v>0.948060941828255</v>
       </c>
@@ -2151,13 +2188,13 @@
       <c r="B131" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="G131" s="4" t="n">
+      <c r="G131" s="3" t="n">
         <v>2</v>
       </c>
-      <c r="H131" s="4" t="n">
+      <c r="H131" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="K131" s="1" t="n">
+      <c r="K131" s="0" t="n">
         <f aca="false">$C$137+H131-$C$124/2-$E$130-50</f>
         <v>93</v>
       </c>
@@ -2166,13 +2203,13 @@
       <c r="B132" s="0" t="s">
         <v>18</v>
       </c>
-      <c r="G132" s="4" t="n">
+      <c r="G132" s="3" t="n">
         <v>3</v>
       </c>
-      <c r="H132" s="4" t="n">
+      <c r="H132" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="K132" s="1" t="n">
+      <c r="K132" s="0" t="n">
         <f aca="false">$C$137+H132-$C$124/2-$E$130-50</f>
         <v>93</v>
       </c>
@@ -2181,24 +2218,24 @@
       <c r="B133" s="0" t="s">
         <v>15</v>
       </c>
-      <c r="C133" s="6" t="n">
+      <c r="C133" s="5" t="n">
         <f aca="false">C130-C124</f>
         <v>245</v>
       </c>
       <c r="D133" s="0" t="s">
         <v>16</v>
       </c>
-      <c r="E133" s="6" t="n">
+      <c r="E133" s="5" t="n">
         <f aca="false">C133-C124/2</f>
         <v>219</v>
       </c>
-      <c r="G133" s="4" t="n">
+      <c r="G133" s="3" t="n">
         <v>4</v>
       </c>
-      <c r="H133" s="4" t="n">
+      <c r="H133" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="K133" s="1" t="n">
+      <c r="K133" s="0" t="n">
         <f aca="false">$C$137+H133-$C$124/2-$E$130-50</f>
         <v>93</v>
       </c>
@@ -2207,13 +2244,13 @@
       <c r="B134" s="0" t="s">
         <v>19</v>
       </c>
-      <c r="G134" s="4" t="n">
+      <c r="G134" s="3" t="n">
         <v>5</v>
       </c>
-      <c r="H134" s="4" t="n">
+      <c r="H134" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="K134" s="1" t="n">
+      <c r="K134" s="0" t="n">
         <f aca="false">$C$137+H134-$C$124/2-$E$130-50</f>
         <v>93</v>
       </c>
@@ -2228,29 +2265,29 @@
       <c r="D135" s="0" t="s">
         <v>16</v>
       </c>
-      <c r="E135" s="6" t="n">
+      <c r="E135" s="5" t="n">
         <f aca="false">C135-C124/2</f>
         <v>124</v>
       </c>
-      <c r="G135" s="4" t="n">
+      <c r="G135" s="3" t="n">
         <v>6</v>
       </c>
-      <c r="H135" s="4" t="n">
+      <c r="H135" s="3" t="n">
         <v>29.5</v>
       </c>
-      <c r="K135" s="1" t="n">
+      <c r="K135" s="0" t="n">
         <f aca="false">$C$137+H135-$C$124/2-$E$130-50</f>
         <v>92.5</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="136">
-      <c r="G136" s="4" t="n">
+      <c r="G136" s="3" t="n">
         <v>7</v>
       </c>
-      <c r="H136" s="4" t="n">
+      <c r="H136" s="3" t="n">
         <v>29</v>
       </c>
-      <c r="K136" s="1" t="n">
+      <c r="K136" s="0" t="n">
         <f aca="false">$C$137+H136-$C$124/2-$E$130-50</f>
         <v>92</v>
       </c>
@@ -2259,40 +2296,40 @@
       <c r="B137" s="0" t="s">
         <v>20</v>
       </c>
-      <c r="C137" s="7" t="n">
+      <c r="C137" s="6" t="n">
         <v>410</v>
       </c>
-      <c r="G137" s="4" t="n">
+      <c r="G137" s="3" t="n">
         <v>8</v>
       </c>
-      <c r="H137" s="4" t="n">
+      <c r="H137" s="3" t="n">
         <v>29</v>
       </c>
-      <c r="K137" s="1" t="n">
+      <c r="K137" s="0" t="n">
         <f aca="false">$C$137+H137-$C$124/2-$E$130-50</f>
         <v>92</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="138">
-      <c r="G138" s="4" t="n">
+      <c r="G138" s="3" t="n">
         <v>9</v>
       </c>
-      <c r="H138" s="4" t="n">
+      <c r="H138" s="3" t="n">
         <v>29.5</v>
       </c>
-      <c r="K138" s="1" t="n">
+      <c r="K138" s="0" t="n">
         <f aca="false">$C$137+H138-$C$124/2-$E$130-50</f>
         <v>92.5</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="139">
-      <c r="G139" s="4" t="n">
+      <c r="G139" s="3" t="n">
         <v>10</v>
       </c>
-      <c r="H139" s="4" t="n">
+      <c r="H139" s="3" t="n">
         <v>29</v>
       </c>
-      <c r="K139" s="1" t="n">
+      <c r="K139" s="0" t="n">
         <f aca="false">$C$137+H139-$C$124/2-$E$130-50</f>
         <v>92</v>
       </c>
@@ -2301,73 +2338,73 @@
       <c r="B141" s="0" t="s">
         <v>0</v>
       </c>
-      <c r="J141" s="8" t="s">
+      <c r="J141" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="K141" s="8" t="s">
+      <c r="K141" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="L141" s="8" t="s">
+      <c r="L141" s="7" t="s">
         <v>23</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="142">
-      <c r="A142" s="2"/>
-      <c r="B142" s="2" t="s">
+      <c r="A142" s="1"/>
+      <c r="B142" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C142" s="2" t="s">
+      <c r="C142" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D142" s="2" t="s">
+      <c r="D142" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="J142" s="6" t="n">
+      <c r="J142" s="5" t="n">
         <f aca="false">AVERAGE(K130:K139)</f>
         <v>92.5</v>
       </c>
-      <c r="K142" s="1" t="n">
+      <c r="K142" s="0" t="n">
         <f aca="false">STDEV(K130:K139)</f>
         <v>0.471404520791032</v>
       </c>
-      <c r="L142" s="1" t="n">
+      <c r="L142" s="0" t="n">
         <f aca="false">K142/SQRT(COUNT(K130:K139))</f>
         <v>0.149071198499986</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="143">
-      <c r="A143" s="2" t="s">
+      <c r="A143" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B143" s="2" t="n">
+      <c r="B143" s="1" t="n">
         <v>233</v>
       </c>
-      <c r="C143" s="2" t="n">
+      <c r="C143" s="1" t="n">
         <v>540</v>
       </c>
-      <c r="D143" s="2" t="n">
+      <c r="D143" s="1" t="n">
         <v>1049</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="144">
-      <c r="A144" s="2" t="s">
+      <c r="A144" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B144" s="2" t="n">
+      <c r="B144" s="1" t="n">
         <v>38</v>
       </c>
-      <c r="C144" s="2" t="n">
+      <c r="C144" s="1" t="n">
         <v>52</v>
       </c>
-      <c r="D144" s="2" t="n">
+      <c r="D144" s="1" t="n">
         <v>65</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="148">
-      <c r="A148" s="3" t="s">
+      <c r="A148" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="B148" s="3" t="s">
+      <c r="B148" s="2" t="s">
         <v>24</v>
       </c>
     </row>
@@ -2375,17 +2412,23 @@
       <c r="B149" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="G149" s="4" t="s">
+      <c r="G149" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="H149" s="4" t="s">
+      <c r="H149" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="J149" s="5" t="s">
+      <c r="J149" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="K149" s="5" t="s">
+      <c r="K149" s="4" t="s">
         <v>12</v>
+      </c>
+      <c r="M149" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="N149" s="0" t="s">
+        <v>14</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="150">
@@ -2398,36 +2441,44 @@
       <c r="D150" s="0" t="s">
         <v>16</v>
       </c>
-      <c r="E150" s="6" t="n">
+      <c r="E150" s="5" t="n">
         <f aca="false">C150-C144/2</f>
         <v>271</v>
       </c>
-      <c r="G150" s="4" t="n">
+      <c r="G150" s="3" t="n">
         <v>1</v>
       </c>
-      <c r="H150" s="4" t="n">
+      <c r="H150" s="3" t="n">
         <v>32</v>
       </c>
-      <c r="J150" s="6" t="n">
+      <c r="J150" s="5" t="n">
         <f aca="false">E153-E155</f>
         <v>95</v>
       </c>
-      <c r="K150" s="1" t="n">
+      <c r="K150" s="0" t="n">
         <f aca="false">$C$157+H150-$C$144/2-$E$150-50</f>
         <v>45</v>
+      </c>
+      <c r="M150" s="5" t="n">
+        <f aca="false">C143*0.001/(C143*0.001)</f>
+        <v>1</v>
+      </c>
+      <c r="N150" s="5" t="n">
+        <f aca="false">$M$150*$J$162^2/$J$150^2</f>
+        <v>0.226876731301939</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="151">
       <c r="B151" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="G151" s="4" t="n">
+      <c r="G151" s="3" t="n">
         <v>2</v>
       </c>
-      <c r="H151" s="4" t="n">
+      <c r="H151" s="3" t="n">
         <v>33</v>
       </c>
-      <c r="K151" s="1" t="n">
+      <c r="K151" s="0" t="n">
         <f aca="false">$C$157+H151-$C$144/2-$E$150-50</f>
         <v>46</v>
       </c>
@@ -2436,13 +2487,13 @@
       <c r="B152" s="0" t="s">
         <v>18</v>
       </c>
-      <c r="G152" s="4" t="n">
+      <c r="G152" s="3" t="n">
         <v>3</v>
       </c>
-      <c r="H152" s="4" t="n">
+      <c r="H152" s="3" t="n">
         <v>33</v>
       </c>
-      <c r="K152" s="1" t="n">
+      <c r="K152" s="0" t="n">
         <f aca="false">$C$157+H152-$C$144/2-$E$150-50</f>
         <v>46</v>
       </c>
@@ -2451,24 +2502,24 @@
       <c r="B153" s="0" t="s">
         <v>15</v>
       </c>
-      <c r="C153" s="6" t="n">
+      <c r="C153" s="5" t="n">
         <f aca="false">C150-C144</f>
         <v>245</v>
       </c>
       <c r="D153" s="0" t="s">
         <v>16</v>
       </c>
-      <c r="E153" s="6" t="n">
+      <c r="E153" s="5" t="n">
         <f aca="false">C153-C144/2</f>
         <v>219</v>
       </c>
-      <c r="G153" s="4" t="n">
+      <c r="G153" s="3" t="n">
         <v>4</v>
       </c>
-      <c r="H153" s="4" t="n">
+      <c r="H153" s="3" t="n">
         <v>32</v>
       </c>
-      <c r="K153" s="1" t="n">
+      <c r="K153" s="0" t="n">
         <f aca="false">$C$157+H153-$C$144/2-$E$150-50</f>
         <v>45</v>
       </c>
@@ -2477,13 +2528,13 @@
       <c r="B154" s="0" t="s">
         <v>19</v>
       </c>
-      <c r="G154" s="4" t="n">
+      <c r="G154" s="3" t="n">
         <v>5</v>
       </c>
-      <c r="H154" s="4" t="n">
+      <c r="H154" s="3" t="n">
         <v>31</v>
       </c>
-      <c r="K154" s="1" t="n">
+      <c r="K154" s="0" t="n">
         <f aca="false">$C$157+H154-$C$144/2-$E$150-50</f>
         <v>44</v>
       </c>
@@ -2498,29 +2549,29 @@
       <c r="D155" s="0" t="s">
         <v>16</v>
       </c>
-      <c r="E155" s="6" t="n">
+      <c r="E155" s="5" t="n">
         <f aca="false">C155-C144/2</f>
         <v>124</v>
       </c>
-      <c r="G155" s="4" t="n">
+      <c r="G155" s="3" t="n">
         <v>6</v>
       </c>
-      <c r="H155" s="4" t="n">
+      <c r="H155" s="3" t="n">
         <v>34.5</v>
       </c>
-      <c r="K155" s="1" t="n">
+      <c r="K155" s="0" t="n">
         <f aca="false">$C$157+H155-$C$144/2-$E$150-50</f>
         <v>47.5</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="156">
-      <c r="G156" s="4" t="n">
+      <c r="G156" s="3" t="n">
         <v>7</v>
       </c>
-      <c r="H156" s="4" t="n">
+      <c r="H156" s="3" t="n">
         <v>31</v>
       </c>
-      <c r="K156" s="1" t="n">
+      <c r="K156" s="0" t="n">
         <f aca="false">$C$157+H156-$C$144/2-$E$150-50</f>
         <v>44</v>
       </c>
@@ -2529,40 +2580,40 @@
       <c r="B157" s="0" t="s">
         <v>20</v>
       </c>
-      <c r="C157" s="7" t="n">
+      <c r="C157" s="6" t="n">
         <v>360</v>
       </c>
-      <c r="G157" s="4" t="n">
+      <c r="G157" s="3" t="n">
         <v>8</v>
       </c>
-      <c r="H157" s="4" t="n">
+      <c r="H157" s="3" t="n">
         <v>31</v>
       </c>
-      <c r="K157" s="1" t="n">
+      <c r="K157" s="0" t="n">
         <f aca="false">$C$157+H157-$C$144/2-$E$150-50</f>
         <v>44</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="158">
-      <c r="G158" s="4" t="n">
+      <c r="G158" s="3" t="n">
         <v>9</v>
       </c>
-      <c r="H158" s="4" t="n">
+      <c r="H158" s="3" t="n">
         <v>31.5</v>
       </c>
-      <c r="K158" s="1" t="n">
+      <c r="K158" s="0" t="n">
         <f aca="false">$C$157+H158-$C$144/2-$E$150-50</f>
         <v>44.5</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="159">
-      <c r="G159" s="4" t="n">
+      <c r="G159" s="3" t="n">
         <v>10</v>
       </c>
-      <c r="H159" s="4" t="n">
+      <c r="H159" s="3" t="n">
         <v>33.5</v>
       </c>
-      <c r="K159" s="1" t="n">
+      <c r="K159" s="0" t="n">
         <f aca="false">$C$157+H159-$C$144/2-$E$150-50</f>
         <v>46.5</v>
       </c>
@@ -2571,73 +2622,73 @@
       <c r="B161" s="0" t="s">
         <v>0</v>
       </c>
-      <c r="J161" s="8" t="s">
+      <c r="J161" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="K161" s="8" t="s">
+      <c r="K161" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="L161" s="8" t="s">
+      <c r="L161" s="7" t="s">
         <v>23</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="162">
-      <c r="A162" s="2"/>
-      <c r="B162" s="2" t="s">
+      <c r="A162" s="1"/>
+      <c r="B162" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C162" s="2" t="s">
+      <c r="C162" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D162" s="2" t="s">
+      <c r="D162" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="J162" s="6" t="n">
+      <c r="J162" s="5" t="n">
         <f aca="false">AVERAGE(K150:K159)</f>
         <v>45.25</v>
       </c>
-      <c r="K162" s="1" t="n">
+      <c r="K162" s="0" t="n">
         <f aca="false">STDEV(K150:K159)</f>
         <v>1.20761472884912</v>
       </c>
-      <c r="L162" s="1" t="n">
+      <c r="L162" s="0" t="n">
         <f aca="false">K162/SQRT(COUNT(K150:K159))</f>
         <v>0.381881307912987</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="163">
-      <c r="A163" s="2" t="s">
+      <c r="A163" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B163" s="2" t="n">
+      <c r="B163" s="1" t="n">
         <v>233</v>
       </c>
-      <c r="C163" s="2" t="n">
+      <c r="C163" s="1" t="n">
         <v>540</v>
       </c>
-      <c r="D163" s="2" t="n">
+      <c r="D163" s="1" t="n">
         <v>1049</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="164">
-      <c r="A164" s="2" t="s">
+      <c r="A164" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B164" s="2" t="n">
+      <c r="B164" s="1" t="n">
         <v>38</v>
       </c>
-      <c r="C164" s="2" t="n">
+      <c r="C164" s="1" t="n">
         <v>52</v>
       </c>
-      <c r="D164" s="2" t="n">
+      <c r="D164" s="1" t="n">
         <v>65</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="168">
-      <c r="A168" s="3" t="s">
+      <c r="A168" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="B168" s="3" t="s">
+      <c r="B168" s="2" t="s">
         <v>7</v>
       </c>
     </row>
@@ -2645,16 +2696,16 @@
       <c r="B169" s="0" t="s">
         <v>26</v>
       </c>
-      <c r="G169" s="4" t="s">
+      <c r="G169" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="H169" s="4" t="s">
+      <c r="H169" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="J169" s="5" t="s">
+      <c r="J169" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="K169" s="5" t="s">
+      <c r="K169" s="4" t="s">
         <v>12</v>
       </c>
       <c r="M169" s="0" t="s">
@@ -2674,29 +2725,29 @@
       <c r="D170" s="0" t="s">
         <v>16</v>
       </c>
-      <c r="E170" s="6" t="n">
+      <c r="E170" s="5" t="n">
         <f aca="false">C170-D164/2</f>
         <v>277</v>
       </c>
-      <c r="G170" s="4" t="n">
+      <c r="G170" s="3" t="n">
         <v>1</v>
       </c>
-      <c r="H170" s="4" t="n">
+      <c r="H170" s="3" t="n">
         <v>36</v>
       </c>
-      <c r="J170" s="6" t="n">
+      <c r="J170" s="5" t="n">
         <f aca="false">E173-E175</f>
         <v>146</v>
       </c>
-      <c r="K170" s="1" t="n">
+      <c r="K170" s="0" t="n">
         <f aca="false">$C$177+H170-$D$164/2-$E$170-50</f>
         <v>96.5</v>
       </c>
-      <c r="M170" s="6" t="n">
+      <c r="M170" s="5" t="n">
         <f aca="false">D163*0.001/(C163*0.001)</f>
         <v>1.94259259259259</v>
       </c>
-      <c r="N170" s="6" t="n">
+      <c r="N170" s="5" t="n">
         <f aca="false">$M$170*$J$182^2/$J$170^2</f>
         <v>0.84865396276836</v>
       </c>
@@ -2705,13 +2756,13 @@
       <c r="B171" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="G171" s="4" t="n">
+      <c r="G171" s="3" t="n">
         <v>2</v>
       </c>
-      <c r="H171" s="4" t="n">
+      <c r="H171" s="3" t="n">
         <v>37</v>
       </c>
-      <c r="K171" s="1" t="n">
+      <c r="K171" s="0" t="n">
         <f aca="false">$C$177+H171-$D$164/2-$E$170-50</f>
         <v>97.5</v>
       </c>
@@ -2720,13 +2771,13 @@
       <c r="B172" s="0" t="s">
         <v>18</v>
       </c>
-      <c r="G172" s="4" t="n">
+      <c r="G172" s="3" t="n">
         <v>3</v>
       </c>
-      <c r="H172" s="4" t="n">
+      <c r="H172" s="3" t="n">
         <v>37</v>
       </c>
-      <c r="K172" s="1" t="n">
+      <c r="K172" s="0" t="n">
         <f aca="false">$C$177+H172-$D$164/2-$E$170-50</f>
         <v>97.5</v>
       </c>
@@ -2741,17 +2792,17 @@
       <c r="D173" s="0" t="s">
         <v>16</v>
       </c>
-      <c r="E173" s="6" t="n">
+      <c r="E173" s="5" t="n">
         <f aca="false">C173-C164/2</f>
         <v>220</v>
       </c>
-      <c r="G173" s="4" t="n">
+      <c r="G173" s="3" t="n">
         <v>4</v>
       </c>
-      <c r="H173" s="4" t="n">
+      <c r="H173" s="3" t="n">
         <v>36.5</v>
       </c>
-      <c r="K173" s="1" t="n">
+      <c r="K173" s="0" t="n">
         <f aca="false">$C$177+H173-$D$164/2-$E$170-50</f>
         <v>97</v>
       </c>
@@ -2760,13 +2811,13 @@
       <c r="B174" s="0" t="s">
         <v>19</v>
       </c>
-      <c r="G174" s="4" t="n">
+      <c r="G174" s="3" t="n">
         <v>5</v>
       </c>
-      <c r="H174" s="4" t="n">
+      <c r="H174" s="3" t="n">
         <v>36</v>
       </c>
-      <c r="K174" s="1" t="n">
+      <c r="K174" s="0" t="n">
         <f aca="false">$C$177+H174-$D$164/2-$E$170-50</f>
         <v>96.5</v>
       </c>
@@ -2781,29 +2832,29 @@
       <c r="D175" s="0" t="s">
         <v>16</v>
       </c>
-      <c r="E175" s="6" t="n">
+      <c r="E175" s="5" t="n">
         <f aca="false">C175-C164/2</f>
         <v>74</v>
       </c>
-      <c r="G175" s="4" t="n">
+      <c r="G175" s="3" t="n">
         <v>6</v>
       </c>
-      <c r="H175" s="4" t="n">
+      <c r="H175" s="3" t="n">
         <v>36</v>
       </c>
-      <c r="K175" s="1" t="n">
+      <c r="K175" s="0" t="n">
         <f aca="false">$C$177+H175-$D$164/2-$E$170-50</f>
         <v>96.5</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="176">
-      <c r="G176" s="4" t="n">
+      <c r="G176" s="3" t="n">
         <v>7</v>
       </c>
-      <c r="H176" s="4" t="n">
+      <c r="H176" s="3" t="n">
         <v>36</v>
       </c>
-      <c r="K176" s="1" t="n">
+      <c r="K176" s="0" t="n">
         <f aca="false">$C$177+H176-$D$164/2-$E$170-50</f>
         <v>96.5</v>
       </c>
@@ -2812,40 +2863,40 @@
       <c r="B177" s="0" t="s">
         <v>20</v>
       </c>
-      <c r="C177" s="7" t="n">
+      <c r="C177" s="6" t="n">
         <v>420</v>
       </c>
-      <c r="G177" s="4" t="n">
+      <c r="G177" s="3" t="n">
         <v>8</v>
       </c>
-      <c r="H177" s="4" t="n">
+      <c r="H177" s="3" t="n">
         <v>34.5</v>
       </c>
-      <c r="K177" s="1" t="n">
+      <c r="K177" s="0" t="n">
         <f aca="false">$C$177+H177-$D$164/2-$E$170-50</f>
         <v>95</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="178">
-      <c r="G178" s="4" t="n">
+      <c r="G178" s="3" t="n">
         <v>9</v>
       </c>
-      <c r="H178" s="4" t="n">
+      <c r="H178" s="3" t="n">
         <v>35</v>
       </c>
-      <c r="K178" s="1" t="n">
+      <c r="K178" s="0" t="n">
         <f aca="false">$C$177+H178-$D$164/2-$E$170-50</f>
         <v>95.5</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="179">
-      <c r="G179" s="4" t="n">
+      <c r="G179" s="3" t="n">
         <v>10</v>
       </c>
-      <c r="H179" s="4" t="n">
+      <c r="H179" s="3" t="n">
         <v>36</v>
       </c>
-      <c r="K179" s="1" t="n">
+      <c r="K179" s="0" t="n">
         <f aca="false">$C$177+H179-$D$164/2-$E$170-50</f>
         <v>96.5</v>
       </c>
@@ -2854,73 +2905,73 @@
       <c r="B181" s="0" t="s">
         <v>0</v>
       </c>
-      <c r="J181" s="8" t="s">
+      <c r="J181" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="K181" s="8" t="s">
+      <c r="K181" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="L181" s="8" t="s">
+      <c r="L181" s="7" t="s">
         <v>23</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="182">
-      <c r="A182" s="2"/>
-      <c r="B182" s="2" t="s">
+      <c r="A182" s="1"/>
+      <c r="B182" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C182" s="2" t="s">
+      <c r="C182" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D182" s="2" t="s">
+      <c r="D182" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="J182" s="6" t="n">
+      <c r="J182" s="5" t="n">
         <f aca="false">AVERAGE(K170:K179)</f>
         <v>96.5</v>
       </c>
-      <c r="K182" s="1" t="n">
+      <c r="K182" s="0" t="n">
         <f aca="false">STDEV(K170:K179)</f>
         <v>0.781735959970572</v>
       </c>
-      <c r="L182" s="1" t="n">
+      <c r="L182" s="0" t="n">
         <f aca="false">K182/SQRT(COUNT(K170:K179))</f>
         <v>0.247206616236522</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="183">
-      <c r="A183" s="2" t="s">
+      <c r="A183" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B183" s="2" t="n">
+      <c r="B183" s="1" t="n">
         <v>233</v>
       </c>
-      <c r="C183" s="2" t="n">
+      <c r="C183" s="1" t="n">
         <v>540</v>
       </c>
-      <c r="D183" s="2" t="n">
+      <c r="D183" s="1" t="n">
         <v>1049</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="184">
-      <c r="A184" s="2" t="s">
+      <c r="A184" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B184" s="2" t="n">
+      <c r="B184" s="1" t="n">
         <v>38</v>
       </c>
-      <c r="C184" s="2" t="n">
+      <c r="C184" s="1" t="n">
         <v>52</v>
       </c>
-      <c r="D184" s="2" t="n">
+      <c r="D184" s="1" t="n">
         <v>65</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="188">
-      <c r="A188" s="3" t="s">
+      <c r="A188" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="B188" s="3" t="s">
+      <c r="B188" s="2" t="s">
         <v>24</v>
       </c>
     </row>
@@ -2928,17 +2979,23 @@
       <c r="B189" s="0" t="s">
         <v>26</v>
       </c>
-      <c r="G189" s="4" t="s">
+      <c r="G189" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="H189" s="4" t="s">
+      <c r="H189" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="J189" s="5" t="s">
+      <c r="J189" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="K189" s="5" t="s">
+      <c r="K189" s="4" t="s">
         <v>12</v>
+      </c>
+      <c r="M189" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="N189" s="0" t="s">
+        <v>14</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="190">
@@ -2951,36 +3008,44 @@
       <c r="D190" s="0" t="s">
         <v>16</v>
       </c>
-      <c r="E190" s="6" t="n">
+      <c r="E190" s="5" t="n">
         <f aca="false">C190-D184/2</f>
         <v>277</v>
       </c>
-      <c r="G190" s="4" t="n">
+      <c r="G190" s="3" t="n">
         <v>1</v>
       </c>
-      <c r="H190" s="4" t="n">
+      <c r="H190" s="3" t="n">
         <v>35</v>
       </c>
-      <c r="J190" s="6" t="n">
+      <c r="J190" s="5" t="n">
         <f aca="false">E193-E195</f>
         <v>146</v>
       </c>
-      <c r="K190" s="1" t="n">
+      <c r="K190" s="0" t="n">
         <f aca="false">$C$197+H190-$D$184/2-$E$190-50</f>
         <v>45.5</v>
+      </c>
+      <c r="M190" s="5" t="n">
+        <f aca="false">D183*0.001/(C183*0.001)</f>
+        <v>1.94259259259259</v>
+      </c>
+      <c r="N190" s="5" t="n">
+        <f aca="false">$M$190*$J$202^2/$J$190^2</f>
+        <v>0.196628947000341</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="191">
       <c r="B191" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="G191" s="4" t="n">
+      <c r="G191" s="3" t="n">
         <v>2</v>
       </c>
-      <c r="H191" s="4" t="n">
+      <c r="H191" s="3" t="n">
         <v>35</v>
       </c>
-      <c r="K191" s="1" t="n">
+      <c r="K191" s="0" t="n">
         <f aca="false">$C$197+H191-$D$184/2-$E$190-50</f>
         <v>45.5</v>
       </c>
@@ -2989,13 +3054,13 @@
       <c r="B192" s="0" t="s">
         <v>18</v>
       </c>
-      <c r="G192" s="4" t="n">
+      <c r="G192" s="3" t="n">
         <v>3</v>
       </c>
-      <c r="H192" s="4" t="n">
+      <c r="H192" s="3" t="n">
         <v>36</v>
       </c>
-      <c r="K192" s="1" t="n">
+      <c r="K192" s="0" t="n">
         <f aca="false">$C$197+H192-$D$184/2-$E$190-50</f>
         <v>46.5</v>
       </c>
@@ -3010,17 +3075,17 @@
       <c r="D193" s="0" t="s">
         <v>16</v>
       </c>
-      <c r="E193" s="6" t="n">
+      <c r="E193" s="5" t="n">
         <f aca="false">C193-C184/2</f>
         <v>220</v>
       </c>
-      <c r="G193" s="4" t="n">
+      <c r="G193" s="3" t="n">
         <v>4</v>
       </c>
-      <c r="H193" s="4" t="n">
+      <c r="H193" s="3" t="n">
         <v>38</v>
       </c>
-      <c r="K193" s="1" t="n">
+      <c r="K193" s="0" t="n">
         <f aca="false">$C$197+H193-$D$184/2-$E$190-50</f>
         <v>48.5</v>
       </c>
@@ -3029,13 +3094,13 @@
       <c r="B194" s="0" t="s">
         <v>19</v>
       </c>
-      <c r="G194" s="4" t="n">
+      <c r="G194" s="3" t="n">
         <v>5</v>
       </c>
-      <c r="H194" s="4" t="n">
+      <c r="H194" s="3" t="n">
         <v>35</v>
       </c>
-      <c r="K194" s="1" t="n">
+      <c r="K194" s="0" t="n">
         <f aca="false">$C$197+H194-$D$184/2-$E$190-50</f>
         <v>45.5</v>
       </c>
@@ -3050,29 +3115,29 @@
       <c r="D195" s="0" t="s">
         <v>16</v>
       </c>
-      <c r="E195" s="6" t="n">
+      <c r="E195" s="5" t="n">
         <f aca="false">C195-C184/2</f>
         <v>74</v>
       </c>
-      <c r="G195" s="4" t="n">
+      <c r="G195" s="3" t="n">
         <v>6</v>
       </c>
-      <c r="H195" s="4" t="n">
+      <c r="H195" s="3" t="n">
         <v>34</v>
       </c>
-      <c r="K195" s="1" t="n">
+      <c r="K195" s="0" t="n">
         <f aca="false">$C$197+H195-$D$184/2-$E$190-50</f>
         <v>44.5</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="196">
-      <c r="G196" s="4" t="n">
+      <c r="G196" s="3" t="n">
         <v>7</v>
       </c>
-      <c r="H196" s="4" t="n">
+      <c r="H196" s="3" t="n">
         <v>37.5</v>
       </c>
-      <c r="K196" s="1" t="n">
+      <c r="K196" s="0" t="n">
         <f aca="false">$C$197+H196-$D$184/2-$E$190-50</f>
         <v>48</v>
       </c>
@@ -3081,40 +3146,40 @@
       <c r="B197" s="0" t="s">
         <v>20</v>
       </c>
-      <c r="C197" s="7" t="n">
+      <c r="C197" s="6" t="n">
         <v>370</v>
       </c>
-      <c r="G197" s="4" t="n">
+      <c r="G197" s="3" t="n">
         <v>8</v>
       </c>
-      <c r="H197" s="4" t="n">
+      <c r="H197" s="3" t="n">
         <v>36.5</v>
       </c>
-      <c r="K197" s="1" t="n">
+      <c r="K197" s="0" t="n">
         <f aca="false">$C$197+H197-$D$184/2-$E$190-50</f>
         <v>47</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="198">
-      <c r="G198" s="4" t="n">
+      <c r="G198" s="3" t="n">
         <v>9</v>
       </c>
-      <c r="H198" s="4" t="n">
+      <c r="H198" s="3" t="n">
         <v>36</v>
       </c>
-      <c r="K198" s="1" t="n">
+      <c r="K198" s="0" t="n">
         <f aca="false">$C$197+H198-$D$184/2-$E$190-50</f>
         <v>46.5</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="199">
-      <c r="G199" s="4" t="n">
+      <c r="G199" s="3" t="n">
         <v>10</v>
       </c>
-      <c r="H199" s="4" t="n">
+      <c r="H199" s="3" t="n">
         <v>36.5</v>
       </c>
-      <c r="K199" s="1" t="n">
+      <c r="K199" s="0" t="n">
         <f aca="false">$C$197+H199-$D$184/2-$E$190-50</f>
         <v>47</v>
       </c>
@@ -3123,73 +3188,73 @@
       <c r="B201" s="0" t="s">
         <v>0</v>
       </c>
-      <c r="J201" s="8" t="s">
+      <c r="J201" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="K201" s="8" t="s">
+      <c r="K201" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="L201" s="8" t="s">
+      <c r="L201" s="7" t="s">
         <v>23</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="202">
-      <c r="A202" s="2"/>
-      <c r="B202" s="2" t="s">
+      <c r="A202" s="1"/>
+      <c r="B202" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C202" s="2" t="s">
+      <c r="C202" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D202" s="2" t="s">
+      <c r="D202" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="J202" s="6" t="n">
+      <c r="J202" s="5" t="n">
         <f aca="false">AVERAGE(K190:K199)</f>
         <v>46.45</v>
       </c>
-      <c r="K202" s="1" t="n">
+      <c r="K202" s="0" t="n">
         <f aca="false">STDEV(K190:K199)</f>
         <v>1.23490890352278</v>
       </c>
-      <c r="L202" s="1" t="n">
+      <c r="L202" s="0" t="n">
         <f aca="false">K202/SQRT(COUNT(K190:K199))</f>
         <v>0.390512483795312</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="203">
-      <c r="A203" s="2" t="s">
+      <c r="A203" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B203" s="2" t="n">
+      <c r="B203" s="1" t="n">
         <v>233</v>
       </c>
-      <c r="C203" s="2" t="n">
+      <c r="C203" s="1" t="n">
         <v>540</v>
       </c>
-      <c r="D203" s="2" t="n">
+      <c r="D203" s="1" t="n">
         <v>1049</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="204">
-      <c r="A204" s="2" t="s">
+      <c r="A204" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B204" s="2" t="n">
+      <c r="B204" s="1" t="n">
         <v>38</v>
       </c>
-      <c r="C204" s="2" t="n">
+      <c r="C204" s="1" t="n">
         <v>52</v>
       </c>
-      <c r="D204" s="2" t="n">
+      <c r="D204" s="1" t="n">
         <v>65</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="208">
-      <c r="A208" s="3" t="s">
+      <c r="A208" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="B208" s="3" t="s">
+      <c r="B208" s="2" t="s">
         <v>7</v>
       </c>
     </row>
@@ -3197,16 +3262,16 @@
       <c r="B209" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="G209" s="4" t="s">
+      <c r="G209" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="H209" s="4" t="s">
+      <c r="H209" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="J209" s="5" t="s">
+      <c r="J209" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="K209" s="5" t="s">
+      <c r="K209" s="4" t="s">
         <v>12</v>
       </c>
       <c r="M209" s="0" t="s">
@@ -3226,29 +3291,29 @@
       <c r="D210" s="0" t="s">
         <v>16</v>
       </c>
-      <c r="E210" s="6" t="n">
+      <c r="E210" s="5" t="n">
         <f aca="false">C210-C204/2</f>
         <v>277.5</v>
       </c>
-      <c r="G210" s="4" t="n">
+      <c r="G210" s="3" t="n">
         <v>1</v>
       </c>
-      <c r="H210" s="4" t="n">
+      <c r="H210" s="3" t="n">
         <v>43</v>
       </c>
-      <c r="J210" s="6" t="n">
+      <c r="J210" s="5" t="n">
         <f aca="false">E213-E215</f>
         <v>72.5</v>
       </c>
-      <c r="K210" s="1" t="n">
+      <c r="K210" s="0" t="n">
         <f aca="false">$C$217+H210-$C$204/2-$E$210-50</f>
         <v>89.5</v>
       </c>
-      <c r="M210" s="6" t="n">
+      <c r="M210" s="5" t="n">
         <f aca="false">C203*0.001/(D203*0.001)</f>
         <v>0.514775977121068</v>
       </c>
-      <c r="N210" s="6" t="n">
+      <c r="N210" s="5" t="n">
         <f aca="false">$M$210*$J$222^2/$J$210^2</f>
         <v>0.786245690080242</v>
       </c>
@@ -3257,13 +3322,13 @@
       <c r="B211" s="0" t="s">
         <v>26</v>
       </c>
-      <c r="G211" s="4" t="n">
+      <c r="G211" s="3" t="n">
         <v>2</v>
       </c>
-      <c r="H211" s="4" t="n">
+      <c r="H211" s="3" t="n">
         <v>43</v>
       </c>
-      <c r="K211" s="1" t="n">
+      <c r="K211" s="0" t="n">
         <f aca="false">$C$217+H211-$C$204/2-$E$210-50</f>
         <v>89.5</v>
       </c>
@@ -3272,13 +3337,13 @@
       <c r="B212" s="0" t="s">
         <v>18</v>
       </c>
-      <c r="G212" s="4" t="n">
+      <c r="G212" s="3" t="n">
         <v>3</v>
       </c>
-      <c r="H212" s="4" t="n">
+      <c r="H212" s="3" t="n">
         <v>43</v>
       </c>
-      <c r="K212" s="1" t="n">
+      <c r="K212" s="0" t="n">
         <f aca="false">$C$217+H212-$C$204/2-$E$210-50</f>
         <v>89.5</v>
       </c>
@@ -3293,17 +3358,17 @@
       <c r="D213" s="0" t="s">
         <v>16</v>
       </c>
-      <c r="E213" s="6" t="n">
+      <c r="E213" s="5" t="n">
         <f aca="false">C213-D204/2</f>
         <v>220</v>
       </c>
-      <c r="G213" s="4" t="n">
+      <c r="G213" s="3" t="n">
         <v>4</v>
       </c>
-      <c r="H213" s="4" t="n">
+      <c r="H213" s="3" t="n">
         <v>43</v>
       </c>
-      <c r="K213" s="1" t="n">
+      <c r="K213" s="0" t="n">
         <f aca="false">$C$217+H213-$C$204/2-$E$210-50</f>
         <v>89.5</v>
       </c>
@@ -3312,13 +3377,13 @@
       <c r="B214" s="0" t="s">
         <v>19</v>
       </c>
-      <c r="G214" s="4" t="n">
+      <c r="G214" s="3" t="n">
         <v>5</v>
       </c>
-      <c r="H214" s="4" t="n">
+      <c r="H214" s="3" t="n">
         <v>43</v>
       </c>
-      <c r="K214" s="1" t="n">
+      <c r="K214" s="0" t="n">
         <f aca="false">$C$217+H214-$C$204/2-$E$210-50</f>
         <v>89.5</v>
       </c>
@@ -3333,29 +3398,29 @@
       <c r="D215" s="0" t="s">
         <v>16</v>
       </c>
-      <c r="E215" s="6" t="n">
+      <c r="E215" s="5" t="n">
         <f aca="false">C215-D204/2</f>
         <v>147.5</v>
       </c>
-      <c r="G215" s="4" t="n">
+      <c r="G215" s="3" t="n">
         <v>6</v>
       </c>
-      <c r="H215" s="4" t="n">
+      <c r="H215" s="3" t="n">
         <v>43</v>
       </c>
-      <c r="K215" s="1" t="n">
+      <c r="K215" s="0" t="n">
         <f aca="false">$C$217+H215-$C$204/2-$E$210-50</f>
         <v>89.5</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="216">
-      <c r="G216" s="4" t="n">
+      <c r="G216" s="3" t="n">
         <v>7</v>
       </c>
-      <c r="H216" s="4" t="n">
+      <c r="H216" s="3" t="n">
         <v>43.5</v>
       </c>
-      <c r="K216" s="1" t="n">
+      <c r="K216" s="0" t="n">
         <f aca="false">$C$217+H216-$C$204/2-$E$210-50</f>
         <v>90</v>
       </c>
@@ -3364,40 +3429,40 @@
       <c r="B217" s="0" t="s">
         <v>20</v>
       </c>
-      <c r="C217" s="7" t="n">
+      <c r="C217" s="6" t="n">
         <v>400</v>
       </c>
-      <c r="G217" s="4" t="n">
+      <c r="G217" s="3" t="n">
         <v>8</v>
       </c>
-      <c r="H217" s="4" t="n">
+      <c r="H217" s="3" t="n">
         <v>43</v>
       </c>
-      <c r="K217" s="1" t="n">
+      <c r="K217" s="0" t="n">
         <f aca="false">$C$217+H217-$C$204/2-$E$210-50</f>
         <v>89.5</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="218">
-      <c r="G218" s="4" t="n">
+      <c r="G218" s="3" t="n">
         <v>9</v>
       </c>
-      <c r="H218" s="4" t="n">
+      <c r="H218" s="3" t="n">
         <v>43.5</v>
       </c>
-      <c r="K218" s="1" t="n">
+      <c r="K218" s="0" t="n">
         <f aca="false">$C$217+H218-$C$204/2-$E$210-50</f>
         <v>90</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="219">
-      <c r="G219" s="4" t="n">
+      <c r="G219" s="3" t="n">
         <v>10</v>
       </c>
-      <c r="H219" s="4" t="n">
+      <c r="H219" s="3" t="n">
         <v>43</v>
       </c>
-      <c r="K219" s="1" t="n">
+      <c r="K219" s="0" t="n">
         <f aca="false">$C$217+H219-$C$204/2-$E$210-50</f>
         <v>89.5</v>
       </c>
@@ -3406,73 +3471,73 @@
       <c r="B221" s="0" t="s">
         <v>0</v>
       </c>
-      <c r="J221" s="8" t="s">
+      <c r="J221" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="K221" s="8" t="s">
+      <c r="K221" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="L221" s="8" t="s">
+      <c r="L221" s="7" t="s">
         <v>23</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="222">
-      <c r="A222" s="2"/>
-      <c r="B222" s="2" t="s">
+      <c r="A222" s="1"/>
+      <c r="B222" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C222" s="2" t="s">
+      <c r="C222" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D222" s="2" t="s">
+      <c r="D222" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="J222" s="6" t="n">
+      <c r="J222" s="5" t="n">
         <f aca="false">AVERAGE(K210:K219)</f>
         <v>89.6</v>
       </c>
-      <c r="K222" s="1" t="n">
+      <c r="K222" s="0" t="n">
         <f aca="false">STDEV(K210:K219)</f>
         <v>0.210818510677892</v>
       </c>
-      <c r="L222" s="1" t="n">
+      <c r="L222" s="0" t="n">
         <f aca="false">K222/SQRT(COUNT(K210:K219))</f>
         <v>0.0666666666666667</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="223">
-      <c r="A223" s="2" t="s">
+      <c r="A223" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B223" s="2" t="n">
+      <c r="B223" s="1" t="n">
         <v>233</v>
       </c>
-      <c r="C223" s="2" t="n">
+      <c r="C223" s="1" t="n">
         <v>540</v>
       </c>
-      <c r="D223" s="2" t="n">
+      <c r="D223" s="1" t="n">
         <v>1049</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="224">
-      <c r="A224" s="2" t="s">
+      <c r="A224" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B224" s="2" t="n">
+      <c r="B224" s="1" t="n">
         <v>38</v>
       </c>
-      <c r="C224" s="2" t="n">
+      <c r="C224" s="1" t="n">
         <v>52</v>
       </c>
-      <c r="D224" s="2" t="n">
+      <c r="D224" s="1" t="n">
         <v>65</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="228">
-      <c r="A228" s="3" t="s">
+      <c r="A228" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="B228" s="3" t="s">
+      <c r="B228" s="2" t="s">
         <v>24</v>
       </c>
     </row>
@@ -3480,17 +3545,23 @@
       <c r="B229" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="G229" s="4" t="s">
+      <c r="G229" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="H229" s="4" t="s">
+      <c r="H229" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="J229" s="5" t="s">
+      <c r="J229" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="K229" s="5" t="s">
+      <c r="K229" s="4" t="s">
         <v>12</v>
+      </c>
+      <c r="M229" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="N229" s="0" t="s">
+        <v>14</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="230">
@@ -3503,36 +3574,44 @@
       <c r="D230" s="0" t="s">
         <v>16</v>
       </c>
-      <c r="E230" s="6" t="n">
+      <c r="E230" s="5" t="n">
         <f aca="false">C230-C224/2</f>
         <v>277.5</v>
       </c>
-      <c r="G230" s="4" t="n">
+      <c r="G230" s="3" t="n">
         <v>1</v>
       </c>
-      <c r="H230" s="4" t="n">
+      <c r="H230" s="3" t="n">
         <v>38</v>
       </c>
-      <c r="J230" s="6" t="n">
+      <c r="J230" s="5" t="n">
         <f aca="false">E233-E235</f>
         <v>72.5</v>
       </c>
-      <c r="K230" s="1" t="n">
+      <c r="K230" s="0" t="n">
         <f aca="false">$C$237+H230-$C$224/2-$E$230-50</f>
         <v>44.5</v>
+      </c>
+      <c r="M230" s="5" t="n">
+        <f aca="false">C223*0.001/(D223*0.001)</f>
+        <v>0.514775977121068</v>
+      </c>
+      <c r="N230" s="5" t="n">
+        <f aca="false">$M$230*$J$242^2/$J$230^2</f>
+        <v>0.186172374119965</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="231">
       <c r="B231" s="0" t="s">
         <v>26</v>
       </c>
-      <c r="G231" s="4" t="n">
+      <c r="G231" s="3" t="n">
         <v>2</v>
       </c>
-      <c r="H231" s="4" t="n">
+      <c r="H231" s="3" t="n">
         <v>38.5</v>
       </c>
-      <c r="K231" s="1" t="n">
+      <c r="K231" s="0" t="n">
         <f aca="false">$C$237+H231-$C$224/2-$E$230-50</f>
         <v>45</v>
       </c>
@@ -3541,13 +3620,13 @@
       <c r="B232" s="0" t="s">
         <v>18</v>
       </c>
-      <c r="G232" s="4" t="n">
+      <c r="G232" s="3" t="n">
         <v>3</v>
       </c>
-      <c r="H232" s="4" t="n">
+      <c r="H232" s="3" t="n">
         <v>37</v>
       </c>
-      <c r="K232" s="1" t="n">
+      <c r="K232" s="0" t="n">
         <f aca="false">$C$237+H232-$C$224/2-$E$230-50</f>
         <v>43.5</v>
       </c>
@@ -3562,17 +3641,17 @@
       <c r="D233" s="0" t="s">
         <v>16</v>
       </c>
-      <c r="E233" s="6" t="n">
+      <c r="E233" s="5" t="n">
         <f aca="false">C233-D224/2</f>
         <v>220</v>
       </c>
-      <c r="G233" s="4" t="n">
+      <c r="G233" s="3" t="n">
         <v>4</v>
       </c>
-      <c r="H233" s="4" t="n">
+      <c r="H233" s="3" t="n">
         <v>37</v>
       </c>
-      <c r="K233" s="1" t="n">
+      <c r="K233" s="0" t="n">
         <f aca="false">$C$237+H233-$C$224/2-$E$230-50</f>
         <v>43.5</v>
       </c>
@@ -3581,13 +3660,13 @@
       <c r="B234" s="0" t="s">
         <v>19</v>
       </c>
-      <c r="G234" s="4" t="n">
+      <c r="G234" s="3" t="n">
         <v>5</v>
       </c>
-      <c r="H234" s="4" t="n">
+      <c r="H234" s="3" t="n">
         <v>37</v>
       </c>
-      <c r="K234" s="1" t="n">
+      <c r="K234" s="0" t="n">
         <f aca="false">$C$237+H234-$C$224/2-$E$230-50</f>
         <v>43.5</v>
       </c>
@@ -3602,29 +3681,29 @@
       <c r="D235" s="0" t="s">
         <v>16</v>
       </c>
-      <c r="E235" s="6" t="n">
+      <c r="E235" s="5" t="n">
         <f aca="false">C235-D224/2</f>
         <v>147.5</v>
       </c>
-      <c r="G235" s="4" t="n">
+      <c r="G235" s="3" t="n">
         <v>6</v>
       </c>
-      <c r="H235" s="4" t="n">
+      <c r="H235" s="3" t="n">
         <v>37</v>
       </c>
-      <c r="K235" s="1" t="n">
+      <c r="K235" s="0" t="n">
         <f aca="false">$C$237+H235-$C$224/2-$E$230-50</f>
         <v>43.5</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="236">
-      <c r="G236" s="4" t="n">
+      <c r="G236" s="3" t="n">
         <v>7</v>
       </c>
-      <c r="H236" s="4" t="n">
+      <c r="H236" s="3" t="n">
         <v>36</v>
       </c>
-      <c r="K236" s="1" t="n">
+      <c r="K236" s="0" t="n">
         <f aca="false">$C$237+H236-$C$224/2-$E$230-50</f>
         <v>42.5</v>
       </c>
@@ -3633,40 +3712,40 @@
       <c r="B237" s="0" t="s">
         <v>20</v>
       </c>
-      <c r="C237" s="7" t="n">
+      <c r="C237" s="6" t="n">
         <v>360</v>
       </c>
-      <c r="G237" s="4" t="n">
+      <c r="G237" s="3" t="n">
         <v>8</v>
       </c>
-      <c r="H237" s="4" t="n">
+      <c r="H237" s="3" t="n">
         <v>37</v>
       </c>
-      <c r="K237" s="1" t="n">
+      <c r="K237" s="0" t="n">
         <f aca="false">$C$237+H237-$C$224/2-$E$230-50</f>
         <v>43.5</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="238">
-      <c r="G238" s="4" t="n">
+      <c r="G238" s="3" t="n">
         <v>9</v>
       </c>
-      <c r="H238" s="4" t="n">
+      <c r="H238" s="3" t="n">
         <v>36</v>
       </c>
-      <c r="K238" s="1" t="n">
+      <c r="K238" s="0" t="n">
         <f aca="false">$C$237+H238-$C$224/2-$E$230-50</f>
         <v>42.5</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="239">
-      <c r="G239" s="4" t="n">
+      <c r="G239" s="3" t="n">
         <v>10</v>
       </c>
-      <c r="H239" s="4" t="n">
+      <c r="H239" s="3" t="n">
         <v>37.5</v>
       </c>
-      <c r="K239" s="1" t="n">
+      <c r="K239" s="0" t="n">
         <f aca="false">$C$237+H239-$C$224/2-$E$230-50</f>
         <v>44</v>
       </c>
@@ -3675,73 +3754,73 @@
       <c r="B241" s="0" t="s">
         <v>0</v>
       </c>
-      <c r="J241" s="8" t="s">
+      <c r="J241" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="K241" s="8" t="s">
+      <c r="K241" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="L241" s="8" t="s">
+      <c r="L241" s="7" t="s">
         <v>23</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="242">
-      <c r="A242" s="2"/>
-      <c r="B242" s="2" t="s">
+      <c r="A242" s="1"/>
+      <c r="B242" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C242" s="2" t="s">
+      <c r="C242" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D242" s="2" t="s">
+      <c r="D242" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="J242" s="6" t="n">
+      <c r="J242" s="5" t="n">
         <f aca="false">AVERAGE(K230:K239)</f>
         <v>43.6</v>
       </c>
-      <c r="K242" s="1" t="n">
+      <c r="K242" s="0" t="n">
         <f aca="false">STDEV(K230:K239)</f>
         <v>0.774596669241588</v>
       </c>
-      <c r="L242" s="1" t="n">
+      <c r="L242" s="0" t="n">
         <f aca="false">K242/SQRT(COUNT(K230:K239))</f>
         <v>0.244948974278351</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="243">
-      <c r="A243" s="2" t="s">
+      <c r="A243" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B243" s="2" t="n">
+      <c r="B243" s="1" t="n">
         <v>233</v>
       </c>
-      <c r="C243" s="2" t="n">
+      <c r="C243" s="1" t="n">
         <v>540</v>
       </c>
-      <c r="D243" s="2" t="n">
+      <c r="D243" s="1" t="n">
         <v>1049</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="244">
-      <c r="A244" s="2" t="s">
+      <c r="A244" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B244" s="2" t="n">
+      <c r="B244" s="1" t="n">
         <v>38</v>
       </c>
-      <c r="C244" s="2" t="n">
+      <c r="C244" s="1" t="n">
         <v>52</v>
       </c>
-      <c r="D244" s="2" t="n">
+      <c r="D244" s="1" t="n">
         <v>65</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="248">
-      <c r="A248" s="3" t="s">
+      <c r="A248" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="B248" s="3" t="s">
+      <c r="B248" s="2" t="s">
         <v>7</v>
       </c>
     </row>
@@ -3749,16 +3828,16 @@
       <c r="B249" s="0" t="s">
         <v>17</v>
       </c>
-      <c r="G249" s="4" t="s">
+      <c r="G249" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="H249" s="4" t="s">
+      <c r="H249" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="J249" s="5" t="s">
+      <c r="J249" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="K249" s="5" t="s">
+      <c r="K249" s="4" t="s">
         <v>12</v>
       </c>
       <c r="M249" s="0" t="s">
@@ -3778,29 +3857,29 @@
       <c r="D250" s="0" t="s">
         <v>16</v>
       </c>
-      <c r="E250" s="6" t="n">
+      <c r="E250" s="5" t="n">
         <f aca="false">C250-B244/2</f>
         <v>271.5</v>
       </c>
-      <c r="G250" s="4" t="n">
+      <c r="G250" s="3" t="n">
         <v>1</v>
       </c>
-      <c r="H250" s="4" t="n">
+      <c r="H250" s="3" t="n">
         <v>18</v>
       </c>
-      <c r="J250" s="6" t="n">
+      <c r="J250" s="5" t="n">
         <f aca="false">E253-E255</f>
         <v>72.5</v>
       </c>
-      <c r="K250" s="1" t="n">
+      <c r="K250" s="0" t="n">
         <f aca="false">$C$257+H250-$B$244/2-$E$250-50</f>
         <v>107.5</v>
       </c>
-      <c r="M250" s="6" t="n">
+      <c r="M250" s="5" t="n">
         <f aca="false">B243*0.001/(D243*0.001)</f>
         <v>0.222116301239275</v>
       </c>
-      <c r="N250" s="6" t="n">
+      <c r="N250" s="5" t="n">
         <f aca="false">$M$250*$J$262^2/$J$250^2</f>
         <v>0.500681202300135</v>
       </c>
@@ -3809,13 +3888,13 @@
       <c r="B251" s="0" t="s">
         <v>26</v>
       </c>
-      <c r="G251" s="4" t="n">
+      <c r="G251" s="3" t="n">
         <v>2</v>
       </c>
-      <c r="H251" s="4" t="n">
+      <c r="H251" s="3" t="n">
         <v>19</v>
       </c>
-      <c r="K251" s="1" t="n">
+      <c r="K251" s="0" t="n">
         <f aca="false">$C$257+H251-$B$244/2-$E$250-50</f>
         <v>108.5</v>
       </c>
@@ -3824,13 +3903,13 @@
       <c r="B252" s="0" t="s">
         <v>18</v>
       </c>
-      <c r="G252" s="4" t="n">
+      <c r="G252" s="3" t="n">
         <v>3</v>
       </c>
-      <c r="H252" s="4" t="n">
+      <c r="H252" s="3" t="n">
         <v>18.5</v>
       </c>
-      <c r="K252" s="1" t="n">
+      <c r="K252" s="0" t="n">
         <f aca="false">$C$257+H252-$B$244/2-$E$250-50</f>
         <v>108</v>
       </c>
@@ -3845,17 +3924,17 @@
       <c r="D253" s="0" t="s">
         <v>16</v>
       </c>
-      <c r="E253" s="6" t="n">
+      <c r="E253" s="5" t="n">
         <f aca="false">C253-D244/2</f>
         <v>220</v>
       </c>
-      <c r="G253" s="4" t="n">
+      <c r="G253" s="3" t="n">
         <v>4</v>
       </c>
-      <c r="H253" s="4" t="n">
+      <c r="H253" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="K253" s="1" t="n">
+      <c r="K253" s="0" t="n">
         <f aca="false">$C$257+H253-$B$244/2-$E$250-50</f>
         <v>109.5</v>
       </c>
@@ -3864,13 +3943,13 @@
       <c r="B254" s="0" t="s">
         <v>19</v>
       </c>
-      <c r="G254" s="4" t="n">
+      <c r="G254" s="3" t="n">
         <v>5</v>
       </c>
-      <c r="H254" s="4" t="n">
+      <c r="H254" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="K254" s="1" t="n">
+      <c r="K254" s="0" t="n">
         <f aca="false">$C$257+H254-$B$244/2-$E$250-50</f>
         <v>109.5</v>
       </c>
@@ -3885,29 +3964,29 @@
       <c r="D255" s="0" t="s">
         <v>16</v>
       </c>
-      <c r="E255" s="6" t="n">
+      <c r="E255" s="5" t="n">
         <f aca="false">C255-D244/2</f>
         <v>147.5</v>
       </c>
-      <c r="G255" s="4" t="n">
+      <c r="G255" s="3" t="n">
         <v>6</v>
       </c>
-      <c r="H255" s="4" t="n">
+      <c r="H255" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="K255" s="1" t="n">
+      <c r="K255" s="0" t="n">
         <f aca="false">$C$257+H255-$B$244/2-$E$250-50</f>
         <v>109.5</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="256">
-      <c r="G256" s="4" t="n">
+      <c r="G256" s="3" t="n">
         <v>7</v>
       </c>
-      <c r="H256" s="4" t="n">
+      <c r="H256" s="3" t="n">
         <v>21</v>
       </c>
-      <c r="K256" s="1" t="n">
+      <c r="K256" s="0" t="n">
         <f aca="false">$C$257+H256-$B$244/2-$E$250-50</f>
         <v>110.5</v>
       </c>
@@ -3916,40 +3995,40 @@
       <c r="B257" s="0" t="s">
         <v>20</v>
       </c>
-      <c r="C257" s="7" t="n">
+      <c r="C257" s="6" t="n">
         <v>430</v>
       </c>
-      <c r="G257" s="4" t="n">
+      <c r="G257" s="3" t="n">
         <v>8</v>
       </c>
-      <c r="H257" s="4" t="n">
+      <c r="H257" s="3" t="n">
         <v>18</v>
       </c>
-      <c r="K257" s="1" t="n">
+      <c r="K257" s="0" t="n">
         <f aca="false">$C$257+H257-$B$244/2-$E$250-50</f>
         <v>107.5</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="258">
-      <c r="G258" s="4" t="n">
+      <c r="G258" s="3" t="n">
         <v>9</v>
       </c>
-      <c r="H258" s="4" t="n">
+      <c r="H258" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="K258" s="1" t="n">
+      <c r="K258" s="0" t="n">
         <f aca="false">$C$257+H258-$B$244/2-$E$250-50</f>
         <v>109.5</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="259">
-      <c r="G259" s="4" t="n">
+      <c r="G259" s="3" t="n">
         <v>10</v>
       </c>
-      <c r="H259" s="4" t="n">
+      <c r="H259" s="3" t="n">
         <v>19</v>
       </c>
-      <c r="K259" s="1" t="n">
+      <c r="K259" s="0" t="n">
         <f aca="false">$C$257+H259-$B$244/2-$E$250-50</f>
         <v>108.5</v>
       </c>
@@ -3958,73 +4037,73 @@
       <c r="B261" s="0" t="s">
         <v>0</v>
       </c>
-      <c r="J261" s="8" t="s">
+      <c r="J261" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="K261" s="8" t="s">
+      <c r="K261" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="L261" s="8" t="s">
+      <c r="L261" s="7" t="s">
         <v>23</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="262">
-      <c r="A262" s="2"/>
-      <c r="B262" s="2" t="s">
+      <c r="A262" s="1"/>
+      <c r="B262" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C262" s="2" t="s">
+      <c r="C262" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D262" s="2" t="s">
+      <c r="D262" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="J262" s="6" t="n">
+      <c r="J262" s="5" t="n">
         <f aca="false">AVERAGE(K250:K259)</f>
         <v>108.85</v>
       </c>
-      <c r="K262" s="1" t="n">
+      <c r="K262" s="0" t="n">
         <f aca="false">STDEV(K250:K259)</f>
         <v>1.00138792571966</v>
       </c>
-      <c r="L262" s="1" t="n">
+      <c r="L262" s="0" t="n">
         <f aca="false">K262/SQRT(COUNT(K250:K259))</f>
         <v>0.316666666666564</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="263">
-      <c r="A263" s="2" t="s">
+      <c r="A263" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B263" s="2" t="n">
+      <c r="B263" s="1" t="n">
         <v>233</v>
       </c>
-      <c r="C263" s="2" t="n">
+      <c r="C263" s="1" t="n">
         <v>540</v>
       </c>
-      <c r="D263" s="2" t="n">
+      <c r="D263" s="1" t="n">
         <v>1049</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="264">
-      <c r="A264" s="2" t="s">
+      <c r="A264" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B264" s="2" t="n">
+      <c r="B264" s="1" t="n">
         <v>38</v>
       </c>
-      <c r="C264" s="2" t="n">
+      <c r="C264" s="1" t="n">
         <v>52</v>
       </c>
-      <c r="D264" s="2" t="n">
+      <c r="D264" s="1" t="n">
         <v>65</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="268">
-      <c r="A268" s="3" t="s">
+      <c r="A268" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="B268" s="3" t="s">
+      <c r="B268" s="2" t="s">
         <v>24</v>
       </c>
     </row>
@@ -4032,17 +4111,23 @@
       <c r="B269" s="0" t="s">
         <v>17</v>
       </c>
-      <c r="G269" s="4" t="s">
+      <c r="G269" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="H269" s="4" t="s">
+      <c r="H269" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="J269" s="5" t="s">
+      <c r="J269" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="K269" s="5" t="s">
+      <c r="K269" s="4" t="s">
         <v>12</v>
+      </c>
+      <c r="M269" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="N269" s="0" t="s">
+        <v>14</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="270">
@@ -4055,36 +4140,44 @@
       <c r="D270" s="0" t="s">
         <v>16</v>
       </c>
-      <c r="E270" s="6" t="n">
+      <c r="E270" s="5" t="n">
         <f aca="false">C270-B264/2</f>
         <v>271.5</v>
       </c>
-      <c r="G270" s="4" t="n">
+      <c r="G270" s="3" t="n">
         <v>1</v>
       </c>
-      <c r="H270" s="4" t="n">
+      <c r="H270" s="3" t="n">
         <v>27</v>
       </c>
-      <c r="J270" s="6" t="n">
+      <c r="J270" s="5" t="n">
         <f aca="false">E273-E275</f>
         <v>72.5</v>
       </c>
-      <c r="K270" s="1" t="n">
+      <c r="K270" s="0" t="n">
         <f aca="false">$C$277+H270-$B$264/2-$E$270-50</f>
         <v>56.5</v>
+      </c>
+      <c r="M270" s="5" t="n">
+        <f aca="false">B263*0.001/(D263*0.001)</f>
+        <v>0.222116301239275</v>
+      </c>
+      <c r="N270" s="5" t="n">
+        <f aca="false">$M$270*$J$282^2/$J$270^2</f>
+        <v>0.137535787098069</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="271">
       <c r="B271" s="0" t="s">
         <v>26</v>
       </c>
-      <c r="G271" s="4" t="n">
+      <c r="G271" s="3" t="n">
         <v>2</v>
       </c>
-      <c r="H271" s="4" t="n">
+      <c r="H271" s="3" t="n">
         <v>28</v>
       </c>
-      <c r="K271" s="1" t="n">
+      <c r="K271" s="0" t="n">
         <f aca="false">$C$277+H271-$B$264/2-$E$270-50</f>
         <v>57.5</v>
       </c>
@@ -4093,13 +4186,13 @@
       <c r="B272" s="0" t="s">
         <v>18</v>
       </c>
-      <c r="G272" s="4" t="n">
+      <c r="G272" s="3" t="n">
         <v>3</v>
       </c>
-      <c r="H272" s="4" t="n">
+      <c r="H272" s="3" t="n">
         <v>28</v>
       </c>
-      <c r="K272" s="1" t="n">
+      <c r="K272" s="0" t="n">
         <f aca="false">$C$277+H272-$B$264/2-$E$270-50</f>
         <v>57.5</v>
       </c>
@@ -4114,17 +4207,17 @@
       <c r="D273" s="0" t="s">
         <v>16</v>
       </c>
-      <c r="E273" s="6" t="n">
+      <c r="E273" s="5" t="n">
         <f aca="false">C273-D264/2</f>
         <v>220</v>
       </c>
-      <c r="G273" s="4" t="n">
+      <c r="G273" s="3" t="n">
         <v>4</v>
       </c>
-      <c r="H273" s="4" t="n">
+      <c r="H273" s="3" t="n">
         <v>28</v>
       </c>
-      <c r="K273" s="1" t="n">
+      <c r="K273" s="0" t="n">
         <f aca="false">$C$277+H273-$B$264/2-$E$270-50</f>
         <v>57.5</v>
       </c>
@@ -4133,13 +4226,13 @@
       <c r="B274" s="0" t="s">
         <v>19</v>
       </c>
-      <c r="G274" s="4" t="n">
+      <c r="G274" s="3" t="n">
         <v>5</v>
       </c>
-      <c r="H274" s="4" t="n">
+      <c r="H274" s="3" t="n">
         <v>27.5</v>
       </c>
-      <c r="K274" s="1" t="n">
+      <c r="K274" s="0" t="n">
         <f aca="false">$C$277+H274-$B$264/2-$E$270-50</f>
         <v>57</v>
       </c>
@@ -4154,29 +4247,29 @@
       <c r="D275" s="0" t="s">
         <v>16</v>
       </c>
-      <c r="E275" s="6" t="n">
+      <c r="E275" s="5" t="n">
         <f aca="false">C275-D264/2</f>
         <v>147.5</v>
       </c>
-      <c r="G275" s="4" t="n">
+      <c r="G275" s="3" t="n">
         <v>6</v>
       </c>
-      <c r="H275" s="4" t="n">
+      <c r="H275" s="3" t="n">
         <v>27.5</v>
       </c>
-      <c r="K275" s="1" t="n">
+      <c r="K275" s="0" t="n">
         <f aca="false">$C$277+H275-$B$264/2-$E$270-50</f>
         <v>57</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="276">
-      <c r="G276" s="4" t="n">
+      <c r="G276" s="3" t="n">
         <v>7</v>
       </c>
-      <c r="H276" s="4" t="n">
+      <c r="H276" s="3" t="n">
         <v>27.5</v>
       </c>
-      <c r="K276" s="1" t="n">
+      <c r="K276" s="0" t="n">
         <f aca="false">$C$277+H276-$B$264/2-$E$270-50</f>
         <v>57</v>
       </c>
@@ -4185,65 +4278,65 @@
       <c r="B277" s="0" t="s">
         <v>20</v>
       </c>
-      <c r="C277" s="7" t="n">
+      <c r="C277" s="6" t="n">
         <v>370</v>
       </c>
-      <c r="G277" s="4" t="n">
+      <c r="G277" s="3" t="n">
         <v>8</v>
       </c>
-      <c r="H277" s="4" t="n">
+      <c r="H277" s="3" t="n">
         <v>27.5</v>
       </c>
-      <c r="K277" s="1" t="n">
+      <c r="K277" s="0" t="n">
         <f aca="false">$C$277+H277-$B$264/2-$E$270-50</f>
         <v>57</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="278">
-      <c r="G278" s="4" t="n">
+      <c r="G278" s="3" t="n">
         <v>9</v>
       </c>
-      <c r="H278" s="4" t="n">
+      <c r="H278" s="3" t="n">
         <v>27</v>
       </c>
-      <c r="K278" s="1" t="n">
+      <c r="K278" s="0" t="n">
         <f aca="false">$C$277+H278-$B$264/2-$E$270-50</f>
         <v>56.5</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="279">
-      <c r="G279" s="4" t="n">
+      <c r="G279" s="3" t="n">
         <v>10</v>
       </c>
-      <c r="H279" s="4" t="n">
+      <c r="H279" s="3" t="n">
         <v>27.5</v>
       </c>
-      <c r="K279" s="1" t="n">
+      <c r="K279" s="0" t="n">
         <f aca="false">$C$277+H279-$B$264/2-$E$270-50</f>
         <v>57</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="281">
-      <c r="J281" s="8" t="s">
+      <c r="J281" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="K281" s="8" t="s">
+      <c r="K281" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="L281" s="8" t="s">
+      <c r="L281" s="7" t="s">
         <v>23</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="282">
-      <c r="J282" s="6" t="n">
+      <c r="J282" s="5" t="n">
         <f aca="false">AVERAGE(K270:K279)</f>
         <v>57.05</v>
       </c>
-      <c r="K282" s="1" t="n">
+      <c r="K282" s="0" t="n">
         <f aca="false">STDEV(K270:K279)</f>
         <v>0.368932393686092</v>
       </c>
-      <c r="L282" s="1" t="n">
+      <c r="L282" s="0" t="n">
         <f aca="false">K282/SQRT(COUNT(K270:K279))</f>
         <v>0.116666666666597</v>
       </c>
@@ -4266,7 +4359,7 @@
   </sheetPr>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100">
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="55" zoomScaleNormal="55" zoomScalePageLayoutView="100">
       <selection activeCell="A1" activeCellId="0" pane="topLeft" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -4292,7 +4385,7 @@
   </sheetPr>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100">
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="55" zoomScaleNormal="55" zoomScalePageLayoutView="100">
       <selection activeCell="A1" activeCellId="0" pane="topLeft" sqref="A1"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Added Q calculation for inelastic collisions
	modified:   exp3/data/values.xlsx
</commit_message>
<xml_diff>
--- a/exp3/data/values.xlsx
+++ b/exp3/data/values.xlsx
@@ -239,7 +239,7 @@
       <protection hidden="false" locked="true"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0">
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
       <protection hidden="false" locked="true"/>
@@ -260,10 +260,6 @@
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
       <protection hidden="false" locked="true"/>
     </xf>
-    <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
     <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="7" fontId="0" numFmtId="164" xfId="0">
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
       <protection hidden="false" locked="true"/>
@@ -280,8 +276,8 @@
     <cellStyle builtinId="4" customBuiltin="false" name="Currency" xfId="17"/>
     <cellStyle builtinId="7" customBuiltin="false" name="Currency [0]" xfId="18"/>
     <cellStyle builtinId="5" customBuiltin="false" name="Percent" xfId="19"/>
-    <cellStyle builtinId="54" customBuiltin="true" name="Excel Built-in Excel Built-in 20% - Accent1" xfId="20"/>
-    <cellStyle builtinId="54" customBuiltin="true" name="Excel Built-in Excel Built-in Good" xfId="21"/>
+    <cellStyle builtinId="54" customBuiltin="true" name="Excel Built-in Excel Built-in Excel Built-in 20% - Accent1" xfId="20"/>
+    <cellStyle builtinId="54" customBuiltin="true" name="Excel Built-in Excel Built-in Excel Built-in Good" xfId="21"/>
   </cellStyles>
   <colors>
     <indexedColors>
@@ -351,10 +347,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A2:N282"/>
+  <dimension ref="A2:O282"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A244" view="normal" windowProtection="false" workbookViewId="0" zoomScale="55" zoomScaleNormal="55" zoomScalePageLayoutView="100">
-      <selection activeCell="N30" activeCellId="0" pane="topLeft" sqref="N30"/>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A247" view="normal" windowProtection="false" workbookViewId="0" zoomScale="55" zoomScaleNormal="55" zoomScalePageLayoutView="100">
+      <selection activeCell="O272" activeCellId="0" pane="topLeft" sqref="O272"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -453,7 +449,7 @@
       <c r="D11" s="0" t="s">
         <v>16</v>
       </c>
-      <c r="E11" s="5" t="n">
+      <c r="E11" s="0" t="n">
         <f aca="false">C11-C5/2</f>
         <v>265</v>
       </c>
@@ -463,7 +459,7 @@
       <c r="H11" s="3" t="n">
         <v>34</v>
       </c>
-      <c r="J11" s="5" t="n">
+      <c r="J11" s="0" t="n">
         <f aca="false">E14-E16</f>
         <v>159</v>
       </c>
@@ -471,11 +467,11 @@
         <f aca="false">$C$18+H11-$C$5/2-$E$11-50</f>
         <v>93</v>
       </c>
-      <c r="M11" s="5" t="n">
+      <c r="M11" s="0" t="n">
         <f aca="false">C4*0.001/(B4*0.001)</f>
         <v>2.31759656652361</v>
       </c>
-      <c r="N11" s="5" t="n">
+      <c r="N11" s="0" t="n">
         <f aca="false">$M$11*$J$23^2/$J$11^2</f>
         <v>0.799718868077318</v>
       </c>
@@ -514,14 +510,14 @@
       <c r="B14" s="0" t="s">
         <v>15</v>
       </c>
-      <c r="C14" s="5" t="n">
+      <c r="C14" s="0" t="n">
         <f aca="false">C11-C5</f>
         <v>239</v>
       </c>
       <c r="D14" s="0" t="s">
         <v>16</v>
       </c>
-      <c r="E14" s="5" t="n">
+      <c r="E14" s="0" t="n">
         <f aca="false">C14-B5/2</f>
         <v>220</v>
       </c>
@@ -561,7 +557,7 @@
       <c r="D16" s="0" t="s">
         <v>16</v>
       </c>
-      <c r="E16" s="5" t="n">
+      <c r="E16" s="0" t="n">
         <f aca="false">C16-B5/2</f>
         <v>61</v>
       </c>
@@ -592,7 +588,7 @@
       <c r="B18" s="0" t="s">
         <v>20</v>
       </c>
-      <c r="C18" s="6" t="n">
+      <c r="C18" s="5" t="n">
         <v>400</v>
       </c>
       <c r="G18" s="3" t="n">
@@ -646,13 +642,13 @@
       <c r="D22" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="J22" s="7" t="s">
+      <c r="J22" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="K22" s="7" t="s">
+      <c r="K22" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="L22" s="7" t="s">
+      <c r="L22" s="6" t="s">
         <v>23</v>
       </c>
     </row>
@@ -669,7 +665,7 @@
       <c r="D23" s="1" t="n">
         <v>1049</v>
       </c>
-      <c r="J23" s="5" t="n">
+      <c r="J23" s="0" t="n">
         <f aca="false">AVERAGE(K11:K20)</f>
         <v>93.4</v>
       </c>
@@ -737,7 +733,7 @@
       <c r="D30" s="0" t="s">
         <v>16</v>
       </c>
-      <c r="E30" s="5" t="n">
+      <c r="E30" s="0" t="n">
         <f aca="false">C30-C24/2</f>
         <v>265</v>
       </c>
@@ -747,7 +743,7 @@
       <c r="H30" s="3" t="n">
         <v>36</v>
       </c>
-      <c r="J30" s="5" t="n">
+      <c r="J30" s="0" t="n">
         <f aca="false">E33-E35</f>
         <v>159</v>
       </c>
@@ -755,13 +751,17 @@
         <f aca="false">$C$37+H30-$C$24/2-$E$30-50</f>
         <v>45</v>
       </c>
-      <c r="M30" s="5" t="n">
+      <c r="M30" s="0" t="n">
         <f aca="false">C23*0.001/(B23*0.001)</f>
         <v>2.31759656652361</v>
       </c>
-      <c r="N30" s="5" t="n">
+      <c r="N30" s="0" t="n">
         <f aca="false">$M$30*$J$42^2/$J$30^2</f>
         <v>0.189786966174024</v>
+      </c>
+      <c r="O30" s="0" t="n">
+        <f aca="false">1-((1+M30)*J42^2/J30^2)</f>
+        <v>0.728323472495332</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="31">
@@ -798,14 +798,14 @@
       <c r="B33" s="0" t="s">
         <v>15</v>
       </c>
-      <c r="C33" s="5" t="n">
+      <c r="C33" s="0" t="n">
         <f aca="false">C30-C24</f>
         <v>239</v>
       </c>
       <c r="D33" s="0" t="s">
         <v>16</v>
       </c>
-      <c r="E33" s="5" t="n">
+      <c r="E33" s="0" t="n">
         <f aca="false">C33-B24/2</f>
         <v>220</v>
       </c>
@@ -845,7 +845,7 @@
       <c r="D35" s="0" t="s">
         <v>16</v>
       </c>
-      <c r="E35" s="5" t="n">
+      <c r="E35" s="0" t="n">
         <f aca="false">C35-B24/2</f>
         <v>61</v>
       </c>
@@ -876,7 +876,7 @@
       <c r="B37" s="0" t="s">
         <v>20</v>
       </c>
-      <c r="C37" s="6" t="n">
+      <c r="C37" s="5" t="n">
         <v>350</v>
       </c>
       <c r="G37" s="3" t="n">
@@ -918,13 +918,13 @@
       <c r="B41" s="0" t="s">
         <v>0</v>
       </c>
-      <c r="J41" s="7" t="s">
+      <c r="J41" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="K41" s="7" t="s">
+      <c r="K41" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="L41" s="7" t="s">
+      <c r="L41" s="6" t="s">
         <v>23</v>
       </c>
     </row>
@@ -939,7 +939,7 @@
       <c r="D42" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="J42" s="5" t="n">
+      <c r="J42" s="0" t="n">
         <f aca="false">AVERAGE(K30:K39)</f>
         <v>45.5</v>
       </c>
@@ -1021,7 +1021,7 @@
       <c r="D50" s="0" t="s">
         <v>16</v>
       </c>
-      <c r="E50" s="5" t="n">
+      <c r="E50" s="0" t="n">
         <f aca="false">C50-D44/2</f>
         <v>270.5</v>
       </c>
@@ -1031,7 +1031,7 @@
       <c r="H50" s="3" t="n">
         <v>39</v>
       </c>
-      <c r="J50" s="5" t="n">
+      <c r="J50" s="0" t="n">
         <f aca="false">E53-E55</f>
         <v>158</v>
       </c>
@@ -1039,11 +1039,11 @@
         <f aca="false">$C$57+H50-$D$44/2-$E$50-50</f>
         <v>56</v>
       </c>
-      <c r="M50" s="5" t="n">
+      <c r="M50" s="0" t="n">
         <f aca="false">D43*0.001/(B43*0.001)</f>
         <v>4.50214592274678</v>
       </c>
-      <c r="N50" s="5" t="n">
+      <c r="N50" s="0" t="n">
         <f aca="false">$M$50*$J$62^2/$J$50^2</f>
         <v>0.555509332580547</v>
       </c>
@@ -1082,14 +1082,14 @@
       <c r="B53" s="0" t="s">
         <v>15</v>
       </c>
-      <c r="C53" s="5" t="n">
+      <c r="C53" s="0" t="n">
         <f aca="false">C50-D44</f>
         <v>238</v>
       </c>
       <c r="D53" s="0" t="s">
         <v>16</v>
       </c>
-      <c r="E53" s="5" t="n">
+      <c r="E53" s="0" t="n">
         <f aca="false">C53-B44/2</f>
         <v>219</v>
       </c>
@@ -1129,7 +1129,7 @@
       <c r="D55" s="0" t="s">
         <v>16</v>
       </c>
-      <c r="E55" s="5" t="n">
+      <c r="E55" s="0" t="n">
         <f aca="false">C55-B44/2</f>
         <v>61</v>
       </c>
@@ -1160,7 +1160,7 @@
       <c r="B57" s="0" t="s">
         <v>20</v>
       </c>
-      <c r="C57" s="6" t="n">
+      <c r="C57" s="5" t="n">
         <v>370</v>
       </c>
       <c r="G57" s="3" t="n">
@@ -1202,13 +1202,13 @@
       <c r="B61" s="0" t="s">
         <v>0</v>
       </c>
-      <c r="J61" s="7" t="s">
+      <c r="J61" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="K61" s="7" t="s">
+      <c r="K61" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="L61" s="7" t="s">
+      <c r="L61" s="6" t="s">
         <v>23</v>
       </c>
     </row>
@@ -1223,7 +1223,7 @@
       <c r="D62" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="J62" s="5" t="n">
+      <c r="J62" s="0" t="n">
         <f aca="false">AVERAGE(K50:K59)</f>
         <v>55.5</v>
       </c>
@@ -1305,7 +1305,7 @@
       <c r="D70" s="0" t="s">
         <v>16</v>
       </c>
-      <c r="E70" s="5" t="n">
+      <c r="E70" s="0" t="n">
         <f aca="false">C70-D64/2</f>
         <v>270.5</v>
       </c>
@@ -1315,7 +1315,7 @@
       <c r="H70" s="3" t="n">
         <v>31</v>
       </c>
-      <c r="J70" s="5" t="n">
+      <c r="J70" s="0" t="n">
         <f aca="false">E73-E75</f>
         <v>158</v>
       </c>
@@ -1323,13 +1323,17 @@
         <f aca="false">$C$77+H70-$D$64/2-$E$70-50</f>
         <v>28</v>
       </c>
-      <c r="M70" s="5" t="n">
+      <c r="M70" s="0" t="n">
         <f aca="false">D63*0.001/(B63*0.001)</f>
         <v>4.50214592274678</v>
       </c>
-      <c r="N70" s="5" t="n">
+      <c r="N70" s="0" t="n">
         <f aca="false">$M$70*$J$82^2/$J$70^2</f>
         <v>0.128566528075106</v>
+      </c>
+      <c r="O70" s="0" t="n">
+        <f aca="false">1-((1+M70)*J82^2/J70^2)</f>
+        <v>0.842876750245676</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="71">
@@ -1366,14 +1370,14 @@
       <c r="B73" s="0" t="s">
         <v>15</v>
       </c>
-      <c r="C73" s="5" t="n">
+      <c r="C73" s="0" t="n">
         <f aca="false">C70-D64</f>
         <v>238</v>
       </c>
       <c r="D73" s="0" t="s">
         <v>16</v>
       </c>
-      <c r="E73" s="5" t="n">
+      <c r="E73" s="0" t="n">
         <f aca="false">C73-B64/2</f>
         <v>219</v>
       </c>
@@ -1413,7 +1417,7 @@
       <c r="D75" s="0" t="s">
         <v>16</v>
       </c>
-      <c r="E75" s="5" t="n">
+      <c r="E75" s="0" t="n">
         <f aca="false">C75-B64/2</f>
         <v>61</v>
       </c>
@@ -1444,7 +1448,7 @@
       <c r="B77" s="0" t="s">
         <v>20</v>
       </c>
-      <c r="C77" s="6" t="n">
+      <c r="C77" s="5" t="n">
         <v>350</v>
       </c>
       <c r="G77" s="3" t="n">
@@ -1486,13 +1490,13 @@
       <c r="B81" s="0" t="s">
         <v>0</v>
       </c>
-      <c r="J81" s="7" t="s">
+      <c r="J81" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="K81" s="7" t="s">
+      <c r="K81" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="L81" s="7" t="s">
+      <c r="L81" s="6" t="s">
         <v>23</v>
       </c>
     </row>
@@ -1507,7 +1511,7 @@
       <c r="D82" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="J82" s="5" t="n">
+      <c r="J82" s="0" t="n">
         <f aca="false">AVERAGE(K70:K79)</f>
         <v>26.7</v>
       </c>
@@ -1589,7 +1593,7 @@
       <c r="D90" s="0" t="s">
         <v>16</v>
       </c>
-      <c r="E90" s="5" t="n">
+      <c r="E90" s="0" t="n">
         <f aca="false">C90-B84/2</f>
         <v>265</v>
       </c>
@@ -1599,7 +1603,7 @@
       <c r="H90" s="3" t="n">
         <v>18</v>
       </c>
-      <c r="J90" s="5" t="n">
+      <c r="J90" s="0" t="n">
         <f aca="false">E93-E95</f>
         <v>86</v>
       </c>
@@ -1607,11 +1611,11 @@
         <f aca="false">$C$97+H90-$B$84/2-$E$90-50</f>
         <v>114</v>
       </c>
-      <c r="M90" s="5" t="n">
+      <c r="M90" s="0" t="n">
         <f aca="false">B83*0.001/(C83*0.001)</f>
         <v>0.431481481481481</v>
       </c>
-      <c r="N90" s="5" t="n">
+      <c r="N90" s="0" t="n">
         <f aca="false">$M$90*$J$102^2/$J$90^2</f>
         <v>0.765518068450414</v>
       </c>
@@ -1650,14 +1654,14 @@
       <c r="B93" s="0" t="s">
         <v>15</v>
       </c>
-      <c r="C93" s="5" t="n">
+      <c r="C93" s="0" t="n">
         <f aca="false">C90-B84</f>
         <v>246</v>
       </c>
       <c r="D93" s="0" t="s">
         <v>16</v>
       </c>
-      <c r="E93" s="5" t="n">
+      <c r="E93" s="0" t="n">
         <f aca="false">C93-C84/2</f>
         <v>220</v>
       </c>
@@ -1697,7 +1701,7 @@
       <c r="D95" s="0" t="s">
         <v>16</v>
       </c>
-      <c r="E95" s="5" t="n">
+      <c r="E95" s="0" t="n">
         <f aca="false">C95-C84/2</f>
         <v>134</v>
       </c>
@@ -1728,7 +1732,7 @@
       <c r="B97" s="0" t="s">
         <v>20</v>
       </c>
-      <c r="C97" s="6" t="n">
+      <c r="C97" s="5" t="n">
         <v>430</v>
       </c>
       <c r="G97" s="3" t="n">
@@ -1770,13 +1774,13 @@
       <c r="B101" s="0" t="s">
         <v>0</v>
       </c>
-      <c r="J101" s="7" t="s">
+      <c r="J101" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="K101" s="7" t="s">
+      <c r="K101" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="L101" s="7" t="s">
+      <c r="L101" s="6" t="s">
         <v>23</v>
       </c>
     </row>
@@ -1791,7 +1795,7 @@
       <c r="D102" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="J102" s="5" t="n">
+      <c r="J102" s="0" t="n">
         <f aca="false">AVERAGE(K90:K99)</f>
         <v>114.55</v>
       </c>
@@ -1873,7 +1877,7 @@
       <c r="D110" s="0" t="s">
         <v>16</v>
       </c>
-      <c r="E110" s="5" t="n">
+      <c r="E110" s="0" t="n">
         <f aca="false">C110-B104/2</f>
         <v>265</v>
       </c>
@@ -1883,7 +1887,7 @@
       <c r="H110" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="J110" s="5" t="n">
+      <c r="J110" s="0" t="n">
         <f aca="false">E113-E115</f>
         <v>86</v>
       </c>
@@ -1891,13 +1895,17 @@
         <f aca="false">$C$117+H110-$B$104/2-$E$110-50</f>
         <v>56</v>
       </c>
-      <c r="M110" s="5" t="n">
+      <c r="M110" s="0" t="n">
         <f aca="false">B103*0.001/(C103*0.001)</f>
         <v>0.431481481481481</v>
       </c>
-      <c r="N110" s="5" t="n">
+      <c r="N110" s="0" t="n">
         <f aca="false">$M$110*$J$122^2/$J$110^2</f>
         <v>0.191881057453478</v>
+      </c>
+      <c r="O110" s="0" t="n">
+        <f aca="false">1-((1+M110)*J122^2/J110^2)</f>
+        <v>0.363416062611422</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="111">
@@ -1934,14 +1942,14 @@
       <c r="B113" s="0" t="s">
         <v>15</v>
       </c>
-      <c r="C113" s="5" t="n">
+      <c r="C113" s="0" t="n">
         <f aca="false">C110-B104</f>
         <v>246</v>
       </c>
       <c r="D113" s="0" t="s">
         <v>16</v>
       </c>
-      <c r="E113" s="5" t="n">
+      <c r="E113" s="0" t="n">
         <f aca="false">C113-C104/2</f>
         <v>220</v>
       </c>
@@ -1981,7 +1989,7 @@
       <c r="D115" s="0" t="s">
         <v>16</v>
       </c>
-      <c r="E115" s="5" t="n">
+      <c r="E115" s="0" t="n">
         <f aca="false">C115-C104/2</f>
         <v>134</v>
       </c>
@@ -2012,7 +2020,7 @@
       <c r="B117" s="0" t="s">
         <v>20</v>
       </c>
-      <c r="C117" s="6" t="n">
+      <c r="C117" s="5" t="n">
         <v>370</v>
       </c>
       <c r="G117" s="3" t="n">
@@ -2054,13 +2062,13 @@
       <c r="B121" s="0" t="s">
         <v>0</v>
       </c>
-      <c r="J121" s="7" t="s">
+      <c r="J121" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="K121" s="7" t="s">
+      <c r="K121" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="L121" s="7" t="s">
+      <c r="L121" s="6" t="s">
         <v>23</v>
       </c>
     </row>
@@ -2075,7 +2083,7 @@
       <c r="D122" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="J122" s="5" t="n">
+      <c r="J122" s="0" t="n">
         <f aca="false">AVERAGE(K110:K119)</f>
         <v>57.35</v>
       </c>
@@ -2157,7 +2165,7 @@
       <c r="D130" s="0" t="s">
         <v>16</v>
       </c>
-      <c r="E130" s="5" t="n">
+      <c r="E130" s="0" t="n">
         <f aca="false">C130-C124/2</f>
         <v>271</v>
       </c>
@@ -2167,7 +2175,7 @@
       <c r="H130" s="3" t="n">
         <v>29</v>
       </c>
-      <c r="J130" s="5" t="n">
+      <c r="J130" s="0" t="n">
         <f aca="false">E133-E135</f>
         <v>95</v>
       </c>
@@ -2175,11 +2183,11 @@
         <f aca="false">$C$137+H130-$C$124/2-$E$130-50</f>
         <v>92</v>
       </c>
-      <c r="M130" s="5" t="n">
+      <c r="M130" s="0" t="n">
         <f aca="false">C123*0.001/(C123*0.001)</f>
         <v>1</v>
       </c>
-      <c r="N130" s="5" t="n">
+      <c r="N130" s="0" t="n">
         <f aca="false">$M$130*$J$142^2/$J$130^2</f>
         <v>0.948060941828255</v>
       </c>
@@ -2218,14 +2226,14 @@
       <c r="B133" s="0" t="s">
         <v>15</v>
       </c>
-      <c r="C133" s="5" t="n">
+      <c r="C133" s="0" t="n">
         <f aca="false">C130-C124</f>
         <v>245</v>
       </c>
       <c r="D133" s="0" t="s">
         <v>16</v>
       </c>
-      <c r="E133" s="5" t="n">
+      <c r="E133" s="0" t="n">
         <f aca="false">C133-C124/2</f>
         <v>219</v>
       </c>
@@ -2265,7 +2273,7 @@
       <c r="D135" s="0" t="s">
         <v>16</v>
       </c>
-      <c r="E135" s="5" t="n">
+      <c r="E135" s="0" t="n">
         <f aca="false">C135-C124/2</f>
         <v>124</v>
       </c>
@@ -2296,7 +2304,7 @@
       <c r="B137" s="0" t="s">
         <v>20</v>
       </c>
-      <c r="C137" s="6" t="n">
+      <c r="C137" s="5" t="n">
         <v>410</v>
       </c>
       <c r="G137" s="3" t="n">
@@ -2338,13 +2346,13 @@
       <c r="B141" s="0" t="s">
         <v>0</v>
       </c>
-      <c r="J141" s="7" t="s">
+      <c r="J141" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="K141" s="7" t="s">
+      <c r="K141" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="L141" s="7" t="s">
+      <c r="L141" s="6" t="s">
         <v>23</v>
       </c>
     </row>
@@ -2359,7 +2367,7 @@
       <c r="D142" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="J142" s="5" t="n">
+      <c r="J142" s="0" t="n">
         <f aca="false">AVERAGE(K130:K139)</f>
         <v>92.5</v>
       </c>
@@ -2441,7 +2449,7 @@
       <c r="D150" s="0" t="s">
         <v>16</v>
       </c>
-      <c r="E150" s="5" t="n">
+      <c r="E150" s="0" t="n">
         <f aca="false">C150-C144/2</f>
         <v>271</v>
       </c>
@@ -2451,7 +2459,7 @@
       <c r="H150" s="3" t="n">
         <v>32</v>
       </c>
-      <c r="J150" s="5" t="n">
+      <c r="J150" s="0" t="n">
         <f aca="false">E153-E155</f>
         <v>95</v>
       </c>
@@ -2459,13 +2467,17 @@
         <f aca="false">$C$157+H150-$C$144/2-$E$150-50</f>
         <v>45</v>
       </c>
-      <c r="M150" s="5" t="n">
+      <c r="M150" s="0" t="n">
         <f aca="false">C143*0.001/(C143*0.001)</f>
         <v>1</v>
       </c>
-      <c r="N150" s="5" t="n">
+      <c r="N150" s="0" t="n">
         <f aca="false">$M$150*$J$162^2/$J$150^2</f>
         <v>0.226876731301939</v>
+      </c>
+      <c r="O150" s="0" t="n">
+        <f aca="false">1-((1+M150)*J162^2/J150^2)</f>
+        <v>0.546246537396122</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="151">
@@ -2502,14 +2514,14 @@
       <c r="B153" s="0" t="s">
         <v>15</v>
       </c>
-      <c r="C153" s="5" t="n">
+      <c r="C153" s="0" t="n">
         <f aca="false">C150-C144</f>
         <v>245</v>
       </c>
       <c r="D153" s="0" t="s">
         <v>16</v>
       </c>
-      <c r="E153" s="5" t="n">
+      <c r="E153" s="0" t="n">
         <f aca="false">C153-C144/2</f>
         <v>219</v>
       </c>
@@ -2549,7 +2561,7 @@
       <c r="D155" s="0" t="s">
         <v>16</v>
       </c>
-      <c r="E155" s="5" t="n">
+      <c r="E155" s="0" t="n">
         <f aca="false">C155-C144/2</f>
         <v>124</v>
       </c>
@@ -2580,7 +2592,7 @@
       <c r="B157" s="0" t="s">
         <v>20</v>
       </c>
-      <c r="C157" s="6" t="n">
+      <c r="C157" s="5" t="n">
         <v>360</v>
       </c>
       <c r="G157" s="3" t="n">
@@ -2622,13 +2634,13 @@
       <c r="B161" s="0" t="s">
         <v>0</v>
       </c>
-      <c r="J161" s="7" t="s">
+      <c r="J161" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="K161" s="7" t="s">
+      <c r="K161" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="L161" s="7" t="s">
+      <c r="L161" s="6" t="s">
         <v>23</v>
       </c>
     </row>
@@ -2643,7 +2655,7 @@
       <c r="D162" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="J162" s="5" t="n">
+      <c r="J162" s="0" t="n">
         <f aca="false">AVERAGE(K150:K159)</f>
         <v>45.25</v>
       </c>
@@ -2725,7 +2737,7 @@
       <c r="D170" s="0" t="s">
         <v>16</v>
       </c>
-      <c r="E170" s="5" t="n">
+      <c r="E170" s="0" t="n">
         <f aca="false">C170-D164/2</f>
         <v>277</v>
       </c>
@@ -2735,7 +2747,7 @@
       <c r="H170" s="3" t="n">
         <v>36</v>
       </c>
-      <c r="J170" s="5" t="n">
+      <c r="J170" s="0" t="n">
         <f aca="false">E173-E175</f>
         <v>146</v>
       </c>
@@ -2743,11 +2755,11 @@
         <f aca="false">$C$177+H170-$D$164/2-$E$170-50</f>
         <v>96.5</v>
       </c>
-      <c r="M170" s="5" t="n">
+      <c r="M170" s="0" t="n">
         <f aca="false">D163*0.001/(C163*0.001)</f>
         <v>1.94259259259259</v>
       </c>
-      <c r="N170" s="5" t="n">
+      <c r="N170" s="0" t="n">
         <f aca="false">$M$170*$J$182^2/$J$170^2</f>
         <v>0.84865396276836</v>
       </c>
@@ -2792,7 +2804,7 @@
       <c r="D173" s="0" t="s">
         <v>16</v>
       </c>
-      <c r="E173" s="5" t="n">
+      <c r="E173" s="0" t="n">
         <f aca="false">C173-C164/2</f>
         <v>220</v>
       </c>
@@ -2832,7 +2844,7 @@
       <c r="D175" s="0" t="s">
         <v>16</v>
       </c>
-      <c r="E175" s="5" t="n">
+      <c r="E175" s="0" t="n">
         <f aca="false">C175-C164/2</f>
         <v>74</v>
       </c>
@@ -2863,7 +2875,7 @@
       <c r="B177" s="0" t="s">
         <v>20</v>
       </c>
-      <c r="C177" s="6" t="n">
+      <c r="C177" s="5" t="n">
         <v>420</v>
       </c>
       <c r="G177" s="3" t="n">
@@ -2905,13 +2917,13 @@
       <c r="B181" s="0" t="s">
         <v>0</v>
       </c>
-      <c r="J181" s="7" t="s">
+      <c r="J181" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="K181" s="7" t="s">
+      <c r="K181" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="L181" s="7" t="s">
+      <c r="L181" s="6" t="s">
         <v>23</v>
       </c>
     </row>
@@ -2926,7 +2938,7 @@
       <c r="D182" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="J182" s="5" t="n">
+      <c r="J182" s="0" t="n">
         <f aca="false">AVERAGE(K170:K179)</f>
         <v>96.5</v>
       </c>
@@ -3008,7 +3020,7 @@
       <c r="D190" s="0" t="s">
         <v>16</v>
       </c>
-      <c r="E190" s="5" t="n">
+      <c r="E190" s="0" t="n">
         <f aca="false">C190-D184/2</f>
         <v>277</v>
       </c>
@@ -3018,7 +3030,7 @@
       <c r="H190" s="3" t="n">
         <v>35</v>
       </c>
-      <c r="J190" s="5" t="n">
+      <c r="J190" s="0" t="n">
         <f aca="false">E193-E195</f>
         <v>146</v>
       </c>
@@ -3026,13 +3038,17 @@
         <f aca="false">$C$197+H190-$D$184/2-$E$190-50</f>
         <v>45.5</v>
       </c>
-      <c r="M190" s="5" t="n">
+      <c r="M190" s="0" t="n">
         <f aca="false">D183*0.001/(C183*0.001)</f>
         <v>1.94259259259259</v>
       </c>
-      <c r="N190" s="5" t="n">
+      <c r="N190" s="0" t="n">
         <f aca="false">$M$190*$J$202^2/$J$190^2</f>
         <v>0.196628947000341</v>
+      </c>
+      <c r="O190" s="0" t="n">
+        <f aca="false">1-((1+M190)*J202^2/J190^2)</f>
+        <v>0.702151194677273</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="191">
@@ -3075,7 +3091,7 @@
       <c r="D193" s="0" t="s">
         <v>16</v>
       </c>
-      <c r="E193" s="5" t="n">
+      <c r="E193" s="0" t="n">
         <f aca="false">C193-C184/2</f>
         <v>220</v>
       </c>
@@ -3115,7 +3131,7 @@
       <c r="D195" s="0" t="s">
         <v>16</v>
       </c>
-      <c r="E195" s="5" t="n">
+      <c r="E195" s="0" t="n">
         <f aca="false">C195-C184/2</f>
         <v>74</v>
       </c>
@@ -3146,7 +3162,7 @@
       <c r="B197" s="0" t="s">
         <v>20</v>
       </c>
-      <c r="C197" s="6" t="n">
+      <c r="C197" s="5" t="n">
         <v>370</v>
       </c>
       <c r="G197" s="3" t="n">
@@ -3188,13 +3204,13 @@
       <c r="B201" s="0" t="s">
         <v>0</v>
       </c>
-      <c r="J201" s="7" t="s">
+      <c r="J201" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="K201" s="7" t="s">
+      <c r="K201" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="L201" s="7" t="s">
+      <c r="L201" s="6" t="s">
         <v>23</v>
       </c>
     </row>
@@ -3209,7 +3225,7 @@
       <c r="D202" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="J202" s="5" t="n">
+      <c r="J202" s="0" t="n">
         <f aca="false">AVERAGE(K190:K199)</f>
         <v>46.45</v>
       </c>
@@ -3291,7 +3307,7 @@
       <c r="D210" s="0" t="s">
         <v>16</v>
       </c>
-      <c r="E210" s="5" t="n">
+      <c r="E210" s="0" t="n">
         <f aca="false">C210-C204/2</f>
         <v>277.5</v>
       </c>
@@ -3301,7 +3317,7 @@
       <c r="H210" s="3" t="n">
         <v>43</v>
       </c>
-      <c r="J210" s="5" t="n">
+      <c r="J210" s="0" t="n">
         <f aca="false">E213-E215</f>
         <v>72.5</v>
       </c>
@@ -3309,11 +3325,11 @@
         <f aca="false">$C$217+H210-$C$204/2-$E$210-50</f>
         <v>89.5</v>
       </c>
-      <c r="M210" s="5" t="n">
+      <c r="M210" s="0" t="n">
         <f aca="false">C203*0.001/(D203*0.001)</f>
         <v>0.514775977121068</v>
       </c>
-      <c r="N210" s="5" t="n">
+      <c r="N210" s="0" t="n">
         <f aca="false">$M$210*$J$222^2/$J$210^2</f>
         <v>0.786245690080242</v>
       </c>
@@ -3358,7 +3374,7 @@
       <c r="D213" s="0" t="s">
         <v>16</v>
       </c>
-      <c r="E213" s="5" t="n">
+      <c r="E213" s="0" t="n">
         <f aca="false">C213-D204/2</f>
         <v>220</v>
       </c>
@@ -3398,7 +3414,7 @@
       <c r="D215" s="0" t="s">
         <v>16</v>
       </c>
-      <c r="E215" s="5" t="n">
+      <c r="E215" s="0" t="n">
         <f aca="false">C215-D204/2</f>
         <v>147.5</v>
       </c>
@@ -3429,7 +3445,7 @@
       <c r="B217" s="0" t="s">
         <v>20</v>
       </c>
-      <c r="C217" s="6" t="n">
+      <c r="C217" s="5" t="n">
         <v>400</v>
       </c>
       <c r="G217" s="3" t="n">
@@ -3471,13 +3487,13 @@
       <c r="B221" s="0" t="s">
         <v>0</v>
       </c>
-      <c r="J221" s="7" t="s">
+      <c r="J221" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="K221" s="7" t="s">
+      <c r="K221" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="L221" s="7" t="s">
+      <c r="L221" s="6" t="s">
         <v>23</v>
       </c>
     </row>
@@ -3492,7 +3508,7 @@
       <c r="D222" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="J222" s="5" t="n">
+      <c r="J222" s="0" t="n">
         <f aca="false">AVERAGE(K210:K219)</f>
         <v>89.6</v>
       </c>
@@ -3574,7 +3590,7 @@
       <c r="D230" s="0" t="s">
         <v>16</v>
       </c>
-      <c r="E230" s="5" t="n">
+      <c r="E230" s="0" t="n">
         <f aca="false">C230-C224/2</f>
         <v>277.5</v>
       </c>
@@ -3584,7 +3600,7 @@
       <c r="H230" s="3" t="n">
         <v>38</v>
       </c>
-      <c r="J230" s="5" t="n">
+      <c r="J230" s="0" t="n">
         <f aca="false">E233-E235</f>
         <v>72.5</v>
       </c>
@@ -3592,13 +3608,17 @@
         <f aca="false">$C$237+H230-$C$224/2-$E$230-50</f>
         <v>44.5</v>
       </c>
-      <c r="M230" s="5" t="n">
+      <c r="M230" s="0" t="n">
         <f aca="false">C223*0.001/(D223*0.001)</f>
         <v>0.514775977121068</v>
       </c>
-      <c r="N230" s="5" t="n">
+      <c r="N230" s="0" t="n">
         <f aca="false">$M$230*$J$242^2/$J$230^2</f>
         <v>0.186172374119965</v>
+      </c>
+      <c r="O230" s="0" t="n">
+        <f aca="false">1-((1+M230)*J242^2/J230^2)</f>
+        <v>0.452170550969215</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="231">
@@ -3641,7 +3661,7 @@
       <c r="D233" s="0" t="s">
         <v>16</v>
       </c>
-      <c r="E233" s="5" t="n">
+      <c r="E233" s="0" t="n">
         <f aca="false">C233-D224/2</f>
         <v>220</v>
       </c>
@@ -3681,7 +3701,7 @@
       <c r="D235" s="0" t="s">
         <v>16</v>
       </c>
-      <c r="E235" s="5" t="n">
+      <c r="E235" s="0" t="n">
         <f aca="false">C235-D224/2</f>
         <v>147.5</v>
       </c>
@@ -3712,7 +3732,7 @@
       <c r="B237" s="0" t="s">
         <v>20</v>
       </c>
-      <c r="C237" s="6" t="n">
+      <c r="C237" s="5" t="n">
         <v>360</v>
       </c>
       <c r="G237" s="3" t="n">
@@ -3754,13 +3774,13 @@
       <c r="B241" s="0" t="s">
         <v>0</v>
       </c>
-      <c r="J241" s="7" t="s">
+      <c r="J241" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="K241" s="7" t="s">
+      <c r="K241" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="L241" s="7" t="s">
+      <c r="L241" s="6" t="s">
         <v>23</v>
       </c>
     </row>
@@ -3775,7 +3795,7 @@
       <c r="D242" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="J242" s="5" t="n">
+      <c r="J242" s="0" t="n">
         <f aca="false">AVERAGE(K230:K239)</f>
         <v>43.6</v>
       </c>
@@ -3857,7 +3877,7 @@
       <c r="D250" s="0" t="s">
         <v>16</v>
       </c>
-      <c r="E250" s="5" t="n">
+      <c r="E250" s="0" t="n">
         <f aca="false">C250-B244/2</f>
         <v>271.5</v>
       </c>
@@ -3867,7 +3887,7 @@
       <c r="H250" s="3" t="n">
         <v>18</v>
       </c>
-      <c r="J250" s="5" t="n">
+      <c r="J250" s="0" t="n">
         <f aca="false">E253-E255</f>
         <v>72.5</v>
       </c>
@@ -3875,11 +3895,11 @@
         <f aca="false">$C$257+H250-$B$244/2-$E$250-50</f>
         <v>107.5</v>
       </c>
-      <c r="M250" s="5" t="n">
+      <c r="M250" s="0" t="n">
         <f aca="false">B243*0.001/(D243*0.001)</f>
         <v>0.222116301239275</v>
       </c>
-      <c r="N250" s="5" t="n">
+      <c r="N250" s="0" t="n">
         <f aca="false">$M$250*$J$262^2/$J$250^2</f>
         <v>0.500681202300135</v>
       </c>
@@ -3924,7 +3944,7 @@
       <c r="D253" s="0" t="s">
         <v>16</v>
       </c>
-      <c r="E253" s="5" t="n">
+      <c r="E253" s="0" t="n">
         <f aca="false">C253-D244/2</f>
         <v>220</v>
       </c>
@@ -3964,7 +3984,7 @@
       <c r="D255" s="0" t="s">
         <v>16</v>
       </c>
-      <c r="E255" s="5" t="n">
+      <c r="E255" s="0" t="n">
         <f aca="false">C255-D244/2</f>
         <v>147.5</v>
       </c>
@@ -3995,7 +4015,7 @@
       <c r="B257" s="0" t="s">
         <v>20</v>
       </c>
-      <c r="C257" s="6" t="n">
+      <c r="C257" s="5" t="n">
         <v>430</v>
       </c>
       <c r="G257" s="3" t="n">
@@ -4037,13 +4057,13 @@
       <c r="B261" s="0" t="s">
         <v>0</v>
       </c>
-      <c r="J261" s="7" t="s">
+      <c r="J261" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="K261" s="7" t="s">
+      <c r="K261" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="L261" s="7" t="s">
+      <c r="L261" s="6" t="s">
         <v>23</v>
       </c>
     </row>
@@ -4058,7 +4078,7 @@
       <c r="D262" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="J262" s="5" t="n">
+      <c r="J262" s="0" t="n">
         <f aca="false">AVERAGE(K250:K259)</f>
         <v>108.85</v>
       </c>
@@ -4140,7 +4160,7 @@
       <c r="D270" s="0" t="s">
         <v>16</v>
       </c>
-      <c r="E270" s="5" t="n">
+      <c r="E270" s="0" t="n">
         <f aca="false">C270-B264/2</f>
         <v>271.5</v>
       </c>
@@ -4150,7 +4170,7 @@
       <c r="H270" s="3" t="n">
         <v>27</v>
       </c>
-      <c r="J270" s="5" t="n">
+      <c r="J270" s="0" t="n">
         <f aca="false">E273-E275</f>
         <v>72.5</v>
       </c>
@@ -4158,13 +4178,17 @@
         <f aca="false">$C$277+H270-$B$264/2-$E$270-50</f>
         <v>56.5</v>
       </c>
-      <c r="M270" s="5" t="n">
+      <c r="M270" s="0" t="n">
         <f aca="false">B263*0.001/(D263*0.001)</f>
         <v>0.222116301239275</v>
       </c>
-      <c r="N270" s="5" t="n">
+      <c r="N270" s="0" t="n">
         <f aca="false">$M$270*$J$282^2/$J$270^2</f>
         <v>0.137535787098069</v>
+      </c>
+      <c r="O270" s="0" t="n">
+        <f aca="false">1-((1+M270)*J282^2/J270^2)</f>
+        <v>0.243258029786593</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="271">
@@ -4207,7 +4231,7 @@
       <c r="D273" s="0" t="s">
         <v>16</v>
       </c>
-      <c r="E273" s="5" t="n">
+      <c r="E273" s="0" t="n">
         <f aca="false">C273-D264/2</f>
         <v>220</v>
       </c>
@@ -4247,7 +4271,7 @@
       <c r="D275" s="0" t="s">
         <v>16</v>
       </c>
-      <c r="E275" s="5" t="n">
+      <c r="E275" s="0" t="n">
         <f aca="false">C275-D264/2</f>
         <v>147.5</v>
       </c>
@@ -4278,7 +4302,7 @@
       <c r="B277" s="0" t="s">
         <v>20</v>
       </c>
-      <c r="C277" s="6" t="n">
+      <c r="C277" s="5" t="n">
         <v>370</v>
       </c>
       <c r="G277" s="3" t="n">
@@ -4317,18 +4341,18 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="281">
-      <c r="J281" s="7" t="s">
+      <c r="J281" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="K281" s="7" t="s">
+      <c r="K281" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="L281" s="7" t="s">
+      <c r="L281" s="6" t="s">
         <v>23</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="282">
-      <c r="J282" s="5" t="n">
+      <c r="J282" s="0" t="n">
         <f aca="false">AVERAGE(K270:K279)</f>
         <v>57.05</v>
       </c>

</xml_diff>

<commit_message>
Ready to add excel diagrams
	modified:   exp3/data/values.xlsx
</commit_message>
<xml_diff>
--- a/exp3/data/values.xlsx
+++ b/exp3/data/values.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="392" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="405" uniqueCount="35">
   <si>
     <t>Balls</t>
   </si>
@@ -43,6 +43,15 @@
     <t>elastic</t>
   </si>
   <si>
+    <t>Theoretical</t>
+  </si>
+  <si>
+    <t>Measurement</t>
+  </si>
+  <si>
+    <t>inelastic</t>
+  </si>
+  <si>
     <t>ball 2:</t>
   </si>
   <si>
@@ -64,6 +73,9 @@
     <t>T2'/T1</t>
   </si>
   <si>
+    <t>ball 1 vs ball 3</t>
+  </si>
+  <si>
     <t>initial right:</t>
   </si>
   <si>
@@ -73,10 +85,25 @@
     <t>ball 1:</t>
   </si>
   <si>
+    <t>ball 3 vs ball 2</t>
+  </si>
+  <si>
     <t>in rest</t>
   </si>
   <si>
+    <t>ball 2 vs ball 2</t>
+  </si>
+  <si>
+    <t>ball 2 vs ball 3</t>
+  </si>
+  <si>
     <t>initial:</t>
+  </si>
+  <si>
+    <t>ball 2 vs ball 1</t>
+  </si>
+  <si>
+    <t>ball 3 vs ball 1</t>
   </si>
   <si>
     <t>slider</t>
@@ -94,25 +121,7 @@
     <t>unelastic</t>
   </si>
   <si>
-    <t>ball 1 vs ball 3</t>
-  </si>
-  <si>
     <t>ball 3:</t>
-  </si>
-  <si>
-    <t>ball 2 vs ball 1</t>
-  </si>
-  <si>
-    <t>ball 2 vs ball 2</t>
-  </si>
-  <si>
-    <t>ball 2 vs ball 3</t>
-  </si>
-  <si>
-    <t>ball 3 vs ball 2</t>
-  </si>
-  <si>
-    <t>ball 3 vs ball 1</t>
   </si>
 </sst>
 </file>
@@ -276,8 +285,8 @@
     <cellStyle builtinId="4" customBuiltin="false" name="Currency" xfId="17"/>
     <cellStyle builtinId="7" customBuiltin="false" name="Currency [0]" xfId="18"/>
     <cellStyle builtinId="5" customBuiltin="false" name="Percent" xfId="19"/>
-    <cellStyle builtinId="54" customBuiltin="true" name="Excel Built-in Excel Built-in Excel Built-in 20% - Accent1" xfId="20"/>
-    <cellStyle builtinId="54" customBuiltin="true" name="Excel Built-in Excel Built-in Excel Built-in Good" xfId="21"/>
+    <cellStyle builtinId="54" customBuiltin="true" name="Excel Built-in Excel Built-in Excel Built-in Excel Built-in 20% - Accent1" xfId="20"/>
+    <cellStyle builtinId="54" customBuiltin="true" name="Excel Built-in Excel Built-in Excel Built-in Excel Built-in Good" xfId="21"/>
   </cellStyles>
   <colors>
     <indexedColors>
@@ -347,10 +356,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A2:O282"/>
+  <dimension ref="A2:V282"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A247" view="normal" windowProtection="false" workbookViewId="0" zoomScale="55" zoomScaleNormal="55" zoomScalePageLayoutView="100">
-      <selection activeCell="O272" activeCellId="0" pane="topLeft" sqref="O272"/>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="E1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="55" zoomScaleNormal="55" zoomScalePageLayoutView="100">
+      <selection activeCell="T20" activeCellId="0" pane="topLeft" sqref="T20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -360,7 +369,11 @@
     <col collapsed="false" hidden="false" max="7" min="7" style="0" width="18.2834008097166"/>
     <col collapsed="false" hidden="false" max="10" min="8" style="0" width="10.5748987854251"/>
     <col collapsed="false" hidden="false" max="12" min="11" style="0" width="11.4251012145749"/>
-    <col collapsed="false" hidden="false" max="1025" min="13" style="0" width="10.5748987854251"/>
+    <col collapsed="false" hidden="false" max="15" min="13" style="0" width="10.5748987854251"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="13.5060728744939"/>
+    <col collapsed="false" hidden="false" max="20" min="17" style="0" width="10.5748987854251"/>
+    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="12.004048582996"/>
+    <col collapsed="false" hidden="false" max="1025" min="22" style="0" width="10.5748987854251"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="2">
@@ -415,39 +428,80 @@
       <c r="B9" s="2" t="s">
         <v>7</v>
       </c>
+      <c r="P9" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="Q9" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="R9" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="T9" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="U9" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="V9" s="0" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="10">
       <c r="B10" s="0" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="G10" s="3" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="H10" s="3" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="J10" s="4" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="K10" s="4" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="M10" s="0" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="N10" s="0" t="s">
-        <v>14</v>
+        <v>17</v>
+      </c>
+      <c r="P10" s="0" t="str">
+        <f aca="false">$A$48</f>
+        <v>ball 1 vs ball 3</v>
+      </c>
+      <c r="Q10" s="0" t="n">
+        <f aca="false">M50*4/(M50+1)^2</f>
+        <v>0.594860799112152</v>
+      </c>
+      <c r="R10" s="0" t="n">
+        <f aca="false">N50</f>
+        <v>0.555509332580547</v>
+      </c>
+      <c r="T10" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="U10" s="0" t="n">
+        <f aca="false">M70/(M70+1)^2</f>
+        <v>0.148715199778038</v>
+      </c>
+      <c r="V10" s="0" t="n">
+        <f aca="false">N70</f>
+        <v>0.128566528075106</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="11">
       <c r="B11" s="0" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="C11" s="0" t="n">
         <v>291</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="E11" s="0" t="n">
         <f aca="false">C11-C5/2</f>
@@ -475,10 +529,33 @@
         <f aca="false">$M$11*$J$23^2/$J$11^2</f>
         <v>0.799718868077318</v>
       </c>
+      <c r="P11" s="0" t="str">
+        <f aca="false">$A$9</f>
+        <v>ball 1 vs ball 2</v>
+      </c>
+      <c r="Q11" s="0" t="n">
+        <f aca="false">M11*4/(M11+1)^2</f>
+        <v>0.842268743441741</v>
+      </c>
+      <c r="R11" s="0" t="n">
+        <f aca="false">N11</f>
+        <v>0.799718868077318</v>
+      </c>
+      <c r="T11" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="U11" s="0" t="n">
+        <f aca="false">M30/(M30+1)^2</f>
+        <v>0.210567185860435</v>
+      </c>
+      <c r="V11" s="0" t="n">
+        <f aca="false">N30</f>
+        <v>0.189786966174024</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="12">
       <c r="B12" s="0" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="G12" s="3" t="n">
         <v>2</v>
@@ -490,10 +567,33 @@
         <f aca="false">$C$18+H12-$C$5/2-$E$11-50</f>
         <v>93</v>
       </c>
+      <c r="P12" s="0" t="str">
+        <f aca="false">$A$208</f>
+        <v>ball 3 vs ball 2</v>
+      </c>
+      <c r="Q12" s="0" t="n">
+        <f aca="false">M210*4/(M210+1)^2</f>
+        <v>0.897390453008233</v>
+      </c>
+      <c r="R12" s="0" t="n">
+        <f aca="false">N210</f>
+        <v>0.786245690080242</v>
+      </c>
+      <c r="T12" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="U12" s="0" t="n">
+        <f aca="false">M230/(M230+1)^2</f>
+        <v>0.224347613252058</v>
+      </c>
+      <c r="V12" s="0" t="n">
+        <f aca="false">N230</f>
+        <v>0.186172374119965</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="13">
       <c r="B13" s="0" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="G13" s="3" t="n">
         <v>3</v>
@@ -505,17 +605,40 @@
         <f aca="false">$C$18+H13-$C$5/2-$E$11-50</f>
         <v>94</v>
       </c>
+      <c r="P13" s="0" t="str">
+        <f aca="false">$A$128</f>
+        <v>ball 2 vs ball 2</v>
+      </c>
+      <c r="Q13" s="0" t="n">
+        <f aca="false">M130*4/(M130+1)^2</f>
+        <v>1</v>
+      </c>
+      <c r="R13" s="0" t="n">
+        <f aca="false">N130</f>
+        <v>0.948060941828255</v>
+      </c>
+      <c r="T13" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="U13" s="0" t="n">
+        <f aca="false">M150/(M150+1)^2</f>
+        <v>0.25</v>
+      </c>
+      <c r="V13" s="0" t="n">
+        <f aca="false">N150</f>
+        <v>0.226876731301939</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="14">
       <c r="B14" s="0" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="C14" s="0" t="n">
         <f aca="false">C11-C5</f>
         <v>239</v>
       </c>
       <c r="D14" s="0" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="E14" s="0" t="n">
         <f aca="false">C14-B5/2</f>
@@ -531,10 +654,33 @@
         <f aca="false">$C$18+H14-$C$5/2-$E$11-50</f>
         <v>94</v>
       </c>
+      <c r="P14" s="0" t="str">
+        <f aca="false">$A$168</f>
+        <v>ball 2 vs ball 3</v>
+      </c>
+      <c r="Q14" s="0" t="n">
+        <f aca="false">M170*4/(M170+1)^2</f>
+        <v>0.897390453008233</v>
+      </c>
+      <c r="R14" s="0" t="n">
+        <f aca="false">N170</f>
+        <v>0.84865396276836</v>
+      </c>
+      <c r="T14" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="U14" s="0" t="n">
+        <f aca="false">M190/(M190+1)^2</f>
+        <v>0.224347613252058</v>
+      </c>
+      <c r="V14" s="0" t="n">
+        <f aca="false">N190</f>
+        <v>0.196628947000341</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="15">
       <c r="B15" s="0" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="G15" s="3" t="n">
         <v>5</v>
@@ -546,16 +692,39 @@
         <f aca="false">$C$18+H15-$C$5/2-$E$11-50</f>
         <v>95</v>
       </c>
+      <c r="P15" s="0" t="str">
+        <f aca="false">$A$88</f>
+        <v>ball 2 vs ball 1</v>
+      </c>
+      <c r="Q15" s="0" t="n">
+        <f aca="false">M90*4/(M90+1)^2</f>
+        <v>0.842268743441741</v>
+      </c>
+      <c r="R15" s="0" t="n">
+        <f aca="false">N90</f>
+        <v>0.765518068450414</v>
+      </c>
+      <c r="T15" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="U15" s="0" t="n">
+        <f aca="false">M110/(M110+1)^2</f>
+        <v>0.210567185860435</v>
+      </c>
+      <c r="V15" s="0" t="n">
+        <f aca="false">N110</f>
+        <v>0.191881057453478</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="16">
       <c r="B16" s="0" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="C16" s="0" t="n">
         <v>80</v>
       </c>
       <c r="D16" s="0" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="E16" s="0" t="n">
         <f aca="false">C16-B5/2</f>
@@ -571,6 +740,29 @@
         <f aca="false">$C$18+H16-$C$5/2-$E$11-50</f>
         <v>93</v>
       </c>
+      <c r="P16" s="0" t="str">
+        <f aca="false">$A$248</f>
+        <v>ball 3 vs ball 1</v>
+      </c>
+      <c r="Q16" s="0" t="n">
+        <f aca="false">M250*4/(M250+1)^2</f>
+        <v>0.594860799112152</v>
+      </c>
+      <c r="R16" s="0" t="n">
+        <f aca="false">N250</f>
+        <v>0.500681202300135</v>
+      </c>
+      <c r="T16" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="U16" s="0" t="n">
+        <f aca="false">M270/(M270+1)^2</f>
+        <v>0.148715199778038</v>
+      </c>
+      <c r="V16" s="0" t="n">
+        <f aca="false">N270</f>
+        <v>0.137535787098069</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="17">
       <c r="G17" s="3" t="n">
@@ -586,7 +778,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="18">
       <c r="B18" s="0" t="s">
-        <v>20</v>
+        <v>29</v>
       </c>
       <c r="C18" s="5" t="n">
         <v>400</v>
@@ -643,13 +835,13 @@
         <v>3</v>
       </c>
       <c r="J22" s="6" t="s">
-        <v>21</v>
+        <v>30</v>
       </c>
       <c r="K22" s="6" t="s">
-        <v>22</v>
+        <v>31</v>
       </c>
       <c r="L22" s="6" t="s">
-        <v>23</v>
+        <v>32</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="23">
@@ -671,11 +863,11 @@
       </c>
       <c r="K23" s="0" t="n">
         <f aca="false">STDEV(K11:K20)</f>
-        <v>0.699205898779639</v>
+        <v>0.699205898780101</v>
       </c>
       <c r="L23" s="0" t="n">
         <f aca="false">K23/SQRT(COUNT(K11:K20))</f>
-        <v>0.22110831935688</v>
+        <v>0.221108319357027</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="24">
@@ -697,41 +889,41 @@
         <v>6</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>24</v>
+        <v>33</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="29">
       <c r="B29" s="0" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="G29" s="3" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="H29" s="3" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="J29" s="4" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="K29" s="4" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="M29" s="0" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="N29" s="0" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="30">
       <c r="B30" s="0" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="C30" s="0" t="n">
         <v>291</v>
       </c>
       <c r="D30" s="0" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="E30" s="0" t="n">
         <f aca="false">C30-C24/2</f>
@@ -761,12 +953,12 @@
       </c>
       <c r="O30" s="0" t="n">
         <f aca="false">1-((1+M30)*J42^2/J30^2)</f>
-        <v>0.728323472495332</v>
+        <v>0.728323472495333</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="31">
       <c r="B31" s="0" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="G31" s="3" t="n">
         <v>2</v>
@@ -781,7 +973,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="32">
       <c r="B32" s="0" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="G32" s="3" t="n">
         <v>3</v>
@@ -796,14 +988,14 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="33">
       <c r="B33" s="0" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="C33" s="0" t="n">
         <f aca="false">C30-C24</f>
         <v>239</v>
       </c>
       <c r="D33" s="0" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="E33" s="0" t="n">
         <f aca="false">C33-B24/2</f>
@@ -822,7 +1014,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="34">
       <c r="B34" s="0" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="G34" s="3" t="n">
         <v>5</v>
@@ -837,13 +1029,13 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="35">
       <c r="B35" s="0" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="C35" s="0" t="n">
         <v>80</v>
       </c>
       <c r="D35" s="0" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="E35" s="0" t="n">
         <f aca="false">C35-B24/2</f>
@@ -874,7 +1066,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="37">
       <c r="B37" s="0" t="s">
-        <v>20</v>
+        <v>29</v>
       </c>
       <c r="C37" s="5" t="n">
         <v>350</v>
@@ -919,13 +1111,13 @@
         <v>0</v>
       </c>
       <c r="J41" s="6" t="s">
-        <v>21</v>
+        <v>30</v>
       </c>
       <c r="K41" s="6" t="s">
-        <v>22</v>
+        <v>31</v>
       </c>
       <c r="L41" s="6" t="s">
-        <v>23</v>
+        <v>32</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="42">
@@ -982,7 +1174,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="48">
       <c r="A48" s="2" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="B48" s="2" t="s">
         <v>7</v>
@@ -990,36 +1182,36 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="49">
       <c r="B49" s="0" t="s">
-        <v>26</v>
+        <v>34</v>
       </c>
       <c r="G49" s="3" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="H49" s="3" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="J49" s="4" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="K49" s="4" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="M49" s="0" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="N49" s="0" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="50">
       <c r="B50" s="0" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="C50" s="0" t="n">
         <v>303</v>
       </c>
       <c r="D50" s="0" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="E50" s="0" t="n">
         <f aca="false">C50-D44/2</f>
@@ -1050,7 +1242,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="51">
       <c r="B51" s="0" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="G51" s="3" t="n">
         <v>2</v>
@@ -1065,7 +1257,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="52">
       <c r="B52" s="0" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="G52" s="3" t="n">
         <v>3</v>
@@ -1080,14 +1272,14 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="53">
       <c r="B53" s="0" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="C53" s="0" t="n">
         <f aca="false">C50-D44</f>
         <v>238</v>
       </c>
       <c r="D53" s="0" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="E53" s="0" t="n">
         <f aca="false">C53-B44/2</f>
@@ -1106,7 +1298,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="54">
       <c r="B54" s="0" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="G54" s="3" t="n">
         <v>5</v>
@@ -1121,13 +1313,13 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="55">
       <c r="B55" s="0" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="C55" s="0" t="n">
         <v>80</v>
       </c>
       <c r="D55" s="0" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="E55" s="0" t="n">
         <f aca="false">C55-B44/2</f>
@@ -1158,7 +1350,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="57">
       <c r="B57" s="0" t="s">
-        <v>20</v>
+        <v>29</v>
       </c>
       <c r="C57" s="5" t="n">
         <v>370</v>
@@ -1203,13 +1395,13 @@
         <v>0</v>
       </c>
       <c r="J61" s="6" t="s">
-        <v>21</v>
+        <v>30</v>
       </c>
       <c r="K61" s="6" t="s">
-        <v>22</v>
+        <v>31</v>
       </c>
       <c r="L61" s="6" t="s">
-        <v>23</v>
+        <v>32</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="62">
@@ -1266,44 +1458,44 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="68">
       <c r="A68" s="2" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>24</v>
+        <v>33</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="69">
       <c r="B69" s="0" t="s">
-        <v>26</v>
+        <v>34</v>
       </c>
       <c r="G69" s="3" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="H69" s="3" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="J69" s="4" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="K69" s="4" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="M69" s="0" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="N69" s="0" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="70">
       <c r="B70" s="0" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="C70" s="0" t="n">
         <v>303</v>
       </c>
       <c r="D70" s="0" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="E70" s="0" t="n">
         <f aca="false">C70-D64/2</f>
@@ -1338,7 +1530,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="71">
       <c r="B71" s="0" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="G71" s="3" t="n">
         <v>2</v>
@@ -1353,7 +1545,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="72">
       <c r="B72" s="0" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="G72" s="3" t="n">
         <v>3</v>
@@ -1368,14 +1560,14 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="73">
       <c r="B73" s="0" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="C73" s="0" t="n">
         <f aca="false">C70-D64</f>
         <v>238</v>
       </c>
       <c r="D73" s="0" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="E73" s="0" t="n">
         <f aca="false">C73-B64/2</f>
@@ -1394,7 +1586,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="74">
       <c r="B74" s="0" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="G74" s="3" t="n">
         <v>5</v>
@@ -1409,13 +1601,13 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="75">
       <c r="B75" s="0" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="C75" s="0" t="n">
         <v>80</v>
       </c>
       <c r="D75" s="0" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="E75" s="0" t="n">
         <f aca="false">C75-B64/2</f>
@@ -1446,7 +1638,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="77">
       <c r="B77" s="0" t="s">
-        <v>20</v>
+        <v>29</v>
       </c>
       <c r="C77" s="5" t="n">
         <v>350</v>
@@ -1491,13 +1683,13 @@
         <v>0</v>
       </c>
       <c r="J81" s="6" t="s">
-        <v>21</v>
+        <v>30</v>
       </c>
       <c r="K81" s="6" t="s">
-        <v>22</v>
+        <v>31</v>
       </c>
       <c r="L81" s="6" t="s">
-        <v>23</v>
+        <v>32</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="82">
@@ -1517,11 +1709,11 @@
       </c>
       <c r="K82" s="0" t="n">
         <f aca="false">STDEV(K70:K79)</f>
-        <v>0.632455532033708</v>
+        <v>0.632455532033676</v>
       </c>
       <c r="L82" s="0" t="n">
         <f aca="false">K82/SQRT(COUNT(K70:K79))</f>
-        <v>0.20000000000001</v>
+        <v>0.2</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="83">
@@ -1562,36 +1754,36 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="89">
       <c r="B89" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="G89" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="H89" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="J89" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="K89" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="M89" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="N89" s="0" t="s">
         <v>17</v>
-      </c>
-      <c r="G89" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="H89" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="J89" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="K89" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="M89" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="N89" s="0" t="s">
-        <v>14</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="90">
       <c r="B90" s="0" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="C90" s="0" t="n">
         <v>284</v>
       </c>
       <c r="D90" s="0" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="E90" s="0" t="n">
         <f aca="false">C90-B84/2</f>
@@ -1622,7 +1814,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="91">
       <c r="B91" s="0" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="G91" s="3" t="n">
         <v>2</v>
@@ -1637,7 +1829,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="92">
       <c r="B92" s="0" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="G92" s="3" t="n">
         <v>3</v>
@@ -1652,14 +1844,14 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="93">
       <c r="B93" s="0" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="C93" s="0" t="n">
         <f aca="false">C90-B84</f>
         <v>246</v>
       </c>
       <c r="D93" s="0" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="E93" s="0" t="n">
         <f aca="false">C93-C84/2</f>
@@ -1678,7 +1870,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="94">
       <c r="B94" s="0" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="G94" s="3" t="n">
         <v>5</v>
@@ -1693,13 +1885,13 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="95">
       <c r="B95" s="0" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="C95" s="0" t="n">
         <v>160</v>
       </c>
       <c r="D95" s="0" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="E95" s="0" t="n">
         <f aca="false">C95-C84/2</f>
@@ -1730,7 +1922,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="97">
       <c r="B97" s="0" t="s">
-        <v>20</v>
+        <v>29</v>
       </c>
       <c r="C97" s="5" t="n">
         <v>430</v>
@@ -1775,13 +1967,13 @@
         <v>0</v>
       </c>
       <c r="J101" s="6" t="s">
-        <v>21</v>
+        <v>30</v>
       </c>
       <c r="K101" s="6" t="s">
-        <v>22</v>
+        <v>31</v>
       </c>
       <c r="L101" s="6" t="s">
-        <v>23</v>
+        <v>32</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="102">
@@ -1801,11 +1993,11 @@
       </c>
       <c r="K102" s="0" t="n">
         <f aca="false">STDEV(K90:K99)</f>
-        <v>0.437797517886195</v>
+        <v>0.437797517885457</v>
       </c>
       <c r="L102" s="0" t="n">
         <f aca="false">K102/SQRT(COUNT(K90:K99))</f>
-        <v>0.138443731048868</v>
+        <v>0.138443731048635</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="103">
@@ -1841,41 +2033,41 @@
         <v>27</v>
       </c>
       <c r="B108" s="2" t="s">
-        <v>24</v>
+        <v>33</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="109">
       <c r="B109" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="G109" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="H109" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="J109" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="K109" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="M109" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="N109" s="0" t="s">
         <v>17</v>
-      </c>
-      <c r="G109" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="H109" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="J109" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="K109" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="M109" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="N109" s="0" t="s">
-        <v>14</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="110">
       <c r="B110" s="0" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="C110" s="0" t="n">
         <v>284</v>
       </c>
       <c r="D110" s="0" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="E110" s="0" t="n">
         <f aca="false">C110-B104/2</f>
@@ -1910,7 +2102,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="111">
       <c r="B111" s="0" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="G111" s="3" t="n">
         <v>2</v>
@@ -1925,7 +2117,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="112">
       <c r="B112" s="0" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="G112" s="3" t="n">
         <v>3</v>
@@ -1940,14 +2132,14 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="113">
       <c r="B113" s="0" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="C113" s="0" t="n">
         <f aca="false">C110-B104</f>
         <v>246</v>
       </c>
       <c r="D113" s="0" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="E113" s="0" t="n">
         <f aca="false">C113-C104/2</f>
@@ -1966,7 +2158,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="114">
       <c r="B114" s="0" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="G114" s="3" t="n">
         <v>5</v>
@@ -1981,13 +2173,13 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="115">
       <c r="B115" s="0" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="C115" s="0" t="n">
         <v>160</v>
       </c>
       <c r="D115" s="0" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="E115" s="0" t="n">
         <f aca="false">C115-C104/2</f>
@@ -2018,7 +2210,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="117">
       <c r="B117" s="0" t="s">
-        <v>20</v>
+        <v>29</v>
       </c>
       <c r="C117" s="5" t="n">
         <v>370</v>
@@ -2063,13 +2255,13 @@
         <v>0</v>
       </c>
       <c r="J121" s="6" t="s">
-        <v>21</v>
+        <v>30</v>
       </c>
       <c r="K121" s="6" t="s">
-        <v>22</v>
+        <v>31</v>
       </c>
       <c r="L121" s="6" t="s">
-        <v>23</v>
+        <v>32</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="122">
@@ -2089,11 +2281,11 @@
       </c>
       <c r="K122" s="0" t="n">
         <f aca="false">STDEV(K110:K119)</f>
-        <v>1.31339255365643</v>
+        <v>1.31339255365637</v>
       </c>
       <c r="L122" s="0" t="n">
         <f aca="false">K122/SQRT(COUNT(K110:K119))</f>
-        <v>0.415331193145923</v>
+        <v>0.415331193145904</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="123">
@@ -2126,7 +2318,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="128">
       <c r="A128" s="2" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="B128" s="2" t="s">
         <v>7</v>
@@ -2134,36 +2326,36 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="129">
       <c r="B129" s="0" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="G129" s="3" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="H129" s="3" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="J129" s="4" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="K129" s="4" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="M129" s="0" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="N129" s="0" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="130">
       <c r="B130" s="0" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="C130" s="0" t="n">
         <v>297</v>
       </c>
       <c r="D130" s="0" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="E130" s="0" t="n">
         <f aca="false">C130-C124/2</f>
@@ -2194,7 +2386,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="131">
       <c r="B131" s="0" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="G131" s="3" t="n">
         <v>2</v>
@@ -2209,7 +2401,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="132">
       <c r="B132" s="0" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="G132" s="3" t="n">
         <v>3</v>
@@ -2224,14 +2416,14 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="133">
       <c r="B133" s="0" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="C133" s="0" t="n">
         <f aca="false">C130-C124</f>
         <v>245</v>
       </c>
       <c r="D133" s="0" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="E133" s="0" t="n">
         <f aca="false">C133-C124/2</f>
@@ -2250,7 +2442,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="134">
       <c r="B134" s="0" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="G134" s="3" t="n">
         <v>5</v>
@@ -2265,13 +2457,13 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="135">
       <c r="B135" s="0" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="C135" s="0" t="n">
         <v>150</v>
       </c>
       <c r="D135" s="0" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="E135" s="0" t="n">
         <f aca="false">C135-C124/2</f>
@@ -2302,7 +2494,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="137">
       <c r="B137" s="0" t="s">
-        <v>20</v>
+        <v>29</v>
       </c>
       <c r="C137" s="5" t="n">
         <v>410</v>
@@ -2347,13 +2539,13 @@
         <v>0</v>
       </c>
       <c r="J141" s="6" t="s">
-        <v>21</v>
+        <v>30</v>
       </c>
       <c r="K141" s="6" t="s">
-        <v>22</v>
+        <v>31</v>
       </c>
       <c r="L141" s="6" t="s">
-        <v>23</v>
+        <v>32</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="142">
@@ -2410,44 +2602,44 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="148">
       <c r="A148" s="2" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="B148" s="2" t="s">
-        <v>24</v>
+        <v>33</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="149">
       <c r="B149" s="0" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="G149" s="3" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="H149" s="3" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="J149" s="4" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="K149" s="4" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="M149" s="0" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="N149" s="0" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="150">
       <c r="B150" s="0" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="C150" s="0" t="n">
         <v>297</v>
       </c>
       <c r="D150" s="0" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="E150" s="0" t="n">
         <f aca="false">C150-C144/2</f>
@@ -2482,7 +2674,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="151">
       <c r="B151" s="0" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="G151" s="3" t="n">
         <v>2</v>
@@ -2497,7 +2689,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="152">
       <c r="B152" s="0" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="G152" s="3" t="n">
         <v>3</v>
@@ -2512,14 +2704,14 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="153">
       <c r="B153" s="0" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="C153" s="0" t="n">
         <f aca="false">C150-C144</f>
         <v>245</v>
       </c>
       <c r="D153" s="0" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="E153" s="0" t="n">
         <f aca="false">C153-C144/2</f>
@@ -2538,7 +2730,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="154">
       <c r="B154" s="0" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="G154" s="3" t="n">
         <v>5</v>
@@ -2553,13 +2745,13 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="155">
       <c r="B155" s="0" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="C155" s="0" t="n">
         <v>150</v>
       </c>
       <c r="D155" s="0" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="E155" s="0" t="n">
         <f aca="false">C155-C144/2</f>
@@ -2590,7 +2782,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="157">
       <c r="B157" s="0" t="s">
-        <v>20</v>
+        <v>29</v>
       </c>
       <c r="C157" s="5" t="n">
         <v>360</v>
@@ -2635,13 +2827,13 @@
         <v>0</v>
       </c>
       <c r="J161" s="6" t="s">
-        <v>21</v>
+        <v>30</v>
       </c>
       <c r="K161" s="6" t="s">
-        <v>22</v>
+        <v>31</v>
       </c>
       <c r="L161" s="6" t="s">
-        <v>23</v>
+        <v>32</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="162">
@@ -2698,7 +2890,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="168">
       <c r="A168" s="2" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="B168" s="2" t="s">
         <v>7</v>
@@ -2706,36 +2898,36 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="169">
       <c r="B169" s="0" t="s">
-        <v>26</v>
+        <v>34</v>
       </c>
       <c r="G169" s="3" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="H169" s="3" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="J169" s="4" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="K169" s="4" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="M169" s="0" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="N169" s="0" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="170">
       <c r="B170" s="0" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="C170" s="0" t="n">
         <v>309.5</v>
       </c>
       <c r="D170" s="0" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="E170" s="0" t="n">
         <f aca="false">C170-D164/2</f>
@@ -2766,7 +2958,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="171">
       <c r="B171" s="0" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="G171" s="3" t="n">
         <v>2</v>
@@ -2781,7 +2973,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="172">
       <c r="B172" s="0" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="G172" s="3" t="n">
         <v>3</v>
@@ -2796,13 +2988,13 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="173">
       <c r="B173" s="0" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="C173" s="0" t="n">
         <v>246</v>
       </c>
       <c r="D173" s="0" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="E173" s="0" t="n">
         <f aca="false">C173-C164/2</f>
@@ -2821,7 +3013,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="174">
       <c r="B174" s="0" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="G174" s="3" t="n">
         <v>5</v>
@@ -2836,13 +3028,13 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="175">
       <c r="B175" s="0" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="C175" s="0" t="n">
         <v>100</v>
       </c>
       <c r="D175" s="0" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="E175" s="0" t="n">
         <f aca="false">C175-C164/2</f>
@@ -2873,7 +3065,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="177">
       <c r="B177" s="0" t="s">
-        <v>20</v>
+        <v>29</v>
       </c>
       <c r="C177" s="5" t="n">
         <v>420</v>
@@ -2918,13 +3110,13 @@
         <v>0</v>
       </c>
       <c r="J181" s="6" t="s">
-        <v>21</v>
+        <v>30</v>
       </c>
       <c r="K181" s="6" t="s">
-        <v>22</v>
+        <v>31</v>
       </c>
       <c r="L181" s="6" t="s">
-        <v>23</v>
+        <v>32</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="182">
@@ -2981,44 +3173,44 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="188">
       <c r="A188" s="2" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="B188" s="2" t="s">
-        <v>24</v>
+        <v>33</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="189">
       <c r="B189" s="0" t="s">
-        <v>26</v>
+        <v>34</v>
       </c>
       <c r="G189" s="3" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="H189" s="3" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="J189" s="4" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="K189" s="4" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="M189" s="0" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="N189" s="0" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="190">
       <c r="B190" s="0" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="C190" s="0" t="n">
         <v>309.5</v>
       </c>
       <c r="D190" s="0" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="E190" s="0" t="n">
         <f aca="false">C190-D184/2</f>
@@ -3048,12 +3240,12 @@
       </c>
       <c r="O190" s="0" t="n">
         <f aca="false">1-((1+M190)*J202^2/J190^2)</f>
-        <v>0.702151194677273</v>
+        <v>0.702151194677272</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="191">
       <c r="B191" s="0" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="G191" s="3" t="n">
         <v>2</v>
@@ -3068,7 +3260,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="192">
       <c r="B192" s="0" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="G192" s="3" t="n">
         <v>3</v>
@@ -3083,13 +3275,13 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="193">
       <c r="B193" s="0" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="C193" s="0" t="n">
         <v>246</v>
       </c>
       <c r="D193" s="0" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="E193" s="0" t="n">
         <f aca="false">C193-C184/2</f>
@@ -3108,7 +3300,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="194">
       <c r="B194" s="0" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="G194" s="3" t="n">
         <v>5</v>
@@ -3123,13 +3315,13 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="195">
       <c r="B195" s="0" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="C195" s="0" t="n">
         <v>100</v>
       </c>
       <c r="D195" s="0" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="E195" s="0" t="n">
         <f aca="false">C195-C184/2</f>
@@ -3160,7 +3352,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="197">
       <c r="B197" s="0" t="s">
-        <v>20</v>
+        <v>29</v>
       </c>
       <c r="C197" s="5" t="n">
         <v>370</v>
@@ -3205,13 +3397,13 @@
         <v>0</v>
       </c>
       <c r="J201" s="6" t="s">
-        <v>21</v>
+        <v>30</v>
       </c>
       <c r="K201" s="6" t="s">
-        <v>22</v>
+        <v>31</v>
       </c>
       <c r="L201" s="6" t="s">
-        <v>23</v>
+        <v>32</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="202">
@@ -3231,11 +3423,11 @@
       </c>
       <c r="K202" s="0" t="n">
         <f aca="false">STDEV(K190:K199)</f>
-        <v>1.23490890352278</v>
+        <v>1.23490890352285</v>
       </c>
       <c r="L202" s="0" t="n">
         <f aca="false">K202/SQRT(COUNT(K190:K199))</f>
-        <v>0.390512483795312</v>
+        <v>0.390512483795333</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="203">
@@ -3268,7 +3460,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="208">
       <c r="A208" s="2" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="B208" s="2" t="s">
         <v>7</v>
@@ -3276,36 +3468,36 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="209">
       <c r="B209" s="0" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="G209" s="3" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="H209" s="3" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="J209" s="4" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="K209" s="4" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="M209" s="0" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="N209" s="0" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="210">
       <c r="B210" s="0" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="C210" s="0" t="n">
         <v>303.5</v>
       </c>
       <c r="D210" s="0" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="E210" s="0" t="n">
         <f aca="false">C210-C204/2</f>
@@ -3336,7 +3528,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="211">
       <c r="B211" s="0" t="s">
-        <v>26</v>
+        <v>34</v>
       </c>
       <c r="G211" s="3" t="n">
         <v>2</v>
@@ -3351,7 +3543,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="212">
       <c r="B212" s="0" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="G212" s="3" t="n">
         <v>3</v>
@@ -3366,13 +3558,13 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="213">
       <c r="B213" s="0" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="C213" s="0" t="n">
         <v>252.5</v>
       </c>
       <c r="D213" s="0" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="E213" s="0" t="n">
         <f aca="false">C213-D204/2</f>
@@ -3391,7 +3583,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="214">
       <c r="B214" s="0" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="G214" s="3" t="n">
         <v>5</v>
@@ -3406,13 +3598,13 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="215">
       <c r="B215" s="0" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="C215" s="0" t="n">
         <v>180</v>
       </c>
       <c r="D215" s="0" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="E215" s="0" t="n">
         <f aca="false">C215-D204/2</f>
@@ -3443,7 +3635,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="217">
       <c r="B217" s="0" t="s">
-        <v>20</v>
+        <v>29</v>
       </c>
       <c r="C217" s="5" t="n">
         <v>400</v>
@@ -3488,13 +3680,13 @@
         <v>0</v>
       </c>
       <c r="J221" s="6" t="s">
-        <v>21</v>
+        <v>30</v>
       </c>
       <c r="K221" s="6" t="s">
-        <v>22</v>
+        <v>31</v>
       </c>
       <c r="L221" s="6" t="s">
-        <v>23</v>
+        <v>32</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="222">
@@ -3551,44 +3743,44 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="228">
       <c r="A228" s="2" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="B228" s="2" t="s">
-        <v>24</v>
+        <v>33</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="229">
       <c r="B229" s="0" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="G229" s="3" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="H229" s="3" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="J229" s="4" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="K229" s="4" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="M229" s="0" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="N229" s="0" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="230">
       <c r="B230" s="0" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="C230" s="0" t="n">
         <v>303.5</v>
       </c>
       <c r="D230" s="0" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="E230" s="0" t="n">
         <f aca="false">C230-C224/2</f>
@@ -3623,7 +3815,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="231">
       <c r="B231" s="0" t="s">
-        <v>26</v>
+        <v>34</v>
       </c>
       <c r="G231" s="3" t="n">
         <v>2</v>
@@ -3638,7 +3830,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="232">
       <c r="B232" s="0" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="G232" s="3" t="n">
         <v>3</v>
@@ -3653,13 +3845,13 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="233">
       <c r="B233" s="0" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="C233" s="0" t="n">
         <v>252.5</v>
       </c>
       <c r="D233" s="0" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="E233" s="0" t="n">
         <f aca="false">C233-D224/2</f>
@@ -3678,7 +3870,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="234">
       <c r="B234" s="0" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="G234" s="3" t="n">
         <v>5</v>
@@ -3693,13 +3885,13 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="235">
       <c r="B235" s="0" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="C235" s="0" t="n">
         <v>180</v>
       </c>
       <c r="D235" s="0" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="E235" s="0" t="n">
         <f aca="false">C235-D224/2</f>
@@ -3730,7 +3922,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="237">
       <c r="B237" s="0" t="s">
-        <v>20</v>
+        <v>29</v>
       </c>
       <c r="C237" s="5" t="n">
         <v>360</v>
@@ -3775,13 +3967,13 @@
         <v>0</v>
       </c>
       <c r="J241" s="6" t="s">
-        <v>21</v>
+        <v>30</v>
       </c>
       <c r="K241" s="6" t="s">
-        <v>22</v>
+        <v>31</v>
       </c>
       <c r="L241" s="6" t="s">
-        <v>23</v>
+        <v>32</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="242">
@@ -3801,11 +3993,11 @@
       </c>
       <c r="K242" s="0" t="n">
         <f aca="false">STDEV(K230:K239)</f>
-        <v>0.774596669241588</v>
+        <v>0.774596669241483</v>
       </c>
       <c r="L242" s="0" t="n">
         <f aca="false">K242/SQRT(COUNT(K230:K239))</f>
-        <v>0.244948974278351</v>
+        <v>0.244948974278318</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="243">
@@ -3838,7 +4030,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="248">
       <c r="A248" s="2" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B248" s="2" t="s">
         <v>7</v>
@@ -3846,36 +4038,36 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="249">
       <c r="B249" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="G249" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="H249" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="J249" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="K249" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="M249" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="N249" s="0" t="s">
         <v>17</v>
-      </c>
-      <c r="G249" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="H249" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="J249" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="K249" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="M249" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="N249" s="0" t="s">
-        <v>14</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="250">
       <c r="B250" s="0" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="C250" s="0" t="n">
         <v>290.5</v>
       </c>
       <c r="D250" s="0" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="E250" s="0" t="n">
         <f aca="false">C250-B244/2</f>
@@ -3906,7 +4098,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="251">
       <c r="B251" s="0" t="s">
-        <v>26</v>
+        <v>34</v>
       </c>
       <c r="G251" s="3" t="n">
         <v>2</v>
@@ -3921,7 +4113,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="252">
       <c r="B252" s="0" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="G252" s="3" t="n">
         <v>3</v>
@@ -3936,13 +4128,13 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="253">
       <c r="B253" s="0" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="C253" s="0" t="n">
         <v>252.5</v>
       </c>
       <c r="D253" s="0" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="E253" s="0" t="n">
         <f aca="false">C253-D244/2</f>
@@ -3961,7 +4153,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="254">
       <c r="B254" s="0" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="G254" s="3" t="n">
         <v>5</v>
@@ -3976,13 +4168,13 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="255">
       <c r="B255" s="0" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="C255" s="0" t="n">
         <v>180</v>
       </c>
       <c r="D255" s="0" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="E255" s="0" t="n">
         <f aca="false">C255-D244/2</f>
@@ -4013,7 +4205,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="257">
       <c r="B257" s="0" t="s">
-        <v>20</v>
+        <v>29</v>
       </c>
       <c r="C257" s="5" t="n">
         <v>430</v>
@@ -4058,13 +4250,13 @@
         <v>0</v>
       </c>
       <c r="J261" s="6" t="s">
-        <v>21</v>
+        <v>30</v>
       </c>
       <c r="K261" s="6" t="s">
-        <v>22</v>
+        <v>31</v>
       </c>
       <c r="L261" s="6" t="s">
-        <v>23</v>
+        <v>32</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="262">
@@ -4084,11 +4276,11 @@
       </c>
       <c r="K262" s="0" t="n">
         <f aca="false">STDEV(K250:K259)</f>
-        <v>1.00138792571966</v>
+        <v>1.00138792571999</v>
       </c>
       <c r="L262" s="0" t="n">
         <f aca="false">K262/SQRT(COUNT(K250:K259))</f>
-        <v>0.316666666666564</v>
+        <v>0.316666666666667</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="263">
@@ -4121,44 +4313,44 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="268">
       <c r="A268" s="2" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B268" s="2" t="s">
-        <v>24</v>
+        <v>33</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="269">
       <c r="B269" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="G269" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="H269" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="J269" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="K269" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="M269" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="N269" s="0" t="s">
         <v>17</v>
-      </c>
-      <c r="G269" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="H269" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="J269" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="K269" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="M269" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="N269" s="0" t="s">
-        <v>14</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="270">
       <c r="B270" s="0" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="C270" s="0" t="n">
         <v>290.5</v>
       </c>
       <c r="D270" s="0" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="E270" s="0" t="n">
         <f aca="false">C270-B264/2</f>
@@ -4188,12 +4380,12 @@
       </c>
       <c r="O270" s="0" t="n">
         <f aca="false">1-((1+M270)*J282^2/J270^2)</f>
-        <v>0.243258029786593</v>
+        <v>0.243258029786592</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="271">
       <c r="B271" s="0" t="s">
-        <v>26</v>
+        <v>34</v>
       </c>
       <c r="G271" s="3" t="n">
         <v>2</v>
@@ -4208,7 +4400,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="272">
       <c r="B272" s="0" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="G272" s="3" t="n">
         <v>3</v>
@@ -4223,13 +4415,13 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="273">
       <c r="B273" s="0" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="C273" s="0" t="n">
         <v>252.5</v>
       </c>
       <c r="D273" s="0" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="E273" s="0" t="n">
         <f aca="false">C273-D264/2</f>
@@ -4248,7 +4440,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="274">
       <c r="B274" s="0" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="G274" s="3" t="n">
         <v>5</v>
@@ -4263,13 +4455,13 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="275">
       <c r="B275" s="0" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="C275" s="0" t="n">
         <v>180</v>
       </c>
       <c r="D275" s="0" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="E275" s="0" t="n">
         <f aca="false">C275-D264/2</f>
@@ -4300,7 +4492,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="277">
       <c r="B277" s="0" t="s">
-        <v>20</v>
+        <v>29</v>
       </c>
       <c r="C277" s="5" t="n">
         <v>370</v>
@@ -4342,13 +4534,13 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="281">
       <c r="J281" s="6" t="s">
-        <v>21</v>
+        <v>30</v>
       </c>
       <c r="K281" s="6" t="s">
-        <v>22</v>
+        <v>31</v>
       </c>
       <c r="L281" s="6" t="s">
-        <v>23</v>
+        <v>32</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="282">
@@ -4358,11 +4550,11 @@
       </c>
       <c r="K282" s="0" t="n">
         <f aca="false">STDEV(K270:K279)</f>
-        <v>0.368932393686092</v>
+        <v>0.368932393686311</v>
       </c>
       <c r="L282" s="0" t="n">
         <f aca="false">K282/SQRT(COUNT(K270:K279))</f>
-        <v>0.116666666666597</v>
+        <v>0.116666666666667</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added error calc to excel
</commit_message>
<xml_diff>
--- a/exp3/data/values.xlsx
+++ b/exp3/data/values.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="398" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="401" uniqueCount="38">
   <si>
     <t>Balls</t>
   </si>
@@ -122,6 +122,15 @@
   <si>
     <t>P: 3, T: 1</t>
   </si>
+  <si>
+    <t>Q/T1 meas</t>
+  </si>
+  <si>
+    <t>Q/T1 Theor</t>
+  </si>
+  <si>
+    <t>Std.Err.Mean</t>
+  </si>
 </sst>
 </file>
 
@@ -143,7 +152,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -186,6 +195,12 @@
         <bgColor rgb="FF808080"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -200,7 +215,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -209,10 +224,11 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
-    <cellStyle name="TableStyleLight1" xfId="1" customBuiltin="1"/>
+    <cellStyle name="TableStyleLight1" xfId="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -324,6 +340,17 @@
           <c:tx>
             <c:v>T2'/T1 measured</c:v>
           </c:tx>
+          <c:errBars>
+            <c:errBarType val="both"/>
+            <c:errValType val="fixedVal"/>
+            <c:val val="3.7000000000000006E-3"/>
+            <c:spPr>
+              <a:ln w="22225">
+                <a:headEnd w="lg" len="lg"/>
+                <a:tailEnd w="lg" len="lg"/>
+              </a:ln>
+            </c:spPr>
+          </c:errBars>
           <c:cat>
             <c:strRef>
               <c:f>Tabelle1!$P$10:$P$16</c:f>
@@ -432,11 +459,11 @@
           </c:val>
         </c:ser>
         <c:overlap val="100"/>
-        <c:axId val="46274048"/>
-        <c:axId val="46953216"/>
+        <c:axId val="84310272"/>
+        <c:axId val="84332544"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="46274048"/>
+        <c:axId val="84310272"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -453,14 +480,14 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="46953216"/>
+        <c:crossAx val="84332544"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="46953216"/>
+        <c:axId val="84332544"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -468,7 +495,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="46274048"/>
+        <c:crossAx val="84310272"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -632,11 +659,11 @@
           </c:val>
         </c:ser>
         <c:overlap val="100"/>
-        <c:axId val="75582080"/>
-        <c:axId val="75592064"/>
+        <c:axId val="81085184"/>
+        <c:axId val="81086720"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="75582080"/>
+        <c:axId val="81085184"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -653,14 +680,14 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="75592064"/>
+        <c:crossAx val="81086720"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="75592064"/>
+        <c:axId val="81086720"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -668,7 +695,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="75582080"/>
+        <c:crossAx val="81085184"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -691,16 +718,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>830035</xdr:colOff>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>379639</xdr:colOff>
       <xdr:row>23</xdr:row>
-      <xdr:rowOff>95250</xdr:rowOff>
+      <xdr:rowOff>40821</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>27</xdr:col>
-      <xdr:colOff>230084</xdr:colOff>
+      <xdr:colOff>611084</xdr:colOff>
       <xdr:row>50</xdr:row>
-      <xdr:rowOff>95250</xdr:rowOff>
+      <xdr:rowOff>40821</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -721,14 +748,14 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>816428</xdr:colOff>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>266700</xdr:colOff>
       <xdr:row>51</xdr:row>
       <xdr:rowOff>163286</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>27</xdr:col>
-      <xdr:colOff>216477</xdr:colOff>
+      <xdr:colOff>488620</xdr:colOff>
       <xdr:row>78</xdr:row>
       <xdr:rowOff>163286</xdr:rowOff>
     </xdr:to>
@@ -1039,8 +1066,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A2:V282"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H14" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="AC52" sqref="AC52"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="M23" sqref="M23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -1050,8 +1077,9 @@
     <col min="7" max="7" width="18.28515625"/>
     <col min="8" max="10" width="10.5703125"/>
     <col min="11" max="12" width="11.42578125"/>
-    <col min="13" max="15" width="10.5703125"/>
-    <col min="16" max="16" width="13.5703125"/>
+    <col min="13" max="13" width="14.28515625" customWidth="1"/>
+    <col min="14" max="15" width="10.5703125"/>
+    <col min="16" max="16" width="12" customWidth="1"/>
     <col min="17" max="17" width="10.5703125"/>
     <col min="18" max="18" width="12.42578125" customWidth="1"/>
     <col min="19" max="19" width="10.5703125"/>
@@ -1091,6 +1119,9 @@
       <c r="D4" s="1">
         <v>1049</v>
       </c>
+      <c r="M4">
+        <v>1E-3</v>
+      </c>
     </row>
     <row r="5" spans="1:22" ht="15" customHeight="1">
       <c r="A5" s="1" t="s">
@@ -1382,6 +1413,9 @@
         <f t="shared" si="0"/>
         <v>95</v>
       </c>
+      <c r="M15" t="s">
+        <v>37</v>
+      </c>
       <c r="P15" t="str">
         <f>$A$88</f>
         <v>P: 2, T: 1</v>
@@ -1431,6 +1465,10 @@
         <f t="shared" si="0"/>
         <v>93</v>
       </c>
+      <c r="M16" s="8">
+        <f>SQRT(4*(M11)^2*((J23*0.001)^4/(J11*0.001)^6*$M$4^2+ (J23*0.001)^2/(J11*0.001)^4*(L23*0.001)^2))</f>
+        <v>1.0748368358313718E-2</v>
+      </c>
       <c r="P16" t="str">
         <f>$A$248</f>
         <v>P: 3, T: 1</v>
@@ -1456,7 +1494,7 @@
         <v>0.1375357870980686</v>
       </c>
     </row>
-    <row r="17" spans="1:15" ht="15" customHeight="1">
+    <row r="17" spans="1:16" ht="15" customHeight="1">
       <c r="G17" s="3">
         <v>7</v>
       </c>
@@ -1468,7 +1506,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="18" spans="1:15" ht="15" customHeight="1">
+    <row r="18" spans="1:16" ht="15" customHeight="1">
       <c r="B18" t="s">
         <v>22</v>
       </c>
@@ -1486,7 +1524,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="19" spans="1:15" ht="15" customHeight="1">
+    <row r="19" spans="1:16" ht="15" customHeight="1">
       <c r="G19" s="3">
         <v>9</v>
       </c>
@@ -1498,7 +1536,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="20" spans="1:15" ht="15" customHeight="1">
+    <row r="20" spans="1:16" ht="15" customHeight="1">
       <c r="G20" s="3">
         <v>10</v>
       </c>
@@ -1510,12 +1548,12 @@
         <v>93</v>
       </c>
     </row>
-    <row r="21" spans="1:15" ht="15" customHeight="1">
+    <row r="21" spans="1:16" ht="15" customHeight="1">
       <c r="B21" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:15" ht="15" customHeight="1">
+    <row r="22" spans="1:16" ht="15" customHeight="1">
       <c r="A22" s="1"/>
       <c r="B22" s="1" t="s">
         <v>1</v>
@@ -1536,7 +1574,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="23" spans="1:15" ht="15" customHeight="1">
+    <row r="23" spans="1:16" ht="15" customHeight="1">
       <c r="A23" s="1" t="s">
         <v>4</v>
       </c>
@@ -1562,7 +1600,7 @@
         <v>0.22110831935688041</v>
       </c>
     </row>
-    <row r="24" spans="1:15" ht="15" customHeight="1">
+    <row r="24" spans="1:16" ht="15" customHeight="1">
       <c r="A24" s="1" t="s">
         <v>5</v>
       </c>
@@ -1576,7 +1614,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="28" spans="1:15" ht="15" customHeight="1">
+    <row r="28" spans="1:16" ht="15" customHeight="1">
       <c r="A28" s="7" t="s">
         <v>28</v>
       </c>
@@ -1584,7 +1622,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="29" spans="1:15" ht="15" customHeight="1">
+    <row r="29" spans="1:16" ht="15" customHeight="1">
       <c r="B29" t="s">
         <v>10</v>
       </c>
@@ -1606,8 +1644,14 @@
       <c r="N29" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="30" spans="1:15" ht="15" customHeight="1">
+      <c r="O29" t="s">
+        <v>35</v>
+      </c>
+      <c r="P29" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="30" spans="1:16" ht="15" customHeight="1">
       <c r="B30" t="s">
         <v>17</v>
       </c>
@@ -1647,8 +1691,12 @@
         <f>1-((1+M30)*J42^2/J30^2)</f>
         <v>0.72832347249533269</v>
       </c>
-    </row>
-    <row r="31" spans="1:15" ht="15" customHeight="1">
+      <c r="P30">
+        <f>M30/(1+M30)</f>
+        <v>0.6985769728331177</v>
+      </c>
+    </row>
+    <row r="31" spans="1:16" ht="15" customHeight="1">
       <c r="B31" t="s">
         <v>19</v>
       </c>
@@ -1663,7 +1711,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="32" spans="1:15" ht="15" customHeight="1">
+    <row r="32" spans="1:16" ht="15" customHeight="1">
       <c r="B32" t="s">
         <v>20</v>
       </c>
@@ -2148,7 +2196,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="68" spans="1:15" ht="15" customHeight="1">
+    <row r="68" spans="1:16" ht="15" customHeight="1">
       <c r="A68" s="7" t="s">
         <v>29</v>
       </c>
@@ -2156,7 +2204,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="69" spans="1:15" ht="15" customHeight="1">
+    <row r="69" spans="1:16" ht="15" customHeight="1">
       <c r="B69" t="s">
         <v>27</v>
       </c>
@@ -2179,7 +2227,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="70" spans="1:15" ht="15" customHeight="1">
+    <row r="70" spans="1:16" ht="15" customHeight="1">
       <c r="B70" t="s">
         <v>17</v>
       </c>
@@ -2219,8 +2267,12 @@
         <f>1-((1+M70)*J82^2/J70^2)</f>
         <v>0.84287675024567565</v>
       </c>
-    </row>
-    <row r="71" spans="1:15" ht="15" customHeight="1">
+      <c r="P70">
+        <f>M70/(1+M70)</f>
+        <v>0.81825273010920441</v>
+      </c>
+    </row>
+    <row r="71" spans="1:16" ht="15" customHeight="1">
       <c r="B71" t="s">
         <v>19</v>
       </c>
@@ -2235,7 +2287,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="72" spans="1:15" ht="15" customHeight="1">
+    <row r="72" spans="1:16" ht="15" customHeight="1">
       <c r="B72" t="s">
         <v>20</v>
       </c>
@@ -2250,7 +2302,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="73" spans="1:15" ht="15" customHeight="1">
+    <row r="73" spans="1:16" ht="15" customHeight="1">
       <c r="B73" t="s">
         <v>17</v>
       </c>
@@ -2276,7 +2328,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="74" spans="1:15" ht="15" customHeight="1">
+    <row r="74" spans="1:16" ht="15" customHeight="1">
       <c r="B74" t="s">
         <v>21</v>
       </c>
@@ -2291,7 +2343,7 @@
         <v>26.5</v>
       </c>
     </row>
-    <row r="75" spans="1:15" ht="15" customHeight="1">
+    <row r="75" spans="1:16" ht="15" customHeight="1">
       <c r="B75" t="s">
         <v>17</v>
       </c>
@@ -2316,7 +2368,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="76" spans="1:15" ht="15" customHeight="1">
+    <row r="76" spans="1:16" ht="15" customHeight="1">
       <c r="G76" s="3">
         <v>7</v>
       </c>
@@ -2328,7 +2380,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="77" spans="1:15" ht="15" customHeight="1">
+    <row r="77" spans="1:16" ht="15" customHeight="1">
       <c r="B77" t="s">
         <v>22</v>
       </c>
@@ -2346,7 +2398,7 @@
         <v>26.5</v>
       </c>
     </row>
-    <row r="78" spans="1:15" ht="15" customHeight="1">
+    <row r="78" spans="1:16" ht="15" customHeight="1">
       <c r="G78" s="3">
         <v>9</v>
       </c>
@@ -2358,7 +2410,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="79" spans="1:15" ht="15" customHeight="1">
+    <row r="79" spans="1:16" ht="15" customHeight="1">
       <c r="G79" s="3">
         <v>10</v>
       </c>
@@ -2612,7 +2664,7 @@
         <v>114.5</v>
       </c>
     </row>
-    <row r="97" spans="1:15" ht="15" customHeight="1">
+    <row r="97" spans="1:16" ht="15" customHeight="1">
       <c r="B97" t="s">
         <v>22</v>
       </c>
@@ -2630,7 +2682,7 @@
         <v>114.5</v>
       </c>
     </row>
-    <row r="98" spans="1:15" ht="15" customHeight="1">
+    <row r="98" spans="1:16" ht="15" customHeight="1">
       <c r="G98" s="3">
         <v>9</v>
       </c>
@@ -2642,7 +2694,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="99" spans="1:15" ht="15" customHeight="1">
+    <row r="99" spans="1:16" ht="15" customHeight="1">
       <c r="G99" s="3">
         <v>10</v>
       </c>
@@ -2654,7 +2706,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="101" spans="1:15" ht="15" customHeight="1">
+    <row r="101" spans="1:16" ht="15" customHeight="1">
       <c r="B101" t="s">
         <v>0</v>
       </c>
@@ -2668,7 +2720,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="102" spans="1:15" ht="15" customHeight="1">
+    <row r="102" spans="1:16" ht="15" customHeight="1">
       <c r="A102" s="1"/>
       <c r="B102" s="1" t="s">
         <v>1</v>
@@ -2692,7 +2744,7 @@
         <v>0.13844373104886815</v>
       </c>
     </row>
-    <row r="103" spans="1:15" ht="15" customHeight="1">
+    <row r="103" spans="1:16" ht="15" customHeight="1">
       <c r="A103" s="1" t="s">
         <v>4</v>
       </c>
@@ -2706,7 +2758,7 @@
         <v>1049</v>
       </c>
     </row>
-    <row r="104" spans="1:15" ht="15" customHeight="1">
+    <row r="104" spans="1:16" ht="15" customHeight="1">
       <c r="A104" s="1" t="s">
         <v>5</v>
       </c>
@@ -2720,7 +2772,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="108" spans="1:15" ht="15" customHeight="1">
+    <row r="108" spans="1:16" ht="15" customHeight="1">
       <c r="A108" s="7" t="s">
         <v>30</v>
       </c>
@@ -2728,7 +2780,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="109" spans="1:15" ht="15" customHeight="1">
+    <row r="109" spans="1:16" ht="15" customHeight="1">
       <c r="B109" t="s">
         <v>19</v>
       </c>
@@ -2751,7 +2803,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="110" spans="1:15" ht="15" customHeight="1">
+    <row r="110" spans="1:16" ht="15" customHeight="1">
       <c r="B110" t="s">
         <v>17</v>
       </c>
@@ -2791,8 +2843,12 @@
         <f>1-((1+M110)*J122^2/J110^2)</f>
         <v>0.36341606261142156</v>
       </c>
-    </row>
-    <row r="111" spans="1:15" ht="15" customHeight="1">
+      <c r="P110">
+        <f>M110/(1+M110)</f>
+        <v>0.30142302716688224</v>
+      </c>
+    </row>
+    <row r="111" spans="1:16" ht="15" customHeight="1">
       <c r="B111" t="s">
         <v>10</v>
       </c>
@@ -2807,7 +2863,7 @@
         <v>56.5</v>
       </c>
     </row>
-    <row r="112" spans="1:15" ht="15" customHeight="1">
+    <row r="112" spans="1:16" ht="15" customHeight="1">
       <c r="B112" t="s">
         <v>20</v>
       </c>
@@ -3292,7 +3348,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="148" spans="1:15" ht="15" customHeight="1">
+    <row r="148" spans="1:16" ht="15" customHeight="1">
       <c r="A148" s="7" t="s">
         <v>31</v>
       </c>
@@ -3300,7 +3356,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="149" spans="1:15" ht="15" customHeight="1">
+    <row r="149" spans="1:16" ht="15" customHeight="1">
       <c r="B149" t="s">
         <v>10</v>
       </c>
@@ -3323,7 +3379,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="150" spans="1:15" ht="15" customHeight="1">
+    <row r="150" spans="1:16" ht="15" customHeight="1">
       <c r="B150" t="s">
         <v>17</v>
       </c>
@@ -3363,8 +3419,12 @@
         <f>1-((1+M150)*J162^2/J150^2)</f>
         <v>0.54624653739612183</v>
       </c>
-    </row>
-    <row r="151" spans="1:15" ht="15" customHeight="1">
+      <c r="P150">
+        <f>M150/(1+M150)</f>
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="151" spans="1:16" ht="15" customHeight="1">
       <c r="B151" t="s">
         <v>10</v>
       </c>
@@ -3379,7 +3439,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="152" spans="1:15" ht="15" customHeight="1">
+    <row r="152" spans="1:16" ht="15" customHeight="1">
       <c r="B152" t="s">
         <v>20</v>
       </c>
@@ -3394,7 +3454,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="153" spans="1:15" ht="15" customHeight="1">
+    <row r="153" spans="1:16" ht="15" customHeight="1">
       <c r="B153" t="s">
         <v>17</v>
       </c>
@@ -3420,7 +3480,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="154" spans="1:15" ht="15" customHeight="1">
+    <row r="154" spans="1:16" ht="15" customHeight="1">
       <c r="B154" t="s">
         <v>21</v>
       </c>
@@ -3435,7 +3495,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="155" spans="1:15" ht="15" customHeight="1">
+    <row r="155" spans="1:16" ht="15" customHeight="1">
       <c r="B155" t="s">
         <v>17</v>
       </c>
@@ -3460,7 +3520,7 @@
         <v>47.5</v>
       </c>
     </row>
-    <row r="156" spans="1:15" ht="15" customHeight="1">
+    <row r="156" spans="1:16" ht="15" customHeight="1">
       <c r="G156" s="3">
         <v>7</v>
       </c>
@@ -3472,7 +3532,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="157" spans="1:15" ht="15" customHeight="1">
+    <row r="157" spans="1:16" ht="15" customHeight="1">
       <c r="B157" t="s">
         <v>22</v>
       </c>
@@ -3490,7 +3550,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="158" spans="1:15" ht="15" customHeight="1">
+    <row r="158" spans="1:16" ht="15" customHeight="1">
       <c r="G158" s="3">
         <v>9</v>
       </c>
@@ -3502,7 +3562,7 @@
         <v>44.5</v>
       </c>
     </row>
-    <row r="159" spans="1:15" ht="15" customHeight="1">
+    <row r="159" spans="1:16" ht="15" customHeight="1">
       <c r="G159" s="3">
         <v>10</v>
       </c>
@@ -3755,7 +3815,7 @@
         <v>96.5</v>
       </c>
     </row>
-    <row r="177" spans="1:15" ht="15" customHeight="1">
+    <row r="177" spans="1:16" ht="15" customHeight="1">
       <c r="B177" t="s">
         <v>22</v>
       </c>
@@ -3773,7 +3833,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="178" spans="1:15" ht="15" customHeight="1">
+    <row r="178" spans="1:16" ht="15" customHeight="1">
       <c r="G178" s="3">
         <v>9</v>
       </c>
@@ -3785,7 +3845,7 @@
         <v>95.5</v>
       </c>
     </row>
-    <row r="179" spans="1:15" ht="15" customHeight="1">
+    <row r="179" spans="1:16" ht="15" customHeight="1">
       <c r="G179" s="3">
         <v>10</v>
       </c>
@@ -3797,7 +3857,7 @@
         <v>96.5</v>
       </c>
     </row>
-    <row r="181" spans="1:15" ht="15" customHeight="1">
+    <row r="181" spans="1:16" ht="15" customHeight="1">
       <c r="B181" t="s">
         <v>0</v>
       </c>
@@ -3811,7 +3871,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="182" spans="1:15" ht="15" customHeight="1">
+    <row r="182" spans="1:16" ht="15" customHeight="1">
       <c r="A182" s="1"/>
       <c r="B182" s="1" t="s">
         <v>1</v>
@@ -3835,7 +3895,7 @@
         <v>0.2472066162365221</v>
       </c>
     </row>
-    <row r="183" spans="1:15" ht="15" customHeight="1">
+    <row r="183" spans="1:16" ht="15" customHeight="1">
       <c r="A183" s="1" t="s">
         <v>4</v>
       </c>
@@ -3849,7 +3909,7 @@
         <v>1049</v>
       </c>
     </row>
-    <row r="184" spans="1:15" ht="15" customHeight="1">
+    <row r="184" spans="1:16" ht="15" customHeight="1">
       <c r="A184" s="1" t="s">
         <v>5</v>
       </c>
@@ -3863,7 +3923,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="188" spans="1:15" ht="15" customHeight="1">
+    <row r="188" spans="1:16" ht="15" customHeight="1">
       <c r="A188" s="7" t="s">
         <v>32</v>
       </c>
@@ -3871,7 +3931,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="189" spans="1:15" ht="15" customHeight="1">
+    <row r="189" spans="1:16" ht="15" customHeight="1">
       <c r="B189" t="s">
         <v>27</v>
       </c>
@@ -3894,7 +3954,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="190" spans="1:15" ht="15" customHeight="1">
+    <row r="190" spans="1:16" ht="15" customHeight="1">
       <c r="B190" t="s">
         <v>17</v>
       </c>
@@ -3934,8 +3994,12 @@
         <f>1-((1+M190)*J202^2/J190^2)</f>
         <v>0.70215119467727249</v>
       </c>
-    </row>
-    <row r="191" spans="1:15" ht="15" customHeight="1">
+      <c r="P190">
+        <f>M190/(1+M190)</f>
+        <v>0.66016362492133418</v>
+      </c>
+    </row>
+    <row r="191" spans="1:16" ht="15" customHeight="1">
       <c r="B191" t="s">
         <v>10</v>
       </c>
@@ -3950,7 +4014,7 @@
         <v>45.5</v>
       </c>
     </row>
-    <row r="192" spans="1:15" ht="15" customHeight="1">
+    <row r="192" spans="1:16" ht="15" customHeight="1">
       <c r="B192" t="s">
         <v>20</v>
       </c>
@@ -4433,7 +4497,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="228" spans="1:15" ht="15" customHeight="1">
+    <row r="228" spans="1:16" ht="15" customHeight="1">
       <c r="A228" s="7" t="s">
         <v>33</v>
       </c>
@@ -4441,7 +4505,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="229" spans="1:15" ht="15" customHeight="1">
+    <row r="229" spans="1:16" ht="15" customHeight="1">
       <c r="B229" t="s">
         <v>10</v>
       </c>
@@ -4464,7 +4528,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="230" spans="1:15" ht="15" customHeight="1">
+    <row r="230" spans="1:16" ht="15" customHeight="1">
       <c r="B230" t="s">
         <v>17</v>
       </c>
@@ -4504,8 +4568,12 @@
         <f>1-((1+M230)*J242^2/J230^2)</f>
         <v>0.45217055096921466</v>
       </c>
-    </row>
-    <row r="231" spans="1:15" ht="15" customHeight="1">
+      <c r="P230">
+        <f>M230/(1+M230)</f>
+        <v>0.33983637507866582</v>
+      </c>
+    </row>
+    <row r="231" spans="1:16" ht="15" customHeight="1">
       <c r="B231" t="s">
         <v>27</v>
       </c>
@@ -4520,7 +4588,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="232" spans="1:15" ht="15" customHeight="1">
+    <row r="232" spans="1:16" ht="15" customHeight="1">
       <c r="B232" t="s">
         <v>20</v>
       </c>
@@ -4535,7 +4603,7 @@
         <v>43.5</v>
       </c>
     </row>
-    <row r="233" spans="1:15" ht="15" customHeight="1">
+    <row r="233" spans="1:16" ht="15" customHeight="1">
       <c r="B233" t="s">
         <v>17</v>
       </c>
@@ -4560,7 +4628,7 @@
         <v>43.5</v>
       </c>
     </row>
-    <row r="234" spans="1:15" ht="15" customHeight="1">
+    <row r="234" spans="1:16" ht="15" customHeight="1">
       <c r="B234" t="s">
         <v>21</v>
       </c>
@@ -4575,7 +4643,7 @@
         <v>43.5</v>
       </c>
     </row>
-    <row r="235" spans="1:15" ht="15" customHeight="1">
+    <row r="235" spans="1:16" ht="15" customHeight="1">
       <c r="B235" t="s">
         <v>17</v>
       </c>
@@ -4600,7 +4668,7 @@
         <v>43.5</v>
       </c>
     </row>
-    <row r="236" spans="1:15" ht="15" customHeight="1">
+    <row r="236" spans="1:16" ht="15" customHeight="1">
       <c r="G236" s="3">
         <v>7</v>
       </c>
@@ -4612,7 +4680,7 @@
         <v>42.5</v>
       </c>
     </row>
-    <row r="237" spans="1:15" ht="15" customHeight="1">
+    <row r="237" spans="1:16" ht="15" customHeight="1">
       <c r="B237" t="s">
         <v>22</v>
       </c>
@@ -4630,7 +4698,7 @@
         <v>43.5</v>
       </c>
     </row>
-    <row r="238" spans="1:15" ht="15" customHeight="1">
+    <row r="238" spans="1:16" ht="15" customHeight="1">
       <c r="G238" s="3">
         <v>9</v>
       </c>
@@ -4642,7 +4710,7 @@
         <v>42.5</v>
       </c>
     </row>
-    <row r="239" spans="1:15" ht="15" customHeight="1">
+    <row r="239" spans="1:16" ht="15" customHeight="1">
       <c r="G239" s="3">
         <v>10</v>
       </c>
@@ -4895,7 +4963,7 @@
         <v>110.5</v>
       </c>
     </row>
-    <row r="257" spans="1:15" ht="15" customHeight="1">
+    <row r="257" spans="1:16" ht="15" customHeight="1">
       <c r="B257" t="s">
         <v>22</v>
       </c>
@@ -4913,7 +4981,7 @@
         <v>107.5</v>
       </c>
     </row>
-    <row r="258" spans="1:15" ht="15" customHeight="1">
+    <row r="258" spans="1:16" ht="15" customHeight="1">
       <c r="G258" s="3">
         <v>9</v>
       </c>
@@ -4925,7 +4993,7 @@
         <v>109.5</v>
       </c>
     </row>
-    <row r="259" spans="1:15" ht="15" customHeight="1">
+    <row r="259" spans="1:16" ht="15" customHeight="1">
       <c r="G259" s="3">
         <v>10</v>
       </c>
@@ -4937,7 +5005,7 @@
         <v>108.5</v>
       </c>
     </row>
-    <row r="261" spans="1:15" ht="15" customHeight="1">
+    <row r="261" spans="1:16" ht="15" customHeight="1">
       <c r="B261" t="s">
         <v>0</v>
       </c>
@@ -4951,7 +5019,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="262" spans="1:15" ht="15" customHeight="1">
+    <row r="262" spans="1:16" ht="15" customHeight="1">
       <c r="A262" s="1"/>
       <c r="B262" s="1" t="s">
         <v>1</v>
@@ -4975,7 +5043,7 @@
         <v>0.31666666666656451</v>
       </c>
     </row>
-    <row r="263" spans="1:15" ht="15" customHeight="1">
+    <row r="263" spans="1:16" ht="15" customHeight="1">
       <c r="A263" s="1" t="s">
         <v>4</v>
       </c>
@@ -4989,7 +5057,7 @@
         <v>1049</v>
       </c>
     </row>
-    <row r="264" spans="1:15" ht="15" customHeight="1">
+    <row r="264" spans="1:16" ht="15" customHeight="1">
       <c r="A264" s="1" t="s">
         <v>5</v>
       </c>
@@ -5003,7 +5071,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="268" spans="1:15" ht="15" customHeight="1">
+    <row r="268" spans="1:16" ht="15" customHeight="1">
       <c r="A268" s="7" t="s">
         <v>34</v>
       </c>
@@ -5011,7 +5079,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="269" spans="1:15" ht="15" customHeight="1">
+    <row r="269" spans="1:16" ht="15" customHeight="1">
       <c r="B269" t="s">
         <v>19</v>
       </c>
@@ -5034,7 +5102,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="270" spans="1:15" ht="15" customHeight="1">
+    <row r="270" spans="1:16" ht="15" customHeight="1">
       <c r="B270" t="s">
         <v>17</v>
       </c>
@@ -5074,8 +5142,12 @@
         <f>1-((1+M270)*J282^2/J270^2)</f>
         <v>0.2432580297865925</v>
       </c>
-    </row>
-    <row r="271" spans="1:15" ht="15" customHeight="1">
+      <c r="P270">
+        <f>M270/(1+M270)</f>
+        <v>0.18174726989079565</v>
+      </c>
+    </row>
+    <row r="271" spans="1:16" ht="15" customHeight="1">
       <c r="B271" t="s">
         <v>27</v>
       </c>
@@ -5090,7 +5162,7 @@
         <v>57.5</v>
       </c>
     </row>
-    <row r="272" spans="1:15" ht="15" customHeight="1">
+    <row r="272" spans="1:16" ht="15" customHeight="1">
       <c r="B272" t="s">
         <v>20</v>
       </c>

</xml_diff>

<commit_message>
Inserted values of elastic measurements
	modified:   exp3/data/values.xlsx
	modified:   exp3/report/report3.tex
</commit_message>
<xml_diff>
--- a/exp3/data/values.xlsx
+++ b/exp3/data/values.xlsx
@@ -139,8 +139,8 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="3">
     <numFmt formatCode="GENERAL" numFmtId="164"/>
-    <numFmt formatCode="0.000" numFmtId="165"/>
-    <numFmt formatCode="GENERAL" numFmtId="166"/>
+    <numFmt formatCode="0.###" numFmtId="165"/>
+    <numFmt formatCode="0.######" numFmtId="166"/>
   </numFmts>
   <fonts count="7">
     <font>
@@ -180,9 +180,8 @@
       <sz val="18"/>
     </font>
     <font>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
-      <color rgb="FF000000"/>
       <sz val="10"/>
     </font>
   </fonts>
@@ -274,12 +273,16 @@
       <protection hidden="false" locked="true"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0">
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
       <protection hidden="false" locked="true"/>
     </xf>
     <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="165" xfId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="166" xfId="0">
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
       <protection hidden="false" locked="true"/>
     </xf>
@@ -299,11 +302,11 @@
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
       <protection hidden="false" locked="true"/>
     </xf>
-    <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="166" xfId="0">
+    <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0">
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
       <protection hidden="false" locked="true"/>
     </xf>
-    <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="7" fontId="0" numFmtId="165" xfId="0">
+    <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="7" fontId="0" numFmtId="166" xfId="0">
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
       <protection hidden="false" locked="true"/>
     </xf>
@@ -323,7 +326,7 @@
     <cellStyle builtinId="4" customBuiltin="false" name="Currency" xfId="17"/>
     <cellStyle builtinId="7" customBuiltin="false" name="Currency [0]" xfId="18"/>
     <cellStyle builtinId="5" customBuiltin="false" name="Percent" xfId="19"/>
-    <cellStyle builtinId="54" customBuiltin="true" name="TableStyleLight1" xfId="20"/>
+    <cellStyle builtinId="54" customBuiltin="true" name="Excel Built-in TableStyleLight1" xfId="20"/>
   </cellStyles>
   <colors>
     <indexedColors>
@@ -583,11 +586,11 @@
         </c:ser>
         <c:overlap val="100"/>
         <c:gapWidth val="150"/>
-        <c:axId val="61577974"/>
-        <c:axId val="99528433"/>
+        <c:axId val="18310463"/>
+        <c:axId val="59290708"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="61577974"/>
+        <c:axId val="18310463"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -595,7 +598,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="low"/>
-        <c:crossAx val="99528433"/>
+        <c:crossAx val="59290708"/>
         <c:crossesAt val="0"/>
         <c:lblAlgn val="ctr"/>
         <c:auto val="1"/>
@@ -610,7 +613,7 @@
         </c:spPr>
       </c:catAx>
       <c:valAx>
-        <c:axId val="99528433"/>
+        <c:axId val="59290708"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -628,7 +631,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="61577974"/>
+        <c:crossAx val="18310463"/>
         <c:crossesAt val="0"/>
         <c:spPr>
           <a:ln w="9360">
@@ -850,11 +853,11 @@
         </c:ser>
         <c:overlap val="100"/>
         <c:gapWidth val="150"/>
-        <c:axId val="61937131"/>
-        <c:axId val="22496495"/>
+        <c:axId val="45333967"/>
+        <c:axId val="8071999"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="61937131"/>
+        <c:axId val="45333967"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -862,7 +865,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="low"/>
-        <c:crossAx val="22496495"/>
+        <c:crossAx val="8071999"/>
         <c:crossesAt val="0"/>
         <c:lblAlgn val="ctr"/>
         <c:auto val="1"/>
@@ -877,7 +880,7 @@
         </c:spPr>
       </c:catAx>
       <c:valAx>
-        <c:axId val="22496495"/>
+        <c:axId val="8071999"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -895,7 +898,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="61937131"/>
+        <c:crossAx val="45333967"/>
         <c:crossesAt val="0"/>
         <c:spPr>
           <a:ln w="9360">
@@ -927,15 +930,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>16</xdr:col>
-      <xdr:colOff>406800</xdr:colOff>
+      <xdr:colOff>433800</xdr:colOff>
       <xdr:row>23</xdr:row>
-      <xdr:rowOff>32040</xdr:rowOff>
+      <xdr:rowOff>23040</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>27</xdr:col>
-      <xdr:colOff>637920</xdr:colOff>
+      <xdr:colOff>664560</xdr:colOff>
       <xdr:row>50</xdr:row>
-      <xdr:rowOff>31320</xdr:rowOff>
+      <xdr:rowOff>21960</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -943,8 +946,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="16966800" y="4413240"/>
-        <a:ext cx="11242080" cy="5142960"/>
+        <a:off x="16993800" y="4404240"/>
+        <a:ext cx="11241720" cy="5142600"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -957,15 +960,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>16</xdr:col>
-      <xdr:colOff>293760</xdr:colOff>
+      <xdr:colOff>320760</xdr:colOff>
       <xdr:row>51</xdr:row>
-      <xdr:rowOff>154800</xdr:rowOff>
+      <xdr:rowOff>145800</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>27</xdr:col>
-      <xdr:colOff>515160</xdr:colOff>
+      <xdr:colOff>541800</xdr:colOff>
       <xdr:row>78</xdr:row>
-      <xdr:rowOff>154080</xdr:rowOff>
+      <xdr:rowOff>144720</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -973,8 +976,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="16853760" y="9870120"/>
-        <a:ext cx="11232360" cy="5142960"/>
+        <a:off x="16880760" y="9861120"/>
+        <a:ext cx="11232000" cy="5142240"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -994,8 +997,8 @@
   </sheetPr>
   <dimension ref="A2:V282"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A130" view="normal" windowProtection="false" workbookViewId="0" zoomScale="55" zoomScaleNormal="55" zoomScalePageLayoutView="100">
-      <selection activeCell="O21" activeCellId="0" pane="topLeft" sqref="O21"/>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="B4" view="normal" windowProtection="false" workbookViewId="0" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100">
+      <selection activeCell="K250" activeCellId="0" pane="topLeft" sqref="K250"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1006,7 +1009,7 @@
     <col collapsed="false" hidden="false" max="9" min="8" style="0" width="10.5708502024292"/>
     <col collapsed="false" hidden="false" max="10" min="10" style="1" width="10.5708502024292"/>
     <col collapsed="false" hidden="false" max="12" min="11" style="1" width="11.4251012145749"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="1" width="14.2834008097166"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="2" width="14.2834008097166"/>
     <col collapsed="false" hidden="false" max="15" min="14" style="1" width="10.5708502024292"/>
     <col collapsed="false" hidden="false" max="16" min="16" style="0" width="11.9959514170041"/>
     <col collapsed="false" hidden="false" max="17" min="17" style="0" width="10.5708502024292"/>
@@ -1024,71 +1027,81 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="3">
-      <c r="A3" s="2"/>
-      <c r="B3" s="2" t="s">
+      <c r="A3" s="3"/>
+      <c r="B3" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="D3" s="3" t="s">
         <v>3</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="4">
-      <c r="A4" s="2" t="s">
+      <c r="A4" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="2" t="n">
+      <c r="B4" s="3" t="n">
         <v>233</v>
       </c>
-      <c r="C4" s="2" t="n">
+      <c r="C4" s="3" t="n">
         <v>540</v>
       </c>
-      <c r="D4" s="2" t="n">
+      <c r="D4" s="3" t="n">
         <v>1049</v>
       </c>
-      <c r="M4" s="1" t="n">
+      <c r="M4" s="2" t="n">
         <v>0.002</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="5">
-      <c r="A5" s="2" t="s">
+      <c r="A5" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="2" t="n">
+      <c r="B5" s="3" t="n">
         <v>38</v>
       </c>
-      <c r="C5" s="2" t="n">
+      <c r="C5" s="3" t="n">
         <v>52</v>
       </c>
-      <c r="D5" s="2" t="n">
+      <c r="D5" s="3" t="n">
         <v>65</v>
       </c>
     </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="8">
+      <c r="P8" s="1"/>
+      <c r="Q8" s="1"/>
+      <c r="R8" s="1"/>
+      <c r="S8" s="1"/>
+      <c r="T8" s="1"/>
+      <c r="U8" s="1"/>
+      <c r="V8" s="1"/>
+    </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="9">
-      <c r="A9" s="3" t="s">
+      <c r="A9" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B9" s="3" t="s">
+      <c r="B9" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="P9" s="0" t="s">
+      <c r="P9" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="Q9" s="0" t="s">
+      <c r="Q9" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="R9" s="0" t="s">
+      <c r="R9" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="T9" s="0" t="s">
+      <c r="S9" s="1"/>
+      <c r="T9" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="U9" s="0" t="s">
+      <c r="U9" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="V9" s="0" t="s">
+      <c r="V9" s="1" t="s">
         <v>9</v>
       </c>
     </row>
@@ -1096,45 +1109,46 @@
       <c r="B10" s="0" t="s">
         <v>11</v>
       </c>
-      <c r="G10" s="4" t="s">
+      <c r="G10" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="H10" s="4" t="s">
+      <c r="H10" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="J10" s="5" t="s">
+      <c r="J10" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="K10" s="5" t="s">
+      <c r="K10" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="M10" s="1" t="s">
+      <c r="M10" s="2" t="s">
         <v>16</v>
       </c>
       <c r="N10" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="P10" s="0" t="str">
+      <c r="P10" s="1" t="str">
         <f aca="false">$A$48</f>
         <v>P: 1, T: 3</v>
       </c>
-      <c r="Q10" s="6" t="n">
+      <c r="Q10" s="2" t="n">
         <f aca="false">M50*4/(M50+1)^2</f>
         <v>0.594860799112152</v>
       </c>
-      <c r="R10" s="6" t="n">
+      <c r="R10" s="1" t="n">
         <f aca="false">N50</f>
         <v>0.555509332580547</v>
       </c>
-      <c r="T10" s="0" t="str">
+      <c r="S10" s="1"/>
+      <c r="T10" s="1" t="str">
         <f aca="false">$A$48</f>
         <v>P: 1, T: 3</v>
       </c>
-      <c r="U10" s="6" t="n">
+      <c r="U10" s="1" t="n">
         <f aca="false">M70/(M70+1)^2</f>
         <v>0.148715199778038</v>
       </c>
-      <c r="V10" s="6" t="n">
+      <c r="V10" s="1" t="n">
         <f aca="false">N70</f>
         <v>0.128566528075106</v>
       </c>
@@ -1149,14 +1163,14 @@
       <c r="D11" s="0" t="s">
         <v>19</v>
       </c>
-      <c r="E11" s="6" t="n">
+      <c r="E11" s="7" t="n">
         <f aca="false">C11-C5/2</f>
         <v>265</v>
       </c>
-      <c r="G11" s="4" t="n">
+      <c r="G11" s="5" t="n">
         <v>1</v>
       </c>
-      <c r="H11" s="4" t="n">
+      <c r="H11" s="5" t="n">
         <v>34</v>
       </c>
       <c r="J11" s="1" t="n">
@@ -1167,7 +1181,7 @@
         <f aca="false">$C$18+H11-$C$5/2-$E$11-50</f>
         <v>93</v>
       </c>
-      <c r="M11" s="1" t="n">
+      <c r="M11" s="2" t="n">
         <f aca="false">C4*0.001/(B4*0.001)</f>
         <v>2.31759656652361</v>
       </c>
@@ -1175,27 +1189,28 @@
         <f aca="false">$M$11*$J$23^2/$J$11^2</f>
         <v>0.799718868077318</v>
       </c>
-      <c r="P11" s="0" t="str">
+      <c r="P11" s="1" t="str">
         <f aca="false">$A$9</f>
         <v>P: 1, T: 2</v>
       </c>
-      <c r="Q11" s="6" t="n">
+      <c r="Q11" s="2" t="n">
         <f aca="false">M11*4/(M11+1)^2</f>
         <v>0.842268743441741</v>
       </c>
-      <c r="R11" s="6" t="n">
+      <c r="R11" s="1" t="n">
         <f aca="false">N11</f>
         <v>0.799718868077318</v>
       </c>
-      <c r="T11" s="0" t="str">
+      <c r="S11" s="1"/>
+      <c r="T11" s="1" t="str">
         <f aca="false">$A$9</f>
         <v>P: 1, T: 2</v>
       </c>
-      <c r="U11" s="6" t="n">
+      <c r="U11" s="1" t="n">
         <f aca="false">M30/(M30+1)^2</f>
         <v>0.210567185860435</v>
       </c>
-      <c r="V11" s="6" t="n">
+      <c r="V11" s="1" t="n">
         <f aca="false">N30</f>
         <v>0.189786966174024</v>
       </c>
@@ -1204,37 +1219,38 @@
       <c r="B12" s="0" t="s">
         <v>20</v>
       </c>
-      <c r="G12" s="4" t="n">
+      <c r="G12" s="5" t="n">
         <v>2</v>
       </c>
-      <c r="H12" s="4" t="n">
+      <c r="H12" s="5" t="n">
         <v>34</v>
       </c>
       <c r="K12" s="1" t="n">
         <f aca="false">$C$18+H12-$C$5/2-$E$11-50</f>
         <v>93</v>
       </c>
-      <c r="P12" s="0" t="str">
+      <c r="P12" s="1" t="str">
         <f aca="false">$A$208</f>
         <v>P: 3, T: 2</v>
       </c>
-      <c r="Q12" s="6" t="n">
+      <c r="Q12" s="2" t="n">
         <f aca="false">M210*4/(M210+1)^2</f>
         <v>0.897390453008233</v>
       </c>
-      <c r="R12" s="6" t="n">
+      <c r="R12" s="1" t="n">
         <f aca="false">N210</f>
         <v>0.786245690080242</v>
       </c>
-      <c r="T12" s="0" t="str">
+      <c r="S12" s="1"/>
+      <c r="T12" s="1" t="str">
         <f aca="false">$A$208</f>
         <v>P: 3, T: 2</v>
       </c>
-      <c r="U12" s="6" t="n">
+      <c r="U12" s="1" t="n">
         <f aca="false">M230/(M230+1)^2</f>
         <v>0.224347613252058</v>
       </c>
-      <c r="V12" s="6" t="n">
+      <c r="V12" s="1" t="n">
         <f aca="false">N230</f>
         <v>0.186172374119965</v>
       </c>
@@ -1243,37 +1259,38 @@
       <c r="B13" s="0" t="s">
         <v>21</v>
       </c>
-      <c r="G13" s="4" t="n">
+      <c r="G13" s="5" t="n">
         <v>3</v>
       </c>
-      <c r="H13" s="4" t="n">
+      <c r="H13" s="5" t="n">
         <v>35</v>
       </c>
       <c r="K13" s="1" t="n">
         <f aca="false">$C$18+H13-$C$5/2-$E$11-50</f>
         <v>94</v>
       </c>
-      <c r="P13" s="0" t="str">
+      <c r="P13" s="1" t="str">
         <f aca="false">$A$128</f>
         <v>P: 2, T: 2</v>
       </c>
-      <c r="Q13" s="6" t="n">
+      <c r="Q13" s="2" t="n">
         <f aca="false">M130*4/(M130+1)^2</f>
         <v>1</v>
       </c>
-      <c r="R13" s="6" t="n">
+      <c r="R13" s="1" t="n">
         <f aca="false">N130</f>
         <v>0.948060941828255</v>
       </c>
-      <c r="T13" s="0" t="str">
+      <c r="S13" s="1"/>
+      <c r="T13" s="1" t="str">
         <f aca="false">$A$128</f>
         <v>P: 2, T: 2</v>
       </c>
-      <c r="U13" s="6" t="n">
+      <c r="U13" s="1" t="n">
         <f aca="false">M150/(M150+1)^2</f>
         <v>0.25</v>
       </c>
-      <c r="V13" s="6" t="n">
+      <c r="V13" s="1" t="n">
         <f aca="false">N150</f>
         <v>0.226876731301939</v>
       </c>
@@ -1282,48 +1299,49 @@
       <c r="B14" s="0" t="s">
         <v>18</v>
       </c>
-      <c r="C14" s="6" t="n">
+      <c r="C14" s="7" t="n">
         <f aca="false">C11-C5</f>
         <v>239</v>
       </c>
       <c r="D14" s="0" t="s">
         <v>19</v>
       </c>
-      <c r="E14" s="6" t="n">
+      <c r="E14" s="7" t="n">
         <f aca="false">C14-B5/2</f>
         <v>220</v>
       </c>
-      <c r="G14" s="4" t="n">
+      <c r="G14" s="5" t="n">
         <v>4</v>
       </c>
-      <c r="H14" s="4" t="n">
+      <c r="H14" s="5" t="n">
         <v>35</v>
       </c>
       <c r="K14" s="1" t="n">
         <f aca="false">$C$18+H14-$C$5/2-$E$11-50</f>
         <v>94</v>
       </c>
-      <c r="P14" s="0" t="str">
+      <c r="P14" s="1" t="str">
         <f aca="false">$A$168</f>
         <v>P: 2, T: 3</v>
       </c>
-      <c r="Q14" s="6" t="n">
+      <c r="Q14" s="2" t="n">
         <f aca="false">M170*4/(M170+1)^2</f>
         <v>0.897390453008233</v>
       </c>
-      <c r="R14" s="6" t="n">
+      <c r="R14" s="1" t="n">
         <f aca="false">N170</f>
         <v>0.84865396276836</v>
       </c>
-      <c r="T14" s="0" t="str">
+      <c r="S14" s="1"/>
+      <c r="T14" s="1" t="str">
         <f aca="false">$A$168</f>
         <v>P: 2, T: 3</v>
       </c>
-      <c r="U14" s="6" t="n">
+      <c r="U14" s="1" t="n">
         <f aca="false">M190/(M190+1)^2</f>
         <v>0.224347613252058</v>
       </c>
-      <c r="V14" s="6" t="n">
+      <c r="V14" s="1" t="n">
         <f aca="false">N190</f>
         <v>0.196628947000341</v>
       </c>
@@ -1332,40 +1350,41 @@
       <c r="B15" s="0" t="s">
         <v>22</v>
       </c>
-      <c r="G15" s="4" t="n">
+      <c r="G15" s="5" t="n">
         <v>5</v>
       </c>
-      <c r="H15" s="4" t="n">
+      <c r="H15" s="5" t="n">
         <v>36</v>
       </c>
       <c r="K15" s="1" t="n">
         <f aca="false">$C$18+H15-$C$5/2-$E$11-50</f>
         <v>95</v>
       </c>
-      <c r="M15" s="1" t="s">
+      <c r="M15" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="P15" s="0" t="str">
+      <c r="P15" s="1" t="str">
         <f aca="false">$A$88</f>
         <v>P: 2, T: 1</v>
       </c>
-      <c r="Q15" s="6" t="n">
+      <c r="Q15" s="2" t="n">
         <f aca="false">M90*4/(M90+1)^2</f>
         <v>0.842268743441741</v>
       </c>
-      <c r="R15" s="6" t="n">
+      <c r="R15" s="1" t="n">
         <f aca="false">N90</f>
         <v>0.765518068450414</v>
       </c>
-      <c r="T15" s="0" t="str">
+      <c r="S15" s="1"/>
+      <c r="T15" s="1" t="str">
         <f aca="false">$A$88</f>
         <v>P: 2, T: 1</v>
       </c>
-      <c r="U15" s="6" t="n">
+      <c r="U15" s="1" t="n">
         <f aca="false">M110/(M110+1)^2</f>
         <v>0.210567185860435</v>
       </c>
-      <c r="V15" s="6" t="n">
+      <c r="V15" s="1" t="n">
         <f aca="false">N110</f>
         <v>0.191881057453478</v>
       </c>
@@ -1380,54 +1399,55 @@
       <c r="D16" s="0" t="s">
         <v>19</v>
       </c>
-      <c r="E16" s="6" t="n">
+      <c r="E16" s="7" t="n">
         <f aca="false">C16-B5/2</f>
         <v>61</v>
       </c>
-      <c r="G16" s="4" t="n">
+      <c r="G16" s="5" t="n">
         <v>6</v>
       </c>
-      <c r="H16" s="4" t="n">
+      <c r="H16" s="5" t="n">
         <v>34</v>
       </c>
       <c r="K16" s="1" t="n">
         <f aca="false">$C$18+H16-$C$5/2-$E$11-50</f>
         <v>93</v>
       </c>
-      <c r="M16" s="7" t="n">
+      <c r="M16" s="8" t="n">
         <f aca="false">SQRT(4*(M11)^2*((J23*0.001)^4/(J11*0.001)^6*$M$4^2+ (J23*0.001)^2/(J11*0.001)^4*(L23*0.001)^2))</f>
         <v>0.0204719173976423</v>
       </c>
-      <c r="P16" s="0" t="str">
+      <c r="P16" s="1" t="str">
         <f aca="false">$A$248</f>
         <v>P: 3, T: 1</v>
       </c>
-      <c r="Q16" s="6" t="n">
+      <c r="Q16" s="2" t="n">
         <f aca="false">M250*4/(M250+1)^2</f>
         <v>0.594860799112152</v>
       </c>
-      <c r="R16" s="6" t="n">
+      <c r="R16" s="1" t="n">
         <f aca="false">N250</f>
         <v>0.500681202300135</v>
       </c>
-      <c r="T16" s="0" t="str">
+      <c r="S16" s="1"/>
+      <c r="T16" s="1" t="str">
         <f aca="false">$A$248</f>
         <v>P: 3, T: 1</v>
       </c>
-      <c r="U16" s="6" t="n">
+      <c r="U16" s="1" t="n">
         <f aca="false">M270/(M270+1)^2</f>
         <v>0.148715199778038</v>
       </c>
-      <c r="V16" s="6" t="n">
+      <c r="V16" s="1" t="n">
         <f aca="false">N270</f>
         <v>0.137535787098069</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="17">
-      <c r="G17" s="4" t="n">
+      <c r="G17" s="5" t="n">
         <v>7</v>
       </c>
-      <c r="H17" s="4" t="n">
+      <c r="H17" s="5" t="n">
         <v>34</v>
       </c>
       <c r="K17" s="1" t="n">
@@ -1439,13 +1459,13 @@
       <c r="B18" s="0" t="s">
         <v>24</v>
       </c>
-      <c r="C18" s="8" t="n">
+      <c r="C18" s="9" t="n">
         <v>400</v>
       </c>
-      <c r="G18" s="4" t="n">
+      <c r="G18" s="5" t="n">
         <v>8</v>
       </c>
-      <c r="H18" s="4" t="n">
+      <c r="H18" s="5" t="n">
         <v>34</v>
       </c>
       <c r="K18" s="1" t="n">
@@ -1454,10 +1474,10 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="19">
-      <c r="G19" s="4" t="n">
+      <c r="G19" s="5" t="n">
         <v>9</v>
       </c>
-      <c r="H19" s="4" t="n">
+      <c r="H19" s="5" t="n">
         <v>34</v>
       </c>
       <c r="K19" s="1" t="n">
@@ -1466,10 +1486,10 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="20">
-      <c r="G20" s="4" t="n">
+      <c r="G20" s="5" t="n">
         <v>10</v>
       </c>
-      <c r="H20" s="4" t="n">
+      <c r="H20" s="5" t="n">
         <v>34</v>
       </c>
       <c r="K20" s="1" t="n">
@@ -1483,37 +1503,37 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="22">
-      <c r="A22" s="2"/>
-      <c r="B22" s="2" t="s">
+      <c r="A22" s="3"/>
+      <c r="B22" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C22" s="2" t="s">
+      <c r="C22" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D22" s="2" t="s">
+      <c r="D22" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="J22" s="9" t="s">
+      <c r="J22" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="K22" s="9" t="s">
+      <c r="K22" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="L22" s="9" t="s">
+      <c r="L22" s="10" t="s">
         <v>27</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="23">
-      <c r="A23" s="2" t="s">
+      <c r="A23" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B23" s="2" t="n">
+      <c r="B23" s="3" t="n">
         <v>233</v>
       </c>
-      <c r="C23" s="2" t="n">
+      <c r="C23" s="3" t="n">
         <v>540</v>
       </c>
-      <c r="D23" s="2" t="n">
+      <c r="D23" s="3" t="n">
         <v>1049</v>
       </c>
       <c r="J23" s="1" t="n">
@@ -1530,24 +1550,24 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="24">
-      <c r="A24" s="2" t="s">
+      <c r="A24" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B24" s="2" t="n">
+      <c r="B24" s="3" t="n">
         <v>38</v>
       </c>
-      <c r="C24" s="2" t="n">
+      <c r="C24" s="3" t="n">
         <v>52</v>
       </c>
-      <c r="D24" s="2" t="n">
+      <c r="D24" s="3" t="n">
         <v>65</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="28">
-      <c r="A28" s="3" t="s">
+      <c r="A28" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B28" s="3" t="s">
+      <c r="B28" s="4" t="s">
         <v>28</v>
       </c>
     </row>
@@ -1555,19 +1575,19 @@
       <c r="B29" s="0" t="s">
         <v>11</v>
       </c>
-      <c r="G29" s="4" t="s">
+      <c r="G29" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="H29" s="4" t="s">
+      <c r="H29" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="J29" s="5" t="s">
+      <c r="J29" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="K29" s="5" t="s">
+      <c r="K29" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="M29" s="1" t="s">
+      <c r="M29" s="2" t="s">
         <v>16</v>
       </c>
       <c r="N29" s="1" t="s">
@@ -1590,14 +1610,14 @@
       <c r="D30" s="0" t="s">
         <v>19</v>
       </c>
-      <c r="E30" s="6" t="n">
+      <c r="E30" s="7" t="n">
         <f aca="false">C30-C24/2</f>
         <v>265</v>
       </c>
-      <c r="G30" s="4" t="n">
+      <c r="G30" s="5" t="n">
         <v>1</v>
       </c>
-      <c r="H30" s="4" t="n">
+      <c r="H30" s="5" t="n">
         <v>36</v>
       </c>
       <c r="J30" s="1" t="n">
@@ -1608,7 +1628,7 @@
         <f aca="false">$C$37+H30-$C$24/2-$E$30-50</f>
         <v>45</v>
       </c>
-      <c r="M30" s="1" t="n">
+      <c r="M30" s="2" t="n">
         <f aca="false">C23*0.001/(B23*0.001)</f>
         <v>2.31759656652361</v>
       </c>
@@ -1620,7 +1640,7 @@
         <f aca="false">1-((1+M30)*J42^2/J30^2)</f>
         <v>0.728323472495333</v>
       </c>
-      <c r="P30" s="6" t="n">
+      <c r="P30" s="7" t="n">
         <f aca="false">M30/(1+M30)</f>
         <v>0.698576972833118</v>
       </c>
@@ -1629,10 +1649,10 @@
       <c r="B31" s="0" t="s">
         <v>20</v>
       </c>
-      <c r="G31" s="4" t="n">
+      <c r="G31" s="5" t="n">
         <v>2</v>
       </c>
-      <c r="H31" s="4" t="n">
+      <c r="H31" s="5" t="n">
         <v>38</v>
       </c>
       <c r="K31" s="1" t="n">
@@ -1644,10 +1664,10 @@
       <c r="B32" s="0" t="s">
         <v>21</v>
       </c>
-      <c r="G32" s="4" t="n">
+      <c r="G32" s="5" t="n">
         <v>3</v>
       </c>
-      <c r="H32" s="4" t="n">
+      <c r="H32" s="5" t="n">
         <v>40</v>
       </c>
       <c r="K32" s="1" t="n">
@@ -1659,21 +1679,21 @@
       <c r="B33" s="0" t="s">
         <v>18</v>
       </c>
-      <c r="C33" s="6" t="n">
+      <c r="C33" s="7" t="n">
         <f aca="false">C30-C24</f>
         <v>239</v>
       </c>
       <c r="D33" s="0" t="s">
         <v>19</v>
       </c>
-      <c r="E33" s="6" t="n">
+      <c r="E33" s="7" t="n">
         <f aca="false">C33-B24/2</f>
         <v>220</v>
       </c>
-      <c r="G33" s="4" t="n">
+      <c r="G33" s="5" t="n">
         <v>4</v>
       </c>
-      <c r="H33" s="4" t="n">
+      <c r="H33" s="5" t="n">
         <v>36</v>
       </c>
       <c r="K33" s="1" t="n">
@@ -1685,17 +1705,17 @@
       <c r="B34" s="0" t="s">
         <v>22</v>
       </c>
-      <c r="G34" s="4" t="n">
+      <c r="G34" s="5" t="n">
         <v>5</v>
       </c>
-      <c r="H34" s="4" t="n">
+      <c r="H34" s="5" t="n">
         <v>37</v>
       </c>
       <c r="K34" s="1" t="n">
         <f aca="false">$C$37+H34-$C$24/2-$E$30-50</f>
         <v>46</v>
       </c>
-      <c r="M34" s="1" t="s">
+      <c r="M34" s="2" t="s">
         <v>23</v>
       </c>
     </row>
@@ -1709,30 +1729,30 @@
       <c r="D35" s="0" t="s">
         <v>19</v>
       </c>
-      <c r="E35" s="6" t="n">
+      <c r="E35" s="7" t="n">
         <f aca="false">C35-B24/2</f>
         <v>61</v>
       </c>
-      <c r="G35" s="4" t="n">
+      <c r="G35" s="5" t="n">
         <v>6</v>
       </c>
-      <c r="H35" s="4" t="n">
+      <c r="H35" s="5" t="n">
         <v>36</v>
       </c>
       <c r="K35" s="1" t="n">
         <f aca="false">$C$37+H35-$C$24/2-$E$30-50</f>
         <v>45</v>
       </c>
-      <c r="M35" s="7" t="n">
+      <c r="M35" s="8" t="n">
         <f aca="false">SQRT(4*(M30)^2*((J42*0.001)^4/(J30*0.001)^6*$M$4^2+ (J42*0.001)^2/(J30*0.001)^4*(L42*0.001)^2))</f>
         <v>0.00621674287675844</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="36">
-      <c r="G36" s="4" t="n">
+      <c r="G36" s="5" t="n">
         <v>7</v>
       </c>
-      <c r="H36" s="4" t="n">
+      <c r="H36" s="5" t="n">
         <v>35</v>
       </c>
       <c r="K36" s="1" t="n">
@@ -1744,13 +1764,13 @@
       <c r="B37" s="0" t="s">
         <v>24</v>
       </c>
-      <c r="C37" s="8" t="n">
+      <c r="C37" s="9" t="n">
         <v>350</v>
       </c>
-      <c r="G37" s="4" t="n">
+      <c r="G37" s="5" t="n">
         <v>8</v>
       </c>
-      <c r="H37" s="4" t="n">
+      <c r="H37" s="5" t="n">
         <v>35</v>
       </c>
       <c r="K37" s="1" t="n">
@@ -1759,10 +1779,10 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="38">
-      <c r="G38" s="4" t="n">
+      <c r="G38" s="5" t="n">
         <v>9</v>
       </c>
-      <c r="H38" s="4" t="n">
+      <c r="H38" s="5" t="n">
         <v>36</v>
       </c>
       <c r="K38" s="1" t="n">
@@ -1771,10 +1791,10 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="39">
-      <c r="G39" s="4" t="n">
+      <c r="G39" s="5" t="n">
         <v>10</v>
       </c>
-      <c r="H39" s="4" t="n">
+      <c r="H39" s="5" t="n">
         <v>36</v>
       </c>
       <c r="K39" s="1" t="n">
@@ -1786,25 +1806,25 @@
       <c r="B41" s="0" t="s">
         <v>0</v>
       </c>
-      <c r="J41" s="9" t="s">
+      <c r="J41" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="K41" s="9" t="s">
+      <c r="K41" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="L41" s="9" t="s">
+      <c r="L41" s="10" t="s">
         <v>27</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="42">
-      <c r="A42" s="2"/>
-      <c r="B42" s="2" t="s">
+      <c r="A42" s="3"/>
+      <c r="B42" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C42" s="2" t="s">
+      <c r="C42" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D42" s="2" t="s">
+      <c r="D42" s="3" t="s">
         <v>3</v>
       </c>
       <c r="J42" s="1" t="n">
@@ -1821,38 +1841,38 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="43">
-      <c r="A43" s="2" t="s">
+      <c r="A43" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B43" s="2" t="n">
+      <c r="B43" s="3" t="n">
         <v>233</v>
       </c>
-      <c r="C43" s="2" t="n">
+      <c r="C43" s="3" t="n">
         <v>540</v>
       </c>
-      <c r="D43" s="2" t="n">
+      <c r="D43" s="3" t="n">
         <v>1049</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="44">
-      <c r="A44" s="2" t="s">
+      <c r="A44" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B44" s="2" t="n">
+      <c r="B44" s="3" t="n">
         <v>38</v>
       </c>
-      <c r="C44" s="2" t="n">
+      <c r="C44" s="3" t="n">
         <v>52</v>
       </c>
-      <c r="D44" s="2" t="n">
+      <c r="D44" s="3" t="n">
         <v>65</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="48">
-      <c r="A48" s="3" t="s">
+      <c r="A48" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="B48" s="3" t="s">
+      <c r="B48" s="4" t="s">
         <v>7</v>
       </c>
     </row>
@@ -1860,19 +1880,19 @@
       <c r="B49" s="0" t="s">
         <v>32</v>
       </c>
-      <c r="G49" s="4" t="s">
+      <c r="G49" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="H49" s="4" t="s">
+      <c r="H49" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="J49" s="5" t="s">
+      <c r="J49" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="K49" s="5" t="s">
+      <c r="K49" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="M49" s="1" t="s">
+      <c r="M49" s="2" t="s">
         <v>16</v>
       </c>
       <c r="N49" s="1" t="s">
@@ -1889,14 +1909,14 @@
       <c r="D50" s="0" t="s">
         <v>19</v>
       </c>
-      <c r="E50" s="6" t="n">
+      <c r="E50" s="7" t="n">
         <f aca="false">C50-D44/2</f>
         <v>270.5</v>
       </c>
-      <c r="G50" s="4" t="n">
+      <c r="G50" s="5" t="n">
         <v>1</v>
       </c>
-      <c r="H50" s="4" t="n">
+      <c r="H50" s="5" t="n">
         <v>39</v>
       </c>
       <c r="J50" s="1" t="n">
@@ -1907,7 +1927,7 @@
         <f aca="false">$C$57+H50-$D$44/2-$E$50-50</f>
         <v>56</v>
       </c>
-      <c r="M50" s="1" t="n">
+      <c r="M50" s="2" t="n">
         <f aca="false">D43*0.001/(B43*0.001)</f>
         <v>4.50214592274678</v>
       </c>
@@ -1920,10 +1940,10 @@
       <c r="B51" s="0" t="s">
         <v>20</v>
       </c>
-      <c r="G51" s="4" t="n">
+      <c r="G51" s="5" t="n">
         <v>2</v>
       </c>
-      <c r="H51" s="4" t="n">
+      <c r="H51" s="5" t="n">
         <v>39</v>
       </c>
       <c r="K51" s="1" t="n">
@@ -1935,10 +1955,10 @@
       <c r="B52" s="0" t="s">
         <v>21</v>
       </c>
-      <c r="G52" s="4" t="n">
+      <c r="G52" s="5" t="n">
         <v>3</v>
       </c>
-      <c r="H52" s="4" t="n">
+      <c r="H52" s="5" t="n">
         <v>38</v>
       </c>
       <c r="K52" s="1" t="n">
@@ -1950,21 +1970,21 @@
       <c r="B53" s="0" t="s">
         <v>18</v>
       </c>
-      <c r="C53" s="6" t="n">
+      <c r="C53" s="7" t="n">
         <f aca="false">C50-D44</f>
         <v>238</v>
       </c>
       <c r="D53" s="0" t="s">
         <v>19</v>
       </c>
-      <c r="E53" s="6" t="n">
+      <c r="E53" s="7" t="n">
         <f aca="false">C53-B44/2</f>
         <v>219</v>
       </c>
-      <c r="G53" s="4" t="n">
+      <c r="G53" s="5" t="n">
         <v>4</v>
       </c>
-      <c r="H53" s="4" t="n">
+      <c r="H53" s="5" t="n">
         <v>38.5</v>
       </c>
       <c r="K53" s="1" t="n">
@@ -1976,17 +1996,17 @@
       <c r="B54" s="0" t="s">
         <v>22</v>
       </c>
-      <c r="G54" s="4" t="n">
+      <c r="G54" s="5" t="n">
         <v>5</v>
       </c>
-      <c r="H54" s="4" t="n">
+      <c r="H54" s="5" t="n">
         <v>38.5</v>
       </c>
       <c r="K54" s="1" t="n">
         <f aca="false">$C$57+H54-$D$44/2-$E$50-50</f>
         <v>55.5</v>
       </c>
-      <c r="M54" s="1" t="s">
+      <c r="M54" s="2" t="s">
         <v>23</v>
       </c>
     </row>
@@ -2000,30 +2020,30 @@
       <c r="D55" s="0" t="s">
         <v>19</v>
       </c>
-      <c r="E55" s="6" t="n">
+      <c r="E55" s="7" t="n">
         <f aca="false">C55-B44/2</f>
         <v>61</v>
       </c>
-      <c r="G55" s="4" t="n">
+      <c r="G55" s="5" t="n">
         <v>6</v>
       </c>
-      <c r="H55" s="4" t="n">
+      <c r="H55" s="5" t="n">
         <v>38.5</v>
       </c>
       <c r="K55" s="1" t="n">
         <f aca="false">$C$57+H55-$D$44/2-$E$50-50</f>
         <v>55.5</v>
       </c>
-      <c r="M55" s="7" t="n">
+      <c r="M55" s="8" t="n">
         <f aca="false">SQRT(4*(M50)^2*((J62*0.001)^4/(J50*0.001)^6*$M$4^2+ (J62*0.001)^2/(J50*0.001)^4*(L62*0.001)^2))</f>
         <v>0.014453868592739</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="56">
-      <c r="G56" s="4" t="n">
+      <c r="G56" s="5" t="n">
         <v>7</v>
       </c>
-      <c r="H56" s="4" t="n">
+      <c r="H56" s="5" t="n">
         <v>38</v>
       </c>
       <c r="K56" s="1" t="n">
@@ -2035,13 +2055,13 @@
       <c r="B57" s="0" t="s">
         <v>24</v>
       </c>
-      <c r="C57" s="8" t="n">
+      <c r="C57" s="9" t="n">
         <v>370</v>
       </c>
-      <c r="G57" s="4" t="n">
+      <c r="G57" s="5" t="n">
         <v>8</v>
       </c>
-      <c r="H57" s="4" t="n">
+      <c r="H57" s="5" t="n">
         <v>37.5</v>
       </c>
       <c r="K57" s="1" t="n">
@@ -2050,10 +2070,10 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="58">
-      <c r="G58" s="4" t="n">
+      <c r="G58" s="5" t="n">
         <v>9</v>
       </c>
-      <c r="H58" s="4" t="n">
+      <c r="H58" s="5" t="n">
         <v>39</v>
       </c>
       <c r="K58" s="1" t="n">
@@ -2062,10 +2082,10 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="59">
-      <c r="G59" s="4" t="n">
+      <c r="G59" s="5" t="n">
         <v>10</v>
       </c>
-      <c r="H59" s="4" t="n">
+      <c r="H59" s="5" t="n">
         <v>39</v>
       </c>
       <c r="K59" s="1" t="n">
@@ -2077,25 +2097,25 @@
       <c r="B61" s="0" t="s">
         <v>0</v>
       </c>
-      <c r="J61" s="9" t="s">
+      <c r="J61" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="K61" s="9" t="s">
+      <c r="K61" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="L61" s="9" t="s">
+      <c r="L61" s="10" t="s">
         <v>27</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="62">
-      <c r="A62" s="2"/>
-      <c r="B62" s="2" t="s">
+      <c r="A62" s="3"/>
+      <c r="B62" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C62" s="2" t="s">
+      <c r="C62" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D62" s="2" t="s">
+      <c r="D62" s="3" t="s">
         <v>3</v>
       </c>
       <c r="J62" s="1" t="n">
@@ -2112,38 +2132,38 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="63">
-      <c r="A63" s="2" t="s">
+      <c r="A63" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B63" s="2" t="n">
+      <c r="B63" s="3" t="n">
         <v>233</v>
       </c>
-      <c r="C63" s="2" t="n">
+      <c r="C63" s="3" t="n">
         <v>540</v>
       </c>
-      <c r="D63" s="2" t="n">
+      <c r="D63" s="3" t="n">
         <v>1049</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="64">
-      <c r="A64" s="2" t="s">
+      <c r="A64" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B64" s="2" t="n">
+      <c r="B64" s="3" t="n">
         <v>38</v>
       </c>
-      <c r="C64" s="2" t="n">
+      <c r="C64" s="3" t="n">
         <v>52</v>
       </c>
-      <c r="D64" s="2" t="n">
+      <c r="D64" s="3" t="n">
         <v>65</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="68">
-      <c r="A68" s="3" t="s">
+      <c r="A68" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="B68" s="3" t="s">
+      <c r="B68" s="4" t="s">
         <v>28</v>
       </c>
     </row>
@@ -2151,19 +2171,19 @@
       <c r="B69" s="0" t="s">
         <v>32</v>
       </c>
-      <c r="G69" s="4" t="s">
+      <c r="G69" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="H69" s="4" t="s">
+      <c r="H69" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="J69" s="5" t="s">
+      <c r="J69" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="K69" s="5" t="s">
+      <c r="K69" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="M69" s="1" t="s">
+      <c r="M69" s="2" t="s">
         <v>16</v>
       </c>
       <c r="N69" s="1" t="s">
@@ -2180,14 +2200,14 @@
       <c r="D70" s="0" t="s">
         <v>19</v>
       </c>
-      <c r="E70" s="6" t="n">
+      <c r="E70" s="7" t="n">
         <f aca="false">C70-D64/2</f>
         <v>270.5</v>
       </c>
-      <c r="G70" s="4" t="n">
+      <c r="G70" s="5" t="n">
         <v>1</v>
       </c>
-      <c r="H70" s="4" t="n">
+      <c r="H70" s="5" t="n">
         <v>31</v>
       </c>
       <c r="J70" s="1" t="n">
@@ -2198,7 +2218,7 @@
         <f aca="false">$C$77+H70-$D$64/2-$E$70-50</f>
         <v>28</v>
       </c>
-      <c r="M70" s="1" t="n">
+      <c r="M70" s="2" t="n">
         <f aca="false">D63*0.001/(B63*0.001)</f>
         <v>4.50214592274678</v>
       </c>
@@ -2210,7 +2230,7 @@
         <f aca="false">1-((1+M70)*J82^2/J70^2)</f>
         <v>0.842876750245675</v>
       </c>
-      <c r="P70" s="6" t="n">
+      <c r="P70" s="7" t="n">
         <f aca="false">M70/(1+M70)</f>
         <v>0.818252730109204</v>
       </c>
@@ -2219,10 +2239,10 @@
       <c r="B71" s="0" t="s">
         <v>20</v>
       </c>
-      <c r="G71" s="4" t="n">
+      <c r="G71" s="5" t="n">
         <v>2</v>
       </c>
-      <c r="H71" s="4" t="n">
+      <c r="H71" s="5" t="n">
         <v>30</v>
       </c>
       <c r="K71" s="1" t="n">
@@ -2234,10 +2254,10 @@
       <c r="B72" s="0" t="s">
         <v>21</v>
       </c>
-      <c r="G72" s="4" t="n">
+      <c r="G72" s="5" t="n">
         <v>3</v>
       </c>
-      <c r="H72" s="4" t="n">
+      <c r="H72" s="5" t="n">
         <v>30</v>
       </c>
       <c r="K72" s="1" t="n">
@@ -2249,21 +2269,21 @@
       <c r="B73" s="0" t="s">
         <v>18</v>
       </c>
-      <c r="C73" s="6" t="n">
+      <c r="C73" s="7" t="n">
         <f aca="false">C70-D64</f>
         <v>238</v>
       </c>
       <c r="D73" s="0" t="s">
         <v>19</v>
       </c>
-      <c r="E73" s="6" t="n">
+      <c r="E73" s="7" t="n">
         <f aca="false">C73-B64/2</f>
         <v>219</v>
       </c>
-      <c r="G73" s="4" t="n">
+      <c r="G73" s="5" t="n">
         <v>4</v>
       </c>
-      <c r="H73" s="4" t="n">
+      <c r="H73" s="5" t="n">
         <v>29</v>
       </c>
       <c r="K73" s="1" t="n">
@@ -2275,17 +2295,17 @@
       <c r="B74" s="0" t="s">
         <v>22</v>
       </c>
-      <c r="G74" s="4" t="n">
+      <c r="G74" s="5" t="n">
         <v>5</v>
       </c>
-      <c r="H74" s="4" t="n">
+      <c r="H74" s="5" t="n">
         <v>29.5</v>
       </c>
       <c r="K74" s="1" t="n">
         <f aca="false">$C$77+H74-$D$64/2-$E$70-50</f>
         <v>26.5</v>
       </c>
-      <c r="M74" s="1" t="s">
+      <c r="M74" s="2" t="s">
         <v>23</v>
       </c>
     </row>
@@ -2299,30 +2319,30 @@
       <c r="D75" s="0" t="s">
         <v>19</v>
       </c>
-      <c r="E75" s="6" t="n">
+      <c r="E75" s="7" t="n">
         <f aca="false">C75-B64/2</f>
         <v>61</v>
       </c>
-      <c r="G75" s="4" t="n">
+      <c r="G75" s="5" t="n">
         <v>6</v>
       </c>
-      <c r="H75" s="4" t="n">
+      <c r="H75" s="5" t="n">
         <v>29</v>
       </c>
       <c r="K75" s="1" t="n">
         <f aca="false">$C$77+H75-$D$64/2-$E$70-50</f>
         <v>26</v>
       </c>
-      <c r="M75" s="7" t="n">
+      <c r="M75" s="8" t="n">
         <f aca="false">SQRT(4*(M70)^2*((J82*0.001)^4/(J70*0.001)^6*$M$4^2+ (J82*0.001)^2/(J70*0.001)^4*(L82*0.001)^2))</f>
         <v>0.00378204503736557</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="76">
-      <c r="G76" s="4" t="n">
+      <c r="G76" s="5" t="n">
         <v>7</v>
       </c>
-      <c r="H76" s="4" t="n">
+      <c r="H76" s="5" t="n">
         <v>30</v>
       </c>
       <c r="K76" s="1" t="n">
@@ -2334,13 +2354,13 @@
       <c r="B77" s="0" t="s">
         <v>24</v>
       </c>
-      <c r="C77" s="8" t="n">
+      <c r="C77" s="9" t="n">
         <v>350</v>
       </c>
-      <c r="G77" s="4" t="n">
+      <c r="G77" s="5" t="n">
         <v>8</v>
       </c>
-      <c r="H77" s="4" t="n">
+      <c r="H77" s="5" t="n">
         <v>29.5</v>
       </c>
       <c r="K77" s="1" t="n">
@@ -2349,10 +2369,10 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="78">
-      <c r="G78" s="4" t="n">
+      <c r="G78" s="5" t="n">
         <v>9</v>
       </c>
-      <c r="H78" s="4" t="n">
+      <c r="H78" s="5" t="n">
         <v>30</v>
       </c>
       <c r="K78" s="1" t="n">
@@ -2361,10 +2381,10 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="79">
-      <c r="G79" s="4" t="n">
+      <c r="G79" s="5" t="n">
         <v>10</v>
       </c>
-      <c r="H79" s="4" t="n">
+      <c r="H79" s="5" t="n">
         <v>29</v>
       </c>
       <c r="K79" s="1" t="n">
@@ -2376,25 +2396,25 @@
       <c r="B81" s="0" t="s">
         <v>0</v>
       </c>
-      <c r="J81" s="9" t="s">
+      <c r="J81" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="K81" s="9" t="s">
+      <c r="K81" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="L81" s="9" t="s">
+      <c r="L81" s="10" t="s">
         <v>27</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="82">
-      <c r="A82" s="2"/>
-      <c r="B82" s="2" t="s">
+      <c r="A82" s="3"/>
+      <c r="B82" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C82" s="2" t="s">
+      <c r="C82" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D82" s="2" t="s">
+      <c r="D82" s="3" t="s">
         <v>3</v>
       </c>
       <c r="J82" s="1" t="n">
@@ -2411,38 +2431,38 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="83">
-      <c r="A83" s="2" t="s">
+      <c r="A83" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B83" s="2" t="n">
+      <c r="B83" s="3" t="n">
         <v>233</v>
       </c>
-      <c r="C83" s="2" t="n">
+      <c r="C83" s="3" t="n">
         <v>540</v>
       </c>
-      <c r="D83" s="2" t="n">
+      <c r="D83" s="3" t="n">
         <v>1049</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="84">
-      <c r="A84" s="2" t="s">
+      <c r="A84" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B84" s="2" t="n">
+      <c r="B84" s="3" t="n">
         <v>38</v>
       </c>
-      <c r="C84" s="2" t="n">
+      <c r="C84" s="3" t="n">
         <v>52</v>
       </c>
-      <c r="D84" s="2" t="n">
+      <c r="D84" s="3" t="n">
         <v>65</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="88">
-      <c r="A88" s="3" t="s">
+      <c r="A88" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="B88" s="3" t="s">
+      <c r="B88" s="4" t="s">
         <v>7</v>
       </c>
     </row>
@@ -2450,19 +2470,19 @@
       <c r="B89" s="0" t="s">
         <v>20</v>
       </c>
-      <c r="G89" s="4" t="s">
+      <c r="G89" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="H89" s="4" t="s">
+      <c r="H89" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="J89" s="5" t="s">
+      <c r="J89" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="K89" s="5" t="s">
+      <c r="K89" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="M89" s="1" t="s">
+      <c r="M89" s="2" t="s">
         <v>16</v>
       </c>
       <c r="N89" s="1" t="s">
@@ -2479,14 +2499,14 @@
       <c r="D90" s="0" t="s">
         <v>19</v>
       </c>
-      <c r="E90" s="6" t="n">
+      <c r="E90" s="7" t="n">
         <f aca="false">C90-B84/2</f>
         <v>265</v>
       </c>
-      <c r="G90" s="4" t="n">
+      <c r="G90" s="5" t="n">
         <v>1</v>
       </c>
-      <c r="H90" s="4" t="n">
+      <c r="H90" s="5" t="n">
         <v>18</v>
       </c>
       <c r="J90" s="1" t="n">
@@ -2497,7 +2517,7 @@
         <f aca="false">$C$97+H90-$B$84/2-$E$90-50</f>
         <v>114</v>
       </c>
-      <c r="M90" s="1" t="n">
+      <c r="M90" s="2" t="n">
         <f aca="false">B83*0.001/(C83*0.001)</f>
         <v>0.431481481481482</v>
       </c>
@@ -2510,10 +2530,10 @@
       <c r="B91" s="0" t="s">
         <v>11</v>
       </c>
-      <c r="G91" s="4" t="n">
+      <c r="G91" s="5" t="n">
         <v>2</v>
       </c>
-      <c r="H91" s="4" t="n">
+      <c r="H91" s="5" t="n">
         <v>19</v>
       </c>
       <c r="K91" s="1" t="n">
@@ -2525,10 +2545,10 @@
       <c r="B92" s="0" t="s">
         <v>21</v>
       </c>
-      <c r="G92" s="4" t="n">
+      <c r="G92" s="5" t="n">
         <v>3</v>
       </c>
-      <c r="H92" s="4" t="n">
+      <c r="H92" s="5" t="n">
         <v>19</v>
       </c>
       <c r="K92" s="1" t="n">
@@ -2540,21 +2560,21 @@
       <c r="B93" s="0" t="s">
         <v>18</v>
       </c>
-      <c r="C93" s="6" t="n">
+      <c r="C93" s="7" t="n">
         <f aca="false">C90-B84</f>
         <v>246</v>
       </c>
       <c r="D93" s="0" t="s">
         <v>19</v>
       </c>
-      <c r="E93" s="6" t="n">
+      <c r="E93" s="7" t="n">
         <f aca="false">C93-C84/2</f>
         <v>220</v>
       </c>
-      <c r="G93" s="4" t="n">
+      <c r="G93" s="5" t="n">
         <v>4</v>
       </c>
-      <c r="H93" s="4" t="n">
+      <c r="H93" s="5" t="n">
         <v>18.5</v>
       </c>
       <c r="K93" s="1" t="n">
@@ -2566,17 +2586,17 @@
       <c r="B94" s="0" t="s">
         <v>22</v>
       </c>
-      <c r="G94" s="4" t="n">
+      <c r="G94" s="5" t="n">
         <v>5</v>
       </c>
-      <c r="H94" s="4" t="n">
+      <c r="H94" s="5" t="n">
         <v>18</v>
       </c>
       <c r="K94" s="1" t="n">
         <f aca="false">$C$97+H94-$B$84/2-$E$90-50</f>
         <v>114</v>
       </c>
-      <c r="M94" s="1" t="s">
+      <c r="M94" s="2" t="s">
         <v>23</v>
       </c>
     </row>
@@ -2590,30 +2610,30 @@
       <c r="D95" s="0" t="s">
         <v>19</v>
       </c>
-      <c r="E95" s="6" t="n">
+      <c r="E95" s="7" t="n">
         <f aca="false">C95-C84/2</f>
         <v>134</v>
       </c>
-      <c r="G95" s="4" t="n">
+      <c r="G95" s="5" t="n">
         <v>6</v>
       </c>
-      <c r="H95" s="4" t="n">
+      <c r="H95" s="5" t="n">
         <v>18</v>
       </c>
       <c r="K95" s="1" t="n">
         <f aca="false">$C$97+H95-$B$84/2-$E$90-50</f>
         <v>114</v>
       </c>
-      <c r="M95" s="7" t="n">
+      <c r="M95" s="8" t="n">
         <f aca="false">SQRT(4*(M90)^2*((J102*0.001)^4/(J90*0.001)^6*$M$4^2+ (J102*0.001)^2/(J90*0.001)^4*(L102*0.001)^2))</f>
         <v>0.0356535408889681</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="96">
-      <c r="G96" s="4" t="n">
+      <c r="G96" s="5" t="n">
         <v>7</v>
       </c>
-      <c r="H96" s="4" t="n">
+      <c r="H96" s="5" t="n">
         <v>18.5</v>
       </c>
       <c r="K96" s="1" t="n">
@@ -2625,13 +2645,13 @@
       <c r="B97" s="0" t="s">
         <v>24</v>
       </c>
-      <c r="C97" s="8" t="n">
+      <c r="C97" s="9" t="n">
         <v>430</v>
       </c>
-      <c r="G97" s="4" t="n">
+      <c r="G97" s="5" t="n">
         <v>8</v>
       </c>
-      <c r="H97" s="4" t="n">
+      <c r="H97" s="5" t="n">
         <v>18.5</v>
       </c>
       <c r="K97" s="1" t="n">
@@ -2640,10 +2660,10 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="98">
-      <c r="G98" s="4" t="n">
+      <c r="G98" s="5" t="n">
         <v>9</v>
       </c>
-      <c r="H98" s="4" t="n">
+      <c r="H98" s="5" t="n">
         <v>19</v>
       </c>
       <c r="K98" s="1" t="n">
@@ -2652,10 +2672,10 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="99">
-      <c r="G99" s="4" t="n">
+      <c r="G99" s="5" t="n">
         <v>10</v>
       </c>
-      <c r="H99" s="4" t="n">
+      <c r="H99" s="5" t="n">
         <v>19</v>
       </c>
       <c r="K99" s="1" t="n">
@@ -2667,25 +2687,25 @@
       <c r="B101" s="0" t="s">
         <v>0</v>
       </c>
-      <c r="J101" s="9" t="s">
+      <c r="J101" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="K101" s="9" t="s">
+      <c r="K101" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="L101" s="9" t="s">
+      <c r="L101" s="10" t="s">
         <v>27</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="102">
-      <c r="A102" s="2"/>
-      <c r="B102" s="2" t="s">
+      <c r="A102" s="3"/>
+      <c r="B102" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C102" s="2" t="s">
+      <c r="C102" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D102" s="2" t="s">
+      <c r="D102" s="3" t="s">
         <v>3</v>
       </c>
       <c r="J102" s="1" t="n">
@@ -2702,38 +2722,38 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="103">
-      <c r="A103" s="2" t="s">
+      <c r="A103" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B103" s="2" t="n">
+      <c r="B103" s="3" t="n">
         <v>233</v>
       </c>
-      <c r="C103" s="2" t="n">
+      <c r="C103" s="3" t="n">
         <v>540</v>
       </c>
-      <c r="D103" s="2" t="n">
+      <c r="D103" s="3" t="n">
         <v>1049</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="104">
-      <c r="A104" s="2" t="s">
+      <c r="A104" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B104" s="2" t="n">
+      <c r="B104" s="3" t="n">
         <v>38</v>
       </c>
-      <c r="C104" s="2" t="n">
+      <c r="C104" s="3" t="n">
         <v>52</v>
       </c>
-      <c r="D104" s="2" t="n">
+      <c r="D104" s="3" t="n">
         <v>65</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="108">
-      <c r="A108" s="3" t="s">
+      <c r="A108" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="B108" s="3" t="s">
+      <c r="B108" s="4" t="s">
         <v>28</v>
       </c>
     </row>
@@ -2741,19 +2761,19 @@
       <c r="B109" s="0" t="s">
         <v>20</v>
       </c>
-      <c r="G109" s="4" t="s">
+      <c r="G109" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="H109" s="4" t="s">
+      <c r="H109" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="J109" s="5" t="s">
+      <c r="J109" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="K109" s="5" t="s">
+      <c r="K109" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="M109" s="1" t="s">
+      <c r="M109" s="2" t="s">
         <v>16</v>
       </c>
       <c r="N109" s="1" t="s">
@@ -2770,14 +2790,14 @@
       <c r="D110" s="0" t="s">
         <v>19</v>
       </c>
-      <c r="E110" s="6" t="n">
+      <c r="E110" s="7" t="n">
         <f aca="false">C110-B104/2</f>
         <v>265</v>
       </c>
-      <c r="G110" s="4" t="n">
+      <c r="G110" s="5" t="n">
         <v>1</v>
       </c>
-      <c r="H110" s="4" t="n">
+      <c r="H110" s="5" t="n">
         <v>20</v>
       </c>
       <c r="J110" s="1" t="n">
@@ -2788,7 +2808,7 @@
         <f aca="false">$C$117+H110-$B$104/2-$E$110-50</f>
         <v>56</v>
       </c>
-      <c r="M110" s="1" t="n">
+      <c r="M110" s="2" t="n">
         <f aca="false">B103*0.001/(C103*0.001)</f>
         <v>0.431481481481482</v>
       </c>
@@ -2800,7 +2820,7 @@
         <f aca="false">1-((1+M110)*J122^2/J110^2)</f>
         <v>0.363416062611422</v>
       </c>
-      <c r="P110" s="6" t="n">
+      <c r="P110" s="7" t="n">
         <f aca="false">M110/(1+M110)</f>
         <v>0.301423027166882</v>
       </c>
@@ -2809,10 +2829,10 @@
       <c r="B111" s="0" t="s">
         <v>11</v>
       </c>
-      <c r="G111" s="4" t="n">
+      <c r="G111" s="5" t="n">
         <v>2</v>
       </c>
-      <c r="H111" s="4" t="n">
+      <c r="H111" s="5" t="n">
         <v>20.5</v>
       </c>
       <c r="K111" s="1" t="n">
@@ -2824,10 +2844,10 @@
       <c r="B112" s="0" t="s">
         <v>21</v>
       </c>
-      <c r="G112" s="4" t="n">
+      <c r="G112" s="5" t="n">
         <v>3</v>
       </c>
-      <c r="H112" s="4" t="n">
+      <c r="H112" s="5" t="n">
         <v>20.5</v>
       </c>
       <c r="K112" s="1" t="n">
@@ -2839,21 +2859,21 @@
       <c r="B113" s="0" t="s">
         <v>18</v>
       </c>
-      <c r="C113" s="6" t="n">
+      <c r="C113" s="7" t="n">
         <f aca="false">C110-B104</f>
         <v>246</v>
       </c>
       <c r="D113" s="0" t="s">
         <v>19</v>
       </c>
-      <c r="E113" s="6" t="n">
+      <c r="E113" s="7" t="n">
         <f aca="false">C113-C104/2</f>
         <v>220</v>
       </c>
-      <c r="G113" s="4" t="n">
+      <c r="G113" s="5" t="n">
         <v>4</v>
       </c>
-      <c r="H113" s="4" t="n">
+      <c r="H113" s="5" t="n">
         <v>20</v>
       </c>
       <c r="K113" s="1" t="n">
@@ -2865,17 +2885,17 @@
       <c r="B114" s="0" t="s">
         <v>22</v>
       </c>
-      <c r="G114" s="4" t="n">
+      <c r="G114" s="5" t="n">
         <v>5</v>
       </c>
-      <c r="H114" s="4" t="n">
+      <c r="H114" s="5" t="n">
         <v>20</v>
       </c>
       <c r="K114" s="1" t="n">
         <f aca="false">$C$117+H114-$B$104/2-$E$110-50</f>
         <v>56</v>
       </c>
-      <c r="M114" s="1" t="s">
+      <c r="M114" s="2" t="s">
         <v>23</v>
       </c>
     </row>
@@ -2889,30 +2909,30 @@
       <c r="D115" s="0" t="s">
         <v>19</v>
       </c>
-      <c r="E115" s="6" t="n">
+      <c r="E115" s="7" t="n">
         <f aca="false">C115-C104/2</f>
         <v>134</v>
       </c>
-      <c r="G115" s="4" t="n">
+      <c r="G115" s="5" t="n">
         <v>6</v>
       </c>
-      <c r="H115" s="4" t="n">
+      <c r="H115" s="5" t="n">
         <v>23</v>
       </c>
       <c r="K115" s="1" t="n">
         <f aca="false">$C$117+H115-$B$104/2-$E$110-50</f>
         <v>59</v>
       </c>
-      <c r="M115" s="7" t="n">
+      <c r="M115" s="8" t="n">
         <f aca="false">SQRT(4*(M110)^2*((J122*0.001)^4/(J110*0.001)^6*$M$4^2+ (J122*0.001)^2/(J110*0.001)^4*(L122*0.001)^2))</f>
         <v>0.00934742481939843</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="116">
-      <c r="G116" s="4" t="n">
+      <c r="G116" s="5" t="n">
         <v>7</v>
       </c>
-      <c r="H116" s="4" t="n">
+      <c r="H116" s="5" t="n">
         <v>23</v>
       </c>
       <c r="K116" s="1" t="n">
@@ -2924,13 +2944,13 @@
       <c r="B117" s="0" t="s">
         <v>24</v>
       </c>
-      <c r="C117" s="8" t="n">
+      <c r="C117" s="9" t="n">
         <v>370</v>
       </c>
-      <c r="G117" s="4" t="n">
+      <c r="G117" s="5" t="n">
         <v>8</v>
       </c>
-      <c r="H117" s="4" t="n">
+      <c r="H117" s="5" t="n">
         <v>21.5</v>
       </c>
       <c r="K117" s="1" t="n">
@@ -2939,10 +2959,10 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="118">
-      <c r="G118" s="4" t="n">
+      <c r="G118" s="5" t="n">
         <v>9</v>
       </c>
-      <c r="H118" s="4" t="n">
+      <c r="H118" s="5" t="n">
         <v>23</v>
       </c>
       <c r="K118" s="1" t="n">
@@ -2951,10 +2971,10 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="119">
-      <c r="G119" s="4" t="n">
+      <c r="G119" s="5" t="n">
         <v>10</v>
       </c>
-      <c r="H119" s="4" t="n">
+      <c r="H119" s="5" t="n">
         <v>22</v>
       </c>
       <c r="K119" s="1" t="n">
@@ -2966,25 +2986,25 @@
       <c r="B121" s="0" t="s">
         <v>0</v>
       </c>
-      <c r="J121" s="9" t="s">
+      <c r="J121" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="K121" s="9" t="s">
+      <c r="K121" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="L121" s="9" t="s">
+      <c r="L121" s="10" t="s">
         <v>27</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="122">
-      <c r="A122" s="2"/>
-      <c r="B122" s="2" t="s">
+      <c r="A122" s="3"/>
+      <c r="B122" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C122" s="2" t="s">
+      <c r="C122" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D122" s="2" t="s">
+      <c r="D122" s="3" t="s">
         <v>3</v>
       </c>
       <c r="J122" s="1" t="n">
@@ -3001,38 +3021,38 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="123">
-      <c r="A123" s="2" t="s">
+      <c r="A123" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B123" s="2" t="n">
+      <c r="B123" s="3" t="n">
         <v>233</v>
       </c>
-      <c r="C123" s="2" t="n">
+      <c r="C123" s="3" t="n">
         <v>540</v>
       </c>
-      <c r="D123" s="2" t="n">
+      <c r="D123" s="3" t="n">
         <v>1049</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="124">
-      <c r="A124" s="2" t="s">
+      <c r="A124" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B124" s="2" t="n">
+      <c r="B124" s="3" t="n">
         <v>38</v>
       </c>
-      <c r="C124" s="2" t="n">
+      <c r="C124" s="3" t="n">
         <v>52</v>
       </c>
-      <c r="D124" s="2" t="n">
+      <c r="D124" s="3" t="n">
         <v>65</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="128">
-      <c r="A128" s="3" t="s">
+      <c r="A128" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="B128" s="3" t="s">
+      <c r="B128" s="4" t="s">
         <v>7</v>
       </c>
     </row>
@@ -3040,19 +3060,19 @@
       <c r="B129" s="0" t="s">
         <v>11</v>
       </c>
-      <c r="G129" s="4" t="s">
+      <c r="G129" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="H129" s="4" t="s">
+      <c r="H129" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="J129" s="5" t="s">
+      <c r="J129" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="K129" s="5" t="s">
+      <c r="K129" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="M129" s="1" t="s">
+      <c r="M129" s="2" t="s">
         <v>16</v>
       </c>
       <c r="N129" s="1" t="s">
@@ -3069,14 +3089,14 @@
       <c r="D130" s="0" t="s">
         <v>19</v>
       </c>
-      <c r="E130" s="6" t="n">
+      <c r="E130" s="7" t="n">
         <f aca="false">C130-C124/2</f>
         <v>271</v>
       </c>
-      <c r="G130" s="4" t="n">
+      <c r="G130" s="5" t="n">
         <v>1</v>
       </c>
-      <c r="H130" s="4" t="n">
+      <c r="H130" s="5" t="n">
         <v>29</v>
       </c>
       <c r="J130" s="1" t="n">
@@ -3087,7 +3107,7 @@
         <f aca="false">$C$137+H130-$C$124/2-$E$130-50</f>
         <v>92</v>
       </c>
-      <c r="M130" s="1" t="n">
+      <c r="M130" s="2" t="n">
         <f aca="false">C123*0.001/(C123*0.001)</f>
         <v>1</v>
       </c>
@@ -3100,10 +3120,10 @@
       <c r="B131" s="0" t="s">
         <v>11</v>
       </c>
-      <c r="G131" s="4" t="n">
+      <c r="G131" s="5" t="n">
         <v>2</v>
       </c>
-      <c r="H131" s="4" t="n">
+      <c r="H131" s="5" t="n">
         <v>30</v>
       </c>
       <c r="K131" s="1" t="n">
@@ -3115,10 +3135,10 @@
       <c r="B132" s="0" t="s">
         <v>21</v>
       </c>
-      <c r="G132" s="4" t="n">
+      <c r="G132" s="5" t="n">
         <v>3</v>
       </c>
-      <c r="H132" s="4" t="n">
+      <c r="H132" s="5" t="n">
         <v>30</v>
       </c>
       <c r="K132" s="1" t="n">
@@ -3130,21 +3150,21 @@
       <c r="B133" s="0" t="s">
         <v>18</v>
       </c>
-      <c r="C133" s="6" t="n">
+      <c r="C133" s="7" t="n">
         <f aca="false">C130-C124</f>
         <v>245</v>
       </c>
       <c r="D133" s="0" t="s">
         <v>19</v>
       </c>
-      <c r="E133" s="6" t="n">
+      <c r="E133" s="7" t="n">
         <f aca="false">C133-C124/2</f>
         <v>219</v>
       </c>
-      <c r="G133" s="4" t="n">
+      <c r="G133" s="5" t="n">
         <v>4</v>
       </c>
-      <c r="H133" s="4" t="n">
+      <c r="H133" s="5" t="n">
         <v>30</v>
       </c>
       <c r="K133" s="1" t="n">
@@ -3156,17 +3176,17 @@
       <c r="B134" s="0" t="s">
         <v>22</v>
       </c>
-      <c r="G134" s="4" t="n">
+      <c r="G134" s="5" t="n">
         <v>5</v>
       </c>
-      <c r="H134" s="4" t="n">
+      <c r="H134" s="5" t="n">
         <v>30</v>
       </c>
       <c r="K134" s="1" t="n">
         <f aca="false">$C$137+H134-$C$124/2-$E$130-50</f>
         <v>93</v>
       </c>
-      <c r="M134" s="1" t="s">
+      <c r="M134" s="2" t="s">
         <v>23</v>
       </c>
     </row>
@@ -3180,30 +3200,30 @@
       <c r="D135" s="0" t="s">
         <v>19</v>
       </c>
-      <c r="E135" s="6" t="n">
+      <c r="E135" s="7" t="n">
         <f aca="false">C135-C124/2</f>
         <v>124</v>
       </c>
-      <c r="G135" s="4" t="n">
+      <c r="G135" s="5" t="n">
         <v>6</v>
       </c>
-      <c r="H135" s="4" t="n">
+      <c r="H135" s="5" t="n">
         <v>29.5</v>
       </c>
       <c r="K135" s="1" t="n">
         <f aca="false">$C$137+H135-$C$124/2-$E$130-50</f>
         <v>92.5</v>
       </c>
-      <c r="M135" s="7" t="n">
+      <c r="M135" s="8" t="n">
         <f aca="false">SQRT(4*(M130)^2*((J142*0.001)^4/(J130*0.001)^6*$M$4^2+ (J142*0.001)^2/(J130*0.001)^4*(L142*0.001)^2))</f>
         <v>0.0400351436674091</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="136">
-      <c r="G136" s="4" t="n">
+      <c r="G136" s="5" t="n">
         <v>7</v>
       </c>
-      <c r="H136" s="4" t="n">
+      <c r="H136" s="5" t="n">
         <v>29</v>
       </c>
       <c r="K136" s="1" t="n">
@@ -3215,13 +3235,13 @@
       <c r="B137" s="0" t="s">
         <v>24</v>
       </c>
-      <c r="C137" s="8" t="n">
+      <c r="C137" s="9" t="n">
         <v>410</v>
       </c>
-      <c r="G137" s="4" t="n">
+      <c r="G137" s="5" t="n">
         <v>8</v>
       </c>
-      <c r="H137" s="4" t="n">
+      <c r="H137" s="5" t="n">
         <v>29</v>
       </c>
       <c r="K137" s="1" t="n">
@@ -3230,10 +3250,10 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="138">
-      <c r="G138" s="4" t="n">
+      <c r="G138" s="5" t="n">
         <v>9</v>
       </c>
-      <c r="H138" s="4" t="n">
+      <c r="H138" s="5" t="n">
         <v>29.5</v>
       </c>
       <c r="K138" s="1" t="n">
@@ -3242,10 +3262,10 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="139">
-      <c r="G139" s="4" t="n">
+      <c r="G139" s="5" t="n">
         <v>10</v>
       </c>
-      <c r="H139" s="4" t="n">
+      <c r="H139" s="5" t="n">
         <v>29</v>
       </c>
       <c r="K139" s="1" t="n">
@@ -3257,25 +3277,25 @@
       <c r="B141" s="0" t="s">
         <v>0</v>
       </c>
-      <c r="J141" s="9" t="s">
+      <c r="J141" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="K141" s="9" t="s">
+      <c r="K141" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="L141" s="9" t="s">
+      <c r="L141" s="10" t="s">
         <v>27</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="142">
-      <c r="A142" s="2"/>
-      <c r="B142" s="2" t="s">
+      <c r="A142" s="3"/>
+      <c r="B142" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C142" s="2" t="s">
+      <c r="C142" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D142" s="2" t="s">
+      <c r="D142" s="3" t="s">
         <v>3</v>
       </c>
       <c r="J142" s="1" t="n">
@@ -3292,38 +3312,38 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="143">
-      <c r="A143" s="2" t="s">
+      <c r="A143" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B143" s="2" t="n">
+      <c r="B143" s="3" t="n">
         <v>233</v>
       </c>
-      <c r="C143" s="2" t="n">
+      <c r="C143" s="3" t="n">
         <v>540</v>
       </c>
-      <c r="D143" s="2" t="n">
+      <c r="D143" s="3" t="n">
         <v>1049</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="144">
-      <c r="A144" s="2" t="s">
+      <c r="A144" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B144" s="2" t="n">
+      <c r="B144" s="3" t="n">
         <v>38</v>
       </c>
-      <c r="C144" s="2" t="n">
+      <c r="C144" s="3" t="n">
         <v>52</v>
       </c>
-      <c r="D144" s="2" t="n">
+      <c r="D144" s="3" t="n">
         <v>65</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="148">
-      <c r="A148" s="3" t="s">
+      <c r="A148" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="B148" s="3" t="s">
+      <c r="B148" s="4" t="s">
         <v>28</v>
       </c>
     </row>
@@ -3331,19 +3351,19 @@
       <c r="B149" s="0" t="s">
         <v>11</v>
       </c>
-      <c r="G149" s="4" t="s">
+      <c r="G149" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="H149" s="4" t="s">
+      <c r="H149" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="J149" s="5" t="s">
+      <c r="J149" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="K149" s="5" t="s">
+      <c r="K149" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="M149" s="1" t="s">
+      <c r="M149" s="2" t="s">
         <v>16</v>
       </c>
       <c r="N149" s="1" t="s">
@@ -3360,14 +3380,14 @@
       <c r="D150" s="0" t="s">
         <v>19</v>
       </c>
-      <c r="E150" s="6" t="n">
+      <c r="E150" s="7" t="n">
         <f aca="false">C150-C144/2</f>
         <v>271</v>
       </c>
-      <c r="G150" s="4" t="n">
+      <c r="G150" s="5" t="n">
         <v>1</v>
       </c>
-      <c r="H150" s="4" t="n">
+      <c r="H150" s="5" t="n">
         <v>32</v>
       </c>
       <c r="J150" s="1" t="n">
@@ -3378,7 +3398,7 @@
         <f aca="false">$C$157+H150-$C$144/2-$E$150-50</f>
         <v>45</v>
       </c>
-      <c r="M150" s="1" t="n">
+      <c r="M150" s="2" t="n">
         <f aca="false">C143*0.001/(C143*0.001)</f>
         <v>1</v>
       </c>
@@ -3390,7 +3410,7 @@
         <f aca="false">1-((1+M150)*J162^2/J150^2)</f>
         <v>0.546246537396122</v>
       </c>
-      <c r="P150" s="6" t="n">
+      <c r="P150" s="7" t="n">
         <f aca="false">M150/(1+M150)</f>
         <v>0.5</v>
       </c>
@@ -3399,10 +3419,10 @@
       <c r="B151" s="0" t="s">
         <v>11</v>
       </c>
-      <c r="G151" s="4" t="n">
+      <c r="G151" s="5" t="n">
         <v>2</v>
       </c>
-      <c r="H151" s="4" t="n">
+      <c r="H151" s="5" t="n">
         <v>33</v>
       </c>
       <c r="K151" s="1" t="n">
@@ -3414,10 +3434,10 @@
       <c r="B152" s="0" t="s">
         <v>21</v>
       </c>
-      <c r="G152" s="4" t="n">
+      <c r="G152" s="5" t="n">
         <v>3</v>
       </c>
-      <c r="H152" s="4" t="n">
+      <c r="H152" s="5" t="n">
         <v>33</v>
       </c>
       <c r="K152" s="1" t="n">
@@ -3429,21 +3449,21 @@
       <c r="B153" s="0" t="s">
         <v>18</v>
       </c>
-      <c r="C153" s="6" t="n">
+      <c r="C153" s="7" t="n">
         <f aca="false">C150-C144</f>
         <v>245</v>
       </c>
       <c r="D153" s="0" t="s">
         <v>19</v>
       </c>
-      <c r="E153" s="6" t="n">
+      <c r="E153" s="7" t="n">
         <f aca="false">C153-C144/2</f>
         <v>219</v>
       </c>
-      <c r="G153" s="4" t="n">
+      <c r="G153" s="5" t="n">
         <v>4</v>
       </c>
-      <c r="H153" s="4" t="n">
+      <c r="H153" s="5" t="n">
         <v>32</v>
       </c>
       <c r="K153" s="1" t="n">
@@ -3455,17 +3475,17 @@
       <c r="B154" s="0" t="s">
         <v>22</v>
       </c>
-      <c r="G154" s="4" t="n">
+      <c r="G154" s="5" t="n">
         <v>5</v>
       </c>
-      <c r="H154" s="4" t="n">
+      <c r="H154" s="5" t="n">
         <v>31</v>
       </c>
       <c r="K154" s="1" t="n">
         <f aca="false">$C$157+H154-$C$144/2-$E$150-50</f>
         <v>44</v>
       </c>
-      <c r="M154" s="1" t="s">
+      <c r="M154" s="2" t="s">
         <v>23</v>
       </c>
     </row>
@@ -3479,30 +3499,30 @@
       <c r="D155" s="0" t="s">
         <v>19</v>
       </c>
-      <c r="E155" s="6" t="n">
+      <c r="E155" s="7" t="n">
         <f aca="false">C155-C144/2</f>
         <v>124</v>
       </c>
-      <c r="G155" s="4" t="n">
+      <c r="G155" s="5" t="n">
         <v>6</v>
       </c>
-      <c r="H155" s="4" t="n">
+      <c r="H155" s="5" t="n">
         <v>34.5</v>
       </c>
       <c r="K155" s="1" t="n">
         <f aca="false">$C$157+H155-$C$144/2-$E$150-50</f>
         <v>47.5</v>
       </c>
-      <c r="M155" s="7" t="n">
+      <c r="M155" s="8" t="n">
         <f aca="false">SQRT(4*(M150)^2*((J162*0.001)^4/(J150*0.001)^6*$M$4^2+ (J162*0.001)^2/(J150*0.001)^4*(L162*0.001)^2))</f>
         <v>0.0102916666352114</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="156">
-      <c r="G156" s="4" t="n">
+      <c r="G156" s="5" t="n">
         <v>7</v>
       </c>
-      <c r="H156" s="4" t="n">
+      <c r="H156" s="5" t="n">
         <v>31</v>
       </c>
       <c r="K156" s="1" t="n">
@@ -3514,13 +3534,13 @@
       <c r="B157" s="0" t="s">
         <v>24</v>
       </c>
-      <c r="C157" s="8" t="n">
+      <c r="C157" s="9" t="n">
         <v>360</v>
       </c>
-      <c r="G157" s="4" t="n">
+      <c r="G157" s="5" t="n">
         <v>8</v>
       </c>
-      <c r="H157" s="4" t="n">
+      <c r="H157" s="5" t="n">
         <v>31</v>
       </c>
       <c r="K157" s="1" t="n">
@@ -3529,10 +3549,10 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="158">
-      <c r="G158" s="4" t="n">
+      <c r="G158" s="5" t="n">
         <v>9</v>
       </c>
-      <c r="H158" s="4" t="n">
+      <c r="H158" s="5" t="n">
         <v>31.5</v>
       </c>
       <c r="K158" s="1" t="n">
@@ -3541,10 +3561,10 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="159">
-      <c r="G159" s="4" t="n">
+      <c r="G159" s="5" t="n">
         <v>10</v>
       </c>
-      <c r="H159" s="4" t="n">
+      <c r="H159" s="5" t="n">
         <v>33.5</v>
       </c>
       <c r="K159" s="1" t="n">
@@ -3556,25 +3576,25 @@
       <c r="B161" s="0" t="s">
         <v>0</v>
       </c>
-      <c r="J161" s="9" t="s">
+      <c r="J161" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="K161" s="9" t="s">
+      <c r="K161" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="L161" s="9" t="s">
+      <c r="L161" s="10" t="s">
         <v>27</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="162">
-      <c r="A162" s="2"/>
-      <c r="B162" s="2" t="s">
+      <c r="A162" s="3"/>
+      <c r="B162" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C162" s="2" t="s">
+      <c r="C162" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D162" s="2" t="s">
+      <c r="D162" s="3" t="s">
         <v>3</v>
       </c>
       <c r="J162" s="1" t="n">
@@ -3591,38 +3611,38 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="163">
-      <c r="A163" s="2" t="s">
+      <c r="A163" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B163" s="2" t="n">
+      <c r="B163" s="3" t="n">
         <v>233</v>
       </c>
-      <c r="C163" s="2" t="n">
+      <c r="C163" s="3" t="n">
         <v>540</v>
       </c>
-      <c r="D163" s="2" t="n">
+      <c r="D163" s="3" t="n">
         <v>1049</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="164">
-      <c r="A164" s="2" t="s">
+      <c r="A164" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B164" s="2" t="n">
+      <c r="B164" s="3" t="n">
         <v>38</v>
       </c>
-      <c r="C164" s="2" t="n">
+      <c r="C164" s="3" t="n">
         <v>52</v>
       </c>
-      <c r="D164" s="2" t="n">
+      <c r="D164" s="3" t="n">
         <v>65</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="168">
-      <c r="A168" s="3" t="s">
+      <c r="A168" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="B168" s="3" t="s">
+      <c r="B168" s="4" t="s">
         <v>7</v>
       </c>
     </row>
@@ -3630,19 +3650,19 @@
       <c r="B169" s="0" t="s">
         <v>32</v>
       </c>
-      <c r="G169" s="4" t="s">
+      <c r="G169" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="H169" s="4" t="s">
+      <c r="H169" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="J169" s="5" t="s">
+      <c r="J169" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="K169" s="5" t="s">
+      <c r="K169" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="M169" s="1" t="s">
+      <c r="M169" s="2" t="s">
         <v>16</v>
       </c>
       <c r="N169" s="1" t="s">
@@ -3659,14 +3679,14 @@
       <c r="D170" s="0" t="s">
         <v>19</v>
       </c>
-      <c r="E170" s="6" t="n">
+      <c r="E170" s="7" t="n">
         <f aca="false">C170-D164/2</f>
         <v>277</v>
       </c>
-      <c r="G170" s="4" t="n">
+      <c r="G170" s="5" t="n">
         <v>1</v>
       </c>
-      <c r="H170" s="4" t="n">
+      <c r="H170" s="5" t="n">
         <v>36</v>
       </c>
       <c r="J170" s="1" t="n">
@@ -3677,7 +3697,7 @@
         <f aca="false">$C$177+H170-$D$164/2-$E$170-50</f>
         <v>96.5</v>
       </c>
-      <c r="M170" s="1" t="n">
+      <c r="M170" s="2" t="n">
         <f aca="false">D163*0.001/(C163*0.001)</f>
         <v>1.94259259259259</v>
       </c>
@@ -3690,10 +3710,10 @@
       <c r="B171" s="0" t="s">
         <v>11</v>
       </c>
-      <c r="G171" s="4" t="n">
+      <c r="G171" s="5" t="n">
         <v>2</v>
       </c>
-      <c r="H171" s="4" t="n">
+      <c r="H171" s="5" t="n">
         <v>37</v>
       </c>
       <c r="K171" s="1" t="n">
@@ -3705,10 +3725,10 @@
       <c r="B172" s="0" t="s">
         <v>21</v>
       </c>
-      <c r="G172" s="4" t="n">
+      <c r="G172" s="5" t="n">
         <v>3</v>
       </c>
-      <c r="H172" s="4" t="n">
+      <c r="H172" s="5" t="n">
         <v>37</v>
       </c>
       <c r="K172" s="1" t="n">
@@ -3726,14 +3746,14 @@
       <c r="D173" s="0" t="s">
         <v>19</v>
       </c>
-      <c r="E173" s="6" t="n">
+      <c r="E173" s="7" t="n">
         <f aca="false">C173-C164/2</f>
         <v>220</v>
       </c>
-      <c r="G173" s="4" t="n">
+      <c r="G173" s="5" t="n">
         <v>4</v>
       </c>
-      <c r="H173" s="4" t="n">
+      <c r="H173" s="5" t="n">
         <v>36.5</v>
       </c>
       <c r="K173" s="1" t="n">
@@ -3745,17 +3765,17 @@
       <c r="B174" s="0" t="s">
         <v>22</v>
       </c>
-      <c r="G174" s="4" t="n">
+      <c r="G174" s="5" t="n">
         <v>5</v>
       </c>
-      <c r="H174" s="4" t="n">
+      <c r="H174" s="5" t="n">
         <v>36</v>
       </c>
       <c r="K174" s="1" t="n">
         <f aca="false">$C$177+H174-$D$164/2-$E$170-50</f>
         <v>96.5</v>
       </c>
-      <c r="M174" s="1" t="s">
+      <c r="M174" s="2" t="s">
         <v>23</v>
       </c>
     </row>
@@ -3769,30 +3789,30 @@
       <c r="D175" s="0" t="s">
         <v>19</v>
       </c>
-      <c r="E175" s="6" t="n">
+      <c r="E175" s="7" t="n">
         <f aca="false">C175-C164/2</f>
         <v>74</v>
       </c>
-      <c r="G175" s="4" t="n">
+      <c r="G175" s="5" t="n">
         <v>6</v>
       </c>
-      <c r="H175" s="4" t="n">
+      <c r="H175" s="5" t="n">
         <v>36</v>
       </c>
       <c r="K175" s="1" t="n">
         <f aca="false">$C$177+H175-$D$164/2-$E$170-50</f>
         <v>96.5</v>
       </c>
-      <c r="M175" s="7" t="n">
+      <c r="M175" s="8" t="n">
         <f aca="false">SQRT(4*(M170)^2*((J182*0.001)^4/(J170*0.001)^6*$M$4^2+ (J182*0.001)^2/(J170*0.001)^4*(L182*0.001)^2))</f>
         <v>0.0236538546592388</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="176">
-      <c r="G176" s="4" t="n">
+      <c r="G176" s="5" t="n">
         <v>7</v>
       </c>
-      <c r="H176" s="4" t="n">
+      <c r="H176" s="5" t="n">
         <v>36</v>
       </c>
       <c r="K176" s="1" t="n">
@@ -3804,13 +3824,13 @@
       <c r="B177" s="0" t="s">
         <v>24</v>
       </c>
-      <c r="C177" s="8" t="n">
+      <c r="C177" s="9" t="n">
         <v>420</v>
       </c>
-      <c r="G177" s="4" t="n">
+      <c r="G177" s="5" t="n">
         <v>8</v>
       </c>
-      <c r="H177" s="4" t="n">
+      <c r="H177" s="5" t="n">
         <v>34.5</v>
       </c>
       <c r="K177" s="1" t="n">
@@ -3819,10 +3839,10 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="178">
-      <c r="G178" s="4" t="n">
+      <c r="G178" s="5" t="n">
         <v>9</v>
       </c>
-      <c r="H178" s="4" t="n">
+      <c r="H178" s="5" t="n">
         <v>35</v>
       </c>
       <c r="K178" s="1" t="n">
@@ -3831,10 +3851,10 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="179">
-      <c r="G179" s="4" t="n">
+      <c r="G179" s="5" t="n">
         <v>10</v>
       </c>
-      <c r="H179" s="4" t="n">
+      <c r="H179" s="5" t="n">
         <v>36</v>
       </c>
       <c r="K179" s="1" t="n">
@@ -3846,25 +3866,25 @@
       <c r="B181" s="0" t="s">
         <v>0</v>
       </c>
-      <c r="J181" s="9" t="s">
+      <c r="J181" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="K181" s="9" t="s">
+      <c r="K181" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="L181" s="9" t="s">
+      <c r="L181" s="10" t="s">
         <v>27</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="182">
-      <c r="A182" s="2"/>
-      <c r="B182" s="2" t="s">
+      <c r="A182" s="3"/>
+      <c r="B182" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C182" s="2" t="s">
+      <c r="C182" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D182" s="2" t="s">
+      <c r="D182" s="3" t="s">
         <v>3</v>
       </c>
       <c r="J182" s="1" t="n">
@@ -3881,38 +3901,38 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="183">
-      <c r="A183" s="2" t="s">
+      <c r="A183" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B183" s="2" t="n">
+      <c r="B183" s="3" t="n">
         <v>233</v>
       </c>
-      <c r="C183" s="2" t="n">
+      <c r="C183" s="3" t="n">
         <v>540</v>
       </c>
-      <c r="D183" s="2" t="n">
+      <c r="D183" s="3" t="n">
         <v>1049</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="184">
-      <c r="A184" s="2" t="s">
+      <c r="A184" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B184" s="2" t="n">
+      <c r="B184" s="3" t="n">
         <v>38</v>
       </c>
-      <c r="C184" s="2" t="n">
+      <c r="C184" s="3" t="n">
         <v>52</v>
       </c>
-      <c r="D184" s="2" t="n">
+      <c r="D184" s="3" t="n">
         <v>65</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="188">
-      <c r="A188" s="3" t="s">
+      <c r="A188" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="B188" s="3" t="s">
+      <c r="B188" s="4" t="s">
         <v>28</v>
       </c>
     </row>
@@ -3920,19 +3940,19 @@
       <c r="B189" s="0" t="s">
         <v>32</v>
       </c>
-      <c r="G189" s="4" t="s">
+      <c r="G189" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="H189" s="4" t="s">
+      <c r="H189" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="J189" s="5" t="s">
+      <c r="J189" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="K189" s="5" t="s">
+      <c r="K189" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="M189" s="1" t="s">
+      <c r="M189" s="2" t="s">
         <v>16</v>
       </c>
       <c r="N189" s="1" t="s">
@@ -3949,14 +3969,14 @@
       <c r="D190" s="0" t="s">
         <v>19</v>
       </c>
-      <c r="E190" s="6" t="n">
+      <c r="E190" s="7" t="n">
         <f aca="false">C190-D184/2</f>
         <v>277</v>
       </c>
-      <c r="G190" s="4" t="n">
+      <c r="G190" s="5" t="n">
         <v>1</v>
       </c>
-      <c r="H190" s="4" t="n">
+      <c r="H190" s="5" t="n">
         <v>35</v>
       </c>
       <c r="J190" s="1" t="n">
@@ -3967,7 +3987,7 @@
         <f aca="false">$C$197+H190-$D$184/2-$E$190-50</f>
         <v>45.5</v>
       </c>
-      <c r="M190" s="1" t="n">
+      <c r="M190" s="2" t="n">
         <f aca="false">D183*0.001/(C183*0.001)</f>
         <v>1.94259259259259</v>
       </c>
@@ -3979,7 +3999,7 @@
         <f aca="false">1-((1+M190)*J202^2/J190^2)</f>
         <v>0.702151194677272</v>
       </c>
-      <c r="P190" s="6" t="n">
+      <c r="P190" s="7" t="n">
         <f aca="false">M190/(1+M190)</f>
         <v>0.660163624921334</v>
       </c>
@@ -3988,10 +4008,10 @@
       <c r="B191" s="0" t="s">
         <v>11</v>
       </c>
-      <c r="G191" s="4" t="n">
+      <c r="G191" s="5" t="n">
         <v>2</v>
       </c>
-      <c r="H191" s="4" t="n">
+      <c r="H191" s="5" t="n">
         <v>35</v>
       </c>
       <c r="K191" s="1" t="n">
@@ -4003,10 +4023,10 @@
       <c r="B192" s="0" t="s">
         <v>21</v>
       </c>
-      <c r="G192" s="4" t="n">
+      <c r="G192" s="5" t="n">
         <v>3</v>
       </c>
-      <c r="H192" s="4" t="n">
+      <c r="H192" s="5" t="n">
         <v>36</v>
       </c>
       <c r="K192" s="1" t="n">
@@ -4024,14 +4044,14 @@
       <c r="D193" s="0" t="s">
         <v>19</v>
       </c>
-      <c r="E193" s="6" t="n">
+      <c r="E193" s="7" t="n">
         <f aca="false">C193-C184/2</f>
         <v>220</v>
       </c>
-      <c r="G193" s="4" t="n">
+      <c r="G193" s="5" t="n">
         <v>4</v>
       </c>
-      <c r="H193" s="4" t="n">
+      <c r="H193" s="5" t="n">
         <v>38</v>
       </c>
       <c r="K193" s="1" t="n">
@@ -4043,17 +4063,17 @@
       <c r="B194" s="0" t="s">
         <v>22</v>
       </c>
-      <c r="G194" s="4" t="n">
+      <c r="G194" s="5" t="n">
         <v>5</v>
       </c>
-      <c r="H194" s="4" t="n">
+      <c r="H194" s="5" t="n">
         <v>35</v>
       </c>
       <c r="K194" s="1" t="n">
         <f aca="false">$C$197+H194-$D$184/2-$E$190-50</f>
         <v>45.5</v>
       </c>
-      <c r="M194" s="1" t="s">
+      <c r="M194" s="2" t="s">
         <v>23</v>
       </c>
     </row>
@@ -4067,30 +4087,30 @@
       <c r="D195" s="0" t="s">
         <v>19</v>
       </c>
-      <c r="E195" s="6" t="n">
+      <c r="E195" s="7" t="n">
         <f aca="false">C195-C184/2</f>
         <v>74</v>
       </c>
-      <c r="G195" s="4" t="n">
+      <c r="G195" s="5" t="n">
         <v>6</v>
       </c>
-      <c r="H195" s="4" t="n">
+      <c r="H195" s="5" t="n">
         <v>34</v>
       </c>
       <c r="K195" s="1" t="n">
         <f aca="false">$C$197+H195-$D$184/2-$E$190-50</f>
         <v>44.5</v>
       </c>
-      <c r="M195" s="7" t="n">
+      <c r="M195" s="8" t="n">
         <f aca="false">SQRT(4*(M190)^2*((J202*0.001)^4/(J190*0.001)^6*$M$4^2+ (J202*0.001)^2/(J190*0.001)^4*(L202*0.001)^2))</f>
         <v>0.00632072943940655</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="196">
-      <c r="G196" s="4" t="n">
+      <c r="G196" s="5" t="n">
         <v>7</v>
       </c>
-      <c r="H196" s="4" t="n">
+      <c r="H196" s="5" t="n">
         <v>37.5</v>
       </c>
       <c r="K196" s="1" t="n">
@@ -4102,13 +4122,13 @@
       <c r="B197" s="0" t="s">
         <v>24</v>
       </c>
-      <c r="C197" s="8" t="n">
+      <c r="C197" s="9" t="n">
         <v>370</v>
       </c>
-      <c r="G197" s="4" t="n">
+      <c r="G197" s="5" t="n">
         <v>8</v>
       </c>
-      <c r="H197" s="4" t="n">
+      <c r="H197" s="5" t="n">
         <v>36.5</v>
       </c>
       <c r="K197" s="1" t="n">
@@ -4117,10 +4137,10 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="198">
-      <c r="G198" s="4" t="n">
+      <c r="G198" s="5" t="n">
         <v>9</v>
       </c>
-      <c r="H198" s="4" t="n">
+      <c r="H198" s="5" t="n">
         <v>36</v>
       </c>
       <c r="K198" s="1" t="n">
@@ -4129,10 +4149,10 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="199">
-      <c r="G199" s="4" t="n">
+      <c r="G199" s="5" t="n">
         <v>10</v>
       </c>
-      <c r="H199" s="4" t="n">
+      <c r="H199" s="5" t="n">
         <v>36.5</v>
       </c>
       <c r="K199" s="1" t="n">
@@ -4144,25 +4164,25 @@
       <c r="B201" s="0" t="s">
         <v>0</v>
       </c>
-      <c r="J201" s="9" t="s">
+      <c r="J201" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="K201" s="9" t="s">
+      <c r="K201" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="L201" s="9" t="s">
+      <c r="L201" s="10" t="s">
         <v>27</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="202">
-      <c r="A202" s="2"/>
-      <c r="B202" s="2" t="s">
+      <c r="A202" s="3"/>
+      <c r="B202" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C202" s="2" t="s">
+      <c r="C202" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D202" s="2" t="s">
+      <c r="D202" s="3" t="s">
         <v>3</v>
       </c>
       <c r="J202" s="1" t="n">
@@ -4179,38 +4199,38 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="203">
-      <c r="A203" s="2" t="s">
+      <c r="A203" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B203" s="2" t="n">
+      <c r="B203" s="3" t="n">
         <v>233</v>
       </c>
-      <c r="C203" s="2" t="n">
+      <c r="C203" s="3" t="n">
         <v>540</v>
       </c>
-      <c r="D203" s="2" t="n">
+      <c r="D203" s="3" t="n">
         <v>1049</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="204">
-      <c r="A204" s="2" t="s">
+      <c r="A204" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B204" s="2" t="n">
+      <c r="B204" s="3" t="n">
         <v>38</v>
       </c>
-      <c r="C204" s="2" t="n">
+      <c r="C204" s="3" t="n">
         <v>52</v>
       </c>
-      <c r="D204" s="2" t="n">
+      <c r="D204" s="3" t="n">
         <v>65</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="208">
-      <c r="A208" s="3" t="s">
+      <c r="A208" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="B208" s="3" t="s">
+      <c r="B208" s="4" t="s">
         <v>7</v>
       </c>
     </row>
@@ -4218,19 +4238,19 @@
       <c r="B209" s="0" t="s">
         <v>11</v>
       </c>
-      <c r="G209" s="4" t="s">
+      <c r="G209" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="H209" s="4" t="s">
+      <c r="H209" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="J209" s="5" t="s">
+      <c r="J209" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="K209" s="5" t="s">
+      <c r="K209" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="M209" s="1" t="s">
+      <c r="M209" s="2" t="s">
         <v>16</v>
       </c>
       <c r="N209" s="1" t="s">
@@ -4247,14 +4267,14 @@
       <c r="D210" s="0" t="s">
         <v>19</v>
       </c>
-      <c r="E210" s="6" t="n">
+      <c r="E210" s="7" t="n">
         <f aca="false">C210-C204/2</f>
         <v>277.5</v>
       </c>
-      <c r="G210" s="4" t="n">
+      <c r="G210" s="5" t="n">
         <v>1</v>
       </c>
-      <c r="H210" s="4" t="n">
+      <c r="H210" s="5" t="n">
         <v>43</v>
       </c>
       <c r="J210" s="1" t="n">
@@ -4265,7 +4285,7 @@
         <f aca="false">$C$217+H210-$C$204/2-$E$210-50</f>
         <v>89.5</v>
       </c>
-      <c r="M210" s="1" t="n">
+      <c r="M210" s="2" t="n">
         <f aca="false">C203*0.001/(D203*0.001)</f>
         <v>0.514775977121068</v>
       </c>
@@ -4278,10 +4298,10 @@
       <c r="B211" s="0" t="s">
         <v>32</v>
       </c>
-      <c r="G211" s="4" t="n">
+      <c r="G211" s="5" t="n">
         <v>2</v>
       </c>
-      <c r="H211" s="4" t="n">
+      <c r="H211" s="5" t="n">
         <v>43</v>
       </c>
       <c r="K211" s="1" t="n">
@@ -4293,10 +4313,10 @@
       <c r="B212" s="0" t="s">
         <v>21</v>
       </c>
-      <c r="G212" s="4" t="n">
+      <c r="G212" s="5" t="n">
         <v>3</v>
       </c>
-      <c r="H212" s="4" t="n">
+      <c r="H212" s="5" t="n">
         <v>43</v>
       </c>
       <c r="K212" s="1" t="n">
@@ -4314,14 +4334,14 @@
       <c r="D213" s="0" t="s">
         <v>19</v>
       </c>
-      <c r="E213" s="6" t="n">
+      <c r="E213" s="7" t="n">
         <f aca="false">C213-D204/2</f>
         <v>220</v>
       </c>
-      <c r="G213" s="4" t="n">
+      <c r="G213" s="5" t="n">
         <v>4</v>
       </c>
-      <c r="H213" s="4" t="n">
+      <c r="H213" s="5" t="n">
         <v>43</v>
       </c>
       <c r="K213" s="1" t="n">
@@ -4333,17 +4353,17 @@
       <c r="B214" s="0" t="s">
         <v>22</v>
       </c>
-      <c r="G214" s="4" t="n">
+      <c r="G214" s="5" t="n">
         <v>5</v>
       </c>
-      <c r="H214" s="4" t="n">
+      <c r="H214" s="5" t="n">
         <v>43</v>
       </c>
       <c r="K214" s="1" t="n">
         <f aca="false">$C$217+H214-$C$204/2-$E$210-50</f>
         <v>89.5</v>
       </c>
-      <c r="M214" s="1" t="s">
+      <c r="M214" s="2" t="s">
         <v>23</v>
       </c>
     </row>
@@ -4357,30 +4377,30 @@
       <c r="D215" s="0" t="s">
         <v>19</v>
       </c>
-      <c r="E215" s="6" t="n">
+      <c r="E215" s="7" t="n">
         <f aca="false">C215-D204/2</f>
         <v>147.5</v>
       </c>
-      <c r="G215" s="4" t="n">
+      <c r="G215" s="5" t="n">
         <v>6</v>
       </c>
-      <c r="H215" s="4" t="n">
+      <c r="H215" s="5" t="n">
         <v>43</v>
       </c>
       <c r="K215" s="1" t="n">
         <f aca="false">$C$217+H215-$C$204/2-$E$210-50</f>
         <v>89.5</v>
       </c>
-      <c r="M215" s="7" t="n">
+      <c r="M215" s="8" t="n">
         <f aca="false">SQRT(4*(M210)^2*((J222*0.001)^4/(J210*0.001)^6*$M$4^2+ (J222*0.001)^2/(J210*0.001)^4*(L222*0.001)^2))</f>
         <v>0.0433948482615803</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="216">
-      <c r="G216" s="4" t="n">
+      <c r="G216" s="5" t="n">
         <v>7</v>
       </c>
-      <c r="H216" s="4" t="n">
+      <c r="H216" s="5" t="n">
         <v>43.5</v>
       </c>
       <c r="K216" s="1" t="n">
@@ -4392,13 +4412,13 @@
       <c r="B217" s="0" t="s">
         <v>24</v>
       </c>
-      <c r="C217" s="8" t="n">
+      <c r="C217" s="9" t="n">
         <v>400</v>
       </c>
-      <c r="G217" s="4" t="n">
+      <c r="G217" s="5" t="n">
         <v>8</v>
       </c>
-      <c r="H217" s="4" t="n">
+      <c r="H217" s="5" t="n">
         <v>43</v>
       </c>
       <c r="K217" s="1" t="n">
@@ -4407,10 +4427,10 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="218">
-      <c r="G218" s="4" t="n">
+      <c r="G218" s="5" t="n">
         <v>9</v>
       </c>
-      <c r="H218" s="4" t="n">
+      <c r="H218" s="5" t="n">
         <v>43.5</v>
       </c>
       <c r="K218" s="1" t="n">
@@ -4419,10 +4439,10 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="219">
-      <c r="G219" s="4" t="n">
+      <c r="G219" s="5" t="n">
         <v>10</v>
       </c>
-      <c r="H219" s="4" t="n">
+      <c r="H219" s="5" t="n">
         <v>43</v>
       </c>
       <c r="K219" s="1" t="n">
@@ -4434,25 +4454,25 @@
       <c r="B221" s="0" t="s">
         <v>0</v>
       </c>
-      <c r="J221" s="9" t="s">
+      <c r="J221" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="K221" s="9" t="s">
+      <c r="K221" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="L221" s="9" t="s">
+      <c r="L221" s="10" t="s">
         <v>27</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="222">
-      <c r="A222" s="2"/>
-      <c r="B222" s="2" t="s">
+      <c r="A222" s="3"/>
+      <c r="B222" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C222" s="2" t="s">
+      <c r="C222" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D222" s="2" t="s">
+      <c r="D222" s="3" t="s">
         <v>3</v>
       </c>
       <c r="J222" s="1" t="n">
@@ -4469,38 +4489,38 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="223">
-      <c r="A223" s="2" t="s">
+      <c r="A223" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B223" s="2" t="n">
+      <c r="B223" s="3" t="n">
         <v>233</v>
       </c>
-      <c r="C223" s="2" t="n">
+      <c r="C223" s="3" t="n">
         <v>540</v>
       </c>
-      <c r="D223" s="2" t="n">
+      <c r="D223" s="3" t="n">
         <v>1049</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="224">
-      <c r="A224" s="2" t="s">
+      <c r="A224" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B224" s="2" t="n">
+      <c r="B224" s="3" t="n">
         <v>38</v>
       </c>
-      <c r="C224" s="2" t="n">
+      <c r="C224" s="3" t="n">
         <v>52</v>
       </c>
-      <c r="D224" s="2" t="n">
+      <c r="D224" s="3" t="n">
         <v>65</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="228">
-      <c r="A228" s="3" t="s">
+      <c r="A228" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="B228" s="3" t="s">
+      <c r="B228" s="4" t="s">
         <v>28</v>
       </c>
     </row>
@@ -4508,19 +4528,19 @@
       <c r="B229" s="0" t="s">
         <v>11</v>
       </c>
-      <c r="G229" s="4" t="s">
+      <c r="G229" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="H229" s="4" t="s">
+      <c r="H229" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="J229" s="5" t="s">
+      <c r="J229" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="K229" s="5" t="s">
+      <c r="K229" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="M229" s="1" t="s">
+      <c r="M229" s="2" t="s">
         <v>16</v>
       </c>
       <c r="N229" s="1" t="s">
@@ -4537,14 +4557,14 @@
       <c r="D230" s="0" t="s">
         <v>19</v>
       </c>
-      <c r="E230" s="6" t="n">
+      <c r="E230" s="7" t="n">
         <f aca="false">C230-C224/2</f>
         <v>277.5</v>
       </c>
-      <c r="G230" s="4" t="n">
+      <c r="G230" s="5" t="n">
         <v>1</v>
       </c>
-      <c r="H230" s="4" t="n">
+      <c r="H230" s="5" t="n">
         <v>38</v>
       </c>
       <c r="J230" s="1" t="n">
@@ -4555,7 +4575,7 @@
         <f aca="false">$C$237+H230-$C$224/2-$E$230-50</f>
         <v>44.5</v>
       </c>
-      <c r="M230" s="1" t="n">
+      <c r="M230" s="2" t="n">
         <f aca="false">C223*0.001/(D223*0.001)</f>
         <v>0.514775977121068</v>
       </c>
@@ -4567,7 +4587,7 @@
         <f aca="false">1-((1+M230)*J242^2/J230^2)</f>
         <v>0.452170550969215</v>
       </c>
-      <c r="P230" s="6" t="n">
+      <c r="P230" s="7" t="n">
         <f aca="false">M230/(1+M230)</f>
         <v>0.339836375078666</v>
       </c>
@@ -4576,10 +4596,10 @@
       <c r="B231" s="0" t="s">
         <v>32</v>
       </c>
-      <c r="G231" s="4" t="n">
+      <c r="G231" s="5" t="n">
         <v>2</v>
       </c>
-      <c r="H231" s="4" t="n">
+      <c r="H231" s="5" t="n">
         <v>38.5</v>
       </c>
       <c r="K231" s="1" t="n">
@@ -4591,10 +4611,10 @@
       <c r="B232" s="0" t="s">
         <v>21</v>
       </c>
-      <c r="G232" s="4" t="n">
+      <c r="G232" s="5" t="n">
         <v>3</v>
       </c>
-      <c r="H232" s="4" t="n">
+      <c r="H232" s="5" t="n">
         <v>37</v>
       </c>
       <c r="K232" s="1" t="n">
@@ -4612,14 +4632,14 @@
       <c r="D233" s="0" t="s">
         <v>19</v>
       </c>
-      <c r="E233" s="6" t="n">
+      <c r="E233" s="7" t="n">
         <f aca="false">C233-D224/2</f>
         <v>220</v>
       </c>
-      <c r="G233" s="4" t="n">
+      <c r="G233" s="5" t="n">
         <v>4</v>
       </c>
-      <c r="H233" s="4" t="n">
+      <c r="H233" s="5" t="n">
         <v>37</v>
       </c>
       <c r="K233" s="1" t="n">
@@ -4631,17 +4651,17 @@
       <c r="B234" s="0" t="s">
         <v>22</v>
       </c>
-      <c r="G234" s="4" t="n">
+      <c r="G234" s="5" t="n">
         <v>5</v>
       </c>
-      <c r="H234" s="4" t="n">
+      <c r="H234" s="5" t="n">
         <v>37</v>
       </c>
       <c r="K234" s="1" t="n">
         <f aca="false">$C$237+H234-$C$224/2-$E$230-50</f>
         <v>43.5</v>
       </c>
-      <c r="M234" s="1" t="s">
+      <c r="M234" s="2" t="s">
         <v>23</v>
       </c>
     </row>
@@ -4655,30 +4675,30 @@
       <c r="D235" s="0" t="s">
         <v>19</v>
       </c>
-      <c r="E235" s="6" t="n">
+      <c r="E235" s="7" t="n">
         <f aca="false">C235-D224/2</f>
         <v>147.5</v>
       </c>
-      <c r="G235" s="4" t="n">
+      <c r="G235" s="5" t="n">
         <v>6</v>
       </c>
-      <c r="H235" s="4" t="n">
+      <c r="H235" s="5" t="n">
         <v>37</v>
       </c>
       <c r="K235" s="1" t="n">
         <f aca="false">$C$237+H235-$C$224/2-$E$230-50</f>
         <v>43.5</v>
       </c>
-      <c r="M235" s="7" t="n">
+      <c r="M235" s="8" t="n">
         <f aca="false">SQRT(4*(M230)^2*((J242*0.001)^4/(J230*0.001)^6*$M$4^2+ (J242*0.001)^2/(J230*0.001)^4*(L242*0.001)^2))</f>
         <v>0.0104824259653168</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="236">
-      <c r="G236" s="4" t="n">
+      <c r="G236" s="5" t="n">
         <v>7</v>
       </c>
-      <c r="H236" s="4" t="n">
+      <c r="H236" s="5" t="n">
         <v>36</v>
       </c>
       <c r="K236" s="1" t="n">
@@ -4690,13 +4710,13 @@
       <c r="B237" s="0" t="s">
         <v>24</v>
       </c>
-      <c r="C237" s="8" t="n">
+      <c r="C237" s="9" t="n">
         <v>360</v>
       </c>
-      <c r="G237" s="4" t="n">
+      <c r="G237" s="5" t="n">
         <v>8</v>
       </c>
-      <c r="H237" s="4" t="n">
+      <c r="H237" s="5" t="n">
         <v>37</v>
       </c>
       <c r="K237" s="1" t="n">
@@ -4705,10 +4725,10 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="238">
-      <c r="G238" s="4" t="n">
+      <c r="G238" s="5" t="n">
         <v>9</v>
       </c>
-      <c r="H238" s="4" t="n">
+      <c r="H238" s="5" t="n">
         <v>36</v>
       </c>
       <c r="K238" s="1" t="n">
@@ -4717,10 +4737,10 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="239">
-      <c r="G239" s="4" t="n">
+      <c r="G239" s="5" t="n">
         <v>10</v>
       </c>
-      <c r="H239" s="4" t="n">
+      <c r="H239" s="5" t="n">
         <v>37.5</v>
       </c>
       <c r="K239" s="1" t="n">
@@ -4732,25 +4752,25 @@
       <c r="B241" s="0" t="s">
         <v>0</v>
       </c>
-      <c r="J241" s="9" t="s">
+      <c r="J241" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="K241" s="9" t="s">
+      <c r="K241" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="L241" s="9" t="s">
+      <c r="L241" s="10" t="s">
         <v>27</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="242">
-      <c r="A242" s="2"/>
-      <c r="B242" s="2" t="s">
+      <c r="A242" s="3"/>
+      <c r="B242" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C242" s="2" t="s">
+      <c r="C242" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D242" s="2" t="s">
+      <c r="D242" s="3" t="s">
         <v>3</v>
       </c>
       <c r="J242" s="1" t="n">
@@ -4767,38 +4787,38 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="243">
-      <c r="A243" s="2" t="s">
+      <c r="A243" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B243" s="2" t="n">
+      <c r="B243" s="3" t="n">
         <v>233</v>
       </c>
-      <c r="C243" s="2" t="n">
+      <c r="C243" s="3" t="n">
         <v>540</v>
       </c>
-      <c r="D243" s="2" t="n">
+      <c r="D243" s="3" t="n">
         <v>1049</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="244">
-      <c r="A244" s="2" t="s">
+      <c r="A244" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B244" s="2" t="n">
+      <c r="B244" s="3" t="n">
         <v>38</v>
       </c>
-      <c r="C244" s="2" t="n">
+      <c r="C244" s="3" t="n">
         <v>52</v>
       </c>
-      <c r="D244" s="2" t="n">
+      <c r="D244" s="3" t="n">
         <v>65</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="248">
-      <c r="A248" s="3" t="s">
+      <c r="A248" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="B248" s="3" t="s">
+      <c r="B248" s="4" t="s">
         <v>7</v>
       </c>
     </row>
@@ -4806,19 +4826,19 @@
       <c r="B249" s="0" t="s">
         <v>20</v>
       </c>
-      <c r="G249" s="4" t="s">
+      <c r="G249" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="H249" s="4" t="s">
+      <c r="H249" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="J249" s="5" t="s">
+      <c r="J249" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="K249" s="5" t="s">
+      <c r="K249" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="M249" s="1" t="s">
+      <c r="M249" s="2" t="s">
         <v>16</v>
       </c>
       <c r="N249" s="1" t="s">
@@ -4835,14 +4855,14 @@
       <c r="D250" s="0" t="s">
         <v>19</v>
       </c>
-      <c r="E250" s="6" t="n">
+      <c r="E250" s="7" t="n">
         <f aca="false">C250-B244/2</f>
         <v>271.5</v>
       </c>
-      <c r="G250" s="4" t="n">
+      <c r="G250" s="5" t="n">
         <v>1</v>
       </c>
-      <c r="H250" s="4" t="n">
+      <c r="H250" s="5" t="n">
         <v>18</v>
       </c>
       <c r="J250" s="1" t="n">
@@ -4853,7 +4873,7 @@
         <f aca="false">$C$257+H250-$B$244/2-$E$250-50</f>
         <v>107.5</v>
       </c>
-      <c r="M250" s="1" t="n">
+      <c r="M250" s="2" t="n">
         <f aca="false">B243*0.001/(D243*0.001)</f>
         <v>0.222116301239276</v>
       </c>
@@ -4866,10 +4886,10 @@
       <c r="B251" s="0" t="s">
         <v>32</v>
       </c>
-      <c r="G251" s="4" t="n">
+      <c r="G251" s="5" t="n">
         <v>2</v>
       </c>
-      <c r="H251" s="4" t="n">
+      <c r="H251" s="5" t="n">
         <v>19</v>
       </c>
       <c r="K251" s="1" t="n">
@@ -4881,10 +4901,10 @@
       <c r="B252" s="0" t="s">
         <v>21</v>
       </c>
-      <c r="G252" s="4" t="n">
+      <c r="G252" s="5" t="n">
         <v>3</v>
       </c>
-      <c r="H252" s="4" t="n">
+      <c r="H252" s="5" t="n">
         <v>18.5</v>
       </c>
       <c r="K252" s="1" t="n">
@@ -4902,14 +4922,14 @@
       <c r="D253" s="0" t="s">
         <v>19</v>
       </c>
-      <c r="E253" s="6" t="n">
+      <c r="E253" s="7" t="n">
         <f aca="false">C253-D244/2</f>
         <v>220</v>
       </c>
-      <c r="G253" s="4" t="n">
+      <c r="G253" s="5" t="n">
         <v>4</v>
       </c>
-      <c r="H253" s="4" t="n">
+      <c r="H253" s="5" t="n">
         <v>20</v>
       </c>
       <c r="K253" s="1" t="n">
@@ -4921,17 +4941,17 @@
       <c r="B254" s="0" t="s">
         <v>22</v>
       </c>
-      <c r="G254" s="4" t="n">
+      <c r="G254" s="5" t="n">
         <v>5</v>
       </c>
-      <c r="H254" s="4" t="n">
+      <c r="H254" s="5" t="n">
         <v>20</v>
       </c>
       <c r="K254" s="1" t="n">
         <f aca="false">$C$257+H254-$B$244/2-$E$250-50</f>
         <v>109.5</v>
       </c>
-      <c r="M254" s="1" t="s">
+      <c r="M254" s="2" t="s">
         <v>23</v>
       </c>
     </row>
@@ -4945,30 +4965,30 @@
       <c r="D255" s="0" t="s">
         <v>19</v>
       </c>
-      <c r="E255" s="6" t="n">
+      <c r="E255" s="7" t="n">
         <f aca="false">C255-D244/2</f>
         <v>147.5</v>
       </c>
-      <c r="G255" s="4" t="n">
+      <c r="G255" s="5" t="n">
         <v>6</v>
       </c>
-      <c r="H255" s="4" t="n">
+      <c r="H255" s="5" t="n">
         <v>20</v>
       </c>
       <c r="K255" s="1" t="n">
         <f aca="false">$C$257+H255-$B$244/2-$E$250-50</f>
         <v>109.5</v>
       </c>
-      <c r="M255" s="7" t="n">
+      <c r="M255" s="8" t="n">
         <f aca="false">SQRT(4*(M250)^2*((J262*0.001)^4/(J250*0.001)^6*$M$4^2+ (J262*0.001)^2/(J250*0.001)^4*(L262*0.001)^2))</f>
         <v>0.0277769749049183</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="256">
-      <c r="G256" s="4" t="n">
+      <c r="G256" s="5" t="n">
         <v>7</v>
       </c>
-      <c r="H256" s="4" t="n">
+      <c r="H256" s="5" t="n">
         <v>21</v>
       </c>
       <c r="K256" s="1" t="n">
@@ -4980,13 +5000,13 @@
       <c r="B257" s="0" t="s">
         <v>24</v>
       </c>
-      <c r="C257" s="8" t="n">
+      <c r="C257" s="9" t="n">
         <v>430</v>
       </c>
-      <c r="G257" s="4" t="n">
+      <c r="G257" s="5" t="n">
         <v>8</v>
       </c>
-      <c r="H257" s="4" t="n">
+      <c r="H257" s="5" t="n">
         <v>18</v>
       </c>
       <c r="K257" s="1" t="n">
@@ -4995,10 +5015,10 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="258">
-      <c r="G258" s="4" t="n">
+      <c r="G258" s="5" t="n">
         <v>9</v>
       </c>
-      <c r="H258" s="4" t="n">
+      <c r="H258" s="5" t="n">
         <v>20</v>
       </c>
       <c r="K258" s="1" t="n">
@@ -5007,10 +5027,10 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="259">
-      <c r="G259" s="4" t="n">
+      <c r="G259" s="5" t="n">
         <v>10</v>
       </c>
-      <c r="H259" s="4" t="n">
+      <c r="H259" s="5" t="n">
         <v>19</v>
       </c>
       <c r="K259" s="1" t="n">
@@ -5022,25 +5042,25 @@
       <c r="B261" s="0" t="s">
         <v>0</v>
       </c>
-      <c r="J261" s="9" t="s">
+      <c r="J261" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="K261" s="9" t="s">
+      <c r="K261" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="L261" s="9" t="s">
+      <c r="L261" s="10" t="s">
         <v>27</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="262">
-      <c r="A262" s="2"/>
-      <c r="B262" s="2" t="s">
+      <c r="A262" s="3"/>
+      <c r="B262" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C262" s="2" t="s">
+      <c r="C262" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D262" s="2" t="s">
+      <c r="D262" s="3" t="s">
         <v>3</v>
       </c>
       <c r="J262" s="1" t="n">
@@ -5057,38 +5077,38 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="263">
-      <c r="A263" s="2" t="s">
+      <c r="A263" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B263" s="2" t="n">
+      <c r="B263" s="3" t="n">
         <v>233</v>
       </c>
-      <c r="C263" s="2" t="n">
+      <c r="C263" s="3" t="n">
         <v>540</v>
       </c>
-      <c r="D263" s="2" t="n">
+      <c r="D263" s="3" t="n">
         <v>1049</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="264">
-      <c r="A264" s="2" t="s">
+      <c r="A264" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B264" s="2" t="n">
+      <c r="B264" s="3" t="n">
         <v>38</v>
       </c>
-      <c r="C264" s="2" t="n">
+      <c r="C264" s="3" t="n">
         <v>52</v>
       </c>
-      <c r="D264" s="2" t="n">
+      <c r="D264" s="3" t="n">
         <v>65</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="268">
-      <c r="A268" s="3" t="s">
+      <c r="A268" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="B268" s="3" t="s">
+      <c r="B268" s="4" t="s">
         <v>28</v>
       </c>
     </row>
@@ -5096,19 +5116,19 @@
       <c r="B269" s="0" t="s">
         <v>20</v>
       </c>
-      <c r="G269" s="4" t="s">
+      <c r="G269" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="H269" s="4" t="s">
+      <c r="H269" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="J269" s="5" t="s">
+      <c r="J269" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="K269" s="5" t="s">
+      <c r="K269" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="M269" s="1" t="s">
+      <c r="M269" s="2" t="s">
         <v>16</v>
       </c>
       <c r="N269" s="1" t="s">
@@ -5125,14 +5145,14 @@
       <c r="D270" s="0" t="s">
         <v>19</v>
       </c>
-      <c r="E270" s="6" t="n">
+      <c r="E270" s="7" t="n">
         <f aca="false">C270-B264/2</f>
         <v>271.5</v>
       </c>
-      <c r="G270" s="4" t="n">
+      <c r="G270" s="5" t="n">
         <v>1</v>
       </c>
-      <c r="H270" s="4" t="n">
+      <c r="H270" s="5" t="n">
         <v>27</v>
       </c>
       <c r="J270" s="1" t="n">
@@ -5143,7 +5163,7 @@
         <f aca="false">$C$277+H270-$B$264/2-$E$270-50</f>
         <v>56.5</v>
       </c>
-      <c r="M270" s="1" t="n">
+      <c r="M270" s="2" t="n">
         <f aca="false">B263*0.001/(D263*0.001)</f>
         <v>0.222116301239276</v>
       </c>
@@ -5155,7 +5175,7 @@
         <f aca="false">1-((1+M270)*J282^2/J270^2)</f>
         <v>0.243258029786592</v>
       </c>
-      <c r="P270" s="6" t="n">
+      <c r="P270" s="7" t="n">
         <f aca="false">M270/(1+M270)</f>
         <v>0.181747269890796</v>
       </c>
@@ -5164,10 +5184,10 @@
       <c r="B271" s="0" t="s">
         <v>32</v>
       </c>
-      <c r="G271" s="4" t="n">
+      <c r="G271" s="5" t="n">
         <v>2</v>
       </c>
-      <c r="H271" s="4" t="n">
+      <c r="H271" s="5" t="n">
         <v>28</v>
       </c>
       <c r="K271" s="1" t="n">
@@ -5179,10 +5199,10 @@
       <c r="B272" s="0" t="s">
         <v>21</v>
       </c>
-      <c r="G272" s="4" t="n">
+      <c r="G272" s="5" t="n">
         <v>3</v>
       </c>
-      <c r="H272" s="4" t="n">
+      <c r="H272" s="5" t="n">
         <v>28</v>
       </c>
       <c r="K272" s="1" t="n">
@@ -5200,14 +5220,14 @@
       <c r="D273" s="0" t="s">
         <v>19</v>
       </c>
-      <c r="E273" s="6" t="n">
+      <c r="E273" s="7" t="n">
         <f aca="false">C273-D264/2</f>
         <v>220</v>
       </c>
-      <c r="G273" s="4" t="n">
+      <c r="G273" s="5" t="n">
         <v>4</v>
       </c>
-      <c r="H273" s="4" t="n">
+      <c r="H273" s="5" t="n">
         <v>28</v>
       </c>
       <c r="K273" s="1" t="n">
@@ -5219,17 +5239,17 @@
       <c r="B274" s="0" t="s">
         <v>22</v>
       </c>
-      <c r="G274" s="4" t="n">
+      <c r="G274" s="5" t="n">
         <v>5</v>
       </c>
-      <c r="H274" s="4" t="n">
+      <c r="H274" s="5" t="n">
         <v>27.5</v>
       </c>
       <c r="K274" s="1" t="n">
         <f aca="false">$C$277+H274-$B$264/2-$E$270-50</f>
         <v>57</v>
       </c>
-      <c r="M274" s="1" t="s">
+      <c r="M274" s="2" t="s">
         <v>23</v>
       </c>
     </row>
@@ -5243,30 +5263,30 @@
       <c r="D275" s="0" t="s">
         <v>19</v>
       </c>
-      <c r="E275" s="6" t="n">
+      <c r="E275" s="7" t="n">
         <f aca="false">C275-D264/2</f>
         <v>147.5</v>
       </c>
-      <c r="G275" s="4" t="n">
+      <c r="G275" s="5" t="n">
         <v>6</v>
       </c>
-      <c r="H275" s="4" t="n">
+      <c r="H275" s="5" t="n">
         <v>27.5</v>
       </c>
       <c r="K275" s="1" t="n">
         <f aca="false">$C$277+H275-$B$264/2-$E$270-50</f>
         <v>57</v>
       </c>
-      <c r="M275" s="7" t="n">
+      <c r="M275" s="8" t="n">
         <f aca="false">SQRT(4*(M270)^2*((J282*0.001)^4/(J270*0.001)^6*$M$4^2+ (J282*0.001)^2/(J270*0.001)^4*(L282*0.001)^2))</f>
         <v>0.00760900278849539</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="276">
-      <c r="G276" s="4" t="n">
+      <c r="G276" s="5" t="n">
         <v>7</v>
       </c>
-      <c r="H276" s="4" t="n">
+      <c r="H276" s="5" t="n">
         <v>27.5</v>
       </c>
       <c r="K276" s="1" t="n">
@@ -5278,13 +5298,13 @@
       <c r="B277" s="0" t="s">
         <v>24</v>
       </c>
-      <c r="C277" s="8" t="n">
+      <c r="C277" s="9" t="n">
         <v>370</v>
       </c>
-      <c r="G277" s="4" t="n">
+      <c r="G277" s="5" t="n">
         <v>8</v>
       </c>
-      <c r="H277" s="4" t="n">
+      <c r="H277" s="5" t="n">
         <v>27.5</v>
       </c>
       <c r="K277" s="1" t="n">
@@ -5293,10 +5313,10 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="278">
-      <c r="G278" s="4" t="n">
+      <c r="G278" s="5" t="n">
         <v>9</v>
       </c>
-      <c r="H278" s="4" t="n">
+      <c r="H278" s="5" t="n">
         <v>27</v>
       </c>
       <c r="K278" s="1" t="n">
@@ -5305,10 +5325,10 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="279">
-      <c r="G279" s="4" t="n">
+      <c r="G279" s="5" t="n">
         <v>10</v>
       </c>
-      <c r="H279" s="4" t="n">
+      <c r="H279" s="5" t="n">
         <v>27.5</v>
       </c>
       <c r="K279" s="1" t="n">
@@ -5317,13 +5337,13 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="281">
-      <c r="J281" s="9" t="s">
+      <c r="J281" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="K281" s="9" t="s">
+      <c r="K281" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="L281" s="9" t="s">
+      <c r="L281" s="10" t="s">
         <v>27</v>
       </c>
     </row>
@@ -5360,7 +5380,7 @@
   </sheetPr>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="55" zoomScaleNormal="55" zoomScalePageLayoutView="100">
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100">
       <selection activeCell="A1" activeCellId="0" pane="topLeft" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -5386,7 +5406,7 @@
   </sheetPr>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="55" zoomScaleNormal="55" zoomScalePageLayoutView="100">
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100">
       <selection activeCell="A1" activeCellId="0" pane="topLeft" sqref="A1"/>
     </sheetView>
   </sheetViews>

</xml_diff>